<commit_message>
Incremento de coluna e alteração da nulidade das colunas null
</commit_message>
<xml_diff>
--- a/Dicionário/Dicionario_de_dados.xlsx
+++ b/Dicionário/Dicionario_de_dados.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luigi\Desktop\Faculdade\3 FASE\Banco de Dados II\ABP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD6B0A5D-396B-4508-9009-1DAB780EB1B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C94E3850-052B-4E8A-9895-BA4A3509F73F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5205" yWindow="2685" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5340" yWindow="2460" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dicionario" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="177">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -85,9 +85,6 @@
   </si>
   <si>
     <t>0 -&gt; 1</t>
-  </si>
-  <si>
-    <t>Conta "Ativa"(1) ou "Inativa"(1)</t>
   </si>
   <si>
     <t>nome</t>
@@ -243,9 +240,6 @@
     <t>saldo_dolar</t>
   </si>
   <si>
-    <t>Null</t>
-  </si>
-  <si>
     <t>Saldo da conta em Dólar, para quando o cliente realizar um Cambio.</t>
   </si>
   <si>
@@ -397,9 +391,6 @@
   </si>
   <si>
     <t>taxa_juros</t>
-  </si>
-  <si>
-    <t>tinyint</t>
   </si>
   <si>
     <t>0 -&gt; 255</t>
@@ -559,6 +550,12 @@
   </si>
   <si>
     <t>pk_Fatura</t>
+  </si>
+  <si>
+    <t>Empréstimo "Ativo"(1) ou "Inativo"(0)</t>
+  </si>
+  <si>
+    <t>Conta "Ativa"(1) ou "Inativa"(0)</t>
   </si>
 </sst>
 </file>
@@ -1107,7 +1104,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="77">
+  <cellXfs count="78">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1195,87 +1192,6 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1284,6 +1200,90 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1500,9 +1500,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z1003"/>
+  <dimension ref="A1:Z1004"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A68" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
@@ -1519,15 +1519,15 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="54" t="s">
+      <c r="B1" s="72" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
-      <c r="G1" s="36"/>
-      <c r="H1" s="37"/>
+      <c r="C1" s="52"/>
+      <c r="D1" s="52"/>
+      <c r="E1" s="52"/>
+      <c r="F1" s="52"/>
+      <c r="G1" s="52"/>
+      <c r="H1" s="53"/>
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
       <c r="K1" s="2"/>
@@ -1551,15 +1551,15 @@
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="41" t="s">
+      <c r="B2" s="66" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="36"/>
-      <c r="D2" s="36"/>
-      <c r="E2" s="36"/>
-      <c r="F2" s="36"/>
-      <c r="G2" s="36"/>
-      <c r="H2" s="37"/>
+      <c r="C2" s="52"/>
+      <c r="D2" s="52"/>
+      <c r="E2" s="52"/>
+      <c r="F2" s="52"/>
+      <c r="G2" s="52"/>
+      <c r="H2" s="53"/>
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
@@ -1580,16 +1580,16 @@
       <c r="Z2" s="2"/>
     </row>
     <row r="3" spans="1:26">
-      <c r="A3" s="42" t="s">
+      <c r="A3" s="54" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="36"/>
-      <c r="C3" s="36"/>
-      <c r="D3" s="36"/>
-      <c r="E3" s="36"/>
-      <c r="F3" s="36"/>
-      <c r="G3" s="36"/>
-      <c r="H3" s="37"/>
+      <c r="B3" s="52"/>
+      <c r="C3" s="52"/>
+      <c r="D3" s="52"/>
+      <c r="E3" s="52"/>
+      <c r="F3" s="52"/>
+      <c r="G3" s="52"/>
+      <c r="H3" s="53"/>
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
@@ -1610,10 +1610,10 @@
       <c r="Z3" s="2"/>
     </row>
     <row r="4" spans="1:26">
-      <c r="A4" s="43" t="s">
+      <c r="A4" s="51" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="44"/>
+      <c r="B4" s="43"/>
       <c r="C4" s="1" t="s">
         <v>6</v>
       </c>
@@ -1652,10 +1652,10 @@
       <c r="Z4" s="2"/>
     </row>
     <row r="5" spans="1:26">
-      <c r="A5" s="45" t="s">
+      <c r="A5" s="42" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="44"/>
+      <c r="B5" s="43"/>
       <c r="C5" s="4" t="s">
         <v>12</v>
       </c>
@@ -1692,10 +1692,10 @@
       <c r="Z5" s="2"/>
     </row>
     <row r="6" spans="1:26">
-      <c r="A6" s="45" t="s">
+      <c r="A6" s="42" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="44"/>
+      <c r="B6" s="43"/>
       <c r="C6" s="4" t="s">
         <v>18</v>
       </c>
@@ -1708,7 +1708,7 @@
       <c r="F6" s="5"/>
       <c r="G6" s="5"/>
       <c r="H6" s="6" t="s">
-        <v>20</v>
+        <v>176</v>
       </c>
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
@@ -1730,15 +1730,15 @@
       <c r="Z6" s="2"/>
     </row>
     <row r="7" spans="1:26">
-      <c r="A7" s="45" t="s">
+      <c r="A7" s="42" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="43"/>
+      <c r="C7" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="44"/>
-      <c r="C7" s="4" t="s">
+      <c r="D7" s="4" t="s">
         <v>22</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>23</v>
       </c>
       <c r="E7" s="4" t="s">
         <v>14</v>
@@ -1746,7 +1746,7 @@
       <c r="F7" s="5"/>
       <c r="G7" s="5"/>
       <c r="H7" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
@@ -1768,15 +1768,15 @@
       <c r="Z7" s="2"/>
     </row>
     <row r="8" spans="1:26">
-      <c r="A8" s="45" t="s">
+      <c r="A8" s="42" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="43"/>
+      <c r="C8" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B8" s="44"/>
-      <c r="C8" s="4" t="s">
+      <c r="D8" s="7" t="s">
         <v>26</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>27</v>
       </c>
       <c r="E8" s="4" t="s">
         <v>14</v>
@@ -1784,7 +1784,7 @@
       <c r="F8" s="5"/>
       <c r="G8" s="5"/>
       <c r="H8" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
@@ -1806,15 +1806,15 @@
       <c r="Z8" s="2"/>
     </row>
     <row r="9" spans="1:26">
-      <c r="A9" s="45" t="s">
+      <c r="A9" s="42" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" s="43"/>
+      <c r="C9" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B9" s="44"/>
-      <c r="C9" s="4" t="s">
+      <c r="D9" s="4" t="s">
         <v>30</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>31</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>14</v>
@@ -1822,7 +1822,7 @@
       <c r="F9" s="5"/>
       <c r="G9" s="5"/>
       <c r="H9" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
@@ -1844,15 +1844,15 @@
       <c r="Z9" s="2"/>
     </row>
     <row r="10" spans="1:26">
-      <c r="A10" s="45" t="s">
+      <c r="A10" s="42" t="s">
+        <v>32</v>
+      </c>
+      <c r="B10" s="43"/>
+      <c r="C10" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B10" s="44"/>
-      <c r="C10" s="4" t="s">
+      <c r="D10" s="4" t="s">
         <v>34</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>35</v>
       </c>
       <c r="E10" s="4" t="s">
         <v>14</v>
@@ -1860,7 +1860,7 @@
       <c r="F10" s="5"/>
       <c r="G10" s="5"/>
       <c r="H10" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
@@ -1882,12 +1882,12 @@
       <c r="Z10" s="2"/>
     </row>
     <row r="11" spans="1:26">
-      <c r="A11" s="58" t="s">
+      <c r="A11" s="68" t="s">
+        <v>36</v>
+      </c>
+      <c r="B11" s="43"/>
+      <c r="C11" s="8" t="s">
         <v>37</v>
-      </c>
-      <c r="B11" s="44"/>
-      <c r="C11" s="8" t="s">
-        <v>38</v>
       </c>
       <c r="D11" s="8" t="s">
         <v>13</v>
@@ -1898,7 +1898,7 @@
       <c r="F11" s="9"/>
       <c r="G11" s="9"/>
       <c r="H11" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
@@ -1920,15 +1920,15 @@
       <c r="Z11" s="2"/>
     </row>
     <row r="12" spans="1:26">
-      <c r="A12" s="58" t="s">
-        <v>40</v>
-      </c>
-      <c r="B12" s="44"/>
+      <c r="A12" s="68" t="s">
+        <v>39</v>
+      </c>
+      <c r="B12" s="43"/>
       <c r="C12" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12" s="8" t="s">
         <v>22</v>
-      </c>
-      <c r="D12" s="8" t="s">
-        <v>23</v>
       </c>
       <c r="E12" s="4" t="s">
         <v>14</v>
@@ -1936,7 +1936,7 @@
       <c r="F12" s="9"/>
       <c r="G12" s="9"/>
       <c r="H12" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
@@ -1958,15 +1958,15 @@
       <c r="Z12" s="2"/>
     </row>
     <row r="13" spans="1:26">
-      <c r="A13" s="58" t="s">
+      <c r="A13" s="68" t="s">
+        <v>41</v>
+      </c>
+      <c r="B13" s="43"/>
+      <c r="C13" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="B13" s="44"/>
-      <c r="C13" s="8" t="s">
+      <c r="D13" s="8" t="s">
         <v>43</v>
-      </c>
-      <c r="D13" s="8" t="s">
-        <v>44</v>
       </c>
       <c r="E13" s="4" t="s">
         <v>14</v>
@@ -1974,7 +1974,7 @@
       <c r="F13" s="9"/>
       <c r="G13" s="9"/>
       <c r="H13" s="10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
@@ -1996,15 +1996,15 @@
       <c r="Z13" s="2"/>
     </row>
     <row r="14" spans="1:26">
-      <c r="A14" s="46" t="s">
-        <v>46</v>
+      <c r="A14" s="73" t="s">
+        <v>45</v>
       </c>
       <c r="B14" s="47"/>
       <c r="C14" s="11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D14" s="11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E14" s="12" t="s">
         <v>14</v>
@@ -2012,7 +2012,7 @@
       <c r="F14" s="13"/>
       <c r="G14" s="13"/>
       <c r="H14" s="14" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
@@ -2034,16 +2034,16 @@
       <c r="Z14" s="2"/>
     </row>
     <row r="15" spans="1:26" ht="15" customHeight="1">
-      <c r="A15" s="48" t="s">
-        <v>49</v>
-      </c>
-      <c r="B15" s="49"/>
-      <c r="C15" s="49"/>
-      <c r="D15" s="49"/>
-      <c r="E15" s="49"/>
-      <c r="F15" s="49"/>
-      <c r="G15" s="49"/>
-      <c r="H15" s="50"/>
+      <c r="A15" s="74" t="s">
+        <v>48</v>
+      </c>
+      <c r="B15" s="75"/>
+      <c r="C15" s="75"/>
+      <c r="D15" s="75"/>
+      <c r="E15" s="75"/>
+      <c r="F15" s="75"/>
+      <c r="G15" s="75"/>
+      <c r="H15" s="76"/>
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
       <c r="K15" s="2"/>
@@ -2064,24 +2064,24 @@
       <c r="Z15" s="2"/>
     </row>
     <row r="16" spans="1:26" ht="15" customHeight="1">
-      <c r="A16" s="43" t="s">
+      <c r="A16" s="51" t="s">
+        <v>49</v>
+      </c>
+      <c r="B16" s="43"/>
+      <c r="C16" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B16" s="44"/>
-      <c r="C16" s="1" t="s">
+      <c r="D16" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="E16" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="E16" s="1" t="s">
+      <c r="F16" s="51" t="s">
         <v>53</v>
       </c>
-      <c r="F16" s="43" t="s">
-        <v>54</v>
-      </c>
-      <c r="G16" s="36"/>
-      <c r="H16" s="37"/>
+      <c r="G16" s="52"/>
+      <c r="H16" s="53"/>
       <c r="I16" s="2"/>
       <c r="J16" s="2"/>
       <c r="K16" s="2"/>
@@ -2102,10 +2102,10 @@
       <c r="Z16" s="2"/>
     </row>
     <row r="17" spans="1:26">
-      <c r="A17" s="35" t="s">
-        <v>55</v>
-      </c>
-      <c r="B17" s="44"/>
+      <c r="A17" s="44" t="s">
+        <v>54</v>
+      </c>
+      <c r="B17" s="43"/>
       <c r="C17" s="15" t="s">
         <v>15</v>
       </c>
@@ -2113,11 +2113,11 @@
       <c r="E17" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="F17" s="35" t="s">
+      <c r="F17" s="44" t="s">
         <v>11</v>
       </c>
-      <c r="G17" s="36"/>
-      <c r="H17" s="37"/>
+      <c r="G17" s="52"/>
+      <c r="H17" s="53"/>
       <c r="I17" s="2"/>
       <c r="J17" s="2"/>
       <c r="K17" s="2"/>
@@ -2138,10 +2138,10 @@
       <c r="Z17" s="2"/>
     </row>
     <row r="18" spans="1:26">
-      <c r="A18" s="35" t="s">
-        <v>56</v>
-      </c>
-      <c r="B18" s="44"/>
+      <c r="A18" s="44" t="s">
+        <v>55</v>
+      </c>
+      <c r="B18" s="43"/>
       <c r="C18" s="15"/>
       <c r="D18" s="15" t="s">
         <v>15</v>
@@ -2149,11 +2149,11 @@
       <c r="E18" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="F18" s="35" t="s">
-        <v>25</v>
-      </c>
-      <c r="G18" s="36"/>
-      <c r="H18" s="37"/>
+      <c r="F18" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="G18" s="52"/>
+      <c r="H18" s="53"/>
       <c r="I18" s="2"/>
       <c r="J18" s="2"/>
       <c r="K18" s="2"/>
@@ -2174,10 +2174,10 @@
       <c r="Z18" s="2"/>
     </row>
     <row r="19" spans="1:26">
-      <c r="A19" s="55" t="s">
-        <v>57</v>
-      </c>
-      <c r="B19" s="44"/>
+      <c r="A19" s="70" t="s">
+        <v>56</v>
+      </c>
+      <c r="B19" s="43"/>
       <c r="C19" s="15"/>
       <c r="D19" s="15" t="s">
         <v>15</v>
@@ -2185,11 +2185,11 @@
       <c r="E19" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="F19" s="55" t="s">
-        <v>40</v>
-      </c>
-      <c r="G19" s="36"/>
-      <c r="H19" s="37"/>
+      <c r="F19" s="70" t="s">
+        <v>39</v>
+      </c>
+      <c r="G19" s="52"/>
+      <c r="H19" s="53"/>
       <c r="I19" s="2"/>
       <c r="J19" s="2"/>
       <c r="K19" s="2"/>
@@ -2210,10 +2210,10 @@
       <c r="Z19" s="2"/>
     </row>
     <row r="20" spans="1:26">
-      <c r="A20" s="56" t="s">
-        <v>58</v>
-      </c>
-      <c r="B20" s="57"/>
+      <c r="A20" s="71" t="s">
+        <v>57</v>
+      </c>
+      <c r="B20" s="39"/>
       <c r="C20" s="17"/>
       <c r="D20" s="18" t="s">
         <v>15</v>
@@ -2221,11 +2221,11 @@
       <c r="E20" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="F20" s="56" t="s">
-        <v>33</v>
-      </c>
-      <c r="G20" s="59"/>
-      <c r="H20" s="60"/>
+      <c r="F20" s="71" t="s">
+        <v>32</v>
+      </c>
+      <c r="G20" s="40"/>
+      <c r="H20" s="41"/>
       <c r="I20" s="2"/>
       <c r="J20" s="2"/>
       <c r="K20" s="2"/>
@@ -2275,17 +2275,17 @@
     </row>
     <row r="22" spans="1:26" ht="15.75" customHeight="1">
       <c r="A22" s="20" t="s">
+        <v>58</v>
+      </c>
+      <c r="B22" s="61" t="s">
         <v>59</v>
       </c>
-      <c r="B22" s="38" t="s">
-        <v>60</v>
-      </c>
-      <c r="C22" s="39"/>
-      <c r="D22" s="39"/>
-      <c r="E22" s="39"/>
-      <c r="F22" s="39"/>
-      <c r="G22" s="39"/>
-      <c r="H22" s="40"/>
+      <c r="C22" s="62"/>
+      <c r="D22" s="62"/>
+      <c r="E22" s="62"/>
+      <c r="F22" s="62"/>
+      <c r="G22" s="62"/>
+      <c r="H22" s="63"/>
       <c r="I22" s="2"/>
       <c r="J22" s="2"/>
       <c r="K22" s="2"/>
@@ -2309,15 +2309,15 @@
       <c r="A23" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B23" s="41" t="s">
-        <v>61</v>
-      </c>
-      <c r="C23" s="36"/>
-      <c r="D23" s="36"/>
-      <c r="E23" s="36"/>
-      <c r="F23" s="36"/>
-      <c r="G23" s="36"/>
-      <c r="H23" s="37"/>
+      <c r="B23" s="66" t="s">
+        <v>60</v>
+      </c>
+      <c r="C23" s="52"/>
+      <c r="D23" s="52"/>
+      <c r="E23" s="52"/>
+      <c r="F23" s="52"/>
+      <c r="G23" s="52"/>
+      <c r="H23" s="53"/>
       <c r="I23" s="2"/>
       <c r="J23" s="2"/>
       <c r="K23" s="2"/>
@@ -2338,16 +2338,16 @@
       <c r="Z23" s="2"/>
     </row>
     <row r="24" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A24" s="42" t="s">
+      <c r="A24" s="54" t="s">
         <v>4</v>
       </c>
-      <c r="B24" s="36"/>
-      <c r="C24" s="36"/>
-      <c r="D24" s="36"/>
-      <c r="E24" s="36"/>
-      <c r="F24" s="36"/>
-      <c r="G24" s="36"/>
-      <c r="H24" s="37"/>
+      <c r="B24" s="52"/>
+      <c r="C24" s="52"/>
+      <c r="D24" s="52"/>
+      <c r="E24" s="52"/>
+      <c r="F24" s="52"/>
+      <c r="G24" s="52"/>
+      <c r="H24" s="53"/>
       <c r="I24" s="2"/>
       <c r="J24" s="2"/>
       <c r="K24" s="2"/>
@@ -2368,10 +2368,10 @@
       <c r="Z24" s="2"/>
     </row>
     <row r="25" spans="1:26" ht="15" customHeight="1">
-      <c r="A25" s="43" t="s">
+      <c r="A25" s="51" t="s">
         <v>5</v>
       </c>
-      <c r="B25" s="44"/>
+      <c r="B25" s="43"/>
       <c r="C25" s="1" t="s">
         <v>6</v>
       </c>
@@ -2410,10 +2410,10 @@
       <c r="Z25" s="2"/>
     </row>
     <row r="26" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A26" s="45" t="s">
-        <v>62</v>
-      </c>
-      <c r="B26" s="44"/>
+      <c r="A26" s="42" t="s">
+        <v>61</v>
+      </c>
+      <c r="B26" s="43"/>
       <c r="C26" s="4" t="s">
         <v>12</v>
       </c>
@@ -2428,7 +2428,7 @@
       </c>
       <c r="G26" s="5"/>
       <c r="H26" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="I26" s="2"/>
       <c r="J26" s="2"/>
@@ -2450,10 +2450,10 @@
       <c r="Z26" s="2"/>
     </row>
     <row r="27" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A27" s="45" t="s">
+      <c r="A27" s="42" t="s">
         <v>11</v>
       </c>
-      <c r="B27" s="44"/>
+      <c r="B27" s="43"/>
       <c r="C27" s="4" t="s">
         <v>12</v>
       </c>
@@ -2468,7 +2468,7 @@
         <v>15</v>
       </c>
       <c r="H27" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I27" s="2"/>
       <c r="J27" s="2"/>
@@ -2490,15 +2490,15 @@
       <c r="Z27" s="2"/>
     </row>
     <row r="28" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A28" s="45" t="s">
-        <v>65</v>
-      </c>
-      <c r="B28" s="44"/>
+      <c r="A28" s="42" t="s">
+        <v>64</v>
+      </c>
+      <c r="B28" s="43"/>
       <c r="C28" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D28" s="4" t="s">
         <v>43</v>
-      </c>
-      <c r="D28" s="4" t="s">
-        <v>44</v>
       </c>
       <c r="E28" s="4" t="s">
         <v>14</v>
@@ -2506,7 +2506,7 @@
       <c r="F28" s="21"/>
       <c r="G28" s="5"/>
       <c r="H28" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I28" s="2"/>
       <c r="J28" s="2"/>
@@ -2528,15 +2528,15 @@
       <c r="Z28" s="2"/>
     </row>
     <row r="29" spans="1:26" ht="15" customHeight="1">
-      <c r="A29" s="45" t="s">
+      <c r="A29" s="42" t="s">
+        <v>66</v>
+      </c>
+      <c r="B29" s="43"/>
+      <c r="C29" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="B29" s="44"/>
-      <c r="C29" s="4" t="s">
+      <c r="D29" s="4" t="s">
         <v>68</v>
-      </c>
-      <c r="D29" s="4" t="s">
-        <v>69</v>
       </c>
       <c r="E29" s="4" t="s">
         <v>14</v>
@@ -2544,7 +2544,7 @@
       <c r="F29" s="21"/>
       <c r="G29" s="5"/>
       <c r="H29" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I29" s="2"/>
       <c r="J29" s="2"/>
@@ -2566,23 +2566,23 @@
       <c r="Z29" s="2"/>
     </row>
     <row r="30" spans="1:26" ht="15" customHeight="1">
-      <c r="A30" s="45" t="s">
-        <v>71</v>
-      </c>
-      <c r="B30" s="44"/>
+      <c r="A30" s="42" t="s">
+        <v>70</v>
+      </c>
+      <c r="B30" s="43"/>
       <c r="C30" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="D30" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="D30" s="4" t="s">
-        <v>69</v>
-      </c>
       <c r="E30" s="4" t="s">
-        <v>72</v>
+        <v>14</v>
       </c>
       <c r="F30" s="21"/>
       <c r="G30" s="5"/>
       <c r="H30" s="6" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="I30" s="2"/>
       <c r="J30" s="2"/>
@@ -2604,23 +2604,23 @@
       <c r="Z30" s="2"/>
     </row>
     <row r="31" spans="1:26" ht="15" customHeight="1">
-      <c r="A31" s="45" t="s">
-        <v>74</v>
-      </c>
-      <c r="B31" s="44"/>
+      <c r="A31" s="42" t="s">
+        <v>72</v>
+      </c>
+      <c r="B31" s="43"/>
       <c r="C31" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="D31" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="D31" s="4" t="s">
-        <v>69</v>
-      </c>
       <c r="E31" s="4" t="s">
-        <v>72</v>
+        <v>14</v>
       </c>
       <c r="F31" s="21"/>
       <c r="G31" s="5"/>
       <c r="H31" s="6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="I31" s="2"/>
       <c r="J31" s="2"/>
@@ -2642,15 +2642,15 @@
       <c r="Z31" s="2"/>
     </row>
     <row r="32" spans="1:26" ht="15" customHeight="1">
-      <c r="A32" s="58" t="s">
-        <v>76</v>
-      </c>
-      <c r="B32" s="44"/>
+      <c r="A32" s="68" t="s">
+        <v>74</v>
+      </c>
+      <c r="B32" s="43"/>
       <c r="C32" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="D32" s="4" t="s">
         <v>68</v>
-      </c>
-      <c r="D32" s="4" t="s">
-        <v>69</v>
       </c>
       <c r="E32" s="4" t="s">
         <v>14</v>
@@ -2658,7 +2658,7 @@
       <c r="F32" s="9"/>
       <c r="G32" s="22"/>
       <c r="H32" s="10" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="I32" s="2"/>
       <c r="J32" s="2"/>
@@ -2680,15 +2680,15 @@
       <c r="Z32" s="2"/>
     </row>
     <row r="33" spans="1:26" ht="15" customHeight="1">
-      <c r="A33" s="61" t="s">
-        <v>78</v>
-      </c>
-      <c r="B33" s="57"/>
+      <c r="A33" s="69" t="s">
+        <v>76</v>
+      </c>
+      <c r="B33" s="39"/>
       <c r="C33" s="23" t="s">
+        <v>67</v>
+      </c>
+      <c r="D33" s="23" t="s">
         <v>68</v>
-      </c>
-      <c r="D33" s="23" t="s">
-        <v>69</v>
       </c>
       <c r="E33" s="23" t="s">
         <v>14</v>
@@ -2696,7 +2696,7 @@
       <c r="F33" s="24"/>
       <c r="G33" s="25"/>
       <c r="H33" s="26" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="I33" s="2"/>
       <c r="J33" s="2"/>
@@ -2718,16 +2718,16 @@
       <c r="Z33" s="2"/>
     </row>
     <row r="34" spans="1:26" ht="15" customHeight="1">
-      <c r="A34" s="51" t="s">
-        <v>49</v>
-      </c>
-      <c r="B34" s="52"/>
-      <c r="C34" s="52"/>
-      <c r="D34" s="52"/>
-      <c r="E34" s="52"/>
-      <c r="F34" s="52"/>
-      <c r="G34" s="52"/>
-      <c r="H34" s="53"/>
+      <c r="A34" s="48" t="s">
+        <v>48</v>
+      </c>
+      <c r="B34" s="49"/>
+      <c r="C34" s="49"/>
+      <c r="D34" s="49"/>
+      <c r="E34" s="49"/>
+      <c r="F34" s="49"/>
+      <c r="G34" s="49"/>
+      <c r="H34" s="50"/>
       <c r="I34" s="2"/>
       <c r="J34" s="2"/>
       <c r="K34" s="2"/>
@@ -2748,24 +2748,24 @@
       <c r="Z34" s="2"/>
     </row>
     <row r="35" spans="1:26" ht="15" customHeight="1">
-      <c r="A35" s="43" t="s">
+      <c r="A35" s="51" t="s">
+        <v>49</v>
+      </c>
+      <c r="B35" s="43"/>
+      <c r="C35" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B35" s="44"/>
-      <c r="C35" s="1" t="s">
+      <c r="D35" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="D35" s="1" t="s">
+      <c r="E35" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="E35" s="1" t="s">
+      <c r="F35" s="51" t="s">
         <v>53</v>
       </c>
-      <c r="F35" s="43" t="s">
-        <v>54</v>
-      </c>
-      <c r="G35" s="36"/>
-      <c r="H35" s="37"/>
+      <c r="G35" s="52"/>
+      <c r="H35" s="53"/>
       <c r="I35" s="2"/>
       <c r="J35" s="2"/>
       <c r="K35" s="2"/>
@@ -2786,10 +2786,10 @@
       <c r="Z35" s="2"/>
     </row>
     <row r="36" spans="1:26" ht="15" customHeight="1">
-      <c r="A36" s="35" t="s">
-        <v>80</v>
-      </c>
-      <c r="B36" s="44"/>
+      <c r="A36" s="44" t="s">
+        <v>78</v>
+      </c>
+      <c r="B36" s="43"/>
       <c r="C36" s="15" t="s">
         <v>15</v>
       </c>
@@ -2797,11 +2797,11 @@
       <c r="E36" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="F36" s="35" t="s">
-        <v>62</v>
-      </c>
-      <c r="G36" s="36"/>
-      <c r="H36" s="37"/>
+      <c r="F36" s="44" t="s">
+        <v>61</v>
+      </c>
+      <c r="G36" s="52"/>
+      <c r="H36" s="53"/>
       <c r="I36" s="2"/>
       <c r="J36" s="2"/>
       <c r="K36" s="2"/>
@@ -2851,17 +2851,17 @@
     </row>
     <row r="38" spans="1:26" ht="15.75" customHeight="1">
       <c r="A38" s="20" t="s">
-        <v>59</v>
-      </c>
-      <c r="B38" s="38" t="s">
-        <v>81</v>
-      </c>
-      <c r="C38" s="39"/>
-      <c r="D38" s="39"/>
-      <c r="E38" s="39"/>
-      <c r="F38" s="39"/>
-      <c r="G38" s="39"/>
-      <c r="H38" s="40"/>
+        <v>58</v>
+      </c>
+      <c r="B38" s="61" t="s">
+        <v>79</v>
+      </c>
+      <c r="C38" s="62"/>
+      <c r="D38" s="62"/>
+      <c r="E38" s="62"/>
+      <c r="F38" s="62"/>
+      <c r="G38" s="62"/>
+      <c r="H38" s="63"/>
       <c r="I38" s="2"/>
       <c r="J38" s="2"/>
       <c r="K38" s="2"/>
@@ -2885,15 +2885,15 @@
       <c r="A39" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B39" s="41" t="s">
-        <v>82</v>
-      </c>
-      <c r="C39" s="36"/>
-      <c r="D39" s="36"/>
-      <c r="E39" s="36"/>
-      <c r="F39" s="36"/>
-      <c r="G39" s="36"/>
-      <c r="H39" s="37"/>
+      <c r="B39" s="66" t="s">
+        <v>80</v>
+      </c>
+      <c r="C39" s="52"/>
+      <c r="D39" s="52"/>
+      <c r="E39" s="52"/>
+      <c r="F39" s="52"/>
+      <c r="G39" s="52"/>
+      <c r="H39" s="53"/>
       <c r="I39" s="2"/>
       <c r="J39" s="2"/>
       <c r="K39" s="2"/>
@@ -2914,16 +2914,16 @@
       <c r="Z39" s="2"/>
     </row>
     <row r="40" spans="1:26" ht="15" customHeight="1">
-      <c r="A40" s="42" t="s">
+      <c r="A40" s="54" t="s">
         <v>4</v>
       </c>
-      <c r="B40" s="36"/>
-      <c r="C40" s="36"/>
-      <c r="D40" s="36"/>
-      <c r="E40" s="36"/>
-      <c r="F40" s="36"/>
-      <c r="G40" s="36"/>
-      <c r="H40" s="37"/>
+      <c r="B40" s="52"/>
+      <c r="C40" s="52"/>
+      <c r="D40" s="52"/>
+      <c r="E40" s="52"/>
+      <c r="F40" s="52"/>
+      <c r="G40" s="52"/>
+      <c r="H40" s="53"/>
       <c r="I40" s="2"/>
       <c r="J40" s="2"/>
       <c r="K40" s="2"/>
@@ -2944,10 +2944,10 @@
       <c r="Z40" s="2"/>
     </row>
     <row r="41" spans="1:26" ht="15" customHeight="1">
-      <c r="A41" s="43" t="s">
+      <c r="A41" s="51" t="s">
         <v>5</v>
       </c>
-      <c r="B41" s="44"/>
+      <c r="B41" s="43"/>
       <c r="C41" s="1" t="s">
         <v>6</v>
       </c>
@@ -2986,10 +2986,10 @@
       <c r="Z41" s="2"/>
     </row>
     <row r="42" spans="1:26" ht="15" customHeight="1">
-      <c r="A42" s="45" t="s">
-        <v>83</v>
-      </c>
-      <c r="B42" s="44"/>
+      <c r="A42" s="42" t="s">
+        <v>81</v>
+      </c>
+      <c r="B42" s="43"/>
       <c r="C42" s="4" t="s">
         <v>12</v>
       </c>
@@ -3004,7 +3004,7 @@
       </c>
       <c r="G42" s="5"/>
       <c r="H42" s="6" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="I42" s="2"/>
       <c r="J42" s="2"/>
@@ -3026,10 +3026,10 @@
       <c r="Z42" s="2"/>
     </row>
     <row r="43" spans="1:26" ht="15" customHeight="1">
-      <c r="A43" s="45" t="s">
-        <v>62</v>
-      </c>
-      <c r="B43" s="44"/>
+      <c r="A43" s="42" t="s">
+        <v>61</v>
+      </c>
+      <c r="B43" s="43"/>
       <c r="C43" s="4" t="s">
         <v>12</v>
       </c>
@@ -3044,7 +3044,7 @@
         <v>15</v>
       </c>
       <c r="H43" s="6" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="I43" s="2"/>
       <c r="J43" s="2"/>
@@ -3066,15 +3066,15 @@
       <c r="Z43" s="2"/>
     </row>
     <row r="44" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A44" s="45" t="s">
+      <c r="A44" s="42" t="s">
+        <v>84</v>
+      </c>
+      <c r="B44" s="43"/>
+      <c r="C44" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="D44" s="4" t="s">
         <v>86</v>
-      </c>
-      <c r="B44" s="44"/>
-      <c r="C44" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="D44" s="4" t="s">
-        <v>88</v>
       </c>
       <c r="E44" s="4" t="s">
         <v>14</v>
@@ -3082,7 +3082,7 @@
       <c r="F44" s="5"/>
       <c r="G44" s="5"/>
       <c r="H44" s="6" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="I44" s="2"/>
       <c r="J44" s="2"/>
@@ -3104,15 +3104,15 @@
       <c r="Z44" s="2"/>
     </row>
     <row r="45" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A45" s="45" t="s">
-        <v>90</v>
-      </c>
-      <c r="B45" s="44"/>
+      <c r="A45" s="42" t="s">
+        <v>88</v>
+      </c>
+      <c r="B45" s="43"/>
       <c r="C45" s="4" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D45" s="4" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E45" s="4" t="s">
         <v>14</v>
@@ -3120,7 +3120,7 @@
       <c r="F45" s="5"/>
       <c r="G45" s="5"/>
       <c r="H45" s="6" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="I45" s="2"/>
       <c r="J45" s="2"/>
@@ -3142,15 +3142,15 @@
       <c r="Z45" s="2"/>
     </row>
     <row r="46" spans="1:26" ht="15" customHeight="1">
-      <c r="A46" s="45" t="s">
-        <v>92</v>
-      </c>
-      <c r="B46" s="44"/>
+      <c r="A46" s="42" t="s">
+        <v>90</v>
+      </c>
+      <c r="B46" s="43"/>
       <c r="C46" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="D46" s="4" t="s">
         <v>68</v>
-      </c>
-      <c r="D46" s="4" t="s">
-        <v>69</v>
       </c>
       <c r="E46" s="4" t="s">
         <v>14</v>
@@ -3158,7 +3158,7 @@
       <c r="F46" s="5"/>
       <c r="G46" s="5"/>
       <c r="H46" s="6" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="I46" s="2"/>
       <c r="J46" s="2"/>
@@ -3180,15 +3180,15 @@
       <c r="Z46" s="2"/>
     </row>
     <row r="47" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A47" s="45" t="s">
-        <v>94</v>
-      </c>
-      <c r="B47" s="44"/>
+      <c r="A47" s="42" t="s">
+        <v>92</v>
+      </c>
+      <c r="B47" s="43"/>
       <c r="C47" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="D47" s="27" t="s">
         <v>68</v>
-      </c>
-      <c r="D47" s="27" t="s">
-        <v>69</v>
       </c>
       <c r="E47" s="4" t="s">
         <v>14</v>
@@ -3196,7 +3196,7 @@
       <c r="F47" s="5"/>
       <c r="G47" s="5"/>
       <c r="H47" s="6" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="I47" s="2"/>
       <c r="J47" s="2"/>
@@ -3218,15 +3218,15 @@
       <c r="Z47" s="2"/>
     </row>
     <row r="48" spans="1:26" ht="15" customHeight="1">
-      <c r="A48" s="46" t="s">
-        <v>96</v>
+      <c r="A48" s="73" t="s">
+        <v>94</v>
       </c>
       <c r="B48" s="47"/>
       <c r="C48" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="D48" s="11" t="s">
         <v>30</v>
-      </c>
-      <c r="D48" s="11" t="s">
-        <v>31</v>
       </c>
       <c r="E48" s="12" t="s">
         <v>14</v>
@@ -3234,7 +3234,7 @@
       <c r="F48" s="28"/>
       <c r="G48" s="13"/>
       <c r="H48" s="14" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="I48" s="2"/>
       <c r="J48" s="2"/>
@@ -3256,16 +3256,16 @@
       <c r="Z48" s="2"/>
     </row>
     <row r="49" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A49" s="48" t="s">
-        <v>49</v>
-      </c>
-      <c r="B49" s="49"/>
-      <c r="C49" s="49"/>
-      <c r="D49" s="49"/>
-      <c r="E49" s="49"/>
-      <c r="F49" s="49"/>
-      <c r="G49" s="49"/>
-      <c r="H49" s="50"/>
+      <c r="A49" s="74" t="s">
+        <v>48</v>
+      </c>
+      <c r="B49" s="75"/>
+      <c r="C49" s="75"/>
+      <c r="D49" s="75"/>
+      <c r="E49" s="75"/>
+      <c r="F49" s="75"/>
+      <c r="G49" s="75"/>
+      <c r="H49" s="76"/>
       <c r="I49" s="2"/>
       <c r="J49" s="2"/>
       <c r="K49" s="2"/>
@@ -3286,24 +3286,24 @@
       <c r="Z49" s="2"/>
     </row>
     <row r="50" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A50" s="43" t="s">
+      <c r="A50" s="51" t="s">
+        <v>49</v>
+      </c>
+      <c r="B50" s="43"/>
+      <c r="C50" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B50" s="44"/>
-      <c r="C50" s="1" t="s">
+      <c r="D50" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="D50" s="1" t="s">
+      <c r="E50" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="E50" s="1" t="s">
+      <c r="F50" s="51" t="s">
         <v>53</v>
       </c>
-      <c r="F50" s="43" t="s">
-        <v>54</v>
-      </c>
-      <c r="G50" s="36"/>
-      <c r="H50" s="37"/>
+      <c r="G50" s="52"/>
+      <c r="H50" s="53"/>
       <c r="I50" s="2"/>
       <c r="J50" s="2"/>
       <c r="K50" s="2"/>
@@ -3324,10 +3324,10 @@
       <c r="Z50" s="2"/>
     </row>
     <row r="51" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A51" s="35" t="s">
-        <v>98</v>
-      </c>
-      <c r="B51" s="44"/>
+      <c r="A51" s="44" t="s">
+        <v>96</v>
+      </c>
+      <c r="B51" s="43"/>
       <c r="C51" s="15" t="s">
         <v>15</v>
       </c>
@@ -3335,11 +3335,11 @@
       <c r="E51" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="F51" s="35" t="s">
-        <v>83</v>
-      </c>
-      <c r="G51" s="36"/>
-      <c r="H51" s="37"/>
+      <c r="F51" s="44" t="s">
+        <v>81</v>
+      </c>
+      <c r="G51" s="52"/>
+      <c r="H51" s="53"/>
       <c r="I51" s="2"/>
       <c r="J51" s="2"/>
       <c r="K51" s="2"/>
@@ -3389,17 +3389,17 @@
     </row>
     <row r="53" spans="1:26" ht="15" customHeight="1">
       <c r="A53" s="20" t="s">
-        <v>59</v>
-      </c>
-      <c r="B53" s="38" t="s">
-        <v>99</v>
-      </c>
-      <c r="C53" s="39"/>
-      <c r="D53" s="39"/>
-      <c r="E53" s="39"/>
-      <c r="F53" s="39"/>
-      <c r="G53" s="39"/>
-      <c r="H53" s="40"/>
+        <v>58</v>
+      </c>
+      <c r="B53" s="61" t="s">
+        <v>97</v>
+      </c>
+      <c r="C53" s="62"/>
+      <c r="D53" s="62"/>
+      <c r="E53" s="62"/>
+      <c r="F53" s="62"/>
+      <c r="G53" s="62"/>
+      <c r="H53" s="63"/>
       <c r="I53" s="2"/>
       <c r="J53" s="2"/>
       <c r="K53" s="2"/>
@@ -3423,15 +3423,15 @@
       <c r="A54" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B54" s="41" t="s">
-        <v>100</v>
-      </c>
-      <c r="C54" s="36"/>
-      <c r="D54" s="36"/>
-      <c r="E54" s="36"/>
-      <c r="F54" s="36"/>
-      <c r="G54" s="36"/>
-      <c r="H54" s="37"/>
+      <c r="B54" s="66" t="s">
+        <v>98</v>
+      </c>
+      <c r="C54" s="52"/>
+      <c r="D54" s="52"/>
+      <c r="E54" s="52"/>
+      <c r="F54" s="52"/>
+      <c r="G54" s="52"/>
+      <c r="H54" s="53"/>
       <c r="I54" s="2"/>
       <c r="J54" s="2"/>
       <c r="K54" s="2"/>
@@ -3452,16 +3452,16 @@
       <c r="Z54" s="2"/>
     </row>
     <row r="55" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A55" s="42" t="s">
+      <c r="A55" s="54" t="s">
         <v>4</v>
       </c>
-      <c r="B55" s="36"/>
-      <c r="C55" s="36"/>
-      <c r="D55" s="36"/>
-      <c r="E55" s="36"/>
-      <c r="F55" s="36"/>
-      <c r="G55" s="36"/>
-      <c r="H55" s="37"/>
+      <c r="B55" s="52"/>
+      <c r="C55" s="52"/>
+      <c r="D55" s="52"/>
+      <c r="E55" s="52"/>
+      <c r="F55" s="52"/>
+      <c r="G55" s="52"/>
+      <c r="H55" s="53"/>
       <c r="I55" s="2"/>
       <c r="J55" s="2"/>
       <c r="K55" s="2"/>
@@ -3482,10 +3482,10 @@
       <c r="Z55" s="2"/>
     </row>
     <row r="56" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A56" s="43" t="s">
+      <c r="A56" s="51" t="s">
         <v>5</v>
       </c>
-      <c r="B56" s="44"/>
+      <c r="B56" s="43"/>
       <c r="C56" s="1" t="s">
         <v>6</v>
       </c>
@@ -3524,10 +3524,10 @@
       <c r="Z56" s="2"/>
     </row>
     <row r="57" spans="1:26" ht="15" customHeight="1">
-      <c r="A57" s="45" t="s">
-        <v>101</v>
-      </c>
-      <c r="B57" s="44"/>
+      <c r="A57" s="42" t="s">
+        <v>99</v>
+      </c>
+      <c r="B57" s="43"/>
       <c r="C57" s="4" t="s">
         <v>12</v>
       </c>
@@ -3542,7 +3542,7 @@
       </c>
       <c r="G57" s="5"/>
       <c r="H57" s="6" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="I57" s="2"/>
       <c r="J57" s="2"/>
@@ -3564,10 +3564,10 @@
       <c r="Z57" s="2"/>
     </row>
     <row r="58" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A58" s="45" t="s">
-        <v>62</v>
-      </c>
-      <c r="B58" s="44"/>
+      <c r="A58" s="42" t="s">
+        <v>61</v>
+      </c>
+      <c r="B58" s="43"/>
       <c r="C58" s="4" t="s">
         <v>12</v>
       </c>
@@ -3582,7 +3582,7 @@
         <v>15</v>
       </c>
       <c r="H58" s="6" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="I58" s="2"/>
       <c r="J58" s="2"/>
@@ -3604,10 +3604,10 @@
       <c r="Z58" s="2"/>
     </row>
     <row r="59" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A59" s="45" t="s">
+      <c r="A59" s="42" t="s">
         <v>11</v>
       </c>
-      <c r="B59" s="44"/>
+      <c r="B59" s="43"/>
       <c r="C59" s="4" t="s">
         <v>12</v>
       </c>
@@ -3622,7 +3622,7 @@
         <v>15</v>
       </c>
       <c r="H59" s="6" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="I59" s="2"/>
       <c r="J59" s="2"/>
@@ -3644,15 +3644,15 @@
       <c r="Z59" s="2"/>
     </row>
     <row r="60" spans="1:26" ht="15" customHeight="1">
-      <c r="A60" s="45" t="s">
-        <v>105</v>
-      </c>
-      <c r="B60" s="44"/>
+      <c r="A60" s="42" t="s">
+        <v>103</v>
+      </c>
+      <c r="B60" s="43"/>
       <c r="C60" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D60" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E60" s="4" t="s">
         <v>14</v>
@@ -3660,7 +3660,7 @@
       <c r="F60" s="5"/>
       <c r="G60" s="5"/>
       <c r="H60" s="6" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="I60" s="2"/>
       <c r="J60" s="2"/>
@@ -3682,15 +3682,15 @@
       <c r="Z60" s="2"/>
     </row>
     <row r="61" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A61" s="45" t="s">
-        <v>107</v>
-      </c>
-      <c r="B61" s="44"/>
+      <c r="A61" s="42" t="s">
+        <v>105</v>
+      </c>
+      <c r="B61" s="43"/>
       <c r="C61" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D61" s="4" t="s">
         <v>43</v>
-      </c>
-      <c r="D61" s="4" t="s">
-        <v>44</v>
       </c>
       <c r="E61" s="4" t="s">
         <v>14</v>
@@ -3698,7 +3698,7 @@
       <c r="F61" s="5"/>
       <c r="G61" s="5"/>
       <c r="H61" s="6" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="I61" s="2"/>
       <c r="J61" s="2"/>
@@ -3720,15 +3720,15 @@
       <c r="Z61" s="2"/>
     </row>
     <row r="62" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A62" s="45" t="s">
+      <c r="A62" s="42" t="s">
+        <v>107</v>
+      </c>
+      <c r="B62" s="43"/>
+      <c r="C62" s="12" t="s">
+        <v>108</v>
+      </c>
+      <c r="D62" s="12" t="s">
         <v>109</v>
-      </c>
-      <c r="B62" s="44"/>
-      <c r="C62" s="12" t="s">
-        <v>110</v>
-      </c>
-      <c r="D62" s="12" t="s">
-        <v>111</v>
       </c>
       <c r="E62" s="12" t="s">
         <v>14</v>
@@ -3736,7 +3736,7 @@
       <c r="F62" s="29"/>
       <c r="G62" s="29"/>
       <c r="H62" s="30" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="I62" s="2"/>
       <c r="J62" s="2"/>
@@ -3758,15 +3758,15 @@
       <c r="Z62" s="2"/>
     </row>
     <row r="63" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A63" s="62" t="s">
-        <v>113</v>
-      </c>
-      <c r="B63" s="57"/>
+      <c r="A63" s="45" t="s">
+        <v>111</v>
+      </c>
+      <c r="B63" s="39"/>
       <c r="C63" s="23" t="s">
+        <v>67</v>
+      </c>
+      <c r="D63" s="23" t="s">
         <v>68</v>
-      </c>
-      <c r="D63" s="23" t="s">
-        <v>69</v>
       </c>
       <c r="E63" s="23" t="s">
         <v>14</v>
@@ -3774,7 +3774,7 @@
       <c r="F63" s="31"/>
       <c r="G63" s="31"/>
       <c r="H63" s="32" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="I63" s="2"/>
       <c r="J63" s="2"/>
@@ -3796,16 +3796,16 @@
       <c r="Z63" s="2"/>
     </row>
     <row r="64" spans="1:26" ht="15" customHeight="1">
-      <c r="A64" s="51" t="s">
-        <v>49</v>
-      </c>
-      <c r="B64" s="52"/>
-      <c r="C64" s="52"/>
-      <c r="D64" s="52"/>
-      <c r="E64" s="52"/>
-      <c r="F64" s="52"/>
-      <c r="G64" s="52"/>
-      <c r="H64" s="53"/>
+      <c r="A64" s="48" t="s">
+        <v>48</v>
+      </c>
+      <c r="B64" s="49"/>
+      <c r="C64" s="49"/>
+      <c r="D64" s="49"/>
+      <c r="E64" s="49"/>
+      <c r="F64" s="49"/>
+      <c r="G64" s="49"/>
+      <c r="H64" s="50"/>
       <c r="I64" s="2"/>
       <c r="J64" s="2"/>
       <c r="K64" s="2"/>
@@ -3826,24 +3826,24 @@
       <c r="Z64" s="2"/>
     </row>
     <row r="65" spans="1:26" ht="15" customHeight="1">
-      <c r="A65" s="43" t="s">
+      <c r="A65" s="51" t="s">
+        <v>49</v>
+      </c>
+      <c r="B65" s="43"/>
+      <c r="C65" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B65" s="44"/>
-      <c r="C65" s="1" t="s">
+      <c r="D65" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="D65" s="1" t="s">
+      <c r="E65" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="E65" s="1" t="s">
+      <c r="F65" s="51" t="s">
         <v>53</v>
       </c>
-      <c r="F65" s="43" t="s">
-        <v>54</v>
-      </c>
-      <c r="G65" s="36"/>
-      <c r="H65" s="37"/>
+      <c r="G65" s="52"/>
+      <c r="H65" s="53"/>
       <c r="I65" s="2"/>
       <c r="J65" s="2"/>
       <c r="K65" s="2"/>
@@ -3864,10 +3864,10 @@
       <c r="Z65" s="2"/>
     </row>
     <row r="66" spans="1:26" ht="15" customHeight="1">
-      <c r="A66" s="35" t="s">
-        <v>115</v>
-      </c>
-      <c r="B66" s="44"/>
+      <c r="A66" s="44" t="s">
+        <v>113</v>
+      </c>
+      <c r="B66" s="43"/>
       <c r="C66" s="15" t="s">
         <v>15</v>
       </c>
@@ -3875,11 +3875,11 @@
       <c r="E66" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="F66" s="35" t="s">
-        <v>101</v>
-      </c>
-      <c r="G66" s="36"/>
-      <c r="H66" s="37"/>
+      <c r="F66" s="44" t="s">
+        <v>99</v>
+      </c>
+      <c r="G66" s="52"/>
+      <c r="H66" s="53"/>
       <c r="I66" s="2"/>
       <c r="J66" s="2"/>
       <c r="K66" s="2"/>
@@ -3929,17 +3929,17 @@
     </row>
     <row r="68" spans="1:26" ht="15" customHeight="1">
       <c r="A68" s="20" t="s">
-        <v>59</v>
-      </c>
-      <c r="B68" s="38" t="s">
-        <v>116</v>
-      </c>
-      <c r="C68" s="39"/>
-      <c r="D68" s="39"/>
-      <c r="E68" s="39"/>
-      <c r="F68" s="39"/>
-      <c r="G68" s="39"/>
-      <c r="H68" s="40"/>
+        <v>58</v>
+      </c>
+      <c r="B68" s="61" t="s">
+        <v>114</v>
+      </c>
+      <c r="C68" s="62"/>
+      <c r="D68" s="62"/>
+      <c r="E68" s="62"/>
+      <c r="F68" s="62"/>
+      <c r="G68" s="62"/>
+      <c r="H68" s="63"/>
       <c r="I68" s="2"/>
       <c r="J68" s="2"/>
       <c r="K68" s="2"/>
@@ -3963,15 +3963,15 @@
       <c r="A69" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B69" s="63" t="s">
-        <v>117</v>
-      </c>
-      <c r="C69" s="39"/>
-      <c r="D69" s="39"/>
-      <c r="E69" s="39"/>
-      <c r="F69" s="39"/>
-      <c r="G69" s="39"/>
-      <c r="H69" s="40"/>
+      <c r="B69" s="67" t="s">
+        <v>115</v>
+      </c>
+      <c r="C69" s="62"/>
+      <c r="D69" s="62"/>
+      <c r="E69" s="62"/>
+      <c r="F69" s="62"/>
+      <c r="G69" s="62"/>
+      <c r="H69" s="63"/>
       <c r="I69" s="2"/>
       <c r="J69" s="2"/>
       <c r="K69" s="2"/>
@@ -3992,16 +3992,16 @@
       <c r="Z69" s="2"/>
     </row>
     <row r="70" spans="1:26" ht="15" customHeight="1">
-      <c r="A70" s="42" t="s">
+      <c r="A70" s="54" t="s">
         <v>4</v>
       </c>
-      <c r="B70" s="36"/>
-      <c r="C70" s="36"/>
-      <c r="D70" s="36"/>
-      <c r="E70" s="36"/>
-      <c r="F70" s="36"/>
-      <c r="G70" s="36"/>
-      <c r="H70" s="64"/>
+      <c r="B70" s="52"/>
+      <c r="C70" s="52"/>
+      <c r="D70" s="52"/>
+      <c r="E70" s="52"/>
+      <c r="F70" s="52"/>
+      <c r="G70" s="52"/>
+      <c r="H70" s="55"/>
       <c r="I70" s="33"/>
       <c r="J70" s="2"/>
       <c r="K70" s="2"/>
@@ -4022,10 +4022,10 @@
       <c r="Z70" s="2"/>
     </row>
     <row r="71" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A71" s="43" t="s">
+      <c r="A71" s="51" t="s">
         <v>5</v>
       </c>
-      <c r="B71" s="44"/>
+      <c r="B71" s="43"/>
       <c r="C71" s="1" t="s">
         <v>6</v>
       </c>
@@ -4064,23 +4064,25 @@
       <c r="Z71" s="2"/>
     </row>
     <row r="72" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A72" s="45" t="s">
-        <v>118</v>
-      </c>
-      <c r="B72" s="44"/>
+      <c r="A72" s="42" t="s">
+        <v>116</v>
+      </c>
+      <c r="B72" s="43"/>
       <c r="C72" s="4" t="s">
         <v>12</v>
       </c>
       <c r="D72" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E72" s="4"/>
+      <c r="E72" s="4" t="s">
+        <v>14</v>
+      </c>
       <c r="F72" s="5" t="s">
         <v>15</v>
       </c>
       <c r="G72" s="5"/>
       <c r="H72" s="6" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="I72" s="2"/>
       <c r="J72" s="2"/>
@@ -4102,23 +4104,23 @@
       <c r="Z72" s="2"/>
     </row>
     <row r="73" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A73" s="45" t="s">
-        <v>62</v>
-      </c>
-      <c r="B73" s="44"/>
+      <c r="A73" s="42" t="s">
+        <v>17</v>
+      </c>
+      <c r="B73" s="77"/>
       <c r="C73" s="4" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="D73" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E73" s="4"/>
+        <v>19</v>
+      </c>
+      <c r="E73" s="4" t="s">
+        <v>14</v>
+      </c>
       <c r="F73" s="5"/>
-      <c r="G73" s="5" t="s">
-        <v>15</v>
-      </c>
+      <c r="G73" s="5"/>
       <c r="H73" s="6" t="s">
-        <v>120</v>
+        <v>175</v>
       </c>
       <c r="I73" s="2"/>
       <c r="J73" s="2"/>
@@ -4140,21 +4142,25 @@
       <c r="Z73" s="2"/>
     </row>
     <row r="74" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A74" s="45" t="s">
-        <v>121</v>
-      </c>
-      <c r="B74" s="44"/>
+      <c r="A74" s="42" t="s">
+        <v>61</v>
+      </c>
+      <c r="B74" s="43"/>
       <c r="C74" s="4" t="s">
-        <v>68</v>
+        <v>12</v>
       </c>
       <c r="D74" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="E74" s="4"/>
+        <v>13</v>
+      </c>
+      <c r="E74" s="4" t="s">
+        <v>14</v>
+      </c>
       <c r="F74" s="5"/>
-      <c r="G74" s="5"/>
+      <c r="G74" s="5" t="s">
+        <v>15</v>
+      </c>
       <c r="H74" s="6" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="I74" s="2"/>
       <c r="J74" s="2"/>
@@ -4176,21 +4182,23 @@
       <c r="Z74" s="2"/>
     </row>
     <row r="75" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A75" s="45" t="s">
-        <v>123</v>
-      </c>
-      <c r="B75" s="44"/>
+      <c r="A75" s="42" t="s">
+        <v>119</v>
+      </c>
+      <c r="B75" s="43"/>
       <c r="C75" s="4" t="s">
-        <v>124</v>
+        <v>67</v>
       </c>
       <c r="D75" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="E75" s="4"/>
+        <v>68</v>
+      </c>
+      <c r="E75" s="4" t="s">
+        <v>14</v>
+      </c>
       <c r="F75" s="5"/>
       <c r="G75" s="5"/>
       <c r="H75" s="6" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="I75" s="2"/>
       <c r="J75" s="2"/>
@@ -4212,21 +4220,23 @@
       <c r="Z75" s="2"/>
     </row>
     <row r="76" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A76" s="45" t="s">
-        <v>127</v>
-      </c>
-      <c r="B76" s="44"/>
+      <c r="A76" s="42" t="s">
+        <v>121</v>
+      </c>
+      <c r="B76" s="43"/>
       <c r="C76" s="4" t="s">
-        <v>30</v>
+        <v>67</v>
       </c>
       <c r="D76" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="E76" s="4"/>
+        <v>122</v>
+      </c>
+      <c r="E76" s="4" t="s">
+        <v>14</v>
+      </c>
       <c r="F76" s="5"/>
       <c r="G76" s="5"/>
       <c r="H76" s="6" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="I76" s="2"/>
       <c r="J76" s="2"/>
@@ -4248,21 +4258,23 @@
       <c r="Z76" s="2"/>
     </row>
     <row r="77" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A77" s="72" t="s">
-        <v>129</v>
-      </c>
-      <c r="B77" s="73"/>
-      <c r="C77" s="12" t="s">
+      <c r="A77" s="42" t="s">
+        <v>124</v>
+      </c>
+      <c r="B77" s="43"/>
+      <c r="C77" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D77" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="D77" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="E77" s="12"/>
-      <c r="F77" s="29"/>
-      <c r="G77" s="29"/>
-      <c r="H77" s="30" t="s">
-        <v>130</v>
+      <c r="E77" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F77" s="5"/>
+      <c r="G77" s="5"/>
+      <c r="H77" s="6" t="s">
+        <v>125</v>
       </c>
       <c r="I77" s="2"/>
       <c r="J77" s="2"/>
@@ -4283,22 +4295,24 @@
       <c r="Y77" s="2"/>
       <c r="Z77" s="2"/>
     </row>
-    <row r="78" spans="1:26" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A78" s="65" t="s">
-        <v>131</v>
-      </c>
-      <c r="B78" s="71"/>
-      <c r="C78" s="74" t="s">
-        <v>68</v>
-      </c>
-      <c r="D78" s="74" t="s">
-        <v>69</v>
-      </c>
-      <c r="E78" s="74"/>
-      <c r="F78" s="75"/>
-      <c r="G78" s="75"/>
-      <c r="H78" s="76" t="s">
-        <v>132</v>
+    <row r="78" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A78" s="56" t="s">
+        <v>126</v>
+      </c>
+      <c r="B78" s="57"/>
+      <c r="C78" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="D78" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="E78" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="F78" s="29"/>
+      <c r="G78" s="29"/>
+      <c r="H78" s="30" t="s">
+        <v>127</v>
       </c>
       <c r="I78" s="2"/>
       <c r="J78" s="2"/>
@@ -4319,17 +4333,25 @@
       <c r="Y78" s="2"/>
       <c r="Z78" s="2"/>
     </row>
-    <row r="79" spans="1:26" ht="15" customHeight="1">
-      <c r="A79" s="68" t="s">
-        <v>49</v>
-      </c>
-      <c r="B79" s="69"/>
-      <c r="C79" s="69"/>
-      <c r="D79" s="69"/>
-      <c r="E79" s="69"/>
-      <c r="F79" s="69"/>
-      <c r="G79" s="69"/>
-      <c r="H79" s="70"/>
+    <row r="79" spans="1:26" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A79" s="64" t="s">
+        <v>128</v>
+      </c>
+      <c r="B79" s="65"/>
+      <c r="C79" s="35" t="s">
+        <v>67</v>
+      </c>
+      <c r="D79" s="35" t="s">
+        <v>68</v>
+      </c>
+      <c r="E79" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="F79" s="36"/>
+      <c r="G79" s="36"/>
+      <c r="H79" s="37" t="s">
+        <v>129</v>
+      </c>
       <c r="I79" s="2"/>
       <c r="J79" s="2"/>
       <c r="K79" s="2"/>
@@ -4349,25 +4371,17 @@
       <c r="Y79" s="2"/>
       <c r="Z79" s="2"/>
     </row>
-    <row r="80" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A80" s="43" t="s">
-        <v>50</v>
-      </c>
-      <c r="B80" s="44"/>
-      <c r="C80" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="D80" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="E80" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="F80" s="43" t="s">
-        <v>54</v>
-      </c>
-      <c r="G80" s="36"/>
-      <c r="H80" s="37"/>
+    <row r="80" spans="1:26" ht="15" customHeight="1">
+      <c r="A80" s="58" t="s">
+        <v>48</v>
+      </c>
+      <c r="B80" s="59"/>
+      <c r="C80" s="59"/>
+      <c r="D80" s="59"/>
+      <c r="E80" s="59"/>
+      <c r="F80" s="59"/>
+      <c r="G80" s="59"/>
+      <c r="H80" s="60"/>
       <c r="I80" s="2"/>
       <c r="J80" s="2"/>
       <c r="K80" s="2"/>
@@ -4388,22 +4402,24 @@
       <c r="Z80" s="2"/>
     </row>
     <row r="81" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A81" s="35" t="s">
-        <v>133</v>
-      </c>
-      <c r="B81" s="44"/>
-      <c r="C81" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="D81" s="16"/>
-      <c r="E81" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="F81" s="35" t="s">
-        <v>118</v>
-      </c>
-      <c r="G81" s="36"/>
-      <c r="H81" s="37"/>
+      <c r="A81" s="51" t="s">
+        <v>49</v>
+      </c>
+      <c r="B81" s="43"/>
+      <c r="C81" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D81" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E81" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F81" s="51" t="s">
+        <v>53</v>
+      </c>
+      <c r="G81" s="52"/>
+      <c r="H81" s="53"/>
       <c r="I81" s="2"/>
       <c r="J81" s="2"/>
       <c r="K81" s="2"/>
@@ -4424,14 +4440,22 @@
       <c r="Z81" s="2"/>
     </row>
     <row r="82" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A82" s="19"/>
-      <c r="B82" s="19"/>
-      <c r="C82" s="19"/>
-      <c r="D82" s="19"/>
-      <c r="E82" s="19"/>
-      <c r="F82" s="19"/>
-      <c r="G82" s="19"/>
-      <c r="H82" s="19"/>
+      <c r="A82" s="44" t="s">
+        <v>130</v>
+      </c>
+      <c r="B82" s="43"/>
+      <c r="C82" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="D82" s="16"/>
+      <c r="E82" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="F82" s="44" t="s">
+        <v>116</v>
+      </c>
+      <c r="G82" s="52"/>
+      <c r="H82" s="53"/>
       <c r="I82" s="2"/>
       <c r="J82" s="2"/>
       <c r="K82" s="2"/>
@@ -4452,18 +4476,14 @@
       <c r="Z82" s="2"/>
     </row>
     <row r="83" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A83" s="20" t="s">
-        <v>59</v>
-      </c>
-      <c r="B83" s="38" t="s">
-        <v>134</v>
-      </c>
-      <c r="C83" s="39"/>
-      <c r="D83" s="39"/>
-      <c r="E83" s="39"/>
-      <c r="F83" s="39"/>
-      <c r="G83" s="39"/>
-      <c r="H83" s="40"/>
+      <c r="A83" s="19"/>
+      <c r="B83" s="19"/>
+      <c r="C83" s="19"/>
+      <c r="D83" s="19"/>
+      <c r="E83" s="19"/>
+      <c r="F83" s="19"/>
+      <c r="G83" s="19"/>
+      <c r="H83" s="19"/>
       <c r="I83" s="2"/>
       <c r="J83" s="2"/>
       <c r="K83" s="2"/>
@@ -4484,18 +4504,18 @@
       <c r="Z83" s="2"/>
     </row>
     <row r="84" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A84" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B84" s="41" t="s">
-        <v>135</v>
-      </c>
-      <c r="C84" s="36"/>
-      <c r="D84" s="36"/>
-      <c r="E84" s="36"/>
-      <c r="F84" s="36"/>
-      <c r="G84" s="36"/>
-      <c r="H84" s="37"/>
+      <c r="A84" s="20" t="s">
+        <v>58</v>
+      </c>
+      <c r="B84" s="61" t="s">
+        <v>131</v>
+      </c>
+      <c r="C84" s="62"/>
+      <c r="D84" s="62"/>
+      <c r="E84" s="62"/>
+      <c r="F84" s="62"/>
+      <c r="G84" s="62"/>
+      <c r="H84" s="63"/>
       <c r="I84" s="2"/>
       <c r="J84" s="2"/>
       <c r="K84" s="2"/>
@@ -4516,16 +4536,18 @@
       <c r="Z84" s="2"/>
     </row>
     <row r="85" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A85" s="42" t="s">
-        <v>4</v>
-      </c>
-      <c r="B85" s="36"/>
-      <c r="C85" s="36"/>
-      <c r="D85" s="36"/>
-      <c r="E85" s="36"/>
-      <c r="F85" s="36"/>
-      <c r="G85" s="36"/>
-      <c r="H85" s="37"/>
+      <c r="A85" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B85" s="66" t="s">
+        <v>132</v>
+      </c>
+      <c r="C85" s="52"/>
+      <c r="D85" s="52"/>
+      <c r="E85" s="52"/>
+      <c r="F85" s="52"/>
+      <c r="G85" s="52"/>
+      <c r="H85" s="53"/>
       <c r="I85" s="2"/>
       <c r="J85" s="2"/>
       <c r="K85" s="2"/>
@@ -4546,28 +4568,16 @@
       <c r="Z85" s="2"/>
     </row>
     <row r="86" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A86" s="43" t="s">
-        <v>5</v>
-      </c>
-      <c r="B86" s="44"/>
-      <c r="C86" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D86" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E86" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F86" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G86" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H86" s="3" t="s">
-        <v>2</v>
-      </c>
+      <c r="A86" s="54" t="s">
+        <v>4</v>
+      </c>
+      <c r="B86" s="52"/>
+      <c r="C86" s="52"/>
+      <c r="D86" s="52"/>
+      <c r="E86" s="52"/>
+      <c r="F86" s="52"/>
+      <c r="G86" s="52"/>
+      <c r="H86" s="53"/>
       <c r="I86" s="2"/>
       <c r="J86" s="2"/>
       <c r="K86" s="2"/>
@@ -4588,25 +4598,27 @@
       <c r="Z86" s="2"/>
     </row>
     <row r="87" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A87" s="45" t="s">
-        <v>136</v>
-      </c>
-      <c r="B87" s="44"/>
-      <c r="C87" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D87" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E87" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="F87" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="G87" s="5"/>
-      <c r="H87" s="6" t="s">
-        <v>137</v>
+      <c r="A87" s="51" t="s">
+        <v>5</v>
+      </c>
+      <c r="B87" s="43"/>
+      <c r="C87" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D87" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E87" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F87" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G87" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H87" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="I87" s="2"/>
       <c r="J87" s="2"/>
@@ -4628,23 +4640,25 @@
       <c r="Z87" s="2"/>
     </row>
     <row r="88" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A88" s="45" t="s">
-        <v>17</v>
-      </c>
-      <c r="B88" s="44"/>
+      <c r="A88" s="42" t="s">
+        <v>133</v>
+      </c>
+      <c r="B88" s="43"/>
       <c r="C88" s="4" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="D88" s="4" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="E88" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="F88" s="5"/>
+      <c r="F88" s="5" t="s">
+        <v>15</v>
+      </c>
       <c r="G88" s="5"/>
       <c r="H88" s="6" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="I88" s="2"/>
       <c r="J88" s="2"/>
@@ -4666,25 +4680,23 @@
       <c r="Z88" s="2"/>
     </row>
     <row r="89" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A89" s="45" t="s">
-        <v>62</v>
-      </c>
-      <c r="B89" s="44"/>
+      <c r="A89" s="42" t="s">
+        <v>17</v>
+      </c>
+      <c r="B89" s="43"/>
       <c r="C89" s="4" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="D89" s="4" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="E89" s="4" t="s">
         <v>14</v>
       </c>
       <c r="F89" s="5"/>
-      <c r="G89" s="5" t="s">
-        <v>15</v>
-      </c>
+      <c r="G89" s="5"/>
       <c r="H89" s="6" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="I89" s="2"/>
       <c r="J89" s="2"/>
@@ -4705,24 +4717,26 @@
       <c r="Y89" s="2"/>
       <c r="Z89" s="2"/>
     </row>
-    <row r="90" spans="1:26" ht="15" customHeight="1">
-      <c r="A90" s="45" t="s">
-        <v>140</v>
-      </c>
-      <c r="B90" s="44"/>
+    <row r="90" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A90" s="42" t="s">
+        <v>61</v>
+      </c>
+      <c r="B90" s="43"/>
       <c r="C90" s="4" t="s">
-        <v>43</v>
+        <v>12</v>
       </c>
       <c r="D90" s="4" t="s">
-        <v>44</v>
+        <v>13</v>
       </c>
       <c r="E90" s="4" t="s">
         <v>14</v>
       </c>
       <c r="F90" s="5"/>
-      <c r="G90" s="5"/>
+      <c r="G90" s="5" t="s">
+        <v>15</v>
+      </c>
       <c r="H90" s="6" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="I90" s="2"/>
       <c r="J90" s="2"/>
@@ -4744,15 +4758,15 @@
       <c r="Z90" s="2"/>
     </row>
     <row r="91" spans="1:26" ht="15" customHeight="1">
-      <c r="A91" s="45" t="s">
-        <v>142</v>
-      </c>
-      <c r="B91" s="44"/>
+      <c r="A91" s="42" t="s">
+        <v>137</v>
+      </c>
+      <c r="B91" s="43"/>
       <c r="C91" s="4" t="s">
-        <v>68</v>
+        <v>42</v>
       </c>
       <c r="D91" s="4" t="s">
-        <v>69</v>
+        <v>43</v>
       </c>
       <c r="E91" s="4" t="s">
         <v>14</v>
@@ -4760,7 +4774,7 @@
       <c r="F91" s="5"/>
       <c r="G91" s="5"/>
       <c r="H91" s="6" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="I91" s="2"/>
       <c r="J91" s="2"/>
@@ -4782,23 +4796,23 @@
       <c r="Z91" s="2"/>
     </row>
     <row r="92" spans="1:26" ht="15" customHeight="1">
-      <c r="A92" s="45" t="s">
-        <v>144</v>
-      </c>
-      <c r="B92" s="44"/>
+      <c r="A92" s="42" t="s">
+        <v>139</v>
+      </c>
+      <c r="B92" s="43"/>
       <c r="C92" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="D92" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="D92" s="4" t="s">
-        <v>69</v>
-      </c>
       <c r="E92" s="4" t="s">
-        <v>72</v>
+        <v>14</v>
       </c>
       <c r="F92" s="5"/>
       <c r="G92" s="5"/>
       <c r="H92" s="6" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="I92" s="2"/>
       <c r="J92" s="2"/>
@@ -4820,23 +4834,23 @@
       <c r="Z92" s="2"/>
     </row>
     <row r="93" spans="1:26" ht="15" customHeight="1">
-      <c r="A93" s="62" t="s">
-        <v>146</v>
-      </c>
-      <c r="B93" s="57"/>
-      <c r="C93" s="23" t="s">
-        <v>30</v>
-      </c>
-      <c r="D93" s="23" t="s">
-        <v>31</v>
-      </c>
-      <c r="E93" s="23" t="s">
+      <c r="A93" s="42" t="s">
+        <v>141</v>
+      </c>
+      <c r="B93" s="43"/>
+      <c r="C93" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="D93" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="E93" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="F93" s="31"/>
-      <c r="G93" s="31"/>
-      <c r="H93" s="32" t="s">
-        <v>147</v>
+      <c r="F93" s="5"/>
+      <c r="G93" s="5"/>
+      <c r="H93" s="6" t="s">
+        <v>142</v>
       </c>
       <c r="I93" s="2"/>
       <c r="J93" s="2"/>
@@ -4857,17 +4871,25 @@
       <c r="Y93" s="2"/>
       <c r="Z93" s="2"/>
     </row>
-    <row r="94" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A94" s="51" t="s">
-        <v>49</v>
-      </c>
-      <c r="B94" s="52"/>
-      <c r="C94" s="52"/>
-      <c r="D94" s="52"/>
-      <c r="E94" s="52"/>
-      <c r="F94" s="52"/>
-      <c r="G94" s="52"/>
-      <c r="H94" s="53"/>
+    <row r="94" spans="1:26" ht="15" customHeight="1" thickBot="1">
+      <c r="A94" s="45" t="s">
+        <v>143</v>
+      </c>
+      <c r="B94" s="39"/>
+      <c r="C94" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="D94" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="E94" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="F94" s="31"/>
+      <c r="G94" s="31"/>
+      <c r="H94" s="32" t="s">
+        <v>144</v>
+      </c>
       <c r="I94" s="2"/>
       <c r="J94" s="2"/>
       <c r="K94" s="2"/>
@@ -4887,25 +4909,17 @@
       <c r="Y94" s="2"/>
       <c r="Z94" s="2"/>
     </row>
-    <row r="95" spans="1:26" ht="15" customHeight="1">
-      <c r="A95" s="43" t="s">
-        <v>50</v>
-      </c>
-      <c r="B95" s="44"/>
-      <c r="C95" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="D95" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="E95" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="F95" s="43" t="s">
-        <v>54</v>
-      </c>
-      <c r="G95" s="36"/>
-      <c r="H95" s="37"/>
+    <row r="95" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A95" s="48" t="s">
+        <v>48</v>
+      </c>
+      <c r="B95" s="49"/>
+      <c r="C95" s="49"/>
+      <c r="D95" s="49"/>
+      <c r="E95" s="49"/>
+      <c r="F95" s="49"/>
+      <c r="G95" s="49"/>
+      <c r="H95" s="50"/>
       <c r="I95" s="2"/>
       <c r="J95" s="2"/>
       <c r="K95" s="2"/>
@@ -4925,23 +4939,25 @@
       <c r="Y95" s="2"/>
       <c r="Z95" s="2"/>
     </row>
-    <row r="96" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A96" s="35" t="s">
-        <v>148</v>
-      </c>
-      <c r="B96" s="44"/>
-      <c r="C96" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="D96" s="16"/>
-      <c r="E96" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="F96" s="35" t="s">
-        <v>136</v>
-      </c>
-      <c r="G96" s="36"/>
-      <c r="H96" s="37"/>
+    <row r="96" spans="1:26" ht="15" customHeight="1">
+      <c r="A96" s="51" t="s">
+        <v>49</v>
+      </c>
+      <c r="B96" s="43"/>
+      <c r="C96" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D96" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E96" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F96" s="51" t="s">
+        <v>53</v>
+      </c>
+      <c r="G96" s="52"/>
+      <c r="H96" s="53"/>
       <c r="I96" s="2"/>
       <c r="J96" s="2"/>
       <c r="K96" s="2"/>
@@ -4962,14 +4978,22 @@
       <c r="Z96" s="2"/>
     </row>
     <row r="97" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A97" s="19"/>
-      <c r="B97" s="19"/>
-      <c r="C97" s="19"/>
-      <c r="D97" s="19"/>
-      <c r="E97" s="19"/>
-      <c r="F97" s="19"/>
-      <c r="G97" s="19"/>
-      <c r="H97" s="19"/>
+      <c r="A97" s="44" t="s">
+        <v>145</v>
+      </c>
+      <c r="B97" s="43"/>
+      <c r="C97" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="D97" s="16"/>
+      <c r="E97" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="F97" s="44" t="s">
+        <v>133</v>
+      </c>
+      <c r="G97" s="52"/>
+      <c r="H97" s="53"/>
       <c r="I97" s="2"/>
       <c r="J97" s="2"/>
       <c r="K97" s="2"/>
@@ -4990,18 +5014,14 @@
       <c r="Z97" s="2"/>
     </row>
     <row r="98" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A98" s="20" t="s">
-        <v>59</v>
-      </c>
-      <c r="B98" s="38" t="s">
-        <v>149</v>
-      </c>
-      <c r="C98" s="39"/>
-      <c r="D98" s="39"/>
-      <c r="E98" s="39"/>
-      <c r="F98" s="39"/>
-      <c r="G98" s="39"/>
-      <c r="H98" s="40"/>
+      <c r="A98" s="19"/>
+      <c r="B98" s="19"/>
+      <c r="C98" s="19"/>
+      <c r="D98" s="19"/>
+      <c r="E98" s="19"/>
+      <c r="F98" s="19"/>
+      <c r="G98" s="19"/>
+      <c r="H98" s="19"/>
       <c r="I98" s="2"/>
       <c r="J98" s="2"/>
       <c r="K98" s="2"/>
@@ -5022,18 +5042,18 @@
       <c r="Z98" s="2"/>
     </row>
     <row r="99" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A99" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B99" s="41" t="s">
-        <v>150</v>
-      </c>
-      <c r="C99" s="36"/>
-      <c r="D99" s="36"/>
-      <c r="E99" s="36"/>
-      <c r="F99" s="36"/>
-      <c r="G99" s="36"/>
-      <c r="H99" s="37"/>
+      <c r="A99" s="20" t="s">
+        <v>58</v>
+      </c>
+      <c r="B99" s="61" t="s">
+        <v>146</v>
+      </c>
+      <c r="C99" s="62"/>
+      <c r="D99" s="62"/>
+      <c r="E99" s="62"/>
+      <c r="F99" s="62"/>
+      <c r="G99" s="62"/>
+      <c r="H99" s="63"/>
       <c r="I99" s="2"/>
       <c r="J99" s="2"/>
       <c r="K99" s="2"/>
@@ -5053,17 +5073,19 @@
       <c r="Y99" s="2"/>
       <c r="Z99" s="2"/>
     </row>
-    <row r="100" spans="1:26" ht="15" customHeight="1">
-      <c r="A100" s="42" t="s">
-        <v>4</v>
-      </c>
-      <c r="B100" s="36"/>
-      <c r="C100" s="36"/>
-      <c r="D100" s="36"/>
-      <c r="E100" s="36"/>
-      <c r="F100" s="36"/>
-      <c r="G100" s="36"/>
-      <c r="H100" s="37"/>
+    <row r="100" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A100" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B100" s="66" t="s">
+        <v>147</v>
+      </c>
+      <c r="C100" s="52"/>
+      <c r="D100" s="52"/>
+      <c r="E100" s="52"/>
+      <c r="F100" s="52"/>
+      <c r="G100" s="52"/>
+      <c r="H100" s="53"/>
       <c r="I100" s="2"/>
       <c r="J100" s="2"/>
       <c r="K100" s="2"/>
@@ -5084,28 +5106,16 @@
       <c r="Z100" s="2"/>
     </row>
     <row r="101" spans="1:26" ht="15" customHeight="1">
-      <c r="A101" s="43" t="s">
-        <v>5</v>
-      </c>
-      <c r="B101" s="44"/>
-      <c r="C101" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D101" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E101" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F101" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G101" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H101" s="3" t="s">
-        <v>151</v>
-      </c>
+      <c r="A101" s="54" t="s">
+        <v>4</v>
+      </c>
+      <c r="B101" s="52"/>
+      <c r="C101" s="52"/>
+      <c r="D101" s="52"/>
+      <c r="E101" s="52"/>
+      <c r="F101" s="52"/>
+      <c r="G101" s="52"/>
+      <c r="H101" s="53"/>
       <c r="I101" s="2"/>
       <c r="J101" s="2"/>
       <c r="K101" s="2"/>
@@ -5126,25 +5136,27 @@
       <c r="Z101" s="2"/>
     </row>
     <row r="102" spans="1:26" ht="15" customHeight="1">
-      <c r="A102" s="45" t="s">
-        <v>152</v>
-      </c>
-      <c r="B102" s="44"/>
-      <c r="C102" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D102" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E102" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="F102" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="G102" s="5"/>
-      <c r="H102" s="6" t="s">
-        <v>151</v>
+      <c r="A102" s="51" t="s">
+        <v>5</v>
+      </c>
+      <c r="B102" s="43"/>
+      <c r="C102" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D102" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E102" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F102" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G102" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H102" s="3" t="s">
+        <v>148</v>
       </c>
       <c r="I102" s="2"/>
       <c r="J102" s="2"/>
@@ -5166,10 +5178,10 @@
       <c r="Z102" s="2"/>
     </row>
     <row r="103" spans="1:26" ht="15" customHeight="1">
-      <c r="A103" s="45" t="s">
-        <v>62</v>
-      </c>
-      <c r="B103" s="44"/>
+      <c r="A103" s="42" t="s">
+        <v>149</v>
+      </c>
+      <c r="B103" s="43"/>
       <c r="C103" s="4" t="s">
         <v>12</v>
       </c>
@@ -5179,12 +5191,12 @@
       <c r="E103" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="F103" s="5"/>
-      <c r="G103" s="5" t="s">
+      <c r="F103" s="5" t="s">
         <v>15</v>
       </c>
+      <c r="G103" s="5"/>
       <c r="H103" s="6" t="s">
-        <v>63</v>
+        <v>148</v>
       </c>
       <c r="I103" s="2"/>
       <c r="J103" s="2"/>
@@ -5206,23 +5218,25 @@
       <c r="Z103" s="2"/>
     </row>
     <row r="104" spans="1:26" ht="15" customHeight="1">
-      <c r="A104" s="45" t="s">
-        <v>153</v>
-      </c>
-      <c r="B104" s="44"/>
+      <c r="A104" s="42" t="s">
+        <v>61</v>
+      </c>
+      <c r="B104" s="43"/>
       <c r="C104" s="4" t="s">
-        <v>154</v>
+        <v>12</v>
       </c>
       <c r="D104" s="4" t="s">
-        <v>155</v>
+        <v>13</v>
       </c>
       <c r="E104" s="4" t="s">
         <v>14</v>
       </c>
       <c r="F104" s="5"/>
-      <c r="G104" s="5"/>
+      <c r="G104" s="5" t="s">
+        <v>15</v>
+      </c>
       <c r="H104" s="6" t="s">
-        <v>156</v>
+        <v>62</v>
       </c>
       <c r="I104" s="2"/>
       <c r="J104" s="2"/>
@@ -5243,16 +5257,16 @@
       <c r="Y104" s="2"/>
       <c r="Z104" s="2"/>
     </row>
-    <row r="105" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A105" s="45" t="s">
-        <v>157</v>
-      </c>
-      <c r="B105" s="44"/>
+    <row r="105" spans="1:26" ht="15" customHeight="1">
+      <c r="A105" s="42" t="s">
+        <v>150</v>
+      </c>
+      <c r="B105" s="43"/>
       <c r="C105" s="4" t="s">
-        <v>22</v>
+        <v>151</v>
       </c>
       <c r="D105" s="4" t="s">
-        <v>23</v>
+        <v>152</v>
       </c>
       <c r="E105" s="4" t="s">
         <v>14</v>
@@ -5260,7 +5274,7 @@
       <c r="F105" s="5"/>
       <c r="G105" s="5"/>
       <c r="H105" s="6" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="I105" s="2"/>
       <c r="J105" s="2"/>
@@ -5282,15 +5296,15 @@
       <c r="Z105" s="2"/>
     </row>
     <row r="106" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A106" s="45" t="s">
-        <v>159</v>
-      </c>
-      <c r="B106" s="44"/>
+      <c r="A106" s="42" t="s">
+        <v>154</v>
+      </c>
+      <c r="B106" s="43"/>
       <c r="C106" s="4" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="D106" s="4" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="E106" s="4" t="s">
         <v>14</v>
@@ -5298,7 +5312,7 @@
       <c r="F106" s="5"/>
       <c r="G106" s="5"/>
       <c r="H106" s="6" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="I106" s="2"/>
       <c r="J106" s="2"/>
@@ -5320,23 +5334,23 @@
       <c r="Z106" s="2"/>
     </row>
     <row r="107" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A107" s="62" t="s">
-        <v>161</v>
-      </c>
-      <c r="B107" s="57"/>
-      <c r="C107" s="23" t="s">
-        <v>162</v>
-      </c>
-      <c r="D107" s="23" t="s">
-        <v>163</v>
-      </c>
-      <c r="E107" s="23" t="s">
+      <c r="A107" s="42" t="s">
+        <v>156</v>
+      </c>
+      <c r="B107" s="43"/>
+      <c r="C107" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D107" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E107" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="F107" s="31"/>
-      <c r="G107" s="31"/>
-      <c r="H107" s="32" t="s">
-        <v>164</v>
+      <c r="F107" s="5"/>
+      <c r="G107" s="5"/>
+      <c r="H107" s="6" t="s">
+        <v>157</v>
       </c>
       <c r="I107" s="2"/>
       <c r="J107" s="2"/>
@@ -5358,16 +5372,24 @@
       <c r="Z107" s="2"/>
     </row>
     <row r="108" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A108" s="51" t="s">
-        <v>49</v>
-      </c>
-      <c r="B108" s="52"/>
-      <c r="C108" s="52"/>
-      <c r="D108" s="52"/>
-      <c r="E108" s="52"/>
-      <c r="F108" s="52"/>
-      <c r="G108" s="52"/>
-      <c r="H108" s="53"/>
+      <c r="A108" s="45" t="s">
+        <v>158</v>
+      </c>
+      <c r="B108" s="39"/>
+      <c r="C108" s="23" t="s">
+        <v>159</v>
+      </c>
+      <c r="D108" s="23" t="s">
+        <v>160</v>
+      </c>
+      <c r="E108" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="F108" s="31"/>
+      <c r="G108" s="31"/>
+      <c r="H108" s="32" t="s">
+        <v>161</v>
+      </c>
       <c r="I108" s="2"/>
       <c r="J108" s="2"/>
       <c r="K108" s="2"/>
@@ -5388,24 +5410,16 @@
       <c r="Z108" s="2"/>
     </row>
     <row r="109" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A109" s="43" t="s">
-        <v>50</v>
-      </c>
-      <c r="B109" s="44"/>
-      <c r="C109" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="D109" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="E109" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="F109" s="43" t="s">
-        <v>54</v>
-      </c>
-      <c r="G109" s="36"/>
-      <c r="H109" s="37"/>
+      <c r="A109" s="48" t="s">
+        <v>48</v>
+      </c>
+      <c r="B109" s="49"/>
+      <c r="C109" s="49"/>
+      <c r="D109" s="49"/>
+      <c r="E109" s="49"/>
+      <c r="F109" s="49"/>
+      <c r="G109" s="49"/>
+      <c r="H109" s="50"/>
       <c r="I109" s="2"/>
       <c r="J109" s="2"/>
       <c r="K109" s="2"/>
@@ -5426,22 +5440,24 @@
       <c r="Z109" s="2"/>
     </row>
     <row r="110" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A110" s="35" t="s">
-        <v>165</v>
-      </c>
-      <c r="B110" s="44"/>
-      <c r="C110" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="D110" s="16"/>
-      <c r="E110" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="F110" s="35" t="s">
-        <v>152</v>
-      </c>
-      <c r="G110" s="36"/>
-      <c r="H110" s="37"/>
+      <c r="A110" s="51" t="s">
+        <v>49</v>
+      </c>
+      <c r="B110" s="43"/>
+      <c r="C110" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D110" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E110" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F110" s="51" t="s">
+        <v>53</v>
+      </c>
+      <c r="G110" s="52"/>
+      <c r="H110" s="53"/>
       <c r="I110" s="2"/>
       <c r="J110" s="2"/>
       <c r="K110" s="2"/>
@@ -5462,22 +5478,22 @@
       <c r="Z110" s="2"/>
     </row>
     <row r="111" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A111" s="35" t="s">
-        <v>166</v>
-      </c>
-      <c r="B111" s="44"/>
-      <c r="C111" s="15"/>
-      <c r="D111" s="15" t="s">
+      <c r="A111" s="44" t="s">
+        <v>162</v>
+      </c>
+      <c r="B111" s="43"/>
+      <c r="C111" s="15" t="s">
         <v>15</v>
       </c>
+      <c r="D111" s="16"/>
       <c r="E111" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="F111" s="35" t="s">
-        <v>153</v>
-      </c>
-      <c r="G111" s="36"/>
-      <c r="H111" s="37"/>
+      <c r="F111" s="44" t="s">
+        <v>149</v>
+      </c>
+      <c r="G111" s="52"/>
+      <c r="H111" s="53"/>
       <c r="I111" s="2"/>
       <c r="J111" s="2"/>
       <c r="K111" s="2"/>
@@ -5498,14 +5514,22 @@
       <c r="Z111" s="2"/>
     </row>
     <row r="112" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A112" s="19"/>
-      <c r="B112" s="19"/>
-      <c r="C112" s="19"/>
-      <c r="D112" s="19"/>
-      <c r="E112" s="19"/>
-      <c r="F112" s="19"/>
-      <c r="G112" s="19"/>
-      <c r="H112" s="19"/>
+      <c r="A112" s="44" t="s">
+        <v>163</v>
+      </c>
+      <c r="B112" s="43"/>
+      <c r="C112" s="15"/>
+      <c r="D112" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="E112" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="F112" s="44" t="s">
+        <v>150</v>
+      </c>
+      <c r="G112" s="52"/>
+      <c r="H112" s="53"/>
       <c r="I112" s="2"/>
       <c r="J112" s="2"/>
       <c r="K112" s="2"/>
@@ -5526,18 +5550,14 @@
       <c r="Z112" s="2"/>
     </row>
     <row r="113" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A113" s="20" t="s">
-        <v>59</v>
-      </c>
-      <c r="B113" s="38" t="s">
-        <v>167</v>
-      </c>
-      <c r="C113" s="39"/>
-      <c r="D113" s="39"/>
-      <c r="E113" s="39"/>
-      <c r="F113" s="39"/>
-      <c r="G113" s="39"/>
-      <c r="H113" s="40"/>
+      <c r="A113" s="19"/>
+      <c r="B113" s="19"/>
+      <c r="C113" s="19"/>
+      <c r="D113" s="19"/>
+      <c r="E113" s="19"/>
+      <c r="F113" s="19"/>
+      <c r="G113" s="19"/>
+      <c r="H113" s="19"/>
       <c r="I113" s="2"/>
       <c r="J113" s="2"/>
       <c r="K113" s="2"/>
@@ -5558,18 +5578,18 @@
       <c r="Z113" s="2"/>
     </row>
     <row r="114" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A114" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B114" s="41" t="s">
-        <v>168</v>
-      </c>
-      <c r="C114" s="36"/>
-      <c r="D114" s="36"/>
-      <c r="E114" s="36"/>
-      <c r="F114" s="36"/>
-      <c r="G114" s="36"/>
-      <c r="H114" s="37"/>
+      <c r="A114" s="20" t="s">
+        <v>58</v>
+      </c>
+      <c r="B114" s="61" t="s">
+        <v>164</v>
+      </c>
+      <c r="C114" s="62"/>
+      <c r="D114" s="62"/>
+      <c r="E114" s="62"/>
+      <c r="F114" s="62"/>
+      <c r="G114" s="62"/>
+      <c r="H114" s="63"/>
       <c r="I114" s="2"/>
       <c r="J114" s="2"/>
       <c r="K114" s="2"/>
@@ -5590,16 +5610,18 @@
       <c r="Z114" s="2"/>
     </row>
     <row r="115" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A115" s="42" t="s">
-        <v>4</v>
-      </c>
-      <c r="B115" s="36"/>
-      <c r="C115" s="36"/>
-      <c r="D115" s="36"/>
-      <c r="E115" s="36"/>
-      <c r="F115" s="36"/>
-      <c r="G115" s="36"/>
-      <c r="H115" s="37"/>
+      <c r="A115" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B115" s="66" t="s">
+        <v>165</v>
+      </c>
+      <c r="C115" s="52"/>
+      <c r="D115" s="52"/>
+      <c r="E115" s="52"/>
+      <c r="F115" s="52"/>
+      <c r="G115" s="52"/>
+      <c r="H115" s="53"/>
       <c r="I115" s="2"/>
       <c r="J115" s="2"/>
       <c r="K115" s="2"/>
@@ -5620,28 +5642,16 @@
       <c r="Z115" s="2"/>
     </row>
     <row r="116" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A116" s="43" t="s">
-        <v>5</v>
-      </c>
-      <c r="B116" s="44"/>
-      <c r="C116" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D116" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E116" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F116" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G116" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H116" s="3" t="s">
-        <v>2</v>
-      </c>
+      <c r="A116" s="54" t="s">
+        <v>4</v>
+      </c>
+      <c r="B116" s="52"/>
+      <c r="C116" s="52"/>
+      <c r="D116" s="52"/>
+      <c r="E116" s="52"/>
+      <c r="F116" s="52"/>
+      <c r="G116" s="52"/>
+      <c r="H116" s="53"/>
       <c r="I116" s="2"/>
       <c r="J116" s="2"/>
       <c r="K116" s="2"/>
@@ -5662,25 +5672,27 @@
       <c r="Z116" s="2"/>
     </row>
     <row r="117" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A117" s="45" t="s">
-        <v>169</v>
-      </c>
-      <c r="B117" s="44"/>
-      <c r="C117" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D117" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E117" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="F117" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="G117" s="5"/>
-      <c r="H117" s="6" t="s">
-        <v>170</v>
+      <c r="A117" s="51" t="s">
+        <v>5</v>
+      </c>
+      <c r="B117" s="43"/>
+      <c r="C117" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D117" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E117" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F117" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G117" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H117" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="I117" s="2"/>
       <c r="J117" s="2"/>
@@ -5702,10 +5714,10 @@
       <c r="Z117" s="2"/>
     </row>
     <row r="118" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A118" s="45" t="s">
-        <v>101</v>
-      </c>
-      <c r="B118" s="44"/>
+      <c r="A118" s="42" t="s">
+        <v>166</v>
+      </c>
+      <c r="B118" s="43"/>
       <c r="C118" s="4" t="s">
         <v>12</v>
       </c>
@@ -5715,12 +5727,12 @@
       <c r="E118" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="F118" s="5"/>
-      <c r="G118" s="5" t="s">
+      <c r="F118" s="5" t="s">
         <v>15</v>
       </c>
+      <c r="G118" s="5"/>
       <c r="H118" s="6" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="I118" s="2"/>
       <c r="J118" s="2"/>
@@ -5742,10 +5754,10 @@
       <c r="Z118" s="2"/>
     </row>
     <row r="119" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A119" s="45" t="s">
-        <v>62</v>
-      </c>
-      <c r="B119" s="44"/>
+      <c r="A119" s="42" t="s">
+        <v>99</v>
+      </c>
+      <c r="B119" s="43"/>
       <c r="C119" s="4" t="s">
         <v>12</v>
       </c>
@@ -5760,7 +5772,7 @@
         <v>15</v>
       </c>
       <c r="H119" s="6" t="s">
-        <v>63</v>
+        <v>168</v>
       </c>
       <c r="I119" s="2"/>
       <c r="J119" s="2"/>
@@ -5782,23 +5794,25 @@
       <c r="Z119" s="2"/>
     </row>
     <row r="120" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A120" s="45" t="s">
-        <v>113</v>
-      </c>
-      <c r="B120" s="44"/>
+      <c r="A120" s="42" t="s">
+        <v>61</v>
+      </c>
+      <c r="B120" s="43"/>
       <c r="C120" s="4" t="s">
-        <v>68</v>
+        <v>12</v>
       </c>
       <c r="D120" s="4" t="s">
-        <v>172</v>
+        <v>13</v>
       </c>
       <c r="E120" s="4" t="s">
-        <v>72</v>
+        <v>14</v>
       </c>
       <c r="F120" s="5"/>
-      <c r="G120" s="5"/>
+      <c r="G120" s="5" t="s">
+        <v>15</v>
+      </c>
       <c r="H120" s="6" t="s">
-        <v>173</v>
+        <v>62</v>
       </c>
       <c r="I120" s="2"/>
       <c r="J120" s="2"/>
@@ -5820,23 +5834,23 @@
       <c r="Z120" s="2"/>
     </row>
     <row r="121" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A121" s="66" t="s">
-        <v>121</v>
-      </c>
-      <c r="B121" s="47"/>
-      <c r="C121" s="12" t="s">
-        <v>68</v>
+      <c r="A121" s="42" t="s">
+        <v>111</v>
+      </c>
+      <c r="B121" s="43"/>
+      <c r="C121" s="4" t="s">
+        <v>67</v>
       </c>
       <c r="D121" s="4" t="s">
-        <v>172</v>
-      </c>
-      <c r="E121" s="12" t="s">
-        <v>72</v>
-      </c>
-      <c r="F121" s="29"/>
-      <c r="G121" s="29"/>
-      <c r="H121" s="30" t="s">
-        <v>174</v>
+        <v>169</v>
+      </c>
+      <c r="E121" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F121" s="5"/>
+      <c r="G121" s="5"/>
+      <c r="H121" s="6" t="s">
+        <v>170</v>
       </c>
       <c r="I121" s="2"/>
       <c r="J121" s="2"/>
@@ -5858,23 +5872,23 @@
       <c r="Z121" s="2"/>
     </row>
     <row r="122" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A122" s="62" t="s">
-        <v>175</v>
-      </c>
-      <c r="B122" s="57"/>
-      <c r="C122" s="23" t="s">
-        <v>30</v>
-      </c>
-      <c r="D122" s="23" t="s">
-        <v>31</v>
-      </c>
-      <c r="E122" s="23" t="s">
+      <c r="A122" s="46" t="s">
+        <v>119</v>
+      </c>
+      <c r="B122" s="47"/>
+      <c r="C122" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="D122" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="E122" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="F122" s="31"/>
-      <c r="G122" s="31"/>
-      <c r="H122" s="32" t="s">
-        <v>176</v>
+      <c r="F122" s="29"/>
+      <c r="G122" s="29"/>
+      <c r="H122" s="30" t="s">
+        <v>171</v>
       </c>
       <c r="I122" s="2"/>
       <c r="J122" s="2"/>
@@ -5895,17 +5909,25 @@
       <c r="Y122" s="2"/>
       <c r="Z122" s="2"/>
     </row>
-    <row r="123" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A123" s="51" t="s">
-        <v>49</v>
-      </c>
-      <c r="B123" s="52"/>
-      <c r="C123" s="52"/>
-      <c r="D123" s="52"/>
-      <c r="E123" s="52"/>
-      <c r="F123" s="52"/>
-      <c r="G123" s="52"/>
-      <c r="H123" s="53"/>
+    <row r="123" spans="1:26" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A123" s="45" t="s">
+        <v>172</v>
+      </c>
+      <c r="B123" s="39"/>
+      <c r="C123" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="D123" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="E123" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="F123" s="31"/>
+      <c r="G123" s="31"/>
+      <c r="H123" s="32" t="s">
+        <v>173</v>
+      </c>
       <c r="I123" s="2"/>
       <c r="J123" s="2"/>
       <c r="K123" s="2"/>
@@ -5926,24 +5948,16 @@
       <c r="Z123" s="2"/>
     </row>
     <row r="124" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A124" s="43" t="s">
-        <v>50</v>
-      </c>
-      <c r="B124" s="44"/>
-      <c r="C124" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="D124" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="E124" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="F124" s="43" t="s">
-        <v>54</v>
-      </c>
-      <c r="G124" s="36"/>
-      <c r="H124" s="37"/>
+      <c r="A124" s="48" t="s">
+        <v>48</v>
+      </c>
+      <c r="B124" s="49"/>
+      <c r="C124" s="49"/>
+      <c r="D124" s="49"/>
+      <c r="E124" s="49"/>
+      <c r="F124" s="49"/>
+      <c r="G124" s="49"/>
+      <c r="H124" s="50"/>
       <c r="I124" s="2"/>
       <c r="J124" s="2"/>
       <c r="K124" s="2"/>
@@ -5964,22 +5978,24 @@
       <c r="Z124" s="2"/>
     </row>
     <row r="125" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A125" s="67" t="s">
-        <v>177</v>
-      </c>
-      <c r="B125" s="57"/>
-      <c r="C125" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="D125" s="34"/>
-      <c r="E125" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="F125" s="67" t="s">
-        <v>169</v>
-      </c>
-      <c r="G125" s="59"/>
-      <c r="H125" s="60"/>
+      <c r="A125" s="51" t="s">
+        <v>49</v>
+      </c>
+      <c r="B125" s="43"/>
+      <c r="C125" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D125" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E125" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F125" s="51" t="s">
+        <v>53</v>
+      </c>
+      <c r="G125" s="52"/>
+      <c r="H125" s="53"/>
       <c r="I125" s="2"/>
       <c r="J125" s="2"/>
       <c r="K125" s="2"/>
@@ -6000,14 +6016,22 @@
       <c r="Z125" s="2"/>
     </row>
     <row r="126" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A126" s="2"/>
-      <c r="B126" s="2"/>
-      <c r="C126" s="2"/>
-      <c r="D126" s="2"/>
-      <c r="E126" s="2"/>
-      <c r="F126" s="2"/>
-      <c r="G126" s="2"/>
-      <c r="H126" s="2"/>
+      <c r="A126" s="38" t="s">
+        <v>174</v>
+      </c>
+      <c r="B126" s="39"/>
+      <c r="C126" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="D126" s="34"/>
+      <c r="E126" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="F126" s="38" t="s">
+        <v>166</v>
+      </c>
+      <c r="G126" s="40"/>
+      <c r="H126" s="41"/>
       <c r="I126" s="2"/>
       <c r="J126" s="2"/>
       <c r="K126" s="2"/>
@@ -6111,7 +6135,7 @@
       <c r="Y129" s="2"/>
       <c r="Z129" s="2"/>
     </row>
-    <row r="130" spans="1:26" ht="15" customHeight="1">
+    <row r="130" spans="1:26" ht="15.75" customHeight="1">
       <c r="A130" s="2"/>
       <c r="B130" s="2"/>
       <c r="C130" s="2"/>
@@ -6139,7 +6163,7 @@
       <c r="Y130" s="2"/>
       <c r="Z130" s="2"/>
     </row>
-    <row r="131" spans="1:26" ht="15.75" customHeight="1">
+    <row r="131" spans="1:26" ht="15" customHeight="1">
       <c r="A131" s="2"/>
       <c r="B131" s="2"/>
       <c r="C131" s="2"/>
@@ -6307,7 +6331,7 @@
       <c r="Y136" s="2"/>
       <c r="Z136" s="2"/>
     </row>
-    <row r="137" spans="1:26" ht="15" customHeight="1">
+    <row r="137" spans="1:26" ht="15.75" customHeight="1">
       <c r="A137" s="2"/>
       <c r="B137" s="2"/>
       <c r="C137" s="2"/>
@@ -6335,7 +6359,7 @@
       <c r="Y137" s="2"/>
       <c r="Z137" s="2"/>
     </row>
-    <row r="138" spans="1:26" ht="15.75" customHeight="1">
+    <row r="138" spans="1:26" ht="15" customHeight="1">
       <c r="A138" s="2"/>
       <c r="B138" s="2"/>
       <c r="C138" s="2"/>
@@ -6363,7 +6387,7 @@
       <c r="Y138" s="2"/>
       <c r="Z138" s="2"/>
     </row>
-    <row r="139" spans="1:26" ht="15" customHeight="1">
+    <row r="139" spans="1:26" ht="15.75" customHeight="1">
       <c r="A139" s="2"/>
       <c r="B139" s="2"/>
       <c r="C139" s="2"/>
@@ -6391,7 +6415,7 @@
       <c r="Y139" s="2"/>
       <c r="Z139" s="2"/>
     </row>
-    <row r="140" spans="1:26" ht="15.75" customHeight="1">
+    <row r="140" spans="1:26" ht="15" customHeight="1">
       <c r="A140" s="2"/>
       <c r="B140" s="2"/>
       <c r="C140" s="2"/>
@@ -30583,95 +30607,63 @@
       <c r="Y1003" s="2"/>
       <c r="Z1003" s="2"/>
     </row>
+    <row r="1004" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A1004" s="2"/>
+      <c r="B1004" s="2"/>
+      <c r="C1004" s="2"/>
+      <c r="D1004" s="2"/>
+      <c r="E1004" s="2"/>
+      <c r="F1004" s="2"/>
+      <c r="G1004" s="2"/>
+      <c r="H1004" s="2"/>
+      <c r="I1004" s="2"/>
+      <c r="J1004" s="2"/>
+      <c r="K1004" s="2"/>
+      <c r="L1004" s="2"/>
+      <c r="M1004" s="2"/>
+      <c r="N1004" s="2"/>
+      <c r="O1004" s="2"/>
+      <c r="P1004" s="2"/>
+      <c r="Q1004" s="2"/>
+      <c r="R1004" s="2"/>
+      <c r="S1004" s="2"/>
+      <c r="T1004" s="2"/>
+      <c r="U1004" s="2"/>
+      <c r="V1004" s="2"/>
+      <c r="W1004" s="2"/>
+      <c r="X1004" s="2"/>
+      <c r="Y1004" s="2"/>
+      <c r="Z1004" s="2"/>
+    </row>
   </sheetData>
-  <mergeCells count="138">
-    <mergeCell ref="A125:B125"/>
-    <mergeCell ref="F125:H125"/>
-    <mergeCell ref="A104:B104"/>
-    <mergeCell ref="A110:B110"/>
-    <mergeCell ref="A111:B111"/>
-    <mergeCell ref="A122:B122"/>
-    <mergeCell ref="A121:B121"/>
-    <mergeCell ref="A119:B119"/>
-    <mergeCell ref="A120:B120"/>
-    <mergeCell ref="A123:H123"/>
-    <mergeCell ref="A124:B124"/>
-    <mergeCell ref="F124:H124"/>
-    <mergeCell ref="A116:B116"/>
-    <mergeCell ref="A117:B117"/>
-    <mergeCell ref="A118:B118"/>
-    <mergeCell ref="A70:H70"/>
-    <mergeCell ref="A71:B71"/>
-    <mergeCell ref="A72:B72"/>
+  <mergeCells count="139">
+    <mergeCell ref="B38:H38"/>
+    <mergeCell ref="B39:H39"/>
+    <mergeCell ref="A40:H40"/>
+    <mergeCell ref="A41:B41"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="A44:B44"/>
+    <mergeCell ref="A45:B45"/>
     <mergeCell ref="A73:B73"/>
-    <mergeCell ref="A74:B74"/>
-    <mergeCell ref="A75:B75"/>
-    <mergeCell ref="A76:B76"/>
-    <mergeCell ref="A77:B77"/>
-    <mergeCell ref="A79:H79"/>
-    <mergeCell ref="A80:B80"/>
-    <mergeCell ref="F80:H80"/>
-    <mergeCell ref="A81:B81"/>
-    <mergeCell ref="F81:H81"/>
-    <mergeCell ref="B83:H83"/>
-    <mergeCell ref="A78:B78"/>
-    <mergeCell ref="B84:H84"/>
-    <mergeCell ref="A85:H85"/>
-    <mergeCell ref="A86:B86"/>
-    <mergeCell ref="A87:B87"/>
-    <mergeCell ref="A89:B89"/>
-    <mergeCell ref="A90:B90"/>
-    <mergeCell ref="A107:B107"/>
-    <mergeCell ref="A108:H108"/>
-    <mergeCell ref="A109:B109"/>
-    <mergeCell ref="F109:H109"/>
-    <mergeCell ref="F110:H110"/>
-    <mergeCell ref="F111:H111"/>
-    <mergeCell ref="B113:H113"/>
-    <mergeCell ref="B114:H114"/>
-    <mergeCell ref="A115:H115"/>
-    <mergeCell ref="A63:B63"/>
-    <mergeCell ref="A65:B65"/>
-    <mergeCell ref="F65:H65"/>
-    <mergeCell ref="A66:B66"/>
-    <mergeCell ref="F66:H66"/>
-    <mergeCell ref="B68:H68"/>
-    <mergeCell ref="B69:H69"/>
-    <mergeCell ref="A105:B105"/>
-    <mergeCell ref="A106:B106"/>
-    <mergeCell ref="A91:B91"/>
-    <mergeCell ref="A88:B88"/>
-    <mergeCell ref="A92:B92"/>
-    <mergeCell ref="A93:B93"/>
-    <mergeCell ref="A94:H94"/>
-    <mergeCell ref="A95:B95"/>
-    <mergeCell ref="F95:H95"/>
-    <mergeCell ref="A96:B96"/>
-    <mergeCell ref="F96:H96"/>
-    <mergeCell ref="B98:H98"/>
-    <mergeCell ref="B99:H99"/>
-    <mergeCell ref="A100:H100"/>
-    <mergeCell ref="A101:B101"/>
-    <mergeCell ref="A102:B102"/>
-    <mergeCell ref="A103:B103"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="A34:H34"/>
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="F35:H35"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="F19:H19"/>
-    <mergeCell ref="F20:H20"/>
-    <mergeCell ref="B22:H22"/>
-    <mergeCell ref="B23:H23"/>
-    <mergeCell ref="A24:H24"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="A48:B48"/>
+    <mergeCell ref="A49:H49"/>
+    <mergeCell ref="F50:H50"/>
+    <mergeCell ref="A50:B50"/>
+    <mergeCell ref="A51:B51"/>
+    <mergeCell ref="F51:H51"/>
+    <mergeCell ref="B53:H53"/>
+    <mergeCell ref="B54:H54"/>
+    <mergeCell ref="A55:H55"/>
+    <mergeCell ref="A56:B56"/>
+    <mergeCell ref="A57:B57"/>
+    <mergeCell ref="A58:B58"/>
+    <mergeCell ref="A59:B59"/>
+    <mergeCell ref="A60:B60"/>
+    <mergeCell ref="A61:B61"/>
+    <mergeCell ref="A62:B62"/>
     <mergeCell ref="A64:H64"/>
     <mergeCell ref="B1:H1"/>
     <mergeCell ref="B2:H2"/>
@@ -30696,33 +30688,94 @@
     <mergeCell ref="F16:H16"/>
     <mergeCell ref="F17:H17"/>
     <mergeCell ref="F18:H18"/>
-    <mergeCell ref="B54:H54"/>
-    <mergeCell ref="A55:H55"/>
-    <mergeCell ref="A56:B56"/>
-    <mergeCell ref="A57:B57"/>
-    <mergeCell ref="A58:B58"/>
-    <mergeCell ref="A59:B59"/>
-    <mergeCell ref="A60:B60"/>
-    <mergeCell ref="A61:B61"/>
-    <mergeCell ref="A62:B62"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="A47:B47"/>
-    <mergeCell ref="A48:B48"/>
-    <mergeCell ref="A49:H49"/>
-    <mergeCell ref="F50:H50"/>
-    <mergeCell ref="A50:B50"/>
-    <mergeCell ref="A51:B51"/>
-    <mergeCell ref="F51:H51"/>
-    <mergeCell ref="B53:H53"/>
+    <mergeCell ref="F19:H19"/>
+    <mergeCell ref="F20:H20"/>
+    <mergeCell ref="B22:H22"/>
+    <mergeCell ref="B23:H23"/>
+    <mergeCell ref="A24:H24"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="A34:H34"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="F35:H35"/>
+    <mergeCell ref="A36:B36"/>
     <mergeCell ref="F36:H36"/>
-    <mergeCell ref="B38:H38"/>
-    <mergeCell ref="B39:H39"/>
-    <mergeCell ref="A40:H40"/>
-    <mergeCell ref="A41:B41"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="A44:B44"/>
-    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="A63:B63"/>
+    <mergeCell ref="A65:B65"/>
+    <mergeCell ref="F65:H65"/>
+    <mergeCell ref="A66:B66"/>
+    <mergeCell ref="F66:H66"/>
+    <mergeCell ref="B68:H68"/>
+    <mergeCell ref="B69:H69"/>
+    <mergeCell ref="A106:B106"/>
+    <mergeCell ref="A107:B107"/>
+    <mergeCell ref="A92:B92"/>
+    <mergeCell ref="A89:B89"/>
+    <mergeCell ref="A93:B93"/>
+    <mergeCell ref="A94:B94"/>
+    <mergeCell ref="A95:H95"/>
+    <mergeCell ref="A96:B96"/>
+    <mergeCell ref="F96:H96"/>
+    <mergeCell ref="A97:B97"/>
+    <mergeCell ref="F97:H97"/>
+    <mergeCell ref="B99:H99"/>
+    <mergeCell ref="B100:H100"/>
+    <mergeCell ref="A101:H101"/>
+    <mergeCell ref="A102:B102"/>
+    <mergeCell ref="A103:B103"/>
+    <mergeCell ref="A104:B104"/>
+    <mergeCell ref="A88:B88"/>
+    <mergeCell ref="A90:B90"/>
+    <mergeCell ref="A91:B91"/>
+    <mergeCell ref="A108:B108"/>
+    <mergeCell ref="A109:H109"/>
+    <mergeCell ref="A110:B110"/>
+    <mergeCell ref="F110:H110"/>
+    <mergeCell ref="F111:H111"/>
+    <mergeCell ref="F112:H112"/>
+    <mergeCell ref="A81:B81"/>
+    <mergeCell ref="F81:H81"/>
+    <mergeCell ref="A82:B82"/>
+    <mergeCell ref="F82:H82"/>
+    <mergeCell ref="B84:H84"/>
+    <mergeCell ref="A79:B79"/>
+    <mergeCell ref="B85:H85"/>
+    <mergeCell ref="A86:H86"/>
+    <mergeCell ref="A87:B87"/>
+    <mergeCell ref="A70:H70"/>
+    <mergeCell ref="A71:B71"/>
+    <mergeCell ref="A72:B72"/>
+    <mergeCell ref="A74:B74"/>
+    <mergeCell ref="A75:B75"/>
+    <mergeCell ref="A76:B76"/>
+    <mergeCell ref="A77:B77"/>
+    <mergeCell ref="A78:B78"/>
+    <mergeCell ref="A80:H80"/>
+    <mergeCell ref="A126:B126"/>
+    <mergeCell ref="F126:H126"/>
+    <mergeCell ref="A105:B105"/>
+    <mergeCell ref="A111:B111"/>
+    <mergeCell ref="A112:B112"/>
+    <mergeCell ref="A123:B123"/>
+    <mergeCell ref="A122:B122"/>
+    <mergeCell ref="A120:B120"/>
+    <mergeCell ref="A121:B121"/>
+    <mergeCell ref="A124:H124"/>
+    <mergeCell ref="A125:B125"/>
+    <mergeCell ref="F125:H125"/>
+    <mergeCell ref="A117:B117"/>
+    <mergeCell ref="A118:B118"/>
+    <mergeCell ref="A119:B119"/>
+    <mergeCell ref="B114:H114"/>
+    <mergeCell ref="B115:H115"/>
+    <mergeCell ref="A116:H116"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>

<commit_message>
Alteração das colunas da tabela empréstimo para datetime
</commit_message>
<xml_diff>
--- a/Dicionário/Dicionario_de_dados.xlsx
+++ b/Dicionário/Dicionario_de_dados.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luigi\Desktop\Faculdade\3 FASE\Banco de Dados II\ABP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C94E3850-052B-4E8A-9895-BA4A3509F73F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCE93C6C-04B7-4EAD-969E-C48550B07B67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5340" yWindow="2460" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5685" yWindow="2805" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dicionario" sheetId="1" r:id="rId1"/>
@@ -1201,32 +1201,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1234,6 +1214,61 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1244,45 +1279,10 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1519,15 +1519,15 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="72" t="s">
+      <c r="B1" s="58" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="52"/>
-      <c r="D1" s="52"/>
-      <c r="E1" s="52"/>
-      <c r="F1" s="52"/>
-      <c r="G1" s="52"/>
-      <c r="H1" s="53"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="42"/>
+      <c r="H1" s="43"/>
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
       <c r="K1" s="2"/>
@@ -1551,15 +1551,15 @@
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="66" t="s">
+      <c r="B2" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="52"/>
-      <c r="D2" s="52"/>
-      <c r="E2" s="52"/>
-      <c r="F2" s="52"/>
-      <c r="G2" s="52"/>
-      <c r="H2" s="53"/>
+      <c r="C2" s="42"/>
+      <c r="D2" s="42"/>
+      <c r="E2" s="42"/>
+      <c r="F2" s="42"/>
+      <c r="G2" s="42"/>
+      <c r="H2" s="43"/>
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
@@ -1580,16 +1580,16 @@
       <c r="Z2" s="2"/>
     </row>
     <row r="3" spans="1:26">
-      <c r="A3" s="54" t="s">
+      <c r="A3" s="44" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="52"/>
-      <c r="C3" s="52"/>
-      <c r="D3" s="52"/>
-      <c r="E3" s="52"/>
-      <c r="F3" s="52"/>
-      <c r="G3" s="52"/>
-      <c r="H3" s="53"/>
+      <c r="B3" s="42"/>
+      <c r="C3" s="42"/>
+      <c r="D3" s="42"/>
+      <c r="E3" s="42"/>
+      <c r="F3" s="42"/>
+      <c r="G3" s="42"/>
+      <c r="H3" s="43"/>
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
@@ -1610,10 +1610,10 @@
       <c r="Z3" s="2"/>
     </row>
     <row r="4" spans="1:26">
-      <c r="A4" s="51" t="s">
+      <c r="A4" s="45" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="43"/>
+      <c r="B4" s="46"/>
       <c r="C4" s="1" t="s">
         <v>6</v>
       </c>
@@ -1652,10 +1652,10 @@
       <c r="Z4" s="2"/>
     </row>
     <row r="5" spans="1:26">
-      <c r="A5" s="42" t="s">
+      <c r="A5" s="47" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="43"/>
+      <c r="B5" s="46"/>
       <c r="C5" s="4" t="s">
         <v>12</v>
       </c>
@@ -1692,10 +1692,10 @@
       <c r="Z5" s="2"/>
     </row>
     <row r="6" spans="1:26">
-      <c r="A6" s="42" t="s">
+      <c r="A6" s="47" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="43"/>
+      <c r="B6" s="46"/>
       <c r="C6" s="4" t="s">
         <v>18</v>
       </c>
@@ -1730,10 +1730,10 @@
       <c r="Z6" s="2"/>
     </row>
     <row r="7" spans="1:26">
-      <c r="A7" s="42" t="s">
+      <c r="A7" s="47" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="43"/>
+      <c r="B7" s="46"/>
       <c r="C7" s="4" t="s">
         <v>21</v>
       </c>
@@ -1768,10 +1768,10 @@
       <c r="Z7" s="2"/>
     </row>
     <row r="8" spans="1:26">
-      <c r="A8" s="42" t="s">
+      <c r="A8" s="47" t="s">
         <v>24</v>
       </c>
-      <c r="B8" s="43"/>
+      <c r="B8" s="46"/>
       <c r="C8" s="4" t="s">
         <v>25</v>
       </c>
@@ -1806,10 +1806,10 @@
       <c r="Z8" s="2"/>
     </row>
     <row r="9" spans="1:26">
-      <c r="A9" s="42" t="s">
+      <c r="A9" s="47" t="s">
         <v>28</v>
       </c>
-      <c r="B9" s="43"/>
+      <c r="B9" s="46"/>
       <c r="C9" s="4" t="s">
         <v>29</v>
       </c>
@@ -1844,10 +1844,10 @@
       <c r="Z9" s="2"/>
     </row>
     <row r="10" spans="1:26">
-      <c r="A10" s="42" t="s">
+      <c r="A10" s="47" t="s">
         <v>32</v>
       </c>
-      <c r="B10" s="43"/>
+      <c r="B10" s="46"/>
       <c r="C10" s="4" t="s">
         <v>33</v>
       </c>
@@ -1882,10 +1882,10 @@
       <c r="Z10" s="2"/>
     </row>
     <row r="11" spans="1:26">
-      <c r="A11" s="68" t="s">
+      <c r="A11" s="62" t="s">
         <v>36</v>
       </c>
-      <c r="B11" s="43"/>
+      <c r="B11" s="46"/>
       <c r="C11" s="8" t="s">
         <v>37</v>
       </c>
@@ -1920,10 +1920,10 @@
       <c r="Z11" s="2"/>
     </row>
     <row r="12" spans="1:26">
-      <c r="A12" s="68" t="s">
+      <c r="A12" s="62" t="s">
         <v>39</v>
       </c>
-      <c r="B12" s="43"/>
+      <c r="B12" s="46"/>
       <c r="C12" s="8" t="s">
         <v>21</v>
       </c>
@@ -1958,10 +1958,10 @@
       <c r="Z12" s="2"/>
     </row>
     <row r="13" spans="1:26">
-      <c r="A13" s="68" t="s">
+      <c r="A13" s="62" t="s">
         <v>41</v>
       </c>
-      <c r="B13" s="43"/>
+      <c r="B13" s="46"/>
       <c r="C13" s="8" t="s">
         <v>42</v>
       </c>
@@ -1996,10 +1996,10 @@
       <c r="Z13" s="2"/>
     </row>
     <row r="14" spans="1:26">
-      <c r="A14" s="73" t="s">
+      <c r="A14" s="49" t="s">
         <v>45</v>
       </c>
-      <c r="B14" s="47"/>
+      <c r="B14" s="50"/>
       <c r="C14" s="11" t="s">
         <v>46</v>
       </c>
@@ -2034,16 +2034,16 @@
       <c r="Z14" s="2"/>
     </row>
     <row r="15" spans="1:26" ht="15" customHeight="1">
-      <c r="A15" s="74" t="s">
+      <c r="A15" s="51" t="s">
         <v>48</v>
       </c>
-      <c r="B15" s="75"/>
-      <c r="C15" s="75"/>
-      <c r="D15" s="75"/>
-      <c r="E15" s="75"/>
-      <c r="F15" s="75"/>
-      <c r="G15" s="75"/>
-      <c r="H15" s="76"/>
+      <c r="B15" s="52"/>
+      <c r="C15" s="52"/>
+      <c r="D15" s="52"/>
+      <c r="E15" s="52"/>
+      <c r="F15" s="52"/>
+      <c r="G15" s="52"/>
+      <c r="H15" s="53"/>
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
       <c r="K15" s="2"/>
@@ -2064,10 +2064,10 @@
       <c r="Z15" s="2"/>
     </row>
     <row r="16" spans="1:26" ht="15" customHeight="1">
-      <c r="A16" s="51" t="s">
+      <c r="A16" s="45" t="s">
         <v>49</v>
       </c>
-      <c r="B16" s="43"/>
+      <c r="B16" s="46"/>
       <c r="C16" s="1" t="s">
         <v>50</v>
       </c>
@@ -2077,11 +2077,11 @@
       <c r="E16" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="F16" s="51" t="s">
+      <c r="F16" s="45" t="s">
         <v>53</v>
       </c>
-      <c r="G16" s="52"/>
-      <c r="H16" s="53"/>
+      <c r="G16" s="42"/>
+      <c r="H16" s="43"/>
       <c r="I16" s="2"/>
       <c r="J16" s="2"/>
       <c r="K16" s="2"/>
@@ -2102,10 +2102,10 @@
       <c r="Z16" s="2"/>
     </row>
     <row r="17" spans="1:26">
-      <c r="A17" s="44" t="s">
+      <c r="A17" s="54" t="s">
         <v>54</v>
       </c>
-      <c r="B17" s="43"/>
+      <c r="B17" s="46"/>
       <c r="C17" s="15" t="s">
         <v>15</v>
       </c>
@@ -2113,11 +2113,11 @@
       <c r="E17" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="F17" s="44" t="s">
+      <c r="F17" s="54" t="s">
         <v>11</v>
       </c>
-      <c r="G17" s="52"/>
-      <c r="H17" s="53"/>
+      <c r="G17" s="42"/>
+      <c r="H17" s="43"/>
       <c r="I17" s="2"/>
       <c r="J17" s="2"/>
       <c r="K17" s="2"/>
@@ -2138,10 +2138,10 @@
       <c r="Z17" s="2"/>
     </row>
     <row r="18" spans="1:26">
-      <c r="A18" s="44" t="s">
+      <c r="A18" s="54" t="s">
         <v>55</v>
       </c>
-      <c r="B18" s="43"/>
+      <c r="B18" s="46"/>
       <c r="C18" s="15"/>
       <c r="D18" s="15" t="s">
         <v>15</v>
@@ -2149,11 +2149,11 @@
       <c r="E18" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="F18" s="44" t="s">
+      <c r="F18" s="54" t="s">
         <v>24</v>
       </c>
-      <c r="G18" s="52"/>
-      <c r="H18" s="53"/>
+      <c r="G18" s="42"/>
+      <c r="H18" s="43"/>
       <c r="I18" s="2"/>
       <c r="J18" s="2"/>
       <c r="K18" s="2"/>
@@ -2174,10 +2174,10 @@
       <c r="Z18" s="2"/>
     </row>
     <row r="19" spans="1:26">
-      <c r="A19" s="70" t="s">
+      <c r="A19" s="59" t="s">
         <v>56</v>
       </c>
-      <c r="B19" s="43"/>
+      <c r="B19" s="46"/>
       <c r="C19" s="15"/>
       <c r="D19" s="15" t="s">
         <v>15</v>
@@ -2185,11 +2185,11 @@
       <c r="E19" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="F19" s="70" t="s">
+      <c r="F19" s="59" t="s">
         <v>39</v>
       </c>
-      <c r="G19" s="52"/>
-      <c r="H19" s="53"/>
+      <c r="G19" s="42"/>
+      <c r="H19" s="43"/>
       <c r="I19" s="2"/>
       <c r="J19" s="2"/>
       <c r="K19" s="2"/>
@@ -2210,10 +2210,10 @@
       <c r="Z19" s="2"/>
     </row>
     <row r="20" spans="1:26">
-      <c r="A20" s="71" t="s">
+      <c r="A20" s="60" t="s">
         <v>57</v>
       </c>
-      <c r="B20" s="39"/>
+      <c r="B20" s="61"/>
       <c r="C20" s="17"/>
       <c r="D20" s="18" t="s">
         <v>15</v>
@@ -2221,11 +2221,11 @@
       <c r="E20" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="F20" s="71" t="s">
+      <c r="F20" s="60" t="s">
         <v>32</v>
       </c>
-      <c r="G20" s="40"/>
-      <c r="H20" s="41"/>
+      <c r="G20" s="63"/>
+      <c r="H20" s="64"/>
       <c r="I20" s="2"/>
       <c r="J20" s="2"/>
       <c r="K20" s="2"/>
@@ -2277,15 +2277,15 @@
       <c r="A22" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="B22" s="61" t="s">
+      <c r="B22" s="38" t="s">
         <v>59</v>
       </c>
-      <c r="C22" s="62"/>
-      <c r="D22" s="62"/>
-      <c r="E22" s="62"/>
-      <c r="F22" s="62"/>
-      <c r="G22" s="62"/>
-      <c r="H22" s="63"/>
+      <c r="C22" s="39"/>
+      <c r="D22" s="39"/>
+      <c r="E22" s="39"/>
+      <c r="F22" s="39"/>
+      <c r="G22" s="39"/>
+      <c r="H22" s="40"/>
       <c r="I22" s="2"/>
       <c r="J22" s="2"/>
       <c r="K22" s="2"/>
@@ -2309,15 +2309,15 @@
       <c r="A23" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B23" s="66" t="s">
+      <c r="B23" s="41" t="s">
         <v>60</v>
       </c>
-      <c r="C23" s="52"/>
-      <c r="D23" s="52"/>
-      <c r="E23" s="52"/>
-      <c r="F23" s="52"/>
-      <c r="G23" s="52"/>
-      <c r="H23" s="53"/>
+      <c r="C23" s="42"/>
+      <c r="D23" s="42"/>
+      <c r="E23" s="42"/>
+      <c r="F23" s="42"/>
+      <c r="G23" s="42"/>
+      <c r="H23" s="43"/>
       <c r="I23" s="2"/>
       <c r="J23" s="2"/>
       <c r="K23" s="2"/>
@@ -2338,16 +2338,16 @@
       <c r="Z23" s="2"/>
     </row>
     <row r="24" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A24" s="54" t="s">
+      <c r="A24" s="44" t="s">
         <v>4</v>
       </c>
-      <c r="B24" s="52"/>
-      <c r="C24" s="52"/>
-      <c r="D24" s="52"/>
-      <c r="E24" s="52"/>
-      <c r="F24" s="52"/>
-      <c r="G24" s="52"/>
-      <c r="H24" s="53"/>
+      <c r="B24" s="42"/>
+      <c r="C24" s="42"/>
+      <c r="D24" s="42"/>
+      <c r="E24" s="42"/>
+      <c r="F24" s="42"/>
+      <c r="G24" s="42"/>
+      <c r="H24" s="43"/>
       <c r="I24" s="2"/>
       <c r="J24" s="2"/>
       <c r="K24" s="2"/>
@@ -2368,10 +2368,10 @@
       <c r="Z24" s="2"/>
     </row>
     <row r="25" spans="1:26" ht="15" customHeight="1">
-      <c r="A25" s="51" t="s">
+      <c r="A25" s="45" t="s">
         <v>5</v>
       </c>
-      <c r="B25" s="43"/>
+      <c r="B25" s="46"/>
       <c r="C25" s="1" t="s">
         <v>6</v>
       </c>
@@ -2410,10 +2410,10 @@
       <c r="Z25" s="2"/>
     </row>
     <row r="26" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A26" s="42" t="s">
+      <c r="A26" s="47" t="s">
         <v>61</v>
       </c>
-      <c r="B26" s="43"/>
+      <c r="B26" s="46"/>
       <c r="C26" s="4" t="s">
         <v>12</v>
       </c>
@@ -2450,10 +2450,10 @@
       <c r="Z26" s="2"/>
     </row>
     <row r="27" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A27" s="42" t="s">
+      <c r="A27" s="47" t="s">
         <v>11</v>
       </c>
-      <c r="B27" s="43"/>
+      <c r="B27" s="46"/>
       <c r="C27" s="4" t="s">
         <v>12</v>
       </c>
@@ -2490,10 +2490,10 @@
       <c r="Z27" s="2"/>
     </row>
     <row r="28" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A28" s="42" t="s">
+      <c r="A28" s="47" t="s">
         <v>64</v>
       </c>
-      <c r="B28" s="43"/>
+      <c r="B28" s="46"/>
       <c r="C28" s="4" t="s">
         <v>42</v>
       </c>
@@ -2528,10 +2528,10 @@
       <c r="Z28" s="2"/>
     </row>
     <row r="29" spans="1:26" ht="15" customHeight="1">
-      <c r="A29" s="42" t="s">
+      <c r="A29" s="47" t="s">
         <v>66</v>
       </c>
-      <c r="B29" s="43"/>
+      <c r="B29" s="46"/>
       <c r="C29" s="4" t="s">
         <v>67</v>
       </c>
@@ -2566,10 +2566,10 @@
       <c r="Z29" s="2"/>
     </row>
     <row r="30" spans="1:26" ht="15" customHeight="1">
-      <c r="A30" s="42" t="s">
+      <c r="A30" s="47" t="s">
         <v>70</v>
       </c>
-      <c r="B30" s="43"/>
+      <c r="B30" s="46"/>
       <c r="C30" s="4" t="s">
         <v>67</v>
       </c>
@@ -2604,10 +2604,10 @@
       <c r="Z30" s="2"/>
     </row>
     <row r="31" spans="1:26" ht="15" customHeight="1">
-      <c r="A31" s="42" t="s">
+      <c r="A31" s="47" t="s">
         <v>72</v>
       </c>
-      <c r="B31" s="43"/>
+      <c r="B31" s="46"/>
       <c r="C31" s="4" t="s">
         <v>67</v>
       </c>
@@ -2642,10 +2642,10 @@
       <c r="Z31" s="2"/>
     </row>
     <row r="32" spans="1:26" ht="15" customHeight="1">
-      <c r="A32" s="68" t="s">
+      <c r="A32" s="62" t="s">
         <v>74</v>
       </c>
-      <c r="B32" s="43"/>
+      <c r="B32" s="46"/>
       <c r="C32" s="4" t="s">
         <v>67</v>
       </c>
@@ -2680,10 +2680,10 @@
       <c r="Z32" s="2"/>
     </row>
     <row r="33" spans="1:26" ht="15" customHeight="1">
-      <c r="A33" s="69" t="s">
+      <c r="A33" s="65" t="s">
         <v>76</v>
       </c>
-      <c r="B33" s="39"/>
+      <c r="B33" s="61"/>
       <c r="C33" s="23" t="s">
         <v>67</v>
       </c>
@@ -2718,16 +2718,16 @@
       <c r="Z33" s="2"/>
     </row>
     <row r="34" spans="1:26" ht="15" customHeight="1">
-      <c r="A34" s="48" t="s">
+      <c r="A34" s="55" t="s">
         <v>48</v>
       </c>
-      <c r="B34" s="49"/>
-      <c r="C34" s="49"/>
-      <c r="D34" s="49"/>
-      <c r="E34" s="49"/>
-      <c r="F34" s="49"/>
-      <c r="G34" s="49"/>
-      <c r="H34" s="50"/>
+      <c r="B34" s="56"/>
+      <c r="C34" s="56"/>
+      <c r="D34" s="56"/>
+      <c r="E34" s="56"/>
+      <c r="F34" s="56"/>
+      <c r="G34" s="56"/>
+      <c r="H34" s="57"/>
       <c r="I34" s="2"/>
       <c r="J34" s="2"/>
       <c r="K34" s="2"/>
@@ -2748,10 +2748,10 @@
       <c r="Z34" s="2"/>
     </row>
     <row r="35" spans="1:26" ht="15" customHeight="1">
-      <c r="A35" s="51" t="s">
+      <c r="A35" s="45" t="s">
         <v>49</v>
       </c>
-      <c r="B35" s="43"/>
+      <c r="B35" s="46"/>
       <c r="C35" s="1" t="s">
         <v>50</v>
       </c>
@@ -2761,11 +2761,11 @@
       <c r="E35" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="F35" s="51" t="s">
+      <c r="F35" s="45" t="s">
         <v>53</v>
       </c>
-      <c r="G35" s="52"/>
-      <c r="H35" s="53"/>
+      <c r="G35" s="42"/>
+      <c r="H35" s="43"/>
       <c r="I35" s="2"/>
       <c r="J35" s="2"/>
       <c r="K35" s="2"/>
@@ -2786,10 +2786,10 @@
       <c r="Z35" s="2"/>
     </row>
     <row r="36" spans="1:26" ht="15" customHeight="1">
-      <c r="A36" s="44" t="s">
+      <c r="A36" s="54" t="s">
         <v>78</v>
       </c>
-      <c r="B36" s="43"/>
+      <c r="B36" s="46"/>
       <c r="C36" s="15" t="s">
         <v>15</v>
       </c>
@@ -2797,11 +2797,11 @@
       <c r="E36" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="F36" s="44" t="s">
+      <c r="F36" s="54" t="s">
         <v>61</v>
       </c>
-      <c r="G36" s="52"/>
-      <c r="H36" s="53"/>
+      <c r="G36" s="42"/>
+      <c r="H36" s="43"/>
       <c r="I36" s="2"/>
       <c r="J36" s="2"/>
       <c r="K36" s="2"/>
@@ -2853,15 +2853,15 @@
       <c r="A38" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="B38" s="61" t="s">
+      <c r="B38" s="38" t="s">
         <v>79</v>
       </c>
-      <c r="C38" s="62"/>
-      <c r="D38" s="62"/>
-      <c r="E38" s="62"/>
-      <c r="F38" s="62"/>
-      <c r="G38" s="62"/>
-      <c r="H38" s="63"/>
+      <c r="C38" s="39"/>
+      <c r="D38" s="39"/>
+      <c r="E38" s="39"/>
+      <c r="F38" s="39"/>
+      <c r="G38" s="39"/>
+      <c r="H38" s="40"/>
       <c r="I38" s="2"/>
       <c r="J38" s="2"/>
       <c r="K38" s="2"/>
@@ -2885,15 +2885,15 @@
       <c r="A39" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B39" s="66" t="s">
+      <c r="B39" s="41" t="s">
         <v>80</v>
       </c>
-      <c r="C39" s="52"/>
-      <c r="D39" s="52"/>
-      <c r="E39" s="52"/>
-      <c r="F39" s="52"/>
-      <c r="G39" s="52"/>
-      <c r="H39" s="53"/>
+      <c r="C39" s="42"/>
+      <c r="D39" s="42"/>
+      <c r="E39" s="42"/>
+      <c r="F39" s="42"/>
+      <c r="G39" s="42"/>
+      <c r="H39" s="43"/>
       <c r="I39" s="2"/>
       <c r="J39" s="2"/>
       <c r="K39" s="2"/>
@@ -2914,16 +2914,16 @@
       <c r="Z39" s="2"/>
     </row>
     <row r="40" spans="1:26" ht="15" customHeight="1">
-      <c r="A40" s="54" t="s">
+      <c r="A40" s="44" t="s">
         <v>4</v>
       </c>
-      <c r="B40" s="52"/>
-      <c r="C40" s="52"/>
-      <c r="D40" s="52"/>
-      <c r="E40" s="52"/>
-      <c r="F40" s="52"/>
-      <c r="G40" s="52"/>
-      <c r="H40" s="53"/>
+      <c r="B40" s="42"/>
+      <c r="C40" s="42"/>
+      <c r="D40" s="42"/>
+      <c r="E40" s="42"/>
+      <c r="F40" s="42"/>
+      <c r="G40" s="42"/>
+      <c r="H40" s="43"/>
       <c r="I40" s="2"/>
       <c r="J40" s="2"/>
       <c r="K40" s="2"/>
@@ -2944,10 +2944,10 @@
       <c r="Z40" s="2"/>
     </row>
     <row r="41" spans="1:26" ht="15" customHeight="1">
-      <c r="A41" s="51" t="s">
+      <c r="A41" s="45" t="s">
         <v>5</v>
       </c>
-      <c r="B41" s="43"/>
+      <c r="B41" s="46"/>
       <c r="C41" s="1" t="s">
         <v>6</v>
       </c>
@@ -2986,10 +2986,10 @@
       <c r="Z41" s="2"/>
     </row>
     <row r="42" spans="1:26" ht="15" customHeight="1">
-      <c r="A42" s="42" t="s">
+      <c r="A42" s="47" t="s">
         <v>81</v>
       </c>
-      <c r="B42" s="43"/>
+      <c r="B42" s="46"/>
       <c r="C42" s="4" t="s">
         <v>12</v>
       </c>
@@ -3026,10 +3026,10 @@
       <c r="Z42" s="2"/>
     </row>
     <row r="43" spans="1:26" ht="15" customHeight="1">
-      <c r="A43" s="42" t="s">
+      <c r="A43" s="47" t="s">
         <v>61</v>
       </c>
-      <c r="B43" s="43"/>
+      <c r="B43" s="46"/>
       <c r="C43" s="4" t="s">
         <v>12</v>
       </c>
@@ -3066,10 +3066,10 @@
       <c r="Z43" s="2"/>
     </row>
     <row r="44" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A44" s="42" t="s">
+      <c r="A44" s="47" t="s">
         <v>84</v>
       </c>
-      <c r="B44" s="43"/>
+      <c r="B44" s="46"/>
       <c r="C44" s="4" t="s">
         <v>85</v>
       </c>
@@ -3104,10 +3104,10 @@
       <c r="Z44" s="2"/>
     </row>
     <row r="45" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A45" s="42" t="s">
+      <c r="A45" s="47" t="s">
         <v>88</v>
       </c>
-      <c r="B45" s="43"/>
+      <c r="B45" s="46"/>
       <c r="C45" s="4" t="s">
         <v>85</v>
       </c>
@@ -3142,10 +3142,10 @@
       <c r="Z45" s="2"/>
     </row>
     <row r="46" spans="1:26" ht="15" customHeight="1">
-      <c r="A46" s="42" t="s">
+      <c r="A46" s="47" t="s">
         <v>90</v>
       </c>
-      <c r="B46" s="43"/>
+      <c r="B46" s="46"/>
       <c r="C46" s="4" t="s">
         <v>67</v>
       </c>
@@ -3180,10 +3180,10 @@
       <c r="Z46" s="2"/>
     </row>
     <row r="47" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A47" s="42" t="s">
+      <c r="A47" s="47" t="s">
         <v>92</v>
       </c>
-      <c r="B47" s="43"/>
+      <c r="B47" s="46"/>
       <c r="C47" s="4" t="s">
         <v>67</v>
       </c>
@@ -3218,10 +3218,10 @@
       <c r="Z47" s="2"/>
     </row>
     <row r="48" spans="1:26" ht="15" customHeight="1">
-      <c r="A48" s="73" t="s">
+      <c r="A48" s="49" t="s">
         <v>94</v>
       </c>
-      <c r="B48" s="47"/>
+      <c r="B48" s="50"/>
       <c r="C48" s="11" t="s">
         <v>29</v>
       </c>
@@ -3256,16 +3256,16 @@
       <c r="Z48" s="2"/>
     </row>
     <row r="49" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A49" s="74" t="s">
+      <c r="A49" s="51" t="s">
         <v>48</v>
       </c>
-      <c r="B49" s="75"/>
-      <c r="C49" s="75"/>
-      <c r="D49" s="75"/>
-      <c r="E49" s="75"/>
-      <c r="F49" s="75"/>
-      <c r="G49" s="75"/>
-      <c r="H49" s="76"/>
+      <c r="B49" s="52"/>
+      <c r="C49" s="52"/>
+      <c r="D49" s="52"/>
+      <c r="E49" s="52"/>
+      <c r="F49" s="52"/>
+      <c r="G49" s="52"/>
+      <c r="H49" s="53"/>
       <c r="I49" s="2"/>
       <c r="J49" s="2"/>
       <c r="K49" s="2"/>
@@ -3286,10 +3286,10 @@
       <c r="Z49" s="2"/>
     </row>
     <row r="50" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A50" s="51" t="s">
+      <c r="A50" s="45" t="s">
         <v>49</v>
       </c>
-      <c r="B50" s="43"/>
+      <c r="B50" s="46"/>
       <c r="C50" s="1" t="s">
         <v>50</v>
       </c>
@@ -3299,11 +3299,11 @@
       <c r="E50" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="F50" s="51" t="s">
+      <c r="F50" s="45" t="s">
         <v>53</v>
       </c>
-      <c r="G50" s="52"/>
-      <c r="H50" s="53"/>
+      <c r="G50" s="42"/>
+      <c r="H50" s="43"/>
       <c r="I50" s="2"/>
       <c r="J50" s="2"/>
       <c r="K50" s="2"/>
@@ -3324,10 +3324,10 @@
       <c r="Z50" s="2"/>
     </row>
     <row r="51" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A51" s="44" t="s">
+      <c r="A51" s="54" t="s">
         <v>96</v>
       </c>
-      <c r="B51" s="43"/>
+      <c r="B51" s="46"/>
       <c r="C51" s="15" t="s">
         <v>15</v>
       </c>
@@ -3335,11 +3335,11 @@
       <c r="E51" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="F51" s="44" t="s">
+      <c r="F51" s="54" t="s">
         <v>81</v>
       </c>
-      <c r="G51" s="52"/>
-      <c r="H51" s="53"/>
+      <c r="G51" s="42"/>
+      <c r="H51" s="43"/>
       <c r="I51" s="2"/>
       <c r="J51" s="2"/>
       <c r="K51" s="2"/>
@@ -3391,15 +3391,15 @@
       <c r="A53" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="B53" s="61" t="s">
+      <c r="B53" s="38" t="s">
         <v>97</v>
       </c>
-      <c r="C53" s="62"/>
-      <c r="D53" s="62"/>
-      <c r="E53" s="62"/>
-      <c r="F53" s="62"/>
-      <c r="G53" s="62"/>
-      <c r="H53" s="63"/>
+      <c r="C53" s="39"/>
+      <c r="D53" s="39"/>
+      <c r="E53" s="39"/>
+      <c r="F53" s="39"/>
+      <c r="G53" s="39"/>
+      <c r="H53" s="40"/>
       <c r="I53" s="2"/>
       <c r="J53" s="2"/>
       <c r="K53" s="2"/>
@@ -3423,15 +3423,15 @@
       <c r="A54" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B54" s="66" t="s">
+      <c r="B54" s="41" t="s">
         <v>98</v>
       </c>
-      <c r="C54" s="52"/>
-      <c r="D54" s="52"/>
-      <c r="E54" s="52"/>
-      <c r="F54" s="52"/>
-      <c r="G54" s="52"/>
-      <c r="H54" s="53"/>
+      <c r="C54" s="42"/>
+      <c r="D54" s="42"/>
+      <c r="E54" s="42"/>
+      <c r="F54" s="42"/>
+      <c r="G54" s="42"/>
+      <c r="H54" s="43"/>
       <c r="I54" s="2"/>
       <c r="J54" s="2"/>
       <c r="K54" s="2"/>
@@ -3452,16 +3452,16 @@
       <c r="Z54" s="2"/>
     </row>
     <row r="55" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A55" s="54" t="s">
+      <c r="A55" s="44" t="s">
         <v>4</v>
       </c>
-      <c r="B55" s="52"/>
-      <c r="C55" s="52"/>
-      <c r="D55" s="52"/>
-      <c r="E55" s="52"/>
-      <c r="F55" s="52"/>
-      <c r="G55" s="52"/>
-      <c r="H55" s="53"/>
+      <c r="B55" s="42"/>
+      <c r="C55" s="42"/>
+      <c r="D55" s="42"/>
+      <c r="E55" s="42"/>
+      <c r="F55" s="42"/>
+      <c r="G55" s="42"/>
+      <c r="H55" s="43"/>
       <c r="I55" s="2"/>
       <c r="J55" s="2"/>
       <c r="K55" s="2"/>
@@ -3482,10 +3482,10 @@
       <c r="Z55" s="2"/>
     </row>
     <row r="56" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A56" s="51" t="s">
+      <c r="A56" s="45" t="s">
         <v>5</v>
       </c>
-      <c r="B56" s="43"/>
+      <c r="B56" s="46"/>
       <c r="C56" s="1" t="s">
         <v>6</v>
       </c>
@@ -3524,10 +3524,10 @@
       <c r="Z56" s="2"/>
     </row>
     <row r="57" spans="1:26" ht="15" customHeight="1">
-      <c r="A57" s="42" t="s">
+      <c r="A57" s="47" t="s">
         <v>99</v>
       </c>
-      <c r="B57" s="43"/>
+      <c r="B57" s="46"/>
       <c r="C57" s="4" t="s">
         <v>12</v>
       </c>
@@ -3564,10 +3564,10 @@
       <c r="Z57" s="2"/>
     </row>
     <row r="58" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A58" s="42" t="s">
+      <c r="A58" s="47" t="s">
         <v>61</v>
       </c>
-      <c r="B58" s="43"/>
+      <c r="B58" s="46"/>
       <c r="C58" s="4" t="s">
         <v>12</v>
       </c>
@@ -3604,10 +3604,10 @@
       <c r="Z58" s="2"/>
     </row>
     <row r="59" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A59" s="42" t="s">
+      <c r="A59" s="47" t="s">
         <v>11</v>
       </c>
-      <c r="B59" s="43"/>
+      <c r="B59" s="46"/>
       <c r="C59" s="4" t="s">
         <v>12</v>
       </c>
@@ -3644,10 +3644,10 @@
       <c r="Z59" s="2"/>
     </row>
     <row r="60" spans="1:26" ht="15" customHeight="1">
-      <c r="A60" s="42" t="s">
+      <c r="A60" s="47" t="s">
         <v>103</v>
       </c>
-      <c r="B60" s="43"/>
+      <c r="B60" s="46"/>
       <c r="C60" s="4" t="s">
         <v>46</v>
       </c>
@@ -3682,10 +3682,10 @@
       <c r="Z60" s="2"/>
     </row>
     <row r="61" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A61" s="42" t="s">
+      <c r="A61" s="47" t="s">
         <v>105</v>
       </c>
-      <c r="B61" s="43"/>
+      <c r="B61" s="46"/>
       <c r="C61" s="4" t="s">
         <v>42</v>
       </c>
@@ -3720,10 +3720,10 @@
       <c r="Z61" s="2"/>
     </row>
     <row r="62" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A62" s="42" t="s">
+      <c r="A62" s="47" t="s">
         <v>107</v>
       </c>
-      <c r="B62" s="43"/>
+      <c r="B62" s="46"/>
       <c r="C62" s="12" t="s">
         <v>108</v>
       </c>
@@ -3758,10 +3758,10 @@
       <c r="Z62" s="2"/>
     </row>
     <row r="63" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A63" s="45" t="s">
+      <c r="A63" s="66" t="s">
         <v>111</v>
       </c>
-      <c r="B63" s="39"/>
+      <c r="B63" s="61"/>
       <c r="C63" s="23" t="s">
         <v>67</v>
       </c>
@@ -3796,16 +3796,16 @@
       <c r="Z63" s="2"/>
     </row>
     <row r="64" spans="1:26" ht="15" customHeight="1">
-      <c r="A64" s="48" t="s">
+      <c r="A64" s="55" t="s">
         <v>48</v>
       </c>
-      <c r="B64" s="49"/>
-      <c r="C64" s="49"/>
-      <c r="D64" s="49"/>
-      <c r="E64" s="49"/>
-      <c r="F64" s="49"/>
-      <c r="G64" s="49"/>
-      <c r="H64" s="50"/>
+      <c r="B64" s="56"/>
+      <c r="C64" s="56"/>
+      <c r="D64" s="56"/>
+      <c r="E64" s="56"/>
+      <c r="F64" s="56"/>
+      <c r="G64" s="56"/>
+      <c r="H64" s="57"/>
       <c r="I64" s="2"/>
       <c r="J64" s="2"/>
       <c r="K64" s="2"/>
@@ -3826,10 +3826,10 @@
       <c r="Z64" s="2"/>
     </row>
     <row r="65" spans="1:26" ht="15" customHeight="1">
-      <c r="A65" s="51" t="s">
+      <c r="A65" s="45" t="s">
         <v>49</v>
       </c>
-      <c r="B65" s="43"/>
+      <c r="B65" s="46"/>
       <c r="C65" s="1" t="s">
         <v>50</v>
       </c>
@@ -3839,11 +3839,11 @@
       <c r="E65" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="F65" s="51" t="s">
+      <c r="F65" s="45" t="s">
         <v>53</v>
       </c>
-      <c r="G65" s="52"/>
-      <c r="H65" s="53"/>
+      <c r="G65" s="42"/>
+      <c r="H65" s="43"/>
       <c r="I65" s="2"/>
       <c r="J65" s="2"/>
       <c r="K65" s="2"/>
@@ -3864,10 +3864,10 @@
       <c r="Z65" s="2"/>
     </row>
     <row r="66" spans="1:26" ht="15" customHeight="1">
-      <c r="A66" s="44" t="s">
+      <c r="A66" s="54" t="s">
         <v>113</v>
       </c>
-      <c r="B66" s="43"/>
+      <c r="B66" s="46"/>
       <c r="C66" s="15" t="s">
         <v>15</v>
       </c>
@@ -3875,11 +3875,11 @@
       <c r="E66" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="F66" s="44" t="s">
+      <c r="F66" s="54" t="s">
         <v>99</v>
       </c>
-      <c r="G66" s="52"/>
-      <c r="H66" s="53"/>
+      <c r="G66" s="42"/>
+      <c r="H66" s="43"/>
       <c r="I66" s="2"/>
       <c r="J66" s="2"/>
       <c r="K66" s="2"/>
@@ -3931,15 +3931,15 @@
       <c r="A68" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="B68" s="61" t="s">
+      <c r="B68" s="38" t="s">
         <v>114</v>
       </c>
-      <c r="C68" s="62"/>
-      <c r="D68" s="62"/>
-      <c r="E68" s="62"/>
-      <c r="F68" s="62"/>
-      <c r="G68" s="62"/>
-      <c r="H68" s="63"/>
+      <c r="C68" s="39"/>
+      <c r="D68" s="39"/>
+      <c r="E68" s="39"/>
+      <c r="F68" s="39"/>
+      <c r="G68" s="39"/>
+      <c r="H68" s="40"/>
       <c r="I68" s="2"/>
       <c r="J68" s="2"/>
       <c r="K68" s="2"/>
@@ -3966,12 +3966,12 @@
       <c r="B69" s="67" t="s">
         <v>115</v>
       </c>
-      <c r="C69" s="62"/>
-      <c r="D69" s="62"/>
-      <c r="E69" s="62"/>
-      <c r="F69" s="62"/>
-      <c r="G69" s="62"/>
-      <c r="H69" s="63"/>
+      <c r="C69" s="39"/>
+      <c r="D69" s="39"/>
+      <c r="E69" s="39"/>
+      <c r="F69" s="39"/>
+      <c r="G69" s="39"/>
+      <c r="H69" s="40"/>
       <c r="I69" s="2"/>
       <c r="J69" s="2"/>
       <c r="K69" s="2"/>
@@ -3992,16 +3992,16 @@
       <c r="Z69" s="2"/>
     </row>
     <row r="70" spans="1:26" ht="15" customHeight="1">
-      <c r="A70" s="54" t="s">
+      <c r="A70" s="44" t="s">
         <v>4</v>
       </c>
-      <c r="B70" s="52"/>
-      <c r="C70" s="52"/>
-      <c r="D70" s="52"/>
-      <c r="E70" s="52"/>
-      <c r="F70" s="52"/>
-      <c r="G70" s="52"/>
-      <c r="H70" s="55"/>
+      <c r="B70" s="42"/>
+      <c r="C70" s="42"/>
+      <c r="D70" s="42"/>
+      <c r="E70" s="42"/>
+      <c r="F70" s="42"/>
+      <c r="G70" s="42"/>
+      <c r="H70" s="70"/>
       <c r="I70" s="33"/>
       <c r="J70" s="2"/>
       <c r="K70" s="2"/>
@@ -4022,10 +4022,10 @@
       <c r="Z70" s="2"/>
     </row>
     <row r="71" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A71" s="51" t="s">
+      <c r="A71" s="45" t="s">
         <v>5</v>
       </c>
-      <c r="B71" s="43"/>
+      <c r="B71" s="46"/>
       <c r="C71" s="1" t="s">
         <v>6</v>
       </c>
@@ -4064,10 +4064,10 @@
       <c r="Z71" s="2"/>
     </row>
     <row r="72" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A72" s="42" t="s">
+      <c r="A72" s="47" t="s">
         <v>116</v>
       </c>
-      <c r="B72" s="43"/>
+      <c r="B72" s="46"/>
       <c r="C72" s="4" t="s">
         <v>12</v>
       </c>
@@ -4104,10 +4104,10 @@
       <c r="Z72" s="2"/>
     </row>
     <row r="73" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A73" s="42" t="s">
+      <c r="A73" s="47" t="s">
         <v>17</v>
       </c>
-      <c r="B73" s="77"/>
+      <c r="B73" s="48"/>
       <c r="C73" s="4" t="s">
         <v>18</v>
       </c>
@@ -4142,10 +4142,10 @@
       <c r="Z73" s="2"/>
     </row>
     <row r="74" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A74" s="42" t="s">
+      <c r="A74" s="47" t="s">
         <v>61</v>
       </c>
-      <c r="B74" s="43"/>
+      <c r="B74" s="46"/>
       <c r="C74" s="4" t="s">
         <v>12</v>
       </c>
@@ -4182,10 +4182,10 @@
       <c r="Z74" s="2"/>
     </row>
     <row r="75" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A75" s="42" t="s">
+      <c r="A75" s="47" t="s">
         <v>119</v>
       </c>
-      <c r="B75" s="43"/>
+      <c r="B75" s="46"/>
       <c r="C75" s="4" t="s">
         <v>67</v>
       </c>
@@ -4220,10 +4220,10 @@
       <c r="Z75" s="2"/>
     </row>
     <row r="76" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A76" s="42" t="s">
+      <c r="A76" s="47" t="s">
         <v>121</v>
       </c>
-      <c r="B76" s="43"/>
+      <c r="B76" s="46"/>
       <c r="C76" s="4" t="s">
         <v>67</v>
       </c>
@@ -4258,12 +4258,12 @@
       <c r="Z76" s="2"/>
     </row>
     <row r="77" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A77" s="42" t="s">
+      <c r="A77" s="47" t="s">
         <v>124</v>
       </c>
-      <c r="B77" s="43"/>
+      <c r="B77" s="46"/>
       <c r="C77" s="4" t="s">
-        <v>29</v>
+        <v>46</v>
       </c>
       <c r="D77" s="4" t="s">
         <v>30</v>
@@ -4296,12 +4296,12 @@
       <c r="Z77" s="2"/>
     </row>
     <row r="78" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A78" s="56" t="s">
+      <c r="A78" s="71" t="s">
         <v>126</v>
       </c>
-      <c r="B78" s="57"/>
+      <c r="B78" s="72"/>
       <c r="C78" s="12" t="s">
-        <v>29</v>
+        <v>46</v>
       </c>
       <c r="D78" s="12" t="s">
         <v>30</v>
@@ -4334,10 +4334,10 @@
       <c r="Z78" s="2"/>
     </row>
     <row r="79" spans="1:26" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A79" s="64" t="s">
+      <c r="A79" s="68" t="s">
         <v>128</v>
       </c>
-      <c r="B79" s="65"/>
+      <c r="B79" s="69"/>
       <c r="C79" s="35" t="s">
         <v>67</v>
       </c>
@@ -4372,16 +4372,16 @@
       <c r="Z79" s="2"/>
     </row>
     <row r="80" spans="1:26" ht="15" customHeight="1">
-      <c r="A80" s="58" t="s">
+      <c r="A80" s="73" t="s">
         <v>48</v>
       </c>
-      <c r="B80" s="59"/>
-      <c r="C80" s="59"/>
-      <c r="D80" s="59"/>
-      <c r="E80" s="59"/>
-      <c r="F80" s="59"/>
-      <c r="G80" s="59"/>
-      <c r="H80" s="60"/>
+      <c r="B80" s="74"/>
+      <c r="C80" s="74"/>
+      <c r="D80" s="74"/>
+      <c r="E80" s="74"/>
+      <c r="F80" s="74"/>
+      <c r="G80" s="74"/>
+      <c r="H80" s="75"/>
       <c r="I80" s="2"/>
       <c r="J80" s="2"/>
       <c r="K80" s="2"/>
@@ -4402,10 +4402,10 @@
       <c r="Z80" s="2"/>
     </row>
     <row r="81" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A81" s="51" t="s">
+      <c r="A81" s="45" t="s">
         <v>49</v>
       </c>
-      <c r="B81" s="43"/>
+      <c r="B81" s="46"/>
       <c r="C81" s="1" t="s">
         <v>50</v>
       </c>
@@ -4415,11 +4415,11 @@
       <c r="E81" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="F81" s="51" t="s">
+      <c r="F81" s="45" t="s">
         <v>53</v>
       </c>
-      <c r="G81" s="52"/>
-      <c r="H81" s="53"/>
+      <c r="G81" s="42"/>
+      <c r="H81" s="43"/>
       <c r="I81" s="2"/>
       <c r="J81" s="2"/>
       <c r="K81" s="2"/>
@@ -4440,10 +4440,10 @@
       <c r="Z81" s="2"/>
     </row>
     <row r="82" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A82" s="44" t="s">
+      <c r="A82" s="54" t="s">
         <v>130</v>
       </c>
-      <c r="B82" s="43"/>
+      <c r="B82" s="46"/>
       <c r="C82" s="15" t="s">
         <v>15</v>
       </c>
@@ -4451,11 +4451,11 @@
       <c r="E82" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="F82" s="44" t="s">
+      <c r="F82" s="54" t="s">
         <v>116</v>
       </c>
-      <c r="G82" s="52"/>
-      <c r="H82" s="53"/>
+      <c r="G82" s="42"/>
+      <c r="H82" s="43"/>
       <c r="I82" s="2"/>
       <c r="J82" s="2"/>
       <c r="K82" s="2"/>
@@ -4507,15 +4507,15 @@
       <c r="A84" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="B84" s="61" t="s">
+      <c r="B84" s="38" t="s">
         <v>131</v>
       </c>
-      <c r="C84" s="62"/>
-      <c r="D84" s="62"/>
-      <c r="E84" s="62"/>
-      <c r="F84" s="62"/>
-      <c r="G84" s="62"/>
-      <c r="H84" s="63"/>
+      <c r="C84" s="39"/>
+      <c r="D84" s="39"/>
+      <c r="E84" s="39"/>
+      <c r="F84" s="39"/>
+      <c r="G84" s="39"/>
+      <c r="H84" s="40"/>
       <c r="I84" s="2"/>
       <c r="J84" s="2"/>
       <c r="K84" s="2"/>
@@ -4539,15 +4539,15 @@
       <c r="A85" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B85" s="66" t="s">
+      <c r="B85" s="41" t="s">
         <v>132</v>
       </c>
-      <c r="C85" s="52"/>
-      <c r="D85" s="52"/>
-      <c r="E85" s="52"/>
-      <c r="F85" s="52"/>
-      <c r="G85" s="52"/>
-      <c r="H85" s="53"/>
+      <c r="C85" s="42"/>
+      <c r="D85" s="42"/>
+      <c r="E85" s="42"/>
+      <c r="F85" s="42"/>
+      <c r="G85" s="42"/>
+      <c r="H85" s="43"/>
       <c r="I85" s="2"/>
       <c r="J85" s="2"/>
       <c r="K85" s="2"/>
@@ -4568,16 +4568,16 @@
       <c r="Z85" s="2"/>
     </row>
     <row r="86" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A86" s="54" t="s">
+      <c r="A86" s="44" t="s">
         <v>4</v>
       </c>
-      <c r="B86" s="52"/>
-      <c r="C86" s="52"/>
-      <c r="D86" s="52"/>
-      <c r="E86" s="52"/>
-      <c r="F86" s="52"/>
-      <c r="G86" s="52"/>
-      <c r="H86" s="53"/>
+      <c r="B86" s="42"/>
+      <c r="C86" s="42"/>
+      <c r="D86" s="42"/>
+      <c r="E86" s="42"/>
+      <c r="F86" s="42"/>
+      <c r="G86" s="42"/>
+      <c r="H86" s="43"/>
       <c r="I86" s="2"/>
       <c r="J86" s="2"/>
       <c r="K86" s="2"/>
@@ -4598,10 +4598,10 @@
       <c r="Z86" s="2"/>
     </row>
     <row r="87" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A87" s="51" t="s">
+      <c r="A87" s="45" t="s">
         <v>5</v>
       </c>
-      <c r="B87" s="43"/>
+      <c r="B87" s="46"/>
       <c r="C87" s="1" t="s">
         <v>6</v>
       </c>
@@ -4640,10 +4640,10 @@
       <c r="Z87" s="2"/>
     </row>
     <row r="88" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A88" s="42" t="s">
+      <c r="A88" s="47" t="s">
         <v>133</v>
       </c>
-      <c r="B88" s="43"/>
+      <c r="B88" s="46"/>
       <c r="C88" s="4" t="s">
         <v>12</v>
       </c>
@@ -4680,10 +4680,10 @@
       <c r="Z88" s="2"/>
     </row>
     <row r="89" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A89" s="42" t="s">
+      <c r="A89" s="47" t="s">
         <v>17</v>
       </c>
-      <c r="B89" s="43"/>
+      <c r="B89" s="46"/>
       <c r="C89" s="4" t="s">
         <v>18</v>
       </c>
@@ -4718,10 +4718,10 @@
       <c r="Z89" s="2"/>
     </row>
     <row r="90" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A90" s="42" t="s">
+      <c r="A90" s="47" t="s">
         <v>61</v>
       </c>
-      <c r="B90" s="43"/>
+      <c r="B90" s="46"/>
       <c r="C90" s="4" t="s">
         <v>12</v>
       </c>
@@ -4758,10 +4758,10 @@
       <c r="Z90" s="2"/>
     </row>
     <row r="91" spans="1:26" ht="15" customHeight="1">
-      <c r="A91" s="42" t="s">
+      <c r="A91" s="47" t="s">
         <v>137</v>
       </c>
-      <c r="B91" s="43"/>
+      <c r="B91" s="46"/>
       <c r="C91" s="4" t="s">
         <v>42</v>
       </c>
@@ -4796,10 +4796,10 @@
       <c r="Z91" s="2"/>
     </row>
     <row r="92" spans="1:26" ht="15" customHeight="1">
-      <c r="A92" s="42" t="s">
+      <c r="A92" s="47" t="s">
         <v>139</v>
       </c>
-      <c r="B92" s="43"/>
+      <c r="B92" s="46"/>
       <c r="C92" s="4" t="s">
         <v>67</v>
       </c>
@@ -4834,10 +4834,10 @@
       <c r="Z92" s="2"/>
     </row>
     <row r="93" spans="1:26" ht="15" customHeight="1">
-      <c r="A93" s="42" t="s">
+      <c r="A93" s="47" t="s">
         <v>141</v>
       </c>
-      <c r="B93" s="43"/>
+      <c r="B93" s="46"/>
       <c r="C93" s="4" t="s">
         <v>67</v>
       </c>
@@ -4872,10 +4872,10 @@
       <c r="Z93" s="2"/>
     </row>
     <row r="94" spans="1:26" ht="15" customHeight="1" thickBot="1">
-      <c r="A94" s="45" t="s">
+      <c r="A94" s="66" t="s">
         <v>143</v>
       </c>
-      <c r="B94" s="39"/>
+      <c r="B94" s="61"/>
       <c r="C94" s="23" t="s">
         <v>29</v>
       </c>
@@ -4910,16 +4910,16 @@
       <c r="Z94" s="2"/>
     </row>
     <row r="95" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A95" s="48" t="s">
+      <c r="A95" s="55" t="s">
         <v>48</v>
       </c>
-      <c r="B95" s="49"/>
-      <c r="C95" s="49"/>
-      <c r="D95" s="49"/>
-      <c r="E95" s="49"/>
-      <c r="F95" s="49"/>
-      <c r="G95" s="49"/>
-      <c r="H95" s="50"/>
+      <c r="B95" s="56"/>
+      <c r="C95" s="56"/>
+      <c r="D95" s="56"/>
+      <c r="E95" s="56"/>
+      <c r="F95" s="56"/>
+      <c r="G95" s="56"/>
+      <c r="H95" s="57"/>
       <c r="I95" s="2"/>
       <c r="J95" s="2"/>
       <c r="K95" s="2"/>
@@ -4940,10 +4940,10 @@
       <c r="Z95" s="2"/>
     </row>
     <row r="96" spans="1:26" ht="15" customHeight="1">
-      <c r="A96" s="51" t="s">
+      <c r="A96" s="45" t="s">
         <v>49</v>
       </c>
-      <c r="B96" s="43"/>
+      <c r="B96" s="46"/>
       <c r="C96" s="1" t="s">
         <v>50</v>
       </c>
@@ -4953,11 +4953,11 @@
       <c r="E96" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="F96" s="51" t="s">
+      <c r="F96" s="45" t="s">
         <v>53</v>
       </c>
-      <c r="G96" s="52"/>
-      <c r="H96" s="53"/>
+      <c r="G96" s="42"/>
+      <c r="H96" s="43"/>
       <c r="I96" s="2"/>
       <c r="J96" s="2"/>
       <c r="K96" s="2"/>
@@ -4978,10 +4978,10 @@
       <c r="Z96" s="2"/>
     </row>
     <row r="97" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A97" s="44" t="s">
+      <c r="A97" s="54" t="s">
         <v>145</v>
       </c>
-      <c r="B97" s="43"/>
+      <c r="B97" s="46"/>
       <c r="C97" s="15" t="s">
         <v>15</v>
       </c>
@@ -4989,11 +4989,11 @@
       <c r="E97" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="F97" s="44" t="s">
+      <c r="F97" s="54" t="s">
         <v>133</v>
       </c>
-      <c r="G97" s="52"/>
-      <c r="H97" s="53"/>
+      <c r="G97" s="42"/>
+      <c r="H97" s="43"/>
       <c r="I97" s="2"/>
       <c r="J97" s="2"/>
       <c r="K97" s="2"/>
@@ -5045,15 +5045,15 @@
       <c r="A99" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="B99" s="61" t="s">
+      <c r="B99" s="38" t="s">
         <v>146</v>
       </c>
-      <c r="C99" s="62"/>
-      <c r="D99" s="62"/>
-      <c r="E99" s="62"/>
-      <c r="F99" s="62"/>
-      <c r="G99" s="62"/>
-      <c r="H99" s="63"/>
+      <c r="C99" s="39"/>
+      <c r="D99" s="39"/>
+      <c r="E99" s="39"/>
+      <c r="F99" s="39"/>
+      <c r="G99" s="39"/>
+      <c r="H99" s="40"/>
       <c r="I99" s="2"/>
       <c r="J99" s="2"/>
       <c r="K99" s="2"/>
@@ -5077,15 +5077,15 @@
       <c r="A100" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B100" s="66" t="s">
+      <c r="B100" s="41" t="s">
         <v>147</v>
       </c>
-      <c r="C100" s="52"/>
-      <c r="D100" s="52"/>
-      <c r="E100" s="52"/>
-      <c r="F100" s="52"/>
-      <c r="G100" s="52"/>
-      <c r="H100" s="53"/>
+      <c r="C100" s="42"/>
+      <c r="D100" s="42"/>
+      <c r="E100" s="42"/>
+      <c r="F100" s="42"/>
+      <c r="G100" s="42"/>
+      <c r="H100" s="43"/>
       <c r="I100" s="2"/>
       <c r="J100" s="2"/>
       <c r="K100" s="2"/>
@@ -5106,16 +5106,16 @@
       <c r="Z100" s="2"/>
     </row>
     <row r="101" spans="1:26" ht="15" customHeight="1">
-      <c r="A101" s="54" t="s">
+      <c r="A101" s="44" t="s">
         <v>4</v>
       </c>
-      <c r="B101" s="52"/>
-      <c r="C101" s="52"/>
-      <c r="D101" s="52"/>
-      <c r="E101" s="52"/>
-      <c r="F101" s="52"/>
-      <c r="G101" s="52"/>
-      <c r="H101" s="53"/>
+      <c r="B101" s="42"/>
+      <c r="C101" s="42"/>
+      <c r="D101" s="42"/>
+      <c r="E101" s="42"/>
+      <c r="F101" s="42"/>
+      <c r="G101" s="42"/>
+      <c r="H101" s="43"/>
       <c r="I101" s="2"/>
       <c r="J101" s="2"/>
       <c r="K101" s="2"/>
@@ -5136,10 +5136,10 @@
       <c r="Z101" s="2"/>
     </row>
     <row r="102" spans="1:26" ht="15" customHeight="1">
-      <c r="A102" s="51" t="s">
+      <c r="A102" s="45" t="s">
         <v>5</v>
       </c>
-      <c r="B102" s="43"/>
+      <c r="B102" s="46"/>
       <c r="C102" s="1" t="s">
         <v>6</v>
       </c>
@@ -5178,10 +5178,10 @@
       <c r="Z102" s="2"/>
     </row>
     <row r="103" spans="1:26" ht="15" customHeight="1">
-      <c r="A103" s="42" t="s">
+      <c r="A103" s="47" t="s">
         <v>149</v>
       </c>
-      <c r="B103" s="43"/>
+      <c r="B103" s="46"/>
       <c r="C103" s="4" t="s">
         <v>12</v>
       </c>
@@ -5218,10 +5218,10 @@
       <c r="Z103" s="2"/>
     </row>
     <row r="104" spans="1:26" ht="15" customHeight="1">
-      <c r="A104" s="42" t="s">
+      <c r="A104" s="47" t="s">
         <v>61</v>
       </c>
-      <c r="B104" s="43"/>
+      <c r="B104" s="46"/>
       <c r="C104" s="4" t="s">
         <v>12</v>
       </c>
@@ -5258,10 +5258,10 @@
       <c r="Z104" s="2"/>
     </row>
     <row r="105" spans="1:26" ht="15" customHeight="1">
-      <c r="A105" s="42" t="s">
+      <c r="A105" s="47" t="s">
         <v>150</v>
       </c>
-      <c r="B105" s="43"/>
+      <c r="B105" s="46"/>
       <c r="C105" s="4" t="s">
         <v>151</v>
       </c>
@@ -5296,10 +5296,10 @@
       <c r="Z105" s="2"/>
     </row>
     <row r="106" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A106" s="42" t="s">
+      <c r="A106" s="47" t="s">
         <v>154</v>
       </c>
-      <c r="B106" s="43"/>
+      <c r="B106" s="46"/>
       <c r="C106" s="4" t="s">
         <v>21</v>
       </c>
@@ -5334,10 +5334,10 @@
       <c r="Z106" s="2"/>
     </row>
     <row r="107" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A107" s="42" t="s">
+      <c r="A107" s="47" t="s">
         <v>156</v>
       </c>
-      <c r="B107" s="43"/>
+      <c r="B107" s="46"/>
       <c r="C107" s="4" t="s">
         <v>29</v>
       </c>
@@ -5372,10 +5372,10 @@
       <c r="Z107" s="2"/>
     </row>
     <row r="108" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A108" s="45" t="s">
+      <c r="A108" s="66" t="s">
         <v>158</v>
       </c>
-      <c r="B108" s="39"/>
+      <c r="B108" s="61"/>
       <c r="C108" s="23" t="s">
         <v>159</v>
       </c>
@@ -5410,16 +5410,16 @@
       <c r="Z108" s="2"/>
     </row>
     <row r="109" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A109" s="48" t="s">
+      <c r="A109" s="55" t="s">
         <v>48</v>
       </c>
-      <c r="B109" s="49"/>
-      <c r="C109" s="49"/>
-      <c r="D109" s="49"/>
-      <c r="E109" s="49"/>
-      <c r="F109" s="49"/>
-      <c r="G109" s="49"/>
-      <c r="H109" s="50"/>
+      <c r="B109" s="56"/>
+      <c r="C109" s="56"/>
+      <c r="D109" s="56"/>
+      <c r="E109" s="56"/>
+      <c r="F109" s="56"/>
+      <c r="G109" s="56"/>
+      <c r="H109" s="57"/>
       <c r="I109" s="2"/>
       <c r="J109" s="2"/>
       <c r="K109" s="2"/>
@@ -5440,10 +5440,10 @@
       <c r="Z109" s="2"/>
     </row>
     <row r="110" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A110" s="51" t="s">
+      <c r="A110" s="45" t="s">
         <v>49</v>
       </c>
-      <c r="B110" s="43"/>
+      <c r="B110" s="46"/>
       <c r="C110" s="1" t="s">
         <v>50</v>
       </c>
@@ -5453,11 +5453,11 @@
       <c r="E110" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="F110" s="51" t="s">
+      <c r="F110" s="45" t="s">
         <v>53</v>
       </c>
-      <c r="G110" s="52"/>
-      <c r="H110" s="53"/>
+      <c r="G110" s="42"/>
+      <c r="H110" s="43"/>
       <c r="I110" s="2"/>
       <c r="J110" s="2"/>
       <c r="K110" s="2"/>
@@ -5478,10 +5478,10 @@
       <c r="Z110" s="2"/>
     </row>
     <row r="111" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A111" s="44" t="s">
+      <c r="A111" s="54" t="s">
         <v>162</v>
       </c>
-      <c r="B111" s="43"/>
+      <c r="B111" s="46"/>
       <c r="C111" s="15" t="s">
         <v>15</v>
       </c>
@@ -5489,11 +5489,11 @@
       <c r="E111" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="F111" s="44" t="s">
+      <c r="F111" s="54" t="s">
         <v>149</v>
       </c>
-      <c r="G111" s="52"/>
-      <c r="H111" s="53"/>
+      <c r="G111" s="42"/>
+      <c r="H111" s="43"/>
       <c r="I111" s="2"/>
       <c r="J111" s="2"/>
       <c r="K111" s="2"/>
@@ -5514,10 +5514,10 @@
       <c r="Z111" s="2"/>
     </row>
     <row r="112" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A112" s="44" t="s">
+      <c r="A112" s="54" t="s">
         <v>163</v>
       </c>
-      <c r="B112" s="43"/>
+      <c r="B112" s="46"/>
       <c r="C112" s="15"/>
       <c r="D112" s="15" t="s">
         <v>15</v>
@@ -5525,11 +5525,11 @@
       <c r="E112" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="F112" s="44" t="s">
+      <c r="F112" s="54" t="s">
         <v>150</v>
       </c>
-      <c r="G112" s="52"/>
-      <c r="H112" s="53"/>
+      <c r="G112" s="42"/>
+      <c r="H112" s="43"/>
       <c r="I112" s="2"/>
       <c r="J112" s="2"/>
       <c r="K112" s="2"/>
@@ -5581,15 +5581,15 @@
       <c r="A114" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="B114" s="61" t="s">
+      <c r="B114" s="38" t="s">
         <v>164</v>
       </c>
-      <c r="C114" s="62"/>
-      <c r="D114" s="62"/>
-      <c r="E114" s="62"/>
-      <c r="F114" s="62"/>
-      <c r="G114" s="62"/>
-      <c r="H114" s="63"/>
+      <c r="C114" s="39"/>
+      <c r="D114" s="39"/>
+      <c r="E114" s="39"/>
+      <c r="F114" s="39"/>
+      <c r="G114" s="39"/>
+      <c r="H114" s="40"/>
       <c r="I114" s="2"/>
       <c r="J114" s="2"/>
       <c r="K114" s="2"/>
@@ -5613,15 +5613,15 @@
       <c r="A115" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B115" s="66" t="s">
+      <c r="B115" s="41" t="s">
         <v>165</v>
       </c>
-      <c r="C115" s="52"/>
-      <c r="D115" s="52"/>
-      <c r="E115" s="52"/>
-      <c r="F115" s="52"/>
-      <c r="G115" s="52"/>
-      <c r="H115" s="53"/>
+      <c r="C115" s="42"/>
+      <c r="D115" s="42"/>
+      <c r="E115" s="42"/>
+      <c r="F115" s="42"/>
+      <c r="G115" s="42"/>
+      <c r="H115" s="43"/>
       <c r="I115" s="2"/>
       <c r="J115" s="2"/>
       <c r="K115" s="2"/>
@@ -5642,16 +5642,16 @@
       <c r="Z115" s="2"/>
     </row>
     <row r="116" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A116" s="54" t="s">
+      <c r="A116" s="44" t="s">
         <v>4</v>
       </c>
-      <c r="B116" s="52"/>
-      <c r="C116" s="52"/>
-      <c r="D116" s="52"/>
-      <c r="E116" s="52"/>
-      <c r="F116" s="52"/>
-      <c r="G116" s="52"/>
-      <c r="H116" s="53"/>
+      <c r="B116" s="42"/>
+      <c r="C116" s="42"/>
+      <c r="D116" s="42"/>
+      <c r="E116" s="42"/>
+      <c r="F116" s="42"/>
+      <c r="G116" s="42"/>
+      <c r="H116" s="43"/>
       <c r="I116" s="2"/>
       <c r="J116" s="2"/>
       <c r="K116" s="2"/>
@@ -5672,10 +5672,10 @@
       <c r="Z116" s="2"/>
     </row>
     <row r="117" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A117" s="51" t="s">
+      <c r="A117" s="45" t="s">
         <v>5</v>
       </c>
-      <c r="B117" s="43"/>
+      <c r="B117" s="46"/>
       <c r="C117" s="1" t="s">
         <v>6</v>
       </c>
@@ -5714,10 +5714,10 @@
       <c r="Z117" s="2"/>
     </row>
     <row r="118" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A118" s="42" t="s">
+      <c r="A118" s="47" t="s">
         <v>166</v>
       </c>
-      <c r="B118" s="43"/>
+      <c r="B118" s="46"/>
       <c r="C118" s="4" t="s">
         <v>12</v>
       </c>
@@ -5754,10 +5754,10 @@
       <c r="Z118" s="2"/>
     </row>
     <row r="119" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A119" s="42" t="s">
+      <c r="A119" s="47" t="s">
         <v>99</v>
       </c>
-      <c r="B119" s="43"/>
+      <c r="B119" s="46"/>
       <c r="C119" s="4" t="s">
         <v>12</v>
       </c>
@@ -5794,10 +5794,10 @@
       <c r="Z119" s="2"/>
     </row>
     <row r="120" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A120" s="42" t="s">
+      <c r="A120" s="47" t="s">
         <v>61</v>
       </c>
-      <c r="B120" s="43"/>
+      <c r="B120" s="46"/>
       <c r="C120" s="4" t="s">
         <v>12</v>
       </c>
@@ -5834,10 +5834,10 @@
       <c r="Z120" s="2"/>
     </row>
     <row r="121" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A121" s="42" t="s">
+      <c r="A121" s="47" t="s">
         <v>111</v>
       </c>
-      <c r="B121" s="43"/>
+      <c r="B121" s="46"/>
       <c r="C121" s="4" t="s">
         <v>67</v>
       </c>
@@ -5872,10 +5872,10 @@
       <c r="Z121" s="2"/>
     </row>
     <row r="122" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A122" s="46" t="s">
+      <c r="A122" s="77" t="s">
         <v>119</v>
       </c>
-      <c r="B122" s="47"/>
+      <c r="B122" s="50"/>
       <c r="C122" s="12" t="s">
         <v>67</v>
       </c>
@@ -5910,10 +5910,10 @@
       <c r="Z122" s="2"/>
     </row>
     <row r="123" spans="1:26" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A123" s="45" t="s">
+      <c r="A123" s="66" t="s">
         <v>172</v>
       </c>
-      <c r="B123" s="39"/>
+      <c r="B123" s="61"/>
       <c r="C123" s="23" t="s">
         <v>29</v>
       </c>
@@ -5948,16 +5948,16 @@
       <c r="Z123" s="2"/>
     </row>
     <row r="124" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A124" s="48" t="s">
+      <c r="A124" s="55" t="s">
         <v>48</v>
       </c>
-      <c r="B124" s="49"/>
-      <c r="C124" s="49"/>
-      <c r="D124" s="49"/>
-      <c r="E124" s="49"/>
-      <c r="F124" s="49"/>
-      <c r="G124" s="49"/>
-      <c r="H124" s="50"/>
+      <c r="B124" s="56"/>
+      <c r="C124" s="56"/>
+      <c r="D124" s="56"/>
+      <c r="E124" s="56"/>
+      <c r="F124" s="56"/>
+      <c r="G124" s="56"/>
+      <c r="H124" s="57"/>
       <c r="I124" s="2"/>
       <c r="J124" s="2"/>
       <c r="K124" s="2"/>
@@ -5978,10 +5978,10 @@
       <c r="Z124" s="2"/>
     </row>
     <row r="125" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A125" s="51" t="s">
+      <c r="A125" s="45" t="s">
         <v>49</v>
       </c>
-      <c r="B125" s="43"/>
+      <c r="B125" s="46"/>
       <c r="C125" s="1" t="s">
         <v>50</v>
       </c>
@@ -5991,11 +5991,11 @@
       <c r="E125" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="F125" s="51" t="s">
+      <c r="F125" s="45" t="s">
         <v>53</v>
       </c>
-      <c r="G125" s="52"/>
-      <c r="H125" s="53"/>
+      <c r="G125" s="42"/>
+      <c r="H125" s="43"/>
       <c r="I125" s="2"/>
       <c r="J125" s="2"/>
       <c r="K125" s="2"/>
@@ -6016,10 +6016,10 @@
       <c r="Z125" s="2"/>
     </row>
     <row r="126" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A126" s="38" t="s">
+      <c r="A126" s="76" t="s">
         <v>174</v>
       </c>
-      <c r="B126" s="39"/>
+      <c r="B126" s="61"/>
       <c r="C126" s="18" t="s">
         <v>15</v>
       </c>
@@ -6027,11 +6027,11 @@
       <c r="E126" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="F126" s="38" t="s">
+      <c r="F126" s="76" t="s">
         <v>166</v>
       </c>
-      <c r="G126" s="40"/>
-      <c r="H126" s="41"/>
+      <c r="G126" s="63"/>
+      <c r="H126" s="64"/>
       <c r="I126" s="2"/>
       <c r="J126" s="2"/>
       <c r="K126" s="2"/>
@@ -30637,6 +30637,121 @@
     </row>
   </sheetData>
   <mergeCells count="139">
+    <mergeCell ref="B115:H115"/>
+    <mergeCell ref="A116:H116"/>
+    <mergeCell ref="A71:B71"/>
+    <mergeCell ref="A72:B72"/>
+    <mergeCell ref="A74:B74"/>
+    <mergeCell ref="A75:B75"/>
+    <mergeCell ref="A76:B76"/>
+    <mergeCell ref="A77:B77"/>
+    <mergeCell ref="A78:B78"/>
+    <mergeCell ref="A80:H80"/>
+    <mergeCell ref="A126:B126"/>
+    <mergeCell ref="F126:H126"/>
+    <mergeCell ref="A105:B105"/>
+    <mergeCell ref="A111:B111"/>
+    <mergeCell ref="A112:B112"/>
+    <mergeCell ref="A123:B123"/>
+    <mergeCell ref="A122:B122"/>
+    <mergeCell ref="A120:B120"/>
+    <mergeCell ref="A121:B121"/>
+    <mergeCell ref="A124:H124"/>
+    <mergeCell ref="A125:B125"/>
+    <mergeCell ref="F125:H125"/>
+    <mergeCell ref="A117:B117"/>
+    <mergeCell ref="A118:B118"/>
+    <mergeCell ref="A119:B119"/>
+    <mergeCell ref="B114:H114"/>
+    <mergeCell ref="A108:B108"/>
+    <mergeCell ref="A109:H109"/>
+    <mergeCell ref="A110:B110"/>
+    <mergeCell ref="F110:H110"/>
+    <mergeCell ref="F111:H111"/>
+    <mergeCell ref="F112:H112"/>
+    <mergeCell ref="A81:B81"/>
+    <mergeCell ref="F81:H81"/>
+    <mergeCell ref="A82:B82"/>
+    <mergeCell ref="F82:H82"/>
+    <mergeCell ref="B84:H84"/>
+    <mergeCell ref="B85:H85"/>
+    <mergeCell ref="A86:H86"/>
+    <mergeCell ref="A87:B87"/>
+    <mergeCell ref="B68:H68"/>
+    <mergeCell ref="B69:H69"/>
+    <mergeCell ref="A106:B106"/>
+    <mergeCell ref="A107:B107"/>
+    <mergeCell ref="A92:B92"/>
+    <mergeCell ref="A89:B89"/>
+    <mergeCell ref="A93:B93"/>
+    <mergeCell ref="A94:B94"/>
+    <mergeCell ref="A95:H95"/>
+    <mergeCell ref="A96:B96"/>
+    <mergeCell ref="F96:H96"/>
+    <mergeCell ref="A97:B97"/>
+    <mergeCell ref="F97:H97"/>
+    <mergeCell ref="B99:H99"/>
+    <mergeCell ref="B100:H100"/>
+    <mergeCell ref="A101:H101"/>
+    <mergeCell ref="A102:B102"/>
+    <mergeCell ref="A103:B103"/>
+    <mergeCell ref="A104:B104"/>
+    <mergeCell ref="A88:B88"/>
+    <mergeCell ref="A90:B90"/>
+    <mergeCell ref="A91:B91"/>
+    <mergeCell ref="A79:B79"/>
+    <mergeCell ref="A70:H70"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="F35:H35"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="F36:H36"/>
+    <mergeCell ref="A63:B63"/>
+    <mergeCell ref="A65:B65"/>
+    <mergeCell ref="F65:H65"/>
+    <mergeCell ref="A66:B66"/>
+    <mergeCell ref="F66:H66"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="A34:H34"/>
+    <mergeCell ref="F16:H16"/>
+    <mergeCell ref="F17:H17"/>
+    <mergeCell ref="F18:H18"/>
+    <mergeCell ref="F19:H19"/>
+    <mergeCell ref="F20:H20"/>
+    <mergeCell ref="B22:H22"/>
+    <mergeCell ref="B23:H23"/>
+    <mergeCell ref="A24:H24"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A60:B60"/>
+    <mergeCell ref="A61:B61"/>
+    <mergeCell ref="A62:B62"/>
+    <mergeCell ref="A64:H64"/>
+    <mergeCell ref="B1:H1"/>
+    <mergeCell ref="B2:H2"/>
+    <mergeCell ref="A3:H3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A15:H15"/>
     <mergeCell ref="B38:H38"/>
     <mergeCell ref="B39:H39"/>
     <mergeCell ref="A40:H40"/>
@@ -30661,121 +30776,6 @@
     <mergeCell ref="A57:B57"/>
     <mergeCell ref="A58:B58"/>
     <mergeCell ref="A59:B59"/>
-    <mergeCell ref="A60:B60"/>
-    <mergeCell ref="A61:B61"/>
-    <mergeCell ref="A62:B62"/>
-    <mergeCell ref="A64:H64"/>
-    <mergeCell ref="B1:H1"/>
-    <mergeCell ref="B2:H2"/>
-    <mergeCell ref="A3:H3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A15:H15"/>
-    <mergeCell ref="F16:H16"/>
-    <mergeCell ref="F17:H17"/>
-    <mergeCell ref="F18:H18"/>
-    <mergeCell ref="F19:H19"/>
-    <mergeCell ref="F20:H20"/>
-    <mergeCell ref="B22:H22"/>
-    <mergeCell ref="B23:H23"/>
-    <mergeCell ref="A24:H24"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="A34:H34"/>
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="F35:H35"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="F36:H36"/>
-    <mergeCell ref="A63:B63"/>
-    <mergeCell ref="A65:B65"/>
-    <mergeCell ref="F65:H65"/>
-    <mergeCell ref="A66:B66"/>
-    <mergeCell ref="F66:H66"/>
-    <mergeCell ref="B68:H68"/>
-    <mergeCell ref="B69:H69"/>
-    <mergeCell ref="A106:B106"/>
-    <mergeCell ref="A107:B107"/>
-    <mergeCell ref="A92:B92"/>
-    <mergeCell ref="A89:B89"/>
-    <mergeCell ref="A93:B93"/>
-    <mergeCell ref="A94:B94"/>
-    <mergeCell ref="A95:H95"/>
-    <mergeCell ref="A96:B96"/>
-    <mergeCell ref="F96:H96"/>
-    <mergeCell ref="A97:B97"/>
-    <mergeCell ref="F97:H97"/>
-    <mergeCell ref="B99:H99"/>
-    <mergeCell ref="B100:H100"/>
-    <mergeCell ref="A101:H101"/>
-    <mergeCell ref="A102:B102"/>
-    <mergeCell ref="A103:B103"/>
-    <mergeCell ref="A104:B104"/>
-    <mergeCell ref="A88:B88"/>
-    <mergeCell ref="A90:B90"/>
-    <mergeCell ref="A91:B91"/>
-    <mergeCell ref="A108:B108"/>
-    <mergeCell ref="A109:H109"/>
-    <mergeCell ref="A110:B110"/>
-    <mergeCell ref="F110:H110"/>
-    <mergeCell ref="F111:H111"/>
-    <mergeCell ref="F112:H112"/>
-    <mergeCell ref="A81:B81"/>
-    <mergeCell ref="F81:H81"/>
-    <mergeCell ref="A82:B82"/>
-    <mergeCell ref="F82:H82"/>
-    <mergeCell ref="B84:H84"/>
-    <mergeCell ref="A79:B79"/>
-    <mergeCell ref="B85:H85"/>
-    <mergeCell ref="A86:H86"/>
-    <mergeCell ref="A87:B87"/>
-    <mergeCell ref="A70:H70"/>
-    <mergeCell ref="A71:B71"/>
-    <mergeCell ref="A72:B72"/>
-    <mergeCell ref="A74:B74"/>
-    <mergeCell ref="A75:B75"/>
-    <mergeCell ref="A76:B76"/>
-    <mergeCell ref="A77:B77"/>
-    <mergeCell ref="A78:B78"/>
-    <mergeCell ref="A80:H80"/>
-    <mergeCell ref="A126:B126"/>
-    <mergeCell ref="F126:H126"/>
-    <mergeCell ref="A105:B105"/>
-    <mergeCell ref="A111:B111"/>
-    <mergeCell ref="A112:B112"/>
-    <mergeCell ref="A123:B123"/>
-    <mergeCell ref="A122:B122"/>
-    <mergeCell ref="A120:B120"/>
-    <mergeCell ref="A121:B121"/>
-    <mergeCell ref="A124:H124"/>
-    <mergeCell ref="A125:B125"/>
-    <mergeCell ref="F125:H125"/>
-    <mergeCell ref="A117:B117"/>
-    <mergeCell ref="A118:B118"/>
-    <mergeCell ref="A119:B119"/>
-    <mergeCell ref="B114:H114"/>
-    <mergeCell ref="B115:H115"/>
-    <mergeCell ref="A116:H116"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>

<commit_message>
Adição de todas as triggers + organização geral
</commit_message>
<xml_diff>
--- a/Dicionário/Dicionario_de_dados.xlsx
+++ b/Dicionário/Dicionario_de_dados.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luigi\Desktop\Faculdade\3 FASE\Banco de Dados II\ABP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luigi\Desktop\Faculdade\3 FASE\Banco de Dados II\ABP\GIT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43DEDA9F-70BA-41DB-BA36-40E71C89992A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A37B8A83-9BFB-4F35-84DB-8DA7A24849F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5685" yWindow="2805" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dicionario" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="574" uniqueCount="191">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -531,9 +531,6 @@
     <t>ID único da fatura do cartão.</t>
   </si>
   <si>
-    <t>ID único da transação realizada que resultou no aumento da fatura.</t>
-  </si>
-  <si>
     <t>0 -&gt; 999999…</t>
   </si>
   <si>
@@ -556,6 +553,51 @@
   </si>
   <si>
     <t>Conta "Ativa"(1) ou "Inativa"(0)</t>
+  </si>
+  <si>
+    <t>Emprestimodesativado</t>
+  </si>
+  <si>
+    <t>Tabela responsável por armazenar os empréstimos desativados.</t>
+  </si>
+  <si>
+    <t>id_empdesat</t>
+  </si>
+  <si>
+    <t>ID único do empréstimo desativado.</t>
+  </si>
+  <si>
+    <t>ID único do empréstimo recém desativado da tabela empréstimo.</t>
+  </si>
+  <si>
+    <t>idx_id_emprest</t>
+  </si>
+  <si>
+    <t>pk_Emprestimodesativado</t>
+  </si>
+  <si>
+    <t>Faturadesativada</t>
+  </si>
+  <si>
+    <t>Tabela responsável por armazenar as faturas recém desativadas da tabela Fatura.</t>
+  </si>
+  <si>
+    <t>id_fatdesat</t>
+  </si>
+  <si>
+    <t>ID único da fatura desativada.</t>
+  </si>
+  <si>
+    <t>ID único da fatura recém desativada da tabela empréstimo.</t>
+  </si>
+  <si>
+    <t>pk_Faturadesativada</t>
+  </si>
+  <si>
+    <t>idx_fatura</t>
+  </si>
+  <si>
+    <t>Null</t>
   </si>
 </sst>
 </file>
@@ -610,7 +652,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="41">
+  <borders count="44">
     <border>
       <left/>
       <right/>
@@ -992,17 +1034,6 @@
         <color rgb="FF000000"/>
       </left>
       <right/>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right/>
       <top style="medium">
         <color indexed="64"/>
       </top>
@@ -1100,11 +1131,59 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="78">
+  <cellXfs count="126">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1192,22 +1271,14 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1216,53 +1287,61 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1271,18 +1350,158 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1500,7 +1719,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z1004"/>
+  <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1509,8 +1728,8 @@
     <col min="1" max="3" width="15.5703125" customWidth="1"/>
     <col min="4" max="4" width="15.42578125" customWidth="1"/>
     <col min="5" max="5" width="15.5703125" customWidth="1"/>
-    <col min="6" max="6" width="3.85546875" customWidth="1"/>
-    <col min="7" max="7" width="3.7109375" customWidth="1"/>
+    <col min="6" max="6" width="3.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="3.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="69" customWidth="1"/>
     <col min="9" max="26" width="15.5703125" customWidth="1"/>
   </cols>
@@ -1519,15 +1738,15 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="72" t="s">
+      <c r="B1" s="62" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="39"/>
-      <c r="D1" s="39"/>
-      <c r="E1" s="39"/>
-      <c r="F1" s="39"/>
-      <c r="G1" s="39"/>
-      <c r="H1" s="40"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="55"/>
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
       <c r="K1" s="2"/>
@@ -1551,15 +1770,15 @@
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="38" t="s">
+      <c r="B2" s="60" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
-      <c r="G2" s="39"/>
-      <c r="H2" s="40"/>
+      <c r="C2" s="54"/>
+      <c r="D2" s="54"/>
+      <c r="E2" s="54"/>
+      <c r="F2" s="54"/>
+      <c r="G2" s="54"/>
+      <c r="H2" s="55"/>
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
@@ -1580,16 +1799,16 @@
       <c r="Z2" s="2"/>
     </row>
     <row r="3" spans="1:26">
-      <c r="A3" s="41" t="s">
+      <c r="A3" s="61" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="39"/>
-      <c r="C3" s="39"/>
-      <c r="D3" s="39"/>
-      <c r="E3" s="39"/>
-      <c r="F3" s="39"/>
-      <c r="G3" s="39"/>
-      <c r="H3" s="40"/>
+      <c r="B3" s="54"/>
+      <c r="C3" s="54"/>
+      <c r="D3" s="54"/>
+      <c r="E3" s="54"/>
+      <c r="F3" s="54"/>
+      <c r="G3" s="54"/>
+      <c r="H3" s="55"/>
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
@@ -1610,10 +1829,10 @@
       <c r="Z3" s="2"/>
     </row>
     <row r="4" spans="1:26">
-      <c r="A4" s="42" t="s">
+      <c r="A4" s="53" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="43"/>
+      <c r="B4" s="49"/>
       <c r="C4" s="1" t="s">
         <v>6</v>
       </c>
@@ -1652,10 +1871,10 @@
       <c r="Z4" s="2"/>
     </row>
     <row r="5" spans="1:26">
-      <c r="A5" s="44" t="s">
+      <c r="A5" s="48" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="43"/>
+      <c r="B5" s="49"/>
       <c r="C5" s="4" t="s">
         <v>12</v>
       </c>
@@ -1692,10 +1911,10 @@
       <c r="Z5" s="2"/>
     </row>
     <row r="6" spans="1:26">
-      <c r="A6" s="44" t="s">
+      <c r="A6" s="48" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="43"/>
+      <c r="B6" s="49"/>
       <c r="C6" s="4" t="s">
         <v>18</v>
       </c>
@@ -1708,7 +1927,7 @@
       <c r="F6" s="5"/>
       <c r="G6" s="5"/>
       <c r="H6" s="6" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
@@ -1730,10 +1949,10 @@
       <c r="Z6" s="2"/>
     </row>
     <row r="7" spans="1:26">
-      <c r="A7" s="44" t="s">
+      <c r="A7" s="48" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="43"/>
+      <c r="B7" s="49"/>
       <c r="C7" s="4" t="s">
         <v>21</v>
       </c>
@@ -1768,10 +1987,10 @@
       <c r="Z7" s="2"/>
     </row>
     <row r="8" spans="1:26">
-      <c r="A8" s="44" t="s">
+      <c r="A8" s="48" t="s">
         <v>24</v>
       </c>
-      <c r="B8" s="43"/>
+      <c r="B8" s="49"/>
       <c r="C8" s="4" t="s">
         <v>25</v>
       </c>
@@ -1806,10 +2025,10 @@
       <c r="Z8" s="2"/>
     </row>
     <row r="9" spans="1:26">
-      <c r="A9" s="44" t="s">
+      <c r="A9" s="48" t="s">
         <v>28</v>
       </c>
-      <c r="B9" s="43"/>
+      <c r="B9" s="49"/>
       <c r="C9" s="4" t="s">
         <v>29</v>
       </c>
@@ -1844,10 +2063,10 @@
       <c r="Z9" s="2"/>
     </row>
     <row r="10" spans="1:26">
-      <c r="A10" s="44" t="s">
+      <c r="A10" s="48" t="s">
         <v>32</v>
       </c>
-      <c r="B10" s="43"/>
+      <c r="B10" s="49"/>
       <c r="C10" s="4" t="s">
         <v>33</v>
       </c>
@@ -1882,10 +2101,10 @@
       <c r="Z10" s="2"/>
     </row>
     <row r="11" spans="1:26">
-      <c r="A11" s="68" t="s">
+      <c r="A11" s="65" t="s">
         <v>36</v>
       </c>
-      <c r="B11" s="43"/>
+      <c r="B11" s="49"/>
       <c r="C11" s="8" t="s">
         <v>37</v>
       </c>
@@ -1920,10 +2139,10 @@
       <c r="Z11" s="2"/>
     </row>
     <row r="12" spans="1:26">
-      <c r="A12" s="68" t="s">
+      <c r="A12" s="65" t="s">
         <v>39</v>
       </c>
-      <c r="B12" s="43"/>
+      <c r="B12" s="49"/>
       <c r="C12" s="8" t="s">
         <v>21</v>
       </c>
@@ -1958,10 +2177,10 @@
       <c r="Z12" s="2"/>
     </row>
     <row r="13" spans="1:26">
-      <c r="A13" s="68" t="s">
+      <c r="A13" s="65" t="s">
         <v>41</v>
       </c>
-      <c r="B13" s="43"/>
+      <c r="B13" s="49"/>
       <c r="C13" s="8" t="s">
         <v>42</v>
       </c>
@@ -1996,10 +2215,10 @@
       <c r="Z13" s="2"/>
     </row>
     <row r="14" spans="1:26">
-      <c r="A14" s="73" t="s">
+      <c r="A14" s="63" t="s">
         <v>45</v>
       </c>
-      <c r="B14" s="57"/>
+      <c r="B14" s="64"/>
       <c r="C14" s="11" t="s">
         <v>46</v>
       </c>
@@ -2034,16 +2253,16 @@
       <c r="Z14" s="2"/>
     </row>
     <row r="15" spans="1:26" ht="15" customHeight="1">
-      <c r="A15" s="74" t="s">
+      <c r="A15" s="50" t="s">
         <v>48</v>
       </c>
-      <c r="B15" s="75"/>
-      <c r="C15" s="75"/>
-      <c r="D15" s="75"/>
-      <c r="E15" s="75"/>
-      <c r="F15" s="75"/>
-      <c r="G15" s="75"/>
-      <c r="H15" s="76"/>
+      <c r="B15" s="51"/>
+      <c r="C15" s="51"/>
+      <c r="D15" s="51"/>
+      <c r="E15" s="51"/>
+      <c r="F15" s="51"/>
+      <c r="G15" s="51"/>
+      <c r="H15" s="52"/>
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
       <c r="K15" s="2"/>
@@ -2064,10 +2283,10 @@
       <c r="Z15" s="2"/>
     </row>
     <row r="16" spans="1:26" ht="15" customHeight="1">
-      <c r="A16" s="42" t="s">
+      <c r="A16" s="53" t="s">
         <v>49</v>
       </c>
-      <c r="B16" s="43"/>
+      <c r="B16" s="49"/>
       <c r="C16" s="1" t="s">
         <v>50</v>
       </c>
@@ -2077,11 +2296,11 @@
       <c r="E16" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="F16" s="42" t="s">
+      <c r="F16" s="53" t="s">
         <v>53</v>
       </c>
-      <c r="G16" s="39"/>
-      <c r="H16" s="40"/>
+      <c r="G16" s="54"/>
+      <c r="H16" s="55"/>
       <c r="I16" s="2"/>
       <c r="J16" s="2"/>
       <c r="K16" s="2"/>
@@ -2102,10 +2321,10 @@
       <c r="Z16" s="2"/>
     </row>
     <row r="17" spans="1:26">
-      <c r="A17" s="54" t="s">
+      <c r="A17" s="56" t="s">
         <v>54</v>
       </c>
-      <c r="B17" s="43"/>
+      <c r="B17" s="49"/>
       <c r="C17" s="15" t="s">
         <v>15</v>
       </c>
@@ -2113,11 +2332,11 @@
       <c r="E17" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="F17" s="54" t="s">
+      <c r="F17" s="56" t="s">
         <v>11</v>
       </c>
-      <c r="G17" s="39"/>
-      <c r="H17" s="40"/>
+      <c r="G17" s="54"/>
+      <c r="H17" s="55"/>
       <c r="I17" s="2"/>
       <c r="J17" s="2"/>
       <c r="K17" s="2"/>
@@ -2138,10 +2357,10 @@
       <c r="Z17" s="2"/>
     </row>
     <row r="18" spans="1:26">
-      <c r="A18" s="54" t="s">
+      <c r="A18" s="56" t="s">
         <v>55</v>
       </c>
-      <c r="B18" s="43"/>
+      <c r="B18" s="49"/>
       <c r="C18" s="15"/>
       <c r="D18" s="15" t="s">
         <v>15</v>
@@ -2149,11 +2368,11 @@
       <c r="E18" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="F18" s="54" t="s">
+      <c r="F18" s="56" t="s">
         <v>24</v>
       </c>
-      <c r="G18" s="39"/>
-      <c r="H18" s="40"/>
+      <c r="G18" s="54"/>
+      <c r="H18" s="55"/>
       <c r="I18" s="2"/>
       <c r="J18" s="2"/>
       <c r="K18" s="2"/>
@@ -2174,10 +2393,10 @@
       <c r="Z18" s="2"/>
     </row>
     <row r="19" spans="1:26">
-      <c r="A19" s="70" t="s">
+      <c r="A19" s="66" t="s">
         <v>56</v>
       </c>
-      <c r="B19" s="43"/>
+      <c r="B19" s="49"/>
       <c r="C19" s="15"/>
       <c r="D19" s="15" t="s">
         <v>15</v>
@@ -2185,11 +2404,11 @@
       <c r="E19" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="F19" s="70" t="s">
+      <c r="F19" s="66" t="s">
         <v>39</v>
       </c>
-      <c r="G19" s="39"/>
-      <c r="H19" s="40"/>
+      <c r="G19" s="54"/>
+      <c r="H19" s="55"/>
       <c r="I19" s="2"/>
       <c r="J19" s="2"/>
       <c r="K19" s="2"/>
@@ -2210,10 +2429,10 @@
       <c r="Z19" s="2"/>
     </row>
     <row r="20" spans="1:26">
-      <c r="A20" s="71" t="s">
+      <c r="A20" s="67" t="s">
         <v>57</v>
       </c>
-      <c r="B20" s="51"/>
+      <c r="B20" s="70"/>
       <c r="C20" s="17"/>
       <c r="D20" s="18" t="s">
         <v>15</v>
@@ -2221,11 +2440,11 @@
       <c r="E20" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="F20" s="71" t="s">
+      <c r="F20" s="67" t="s">
         <v>32</v>
       </c>
-      <c r="G20" s="52"/>
-      <c r="H20" s="53"/>
+      <c r="G20" s="68"/>
+      <c r="H20" s="69"/>
       <c r="I20" s="2"/>
       <c r="J20" s="2"/>
       <c r="K20" s="2"/>
@@ -2277,15 +2496,15 @@
       <c r="A22" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="B22" s="61" t="s">
+      <c r="B22" s="57" t="s">
         <v>59</v>
       </c>
-      <c r="C22" s="62"/>
-      <c r="D22" s="62"/>
-      <c r="E22" s="62"/>
-      <c r="F22" s="62"/>
-      <c r="G22" s="62"/>
-      <c r="H22" s="63"/>
+      <c r="C22" s="58"/>
+      <c r="D22" s="58"/>
+      <c r="E22" s="58"/>
+      <c r="F22" s="58"/>
+      <c r="G22" s="58"/>
+      <c r="H22" s="59"/>
       <c r="I22" s="2"/>
       <c r="J22" s="2"/>
       <c r="K22" s="2"/>
@@ -2309,15 +2528,15 @@
       <c r="A23" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B23" s="38" t="s">
+      <c r="B23" s="60" t="s">
         <v>60</v>
       </c>
-      <c r="C23" s="39"/>
-      <c r="D23" s="39"/>
-      <c r="E23" s="39"/>
-      <c r="F23" s="39"/>
-      <c r="G23" s="39"/>
-      <c r="H23" s="40"/>
+      <c r="C23" s="54"/>
+      <c r="D23" s="54"/>
+      <c r="E23" s="54"/>
+      <c r="F23" s="54"/>
+      <c r="G23" s="54"/>
+      <c r="H23" s="55"/>
       <c r="I23" s="2"/>
       <c r="J23" s="2"/>
       <c r="K23" s="2"/>
@@ -2338,16 +2557,16 @@
       <c r="Z23" s="2"/>
     </row>
     <row r="24" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A24" s="41" t="s">
+      <c r="A24" s="61" t="s">
         <v>4</v>
       </c>
-      <c r="B24" s="39"/>
-      <c r="C24" s="39"/>
-      <c r="D24" s="39"/>
-      <c r="E24" s="39"/>
-      <c r="F24" s="39"/>
-      <c r="G24" s="39"/>
-      <c r="H24" s="40"/>
+      <c r="B24" s="54"/>
+      <c r="C24" s="54"/>
+      <c r="D24" s="54"/>
+      <c r="E24" s="54"/>
+      <c r="F24" s="54"/>
+      <c r="G24" s="54"/>
+      <c r="H24" s="55"/>
       <c r="I24" s="2"/>
       <c r="J24" s="2"/>
       <c r="K24" s="2"/>
@@ -2368,10 +2587,10 @@
       <c r="Z24" s="2"/>
     </row>
     <row r="25" spans="1:26" ht="15" customHeight="1">
-      <c r="A25" s="42" t="s">
+      <c r="A25" s="53" t="s">
         <v>5</v>
       </c>
-      <c r="B25" s="43"/>
+      <c r="B25" s="49"/>
       <c r="C25" s="1" t="s">
         <v>6</v>
       </c>
@@ -2410,10 +2629,10 @@
       <c r="Z25" s="2"/>
     </row>
     <row r="26" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A26" s="44" t="s">
+      <c r="A26" s="48" t="s">
         <v>61</v>
       </c>
-      <c r="B26" s="43"/>
+      <c r="B26" s="49"/>
       <c r="C26" s="4" t="s">
         <v>12</v>
       </c>
@@ -2450,10 +2669,10 @@
       <c r="Z26" s="2"/>
     </row>
     <row r="27" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A27" s="44" t="s">
+      <c r="A27" s="48" t="s">
         <v>11</v>
       </c>
-      <c r="B27" s="43"/>
+      <c r="B27" s="49"/>
       <c r="C27" s="4" t="s">
         <v>12</v>
       </c>
@@ -2490,10 +2709,10 @@
       <c r="Z27" s="2"/>
     </row>
     <row r="28" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A28" s="44" t="s">
+      <c r="A28" s="48" t="s">
         <v>64</v>
       </c>
-      <c r="B28" s="43"/>
+      <c r="B28" s="49"/>
       <c r="C28" s="4" t="s">
         <v>42</v>
       </c>
@@ -2528,10 +2747,10 @@
       <c r="Z28" s="2"/>
     </row>
     <row r="29" spans="1:26" ht="15" customHeight="1">
-      <c r="A29" s="44" t="s">
+      <c r="A29" s="48" t="s">
         <v>66</v>
       </c>
-      <c r="B29" s="43"/>
+      <c r="B29" s="49"/>
       <c r="C29" s="4" t="s">
         <v>67</v>
       </c>
@@ -2566,10 +2785,10 @@
       <c r="Z29" s="2"/>
     </row>
     <row r="30" spans="1:26" ht="15" customHeight="1">
-      <c r="A30" s="44" t="s">
+      <c r="A30" s="48" t="s">
         <v>70</v>
       </c>
-      <c r="B30" s="43"/>
+      <c r="B30" s="49"/>
       <c r="C30" s="4" t="s">
         <v>67</v>
       </c>
@@ -2604,10 +2823,10 @@
       <c r="Z30" s="2"/>
     </row>
     <row r="31" spans="1:26" ht="15" customHeight="1">
-      <c r="A31" s="44" t="s">
+      <c r="A31" s="48" t="s">
         <v>72</v>
       </c>
-      <c r="B31" s="43"/>
+      <c r="B31" s="49"/>
       <c r="C31" s="4" t="s">
         <v>67</v>
       </c>
@@ -2642,10 +2861,10 @@
       <c r="Z31" s="2"/>
     </row>
     <row r="32" spans="1:26" ht="15" customHeight="1">
-      <c r="A32" s="68" t="s">
+      <c r="A32" s="65" t="s">
         <v>74</v>
       </c>
-      <c r="B32" s="43"/>
+      <c r="B32" s="49"/>
       <c r="C32" s="4" t="s">
         <v>67</v>
       </c>
@@ -2680,10 +2899,10 @@
       <c r="Z32" s="2"/>
     </row>
     <row r="33" spans="1:26" ht="15" customHeight="1">
-      <c r="A33" s="69" t="s">
+      <c r="A33" s="71" t="s">
         <v>76</v>
       </c>
-      <c r="B33" s="51"/>
+      <c r="B33" s="70"/>
       <c r="C33" s="23" t="s">
         <v>67</v>
       </c>
@@ -2718,16 +2937,16 @@
       <c r="Z33" s="2"/>
     </row>
     <row r="34" spans="1:26" ht="15" customHeight="1">
-      <c r="A34" s="58" t="s">
+      <c r="A34" s="72" t="s">
         <v>48</v>
       </c>
-      <c r="B34" s="59"/>
-      <c r="C34" s="59"/>
-      <c r="D34" s="59"/>
-      <c r="E34" s="59"/>
-      <c r="F34" s="59"/>
-      <c r="G34" s="59"/>
-      <c r="H34" s="60"/>
+      <c r="B34" s="73"/>
+      <c r="C34" s="73"/>
+      <c r="D34" s="73"/>
+      <c r="E34" s="73"/>
+      <c r="F34" s="73"/>
+      <c r="G34" s="73"/>
+      <c r="H34" s="74"/>
       <c r="I34" s="2"/>
       <c r="J34" s="2"/>
       <c r="K34" s="2"/>
@@ -2748,10 +2967,10 @@
       <c r="Z34" s="2"/>
     </row>
     <row r="35" spans="1:26" ht="15" customHeight="1">
-      <c r="A35" s="42" t="s">
+      <c r="A35" s="53" t="s">
         <v>49</v>
       </c>
-      <c r="B35" s="43"/>
+      <c r="B35" s="49"/>
       <c r="C35" s="1" t="s">
         <v>50</v>
       </c>
@@ -2761,11 +2980,11 @@
       <c r="E35" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="F35" s="42" t="s">
+      <c r="F35" s="53" t="s">
         <v>53</v>
       </c>
-      <c r="G35" s="39"/>
-      <c r="H35" s="40"/>
+      <c r="G35" s="54"/>
+      <c r="H35" s="55"/>
       <c r="I35" s="2"/>
       <c r="J35" s="2"/>
       <c r="K35" s="2"/>
@@ -2785,11 +3004,11 @@
       <c r="Y35" s="2"/>
       <c r="Z35" s="2"/>
     </row>
-    <row r="36" spans="1:26" ht="15" customHeight="1">
-      <c r="A36" s="54" t="s">
+    <row r="36" spans="1:26" ht="15" customHeight="1" thickBot="1">
+      <c r="A36" s="56" t="s">
         <v>78</v>
       </c>
-      <c r="B36" s="43"/>
+      <c r="B36" s="49"/>
       <c r="C36" s="15" t="s">
         <v>15</v>
       </c>
@@ -2797,11 +3016,11 @@
       <c r="E36" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="F36" s="54" t="s">
+      <c r="F36" s="56" t="s">
         <v>61</v>
       </c>
-      <c r="G36" s="39"/>
-      <c r="H36" s="40"/>
+      <c r="G36" s="54"/>
+      <c r="H36" s="55"/>
       <c r="I36" s="2"/>
       <c r="J36" s="2"/>
       <c r="K36" s="2"/>
@@ -2821,7 +3040,7 @@
       <c r="Y36" s="2"/>
       <c r="Z36" s="2"/>
     </row>
-    <row r="37" spans="1:26" ht="15.75" customHeight="1">
+    <row r="37" spans="1:26" ht="15.75" customHeight="1" thickBot="1">
       <c r="A37" s="19"/>
       <c r="B37" s="19"/>
       <c r="C37" s="19"/>
@@ -2853,15 +3072,15 @@
       <c r="A38" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="B38" s="61" t="s">
+      <c r="B38" s="57" t="s">
         <v>79</v>
       </c>
-      <c r="C38" s="62"/>
-      <c r="D38" s="62"/>
-      <c r="E38" s="62"/>
-      <c r="F38" s="62"/>
-      <c r="G38" s="62"/>
-      <c r="H38" s="63"/>
+      <c r="C38" s="58"/>
+      <c r="D38" s="58"/>
+      <c r="E38" s="58"/>
+      <c r="F38" s="58"/>
+      <c r="G38" s="58"/>
+      <c r="H38" s="59"/>
       <c r="I38" s="2"/>
       <c r="J38" s="2"/>
       <c r="K38" s="2"/>
@@ -2885,15 +3104,15 @@
       <c r="A39" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B39" s="38" t="s">
+      <c r="B39" s="60" t="s">
         <v>80</v>
       </c>
-      <c r="C39" s="39"/>
-      <c r="D39" s="39"/>
-      <c r="E39" s="39"/>
-      <c r="F39" s="39"/>
-      <c r="G39" s="39"/>
-      <c r="H39" s="40"/>
+      <c r="C39" s="54"/>
+      <c r="D39" s="54"/>
+      <c r="E39" s="54"/>
+      <c r="F39" s="54"/>
+      <c r="G39" s="54"/>
+      <c r="H39" s="55"/>
       <c r="I39" s="2"/>
       <c r="J39" s="2"/>
       <c r="K39" s="2"/>
@@ -2914,16 +3133,16 @@
       <c r="Z39" s="2"/>
     </row>
     <row r="40" spans="1:26" ht="15" customHeight="1">
-      <c r="A40" s="41" t="s">
+      <c r="A40" s="61" t="s">
         <v>4</v>
       </c>
-      <c r="B40" s="39"/>
-      <c r="C40" s="39"/>
-      <c r="D40" s="39"/>
-      <c r="E40" s="39"/>
-      <c r="F40" s="39"/>
-      <c r="G40" s="39"/>
-      <c r="H40" s="40"/>
+      <c r="B40" s="54"/>
+      <c r="C40" s="54"/>
+      <c r="D40" s="54"/>
+      <c r="E40" s="54"/>
+      <c r="F40" s="54"/>
+      <c r="G40" s="54"/>
+      <c r="H40" s="55"/>
       <c r="I40" s="2"/>
       <c r="J40" s="2"/>
       <c r="K40" s="2"/>
@@ -2944,10 +3163,10 @@
       <c r="Z40" s="2"/>
     </row>
     <row r="41" spans="1:26" ht="15" customHeight="1">
-      <c r="A41" s="42" t="s">
+      <c r="A41" s="53" t="s">
         <v>5</v>
       </c>
-      <c r="B41" s="43"/>
+      <c r="B41" s="49"/>
       <c r="C41" s="1" t="s">
         <v>6</v>
       </c>
@@ -2986,10 +3205,10 @@
       <c r="Z41" s="2"/>
     </row>
     <row r="42" spans="1:26" ht="15" customHeight="1">
-      <c r="A42" s="44" t="s">
+      <c r="A42" s="48" t="s">
         <v>81</v>
       </c>
-      <c r="B42" s="43"/>
+      <c r="B42" s="49"/>
       <c r="C42" s="4" t="s">
         <v>12</v>
       </c>
@@ -3026,10 +3245,10 @@
       <c r="Z42" s="2"/>
     </row>
     <row r="43" spans="1:26" ht="15" customHeight="1">
-      <c r="A43" s="44" t="s">
+      <c r="A43" s="48" t="s">
         <v>61</v>
       </c>
-      <c r="B43" s="43"/>
+      <c r="B43" s="49"/>
       <c r="C43" s="4" t="s">
         <v>12</v>
       </c>
@@ -3066,10 +3285,10 @@
       <c r="Z43" s="2"/>
     </row>
     <row r="44" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A44" s="44" t="s">
+      <c r="A44" s="48" t="s">
         <v>84</v>
       </c>
-      <c r="B44" s="43"/>
+      <c r="B44" s="49"/>
       <c r="C44" s="4" t="s">
         <v>85</v>
       </c>
@@ -3104,10 +3323,10 @@
       <c r="Z44" s="2"/>
     </row>
     <row r="45" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A45" s="44" t="s">
+      <c r="A45" s="48" t="s">
         <v>88</v>
       </c>
-      <c r="B45" s="43"/>
+      <c r="B45" s="49"/>
       <c r="C45" s="4" t="s">
         <v>85</v>
       </c>
@@ -3142,10 +3361,10 @@
       <c r="Z45" s="2"/>
     </row>
     <row r="46" spans="1:26" ht="15" customHeight="1">
-      <c r="A46" s="44" t="s">
+      <c r="A46" s="48" t="s">
         <v>90</v>
       </c>
-      <c r="B46" s="43"/>
+      <c r="B46" s="49"/>
       <c r="C46" s="4" t="s">
         <v>67</v>
       </c>
@@ -3180,10 +3399,10 @@
       <c r="Z46" s="2"/>
     </row>
     <row r="47" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A47" s="44" t="s">
+      <c r="A47" s="48" t="s">
         <v>92</v>
       </c>
-      <c r="B47" s="43"/>
+      <c r="B47" s="49"/>
       <c r="C47" s="4" t="s">
         <v>67</v>
       </c>
@@ -3218,12 +3437,12 @@
       <c r="Z47" s="2"/>
     </row>
     <row r="48" spans="1:26" ht="15" customHeight="1">
-      <c r="A48" s="73" t="s">
+      <c r="A48" s="63" t="s">
         <v>94</v>
       </c>
-      <c r="B48" s="57"/>
+      <c r="B48" s="64"/>
       <c r="C48" s="11" t="s">
-        <v>29</v>
+        <v>46</v>
       </c>
       <c r="D48" s="11" t="s">
         <v>30</v>
@@ -3256,16 +3475,16 @@
       <c r="Z48" s="2"/>
     </row>
     <row r="49" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A49" s="74" t="s">
+      <c r="A49" s="50" t="s">
         <v>48</v>
       </c>
-      <c r="B49" s="75"/>
-      <c r="C49" s="75"/>
-      <c r="D49" s="75"/>
-      <c r="E49" s="75"/>
-      <c r="F49" s="75"/>
-      <c r="G49" s="75"/>
-      <c r="H49" s="76"/>
+      <c r="B49" s="51"/>
+      <c r="C49" s="51"/>
+      <c r="D49" s="51"/>
+      <c r="E49" s="51"/>
+      <c r="F49" s="51"/>
+      <c r="G49" s="51"/>
+      <c r="H49" s="52"/>
       <c r="I49" s="2"/>
       <c r="J49" s="2"/>
       <c r="K49" s="2"/>
@@ -3286,10 +3505,10 @@
       <c r="Z49" s="2"/>
     </row>
     <row r="50" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A50" s="42" t="s">
+      <c r="A50" s="53" t="s">
         <v>49</v>
       </c>
-      <c r="B50" s="43"/>
+      <c r="B50" s="49"/>
       <c r="C50" s="1" t="s">
         <v>50</v>
       </c>
@@ -3299,11 +3518,11 @@
       <c r="E50" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="F50" s="42" t="s">
+      <c r="F50" s="53" t="s">
         <v>53</v>
       </c>
-      <c r="G50" s="39"/>
-      <c r="H50" s="40"/>
+      <c r="G50" s="54"/>
+      <c r="H50" s="55"/>
       <c r="I50" s="2"/>
       <c r="J50" s="2"/>
       <c r="K50" s="2"/>
@@ -3324,10 +3543,10 @@
       <c r="Z50" s="2"/>
     </row>
     <row r="51" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A51" s="54" t="s">
+      <c r="A51" s="56" t="s">
         <v>96</v>
       </c>
-      <c r="B51" s="43"/>
+      <c r="B51" s="49"/>
       <c r="C51" s="15" t="s">
         <v>15</v>
       </c>
@@ -3335,11 +3554,11 @@
       <c r="E51" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="F51" s="54" t="s">
+      <c r="F51" s="56" t="s">
         <v>81</v>
       </c>
-      <c r="G51" s="39"/>
-      <c r="H51" s="40"/>
+      <c r="G51" s="54"/>
+      <c r="H51" s="55"/>
       <c r="I51" s="2"/>
       <c r="J51" s="2"/>
       <c r="K51" s="2"/>
@@ -3391,15 +3610,15 @@
       <c r="A53" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="B53" s="61" t="s">
+      <c r="B53" s="57" t="s">
         <v>97</v>
       </c>
-      <c r="C53" s="62"/>
-      <c r="D53" s="62"/>
-      <c r="E53" s="62"/>
-      <c r="F53" s="62"/>
-      <c r="G53" s="62"/>
-      <c r="H53" s="63"/>
+      <c r="C53" s="58"/>
+      <c r="D53" s="58"/>
+      <c r="E53" s="58"/>
+      <c r="F53" s="58"/>
+      <c r="G53" s="58"/>
+      <c r="H53" s="59"/>
       <c r="I53" s="2"/>
       <c r="J53" s="2"/>
       <c r="K53" s="2"/>
@@ -3423,15 +3642,15 @@
       <c r="A54" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B54" s="38" t="s">
+      <c r="B54" s="60" t="s">
         <v>98</v>
       </c>
-      <c r="C54" s="39"/>
-      <c r="D54" s="39"/>
-      <c r="E54" s="39"/>
-      <c r="F54" s="39"/>
-      <c r="G54" s="39"/>
-      <c r="H54" s="40"/>
+      <c r="C54" s="54"/>
+      <c r="D54" s="54"/>
+      <c r="E54" s="54"/>
+      <c r="F54" s="54"/>
+      <c r="G54" s="54"/>
+      <c r="H54" s="55"/>
       <c r="I54" s="2"/>
       <c r="J54" s="2"/>
       <c r="K54" s="2"/>
@@ -3452,16 +3671,16 @@
       <c r="Z54" s="2"/>
     </row>
     <row r="55" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A55" s="41" t="s">
+      <c r="A55" s="61" t="s">
         <v>4</v>
       </c>
-      <c r="B55" s="39"/>
-      <c r="C55" s="39"/>
-      <c r="D55" s="39"/>
-      <c r="E55" s="39"/>
-      <c r="F55" s="39"/>
-      <c r="G55" s="39"/>
-      <c r="H55" s="40"/>
+      <c r="B55" s="54"/>
+      <c r="C55" s="54"/>
+      <c r="D55" s="54"/>
+      <c r="E55" s="54"/>
+      <c r="F55" s="54"/>
+      <c r="G55" s="54"/>
+      <c r="H55" s="55"/>
       <c r="I55" s="2"/>
       <c r="J55" s="2"/>
       <c r="K55" s="2"/>
@@ -3482,10 +3701,10 @@
       <c r="Z55" s="2"/>
     </row>
     <row r="56" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A56" s="42" t="s">
+      <c r="A56" s="53" t="s">
         <v>5</v>
       </c>
-      <c r="B56" s="43"/>
+      <c r="B56" s="49"/>
       <c r="C56" s="1" t="s">
         <v>6</v>
       </c>
@@ -3524,10 +3743,10 @@
       <c r="Z56" s="2"/>
     </row>
     <row r="57" spans="1:26" ht="15" customHeight="1">
-      <c r="A57" s="44" t="s">
+      <c r="A57" s="48" t="s">
         <v>99</v>
       </c>
-      <c r="B57" s="43"/>
+      <c r="B57" s="49"/>
       <c r="C57" s="4" t="s">
         <v>12</v>
       </c>
@@ -3564,10 +3783,10 @@
       <c r="Z57" s="2"/>
     </row>
     <row r="58" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A58" s="44" t="s">
+      <c r="A58" s="48" t="s">
         <v>61</v>
       </c>
-      <c r="B58" s="43"/>
+      <c r="B58" s="49"/>
       <c r="C58" s="4" t="s">
         <v>12</v>
       </c>
@@ -3604,10 +3823,10 @@
       <c r="Z58" s="2"/>
     </row>
     <row r="59" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A59" s="44" t="s">
+      <c r="A59" s="48" t="s">
         <v>11</v>
       </c>
-      <c r="B59" s="43"/>
+      <c r="B59" s="49"/>
       <c r="C59" s="4" t="s">
         <v>12</v>
       </c>
@@ -3644,10 +3863,10 @@
       <c r="Z59" s="2"/>
     </row>
     <row r="60" spans="1:26" ht="15" customHeight="1">
-      <c r="A60" s="44" t="s">
+      <c r="A60" s="48" t="s">
         <v>103</v>
       </c>
-      <c r="B60" s="43"/>
+      <c r="B60" s="49"/>
       <c r="C60" s="4" t="s">
         <v>46</v>
       </c>
@@ -3682,10 +3901,10 @@
       <c r="Z60" s="2"/>
     </row>
     <row r="61" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A61" s="44" t="s">
+      <c r="A61" s="48" t="s">
         <v>105</v>
       </c>
-      <c r="B61" s="43"/>
+      <c r="B61" s="49"/>
       <c r="C61" s="4" t="s">
         <v>42</v>
       </c>
@@ -3720,10 +3939,10 @@
       <c r="Z61" s="2"/>
     </row>
     <row r="62" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A62" s="44" t="s">
+      <c r="A62" s="48" t="s">
         <v>107</v>
       </c>
-      <c r="B62" s="43"/>
+      <c r="B62" s="49"/>
       <c r="C62" s="12" t="s">
         <v>108</v>
       </c>
@@ -3731,7 +3950,7 @@
         <v>109</v>
       </c>
       <c r="E62" s="12" t="s">
-        <v>14</v>
+        <v>190</v>
       </c>
       <c r="F62" s="29"/>
       <c r="G62" s="29"/>
@@ -3758,10 +3977,10 @@
       <c r="Z62" s="2"/>
     </row>
     <row r="63" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A63" s="55" t="s">
+      <c r="A63" s="75" t="s">
         <v>111</v>
       </c>
-      <c r="B63" s="51"/>
+      <c r="B63" s="70"/>
       <c r="C63" s="23" t="s">
         <v>67</v>
       </c>
@@ -3796,16 +4015,16 @@
       <c r="Z63" s="2"/>
     </row>
     <row r="64" spans="1:26" ht="15" customHeight="1">
-      <c r="A64" s="58" t="s">
+      <c r="A64" s="72" t="s">
         <v>48</v>
       </c>
-      <c r="B64" s="59"/>
-      <c r="C64" s="59"/>
-      <c r="D64" s="59"/>
-      <c r="E64" s="59"/>
-      <c r="F64" s="59"/>
-      <c r="G64" s="59"/>
-      <c r="H64" s="60"/>
+      <c r="B64" s="73"/>
+      <c r="C64" s="73"/>
+      <c r="D64" s="73"/>
+      <c r="E64" s="73"/>
+      <c r="F64" s="73"/>
+      <c r="G64" s="73"/>
+      <c r="H64" s="74"/>
       <c r="I64" s="2"/>
       <c r="J64" s="2"/>
       <c r="K64" s="2"/>
@@ -3826,10 +4045,10 @@
       <c r="Z64" s="2"/>
     </row>
     <row r="65" spans="1:26" ht="15" customHeight="1">
-      <c r="A65" s="42" t="s">
+      <c r="A65" s="53" t="s">
         <v>49</v>
       </c>
-      <c r="B65" s="43"/>
+      <c r="B65" s="49"/>
       <c r="C65" s="1" t="s">
         <v>50</v>
       </c>
@@ -3839,11 +4058,11 @@
       <c r="E65" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="F65" s="42" t="s">
+      <c r="F65" s="53" t="s">
         <v>53</v>
       </c>
-      <c r="G65" s="39"/>
-      <c r="H65" s="40"/>
+      <c r="G65" s="54"/>
+      <c r="H65" s="55"/>
       <c r="I65" s="2"/>
       <c r="J65" s="2"/>
       <c r="K65" s="2"/>
@@ -3864,10 +4083,10 @@
       <c r="Z65" s="2"/>
     </row>
     <row r="66" spans="1:26" ht="15" customHeight="1">
-      <c r="A66" s="54" t="s">
+      <c r="A66" s="56" t="s">
         <v>113</v>
       </c>
-      <c r="B66" s="43"/>
+      <c r="B66" s="49"/>
       <c r="C66" s="15" t="s">
         <v>15</v>
       </c>
@@ -3875,11 +4094,11 @@
       <c r="E66" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="F66" s="54" t="s">
+      <c r="F66" s="56" t="s">
         <v>99</v>
       </c>
-      <c r="G66" s="39"/>
-      <c r="H66" s="40"/>
+      <c r="G66" s="54"/>
+      <c r="H66" s="55"/>
       <c r="I66" s="2"/>
       <c r="J66" s="2"/>
       <c r="K66" s="2"/>
@@ -3931,15 +4150,15 @@
       <c r="A68" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="B68" s="61" t="s">
+      <c r="B68" s="57" t="s">
         <v>114</v>
       </c>
-      <c r="C68" s="62"/>
-      <c r="D68" s="62"/>
-      <c r="E68" s="62"/>
-      <c r="F68" s="62"/>
-      <c r="G68" s="62"/>
-      <c r="H68" s="63"/>
+      <c r="C68" s="58"/>
+      <c r="D68" s="58"/>
+      <c r="E68" s="58"/>
+      <c r="F68" s="58"/>
+      <c r="G68" s="58"/>
+      <c r="H68" s="59"/>
       <c r="I68" s="2"/>
       <c r="J68" s="2"/>
       <c r="K68" s="2"/>
@@ -3963,15 +4182,15 @@
       <c r="A69" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B69" s="64" t="s">
+      <c r="B69" s="76" t="s">
         <v>115</v>
       </c>
-      <c r="C69" s="62"/>
-      <c r="D69" s="62"/>
-      <c r="E69" s="62"/>
-      <c r="F69" s="62"/>
-      <c r="G69" s="62"/>
-      <c r="H69" s="63"/>
+      <c r="C69" s="58"/>
+      <c r="D69" s="58"/>
+      <c r="E69" s="58"/>
+      <c r="F69" s="58"/>
+      <c r="G69" s="58"/>
+      <c r="H69" s="59"/>
       <c r="I69" s="2"/>
       <c r="J69" s="2"/>
       <c r="K69" s="2"/>
@@ -3992,16 +4211,16 @@
       <c r="Z69" s="2"/>
     </row>
     <row r="70" spans="1:26" ht="15" customHeight="1">
-      <c r="A70" s="41" t="s">
+      <c r="A70" s="61" t="s">
         <v>4</v>
       </c>
-      <c r="B70" s="39"/>
-      <c r="C70" s="39"/>
-      <c r="D70" s="39"/>
-      <c r="E70" s="39"/>
-      <c r="F70" s="39"/>
-      <c r="G70" s="39"/>
-      <c r="H70" s="67"/>
+      <c r="B70" s="54"/>
+      <c r="C70" s="54"/>
+      <c r="D70" s="54"/>
+      <c r="E70" s="54"/>
+      <c r="F70" s="54"/>
+      <c r="G70" s="54"/>
+      <c r="H70" s="79"/>
       <c r="I70" s="33"/>
       <c r="J70" s="2"/>
       <c r="K70" s="2"/>
@@ -4022,10 +4241,10 @@
       <c r="Z70" s="2"/>
     </row>
     <row r="71" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A71" s="42" t="s">
+      <c r="A71" s="53" t="s">
         <v>5</v>
       </c>
-      <c r="B71" s="43"/>
+      <c r="B71" s="49"/>
       <c r="C71" s="1" t="s">
         <v>6</v>
       </c>
@@ -4035,7 +4254,7 @@
       <c r="E71" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F71" s="1" t="s">
+      <c r="F71" s="100" t="s">
         <v>9</v>
       </c>
       <c r="G71" s="1" t="s">
@@ -4064,10 +4283,10 @@
       <c r="Z71" s="2"/>
     </row>
     <row r="72" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A72" s="44" t="s">
+      <c r="A72" s="48" t="s">
         <v>116</v>
       </c>
-      <c r="B72" s="43"/>
+      <c r="B72" s="49"/>
       <c r="C72" s="4" t="s">
         <v>12</v>
       </c>
@@ -4104,10 +4323,10 @@
       <c r="Z72" s="2"/>
     </row>
     <row r="73" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A73" s="44" t="s">
+      <c r="A73" s="48" t="s">
         <v>17</v>
       </c>
-      <c r="B73" s="77"/>
+      <c r="B73" s="82"/>
       <c r="C73" s="4" t="s">
         <v>18</v>
       </c>
@@ -4120,7 +4339,7 @@
       <c r="F73" s="5"/>
       <c r="G73" s="5"/>
       <c r="H73" s="6" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="I73" s="2"/>
       <c r="J73" s="2"/>
@@ -4142,10 +4361,10 @@
       <c r="Z73" s="2"/>
     </row>
     <row r="74" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A74" s="44" t="s">
+      <c r="A74" s="48" t="s">
         <v>61</v>
       </c>
-      <c r="B74" s="43"/>
+      <c r="B74" s="49"/>
       <c r="C74" s="4" t="s">
         <v>12</v>
       </c>
@@ -4182,10 +4401,10 @@
       <c r="Z74" s="2"/>
     </row>
     <row r="75" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A75" s="44" t="s">
+      <c r="A75" s="48" t="s">
         <v>119</v>
       </c>
-      <c r="B75" s="43"/>
+      <c r="B75" s="49"/>
       <c r="C75" s="4" t="s">
         <v>67</v>
       </c>
@@ -4220,10 +4439,10 @@
       <c r="Z75" s="2"/>
     </row>
     <row r="76" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A76" s="44" t="s">
+      <c r="A76" s="48" t="s">
         <v>121</v>
       </c>
-      <c r="B76" s="43"/>
+      <c r="B76" s="49"/>
       <c r="C76" s="4" t="s">
         <v>67</v>
       </c>
@@ -4258,10 +4477,10 @@
       <c r="Z76" s="2"/>
     </row>
     <row r="77" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A77" s="44" t="s">
+      <c r="A77" s="48" t="s">
         <v>124</v>
       </c>
-      <c r="B77" s="43"/>
+      <c r="B77" s="49"/>
       <c r="C77" s="4" t="s">
         <v>46</v>
       </c>
@@ -4296,10 +4515,10 @@
       <c r="Z77" s="2"/>
     </row>
     <row r="78" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A78" s="45" t="s">
+      <c r="A78" s="80" t="s">
         <v>126</v>
       </c>
-      <c r="B78" s="46"/>
+      <c r="B78" s="81"/>
       <c r="C78" s="12" t="s">
         <v>46</v>
       </c>
@@ -4334,10 +4553,10 @@
       <c r="Z78" s="2"/>
     </row>
     <row r="79" spans="1:26" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A79" s="65" t="s">
+      <c r="A79" s="77" t="s">
         <v>128</v>
       </c>
-      <c r="B79" s="66"/>
+      <c r="B79" s="78"/>
       <c r="C79" s="35" t="s">
         <v>67</v>
       </c>
@@ -4372,16 +4591,16 @@
       <c r="Z79" s="2"/>
     </row>
     <row r="80" spans="1:26" ht="15" customHeight="1">
-      <c r="A80" s="47" t="s">
+      <c r="A80" s="123" t="s">
         <v>48</v>
       </c>
-      <c r="B80" s="48"/>
-      <c r="C80" s="48"/>
-      <c r="D80" s="48"/>
-      <c r="E80" s="48"/>
-      <c r="F80" s="48"/>
-      <c r="G80" s="48"/>
-      <c r="H80" s="49"/>
+      <c r="B80" s="124"/>
+      <c r="C80" s="124"/>
+      <c r="D80" s="124"/>
+      <c r="E80" s="124"/>
+      <c r="F80" s="124"/>
+      <c r="G80" s="124"/>
+      <c r="H80" s="125"/>
       <c r="I80" s="2"/>
       <c r="J80" s="2"/>
       <c r="K80" s="2"/>
@@ -4402,10 +4621,10 @@
       <c r="Z80" s="2"/>
     </row>
     <row r="81" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A81" s="42" t="s">
+      <c r="A81" s="53" t="s">
         <v>49</v>
       </c>
-      <c r="B81" s="43"/>
+      <c r="B81" s="49"/>
       <c r="C81" s="1" t="s">
         <v>50</v>
       </c>
@@ -4415,11 +4634,11 @@
       <c r="E81" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="F81" s="42" t="s">
+      <c r="F81" s="53" t="s">
         <v>53</v>
       </c>
-      <c r="G81" s="39"/>
-      <c r="H81" s="40"/>
+      <c r="G81" s="54"/>
+      <c r="H81" s="55"/>
       <c r="I81" s="2"/>
       <c r="J81" s="2"/>
       <c r="K81" s="2"/>
@@ -4439,11 +4658,11 @@
       <c r="Y81" s="2"/>
       <c r="Z81" s="2"/>
     </row>
-    <row r="82" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A82" s="54" t="s">
+    <row r="82" spans="1:26" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A82" s="56" t="s">
         <v>130</v>
       </c>
-      <c r="B82" s="43"/>
+      <c r="B82" s="49"/>
       <c r="C82" s="15" t="s">
         <v>15</v>
       </c>
@@ -4451,11 +4670,11 @@
       <c r="E82" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="F82" s="54" t="s">
+      <c r="F82" s="56" t="s">
         <v>116</v>
       </c>
-      <c r="G82" s="39"/>
-      <c r="H82" s="40"/>
+      <c r="G82" s="54"/>
+      <c r="H82" s="55"/>
       <c r="I82" s="2"/>
       <c r="J82" s="2"/>
       <c r="K82" s="2"/>
@@ -4475,15 +4694,15 @@
       <c r="Y82" s="2"/>
       <c r="Z82" s="2"/>
     </row>
-    <row r="83" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A83" s="19"/>
-      <c r="B83" s="19"/>
-      <c r="C83" s="19"/>
-      <c r="D83" s="19"/>
-      <c r="E83" s="19"/>
-      <c r="F83" s="19"/>
-      <c r="G83" s="19"/>
-      <c r="H83" s="19"/>
+    <row r="83" spans="1:26" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A83" s="95"/>
+      <c r="B83" s="95"/>
+      <c r="C83" s="95"/>
+      <c r="D83" s="95"/>
+      <c r="E83" s="95"/>
+      <c r="F83" s="95"/>
+      <c r="G83" s="95"/>
+      <c r="H83" s="95"/>
       <c r="I83" s="2"/>
       <c r="J83" s="2"/>
       <c r="K83" s="2"/>
@@ -4504,18 +4723,18 @@
       <c r="Z83" s="2"/>
     </row>
     <row r="84" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A84" s="20" t="s">
+      <c r="A84" s="107" t="s">
         <v>58</v>
       </c>
-      <c r="B84" s="61" t="s">
-        <v>131</v>
-      </c>
-      <c r="C84" s="62"/>
-      <c r="D84" s="62"/>
-      <c r="E84" s="62"/>
-      <c r="F84" s="62"/>
-      <c r="G84" s="62"/>
-      <c r="H84" s="63"/>
+      <c r="B84" s="111" t="s">
+        <v>176</v>
+      </c>
+      <c r="C84" s="112"/>
+      <c r="D84" s="112"/>
+      <c r="E84" s="112"/>
+      <c r="F84" s="112"/>
+      <c r="G84" s="112"/>
+      <c r="H84" s="113"/>
       <c r="I84" s="2"/>
       <c r="J84" s="2"/>
       <c r="K84" s="2"/>
@@ -4539,15 +4758,15 @@
       <c r="A85" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B85" s="38" t="s">
-        <v>132</v>
-      </c>
-      <c r="C85" s="39"/>
-      <c r="D85" s="39"/>
-      <c r="E85" s="39"/>
-      <c r="F85" s="39"/>
-      <c r="G85" s="39"/>
-      <c r="H85" s="40"/>
+      <c r="B85" s="48" t="s">
+        <v>177</v>
+      </c>
+      <c r="C85" s="109"/>
+      <c r="D85" s="109"/>
+      <c r="E85" s="109"/>
+      <c r="F85" s="109"/>
+      <c r="G85" s="109"/>
+      <c r="H85" s="110"/>
       <c r="I85" s="2"/>
       <c r="J85" s="2"/>
       <c r="K85" s="2"/>
@@ -4568,16 +4787,16 @@
       <c r="Z85" s="2"/>
     </row>
     <row r="86" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A86" s="41" t="s">
+      <c r="A86" s="61" t="s">
         <v>4</v>
       </c>
-      <c r="B86" s="39"/>
-      <c r="C86" s="39"/>
-      <c r="D86" s="39"/>
-      <c r="E86" s="39"/>
-      <c r="F86" s="39"/>
-      <c r="G86" s="39"/>
-      <c r="H86" s="40"/>
+      <c r="B86" s="83"/>
+      <c r="C86" s="83"/>
+      <c r="D86" s="83"/>
+      <c r="E86" s="83"/>
+      <c r="F86" s="83"/>
+      <c r="G86" s="83"/>
+      <c r="H86" s="84"/>
       <c r="I86" s="2"/>
       <c r="J86" s="2"/>
       <c r="K86" s="2"/>
@@ -4598,10 +4817,10 @@
       <c r="Z86" s="2"/>
     </row>
     <row r="87" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A87" s="42" t="s">
+      <c r="A87" s="101" t="s">
         <v>5</v>
       </c>
-      <c r="B87" s="43"/>
+      <c r="B87" s="121"/>
       <c r="C87" s="1" t="s">
         <v>6</v>
       </c>
@@ -4640,10 +4859,10 @@
       <c r="Z87" s="2"/>
     </row>
     <row r="88" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A88" s="44" t="s">
-        <v>133</v>
-      </c>
-      <c r="B88" s="43"/>
+      <c r="A88" s="40" t="s">
+        <v>178</v>
+      </c>
+      <c r="B88" s="47"/>
       <c r="C88" s="4" t="s">
         <v>12</v>
       </c>
@@ -4658,7 +4877,7 @@
       </c>
       <c r="G88" s="5"/>
       <c r="H88" s="6" t="s">
-        <v>134</v>
+        <v>179</v>
       </c>
       <c r="I88" s="2"/>
       <c r="J88" s="2"/>
@@ -4679,24 +4898,26 @@
       <c r="Y88" s="2"/>
       <c r="Z88" s="2"/>
     </row>
-    <row r="89" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A89" s="44" t="s">
-        <v>17</v>
-      </c>
-      <c r="B89" s="43"/>
+    <row r="89" spans="1:26" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A89" s="40" t="s">
+        <v>116</v>
+      </c>
+      <c r="B89" s="47"/>
       <c r="C89" s="4" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="D89" s="4" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="E89" s="4" t="s">
         <v>14</v>
       </c>
       <c r="F89" s="5"/>
-      <c r="G89" s="5"/>
+      <c r="G89" s="5" t="s">
+        <v>15</v>
+      </c>
       <c r="H89" s="6" t="s">
-        <v>135</v>
+        <v>180</v>
       </c>
       <c r="I89" s="2"/>
       <c r="J89" s="2"/>
@@ -4718,26 +4939,16 @@
       <c r="Z89" s="2"/>
     </row>
     <row r="90" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A90" s="44" t="s">
-        <v>61</v>
-      </c>
-      <c r="B90" s="43"/>
-      <c r="C90" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D90" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E90" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="F90" s="5"/>
-      <c r="G90" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="H90" s="6" t="s">
-        <v>136</v>
-      </c>
+      <c r="A90" s="114" t="s">
+        <v>48</v>
+      </c>
+      <c r="B90" s="115"/>
+      <c r="C90" s="115"/>
+      <c r="D90" s="115"/>
+      <c r="E90" s="115"/>
+      <c r="F90" s="115"/>
+      <c r="G90" s="115"/>
+      <c r="H90" s="116"/>
       <c r="I90" s="2"/>
       <c r="J90" s="2"/>
       <c r="K90" s="2"/>
@@ -4757,25 +4968,25 @@
       <c r="Y90" s="2"/>
       <c r="Z90" s="2"/>
     </row>
-    <row r="91" spans="1:26" ht="15" customHeight="1">
-      <c r="A91" s="44" t="s">
-        <v>137</v>
-      </c>
-      <c r="B91" s="43"/>
-      <c r="C91" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="D91" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="E91" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="F91" s="5"/>
-      <c r="G91" s="5"/>
-      <c r="H91" s="6" t="s">
-        <v>138</v>
-      </c>
+    <row r="91" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A91" s="101" t="s">
+        <v>49</v>
+      </c>
+      <c r="B91" s="121"/>
+      <c r="C91" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D91" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E91" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F91" s="101" t="s">
+        <v>53</v>
+      </c>
+      <c r="G91" s="102"/>
+      <c r="H91" s="103"/>
       <c r="I91" s="2"/>
       <c r="J91" s="2"/>
       <c r="K91" s="2"/>
@@ -4796,24 +5007,22 @@
       <c r="Z91" s="2"/>
     </row>
     <row r="92" spans="1:26" ht="15" customHeight="1">
-      <c r="A92" s="44" t="s">
-        <v>139</v>
-      </c>
-      <c r="B92" s="43"/>
-      <c r="C92" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="D92" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="E92" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="F92" s="5"/>
-      <c r="G92" s="5"/>
-      <c r="H92" s="6" t="s">
-        <v>140</v>
-      </c>
+      <c r="A92" s="45" t="s">
+        <v>182</v>
+      </c>
+      <c r="B92" s="108"/>
+      <c r="C92" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="D92" s="16"/>
+      <c r="E92" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="F92" s="66" t="s">
+        <v>178</v>
+      </c>
+      <c r="G92" s="96"/>
+      <c r="H92" s="97"/>
       <c r="I92" s="2"/>
       <c r="J92" s="2"/>
       <c r="K92" s="2"/>
@@ -4833,25 +5042,23 @@
       <c r="Y92" s="2"/>
       <c r="Z92" s="2"/>
     </row>
-    <row r="93" spans="1:26" ht="15" customHeight="1">
-      <c r="A93" s="44" t="s">
-        <v>141</v>
-      </c>
-      <c r="B93" s="43"/>
-      <c r="C93" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="D93" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="E93" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="F93" s="5"/>
-      <c r="G93" s="5"/>
-      <c r="H93" s="6" t="s">
-        <v>142</v>
-      </c>
+    <row r="93" spans="1:26" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A93" s="67" t="s">
+        <v>181</v>
+      </c>
+      <c r="B93" s="104"/>
+      <c r="C93" s="106"/>
+      <c r="D93" s="106" t="s">
+        <v>15</v>
+      </c>
+      <c r="E93" s="106" t="s">
+        <v>15</v>
+      </c>
+      <c r="F93" s="67" t="s">
+        <v>116</v>
+      </c>
+      <c r="G93" s="98"/>
+      <c r="H93" s="99"/>
       <c r="I93" s="2"/>
       <c r="J93" s="2"/>
       <c r="K93" s="2"/>
@@ -4871,25 +5078,15 @@
       <c r="Y93" s="2"/>
       <c r="Z93" s="2"/>
     </row>
-    <row r="94" spans="1:26" ht="15" customHeight="1" thickBot="1">
-      <c r="A94" s="55" t="s">
-        <v>143</v>
-      </c>
-      <c r="B94" s="51"/>
-      <c r="C94" s="23" t="s">
-        <v>29</v>
-      </c>
-      <c r="D94" s="23" t="s">
-        <v>30</v>
-      </c>
-      <c r="E94" s="23" t="s">
-        <v>14</v>
-      </c>
-      <c r="F94" s="31"/>
-      <c r="G94" s="31"/>
-      <c r="H94" s="32" t="s">
-        <v>144</v>
-      </c>
+    <row r="94" spans="1:26" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A94" s="122"/>
+      <c r="B94" s="122"/>
+      <c r="C94" s="122"/>
+      <c r="D94" s="122"/>
+      <c r="E94" s="122"/>
+      <c r="F94" s="122"/>
+      <c r="G94" s="122"/>
+      <c r="H94" s="122"/>
       <c r="I94" s="2"/>
       <c r="J94" s="2"/>
       <c r="K94" s="2"/>
@@ -4910,16 +5107,18 @@
       <c r="Z94" s="2"/>
     </row>
     <row r="95" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A95" s="58" t="s">
-        <v>48</v>
-      </c>
-      <c r="B95" s="59"/>
-      <c r="C95" s="59"/>
-      <c r="D95" s="59"/>
-      <c r="E95" s="59"/>
-      <c r="F95" s="59"/>
-      <c r="G95" s="59"/>
-      <c r="H95" s="60"/>
+      <c r="A95" s="20" t="s">
+        <v>58</v>
+      </c>
+      <c r="B95" s="117" t="s">
+        <v>131</v>
+      </c>
+      <c r="C95" s="118"/>
+      <c r="D95" s="118"/>
+      <c r="E95" s="118"/>
+      <c r="F95" s="118"/>
+      <c r="G95" s="118"/>
+      <c r="H95" s="119"/>
       <c r="I95" s="2"/>
       <c r="J95" s="2"/>
       <c r="K95" s="2"/>
@@ -4939,25 +5138,19 @@
       <c r="Y95" s="2"/>
       <c r="Z95" s="2"/>
     </row>
-    <row r="96" spans="1:26" ht="15" customHeight="1">
-      <c r="A96" s="42" t="s">
-        <v>49</v>
-      </c>
-      <c r="B96" s="43"/>
-      <c r="C96" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D96" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="E96" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="F96" s="42" t="s">
-        <v>53</v>
-      </c>
-      <c r="G96" s="39"/>
-      <c r="H96" s="40"/>
+    <row r="96" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A96" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B96" s="48" t="s">
+        <v>132</v>
+      </c>
+      <c r="C96" s="109"/>
+      <c r="D96" s="109"/>
+      <c r="E96" s="109"/>
+      <c r="F96" s="109"/>
+      <c r="G96" s="109"/>
+      <c r="H96" s="110"/>
       <c r="I96" s="2"/>
       <c r="J96" s="2"/>
       <c r="K96" s="2"/>
@@ -4977,23 +5170,17 @@
       <c r="Y96" s="2"/>
       <c r="Z96" s="2"/>
     </row>
-    <row r="97" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A97" s="54" t="s">
-        <v>145</v>
-      </c>
-      <c r="B97" s="43"/>
-      <c r="C97" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="D97" s="16"/>
-      <c r="E97" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="F97" s="54" t="s">
-        <v>133</v>
-      </c>
-      <c r="G97" s="39"/>
-      <c r="H97" s="40"/>
+    <row r="97" spans="1:26" ht="15" customHeight="1">
+      <c r="A97" s="61" t="s">
+        <v>4</v>
+      </c>
+      <c r="B97" s="83"/>
+      <c r="C97" s="83"/>
+      <c r="D97" s="83"/>
+      <c r="E97" s="83"/>
+      <c r="F97" s="83"/>
+      <c r="G97" s="83"/>
+      <c r="H97" s="84"/>
       <c r="I97" s="2"/>
       <c r="J97" s="2"/>
       <c r="K97" s="2"/>
@@ -5013,15 +5200,29 @@
       <c r="Y97" s="2"/>
       <c r="Z97" s="2"/>
     </row>
-    <row r="98" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A98" s="19"/>
-      <c r="B98" s="19"/>
-      <c r="C98" s="19"/>
-      <c r="D98" s="19"/>
-      <c r="E98" s="19"/>
-      <c r="F98" s="19"/>
-      <c r="G98" s="19"/>
-      <c r="H98" s="19"/>
+    <row r="98" spans="1:26" ht="15" customHeight="1">
+      <c r="A98" s="101" t="s">
+        <v>5</v>
+      </c>
+      <c r="B98" s="121"/>
+      <c r="C98" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D98" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E98" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F98" s="100" t="s">
+        <v>9</v>
+      </c>
+      <c r="G98" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H98" s="3" t="s">
+        <v>2</v>
+      </c>
       <c r="I98" s="2"/>
       <c r="J98" s="2"/>
       <c r="K98" s="2"/>
@@ -5041,19 +5242,27 @@
       <c r="Y98" s="2"/>
       <c r="Z98" s="2"/>
     </row>
-    <row r="99" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A99" s="20" t="s">
-        <v>58</v>
-      </c>
-      <c r="B99" s="61" t="s">
-        <v>146</v>
-      </c>
-      <c r="C99" s="62"/>
-      <c r="D99" s="62"/>
-      <c r="E99" s="62"/>
-      <c r="F99" s="62"/>
-      <c r="G99" s="62"/>
-      <c r="H99" s="63"/>
+    <row r="99" spans="1:26" ht="15" customHeight="1">
+      <c r="A99" s="40" t="s">
+        <v>133</v>
+      </c>
+      <c r="B99" s="39"/>
+      <c r="C99" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D99" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E99" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F99" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G99" s="5"/>
+      <c r="H99" s="6" t="s">
+        <v>134</v>
+      </c>
       <c r="I99" s="2"/>
       <c r="J99" s="2"/>
       <c r="K99" s="2"/>
@@ -5073,19 +5282,25 @@
       <c r="Y99" s="2"/>
       <c r="Z99" s="2"/>
     </row>
-    <row r="100" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A100" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B100" s="38" t="s">
-        <v>147</v>
-      </c>
-      <c r="C100" s="39"/>
-      <c r="D100" s="39"/>
-      <c r="E100" s="39"/>
-      <c r="F100" s="39"/>
-      <c r="G100" s="39"/>
-      <c r="H100" s="40"/>
+    <row r="100" spans="1:26" ht="15" customHeight="1">
+      <c r="A100" s="40" t="s">
+        <v>17</v>
+      </c>
+      <c r="B100" s="39"/>
+      <c r="C100" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D100" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E100" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F100" s="5"/>
+      <c r="G100" s="5"/>
+      <c r="H100" s="6" t="s">
+        <v>135</v>
+      </c>
       <c r="I100" s="2"/>
       <c r="J100" s="2"/>
       <c r="K100" s="2"/>
@@ -5106,16 +5321,26 @@
       <c r="Z100" s="2"/>
     </row>
     <row r="101" spans="1:26" ht="15" customHeight="1">
-      <c r="A101" s="41" t="s">
-        <v>4</v>
+      <c r="A101" s="40" t="s">
+        <v>61</v>
       </c>
       <c r="B101" s="39"/>
-      <c r="C101" s="39"/>
-      <c r="D101" s="39"/>
-      <c r="E101" s="39"/>
-      <c r="F101" s="39"/>
-      <c r="G101" s="39"/>
-      <c r="H101" s="40"/>
+      <c r="C101" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D101" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E101" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F101" s="5"/>
+      <c r="G101" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H101" s="6" t="s">
+        <v>136</v>
+      </c>
       <c r="I101" s="2"/>
       <c r="J101" s="2"/>
       <c r="K101" s="2"/>
@@ -5135,28 +5360,24 @@
       <c r="Y101" s="2"/>
       <c r="Z101" s="2"/>
     </row>
-    <row r="102" spans="1:26" ht="15" customHeight="1">
-      <c r="A102" s="42" t="s">
-        <v>5</v>
-      </c>
-      <c r="B102" s="43"/>
-      <c r="C102" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D102" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E102" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F102" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G102" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H102" s="3" t="s">
-        <v>148</v>
+    <row r="102" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A102" s="40" t="s">
+        <v>137</v>
+      </c>
+      <c r="B102" s="39"/>
+      <c r="C102" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D102" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E102" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F102" s="5"/>
+      <c r="G102" s="5"/>
+      <c r="H102" s="6" t="s">
+        <v>138</v>
       </c>
       <c r="I102" s="2"/>
       <c r="J102" s="2"/>
@@ -5177,26 +5398,24 @@
       <c r="Y102" s="2"/>
       <c r="Z102" s="2"/>
     </row>
-    <row r="103" spans="1:26" ht="15" customHeight="1">
-      <c r="A103" s="44" t="s">
-        <v>149</v>
-      </c>
-      <c r="B103" s="43"/>
+    <row r="103" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A103" s="40" t="s">
+        <v>139</v>
+      </c>
+      <c r="B103" s="39"/>
       <c r="C103" s="4" t="s">
-        <v>12</v>
+        <v>67</v>
       </c>
       <c r="D103" s="4" t="s">
-        <v>13</v>
+        <v>68</v>
       </c>
       <c r="E103" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="F103" s="5" t="s">
-        <v>15</v>
-      </c>
+      <c r="F103" s="5"/>
       <c r="G103" s="5"/>
       <c r="H103" s="6" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="I103" s="2"/>
       <c r="J103" s="2"/>
@@ -5217,26 +5436,24 @@
       <c r="Y103" s="2"/>
       <c r="Z103" s="2"/>
     </row>
-    <row r="104" spans="1:26" ht="15" customHeight="1">
-      <c r="A104" s="44" t="s">
-        <v>61</v>
-      </c>
-      <c r="B104" s="43"/>
+    <row r="104" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A104" s="40" t="s">
+        <v>141</v>
+      </c>
+      <c r="B104" s="39"/>
       <c r="C104" s="4" t="s">
-        <v>12</v>
+        <v>67</v>
       </c>
       <c r="D104" s="4" t="s">
-        <v>13</v>
+        <v>68</v>
       </c>
       <c r="E104" s="4" t="s">
         <v>14</v>
       </c>
       <c r="F104" s="5"/>
-      <c r="G104" s="5" t="s">
-        <v>15</v>
-      </c>
+      <c r="G104" s="5"/>
       <c r="H104" s="6" t="s">
-        <v>62</v>
+        <v>142</v>
       </c>
       <c r="I104" s="2"/>
       <c r="J104" s="2"/>
@@ -5257,24 +5474,24 @@
       <c r="Y104" s="2"/>
       <c r="Z104" s="2"/>
     </row>
-    <row r="105" spans="1:26" ht="15" customHeight="1">
+    <row r="105" spans="1:26" ht="15.75" customHeight="1" thickBot="1">
       <c r="A105" s="44" t="s">
-        <v>150</v>
-      </c>
-      <c r="B105" s="43"/>
-      <c r="C105" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="D105" s="4" t="s">
-        <v>152</v>
-      </c>
-      <c r="E105" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="B105" s="42"/>
+      <c r="C105" s="23" t="s">
+        <v>46</v>
+      </c>
+      <c r="D105" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="E105" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="F105" s="5"/>
-      <c r="G105" s="5"/>
-      <c r="H105" s="6" t="s">
-        <v>153</v>
+      <c r="F105" s="31"/>
+      <c r="G105" s="31"/>
+      <c r="H105" s="32" t="s">
+        <v>144</v>
       </c>
       <c r="I105" s="2"/>
       <c r="J105" s="2"/>
@@ -5296,24 +5513,16 @@
       <c r="Z105" s="2"/>
     </row>
     <row r="106" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A106" s="44" t="s">
-        <v>154</v>
-      </c>
-      <c r="B106" s="43"/>
-      <c r="C106" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D106" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="E106" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="F106" s="5"/>
-      <c r="G106" s="5"/>
-      <c r="H106" s="6" t="s">
-        <v>155</v>
-      </c>
+      <c r="A106" s="114" t="s">
+        <v>48</v>
+      </c>
+      <c r="B106" s="115"/>
+      <c r="C106" s="115"/>
+      <c r="D106" s="115"/>
+      <c r="E106" s="115"/>
+      <c r="F106" s="115"/>
+      <c r="G106" s="115"/>
+      <c r="H106" s="116"/>
       <c r="I106" s="2"/>
       <c r="J106" s="2"/>
       <c r="K106" s="2"/>
@@ -5334,24 +5543,24 @@
       <c r="Z106" s="2"/>
     </row>
     <row r="107" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A107" s="44" t="s">
-        <v>156</v>
-      </c>
-      <c r="B107" s="43"/>
-      <c r="C107" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="D107" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="E107" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="F107" s="5"/>
-      <c r="G107" s="5"/>
-      <c r="H107" s="6" t="s">
-        <v>157</v>
-      </c>
+      <c r="A107" s="61" t="s">
+        <v>49</v>
+      </c>
+      <c r="B107" s="120"/>
+      <c r="C107" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D107" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E107" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F107" s="101" t="s">
+        <v>53</v>
+      </c>
+      <c r="G107" s="102"/>
+      <c r="H107" s="103"/>
       <c r="I107" s="2"/>
       <c r="J107" s="2"/>
       <c r="K107" s="2"/>
@@ -5371,25 +5580,23 @@
       <c r="Y107" s="2"/>
       <c r="Z107" s="2"/>
     </row>
-    <row r="108" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A108" s="55" t="s">
-        <v>158</v>
-      </c>
-      <c r="B108" s="51"/>
-      <c r="C108" s="23" t="s">
-        <v>159</v>
-      </c>
-      <c r="D108" s="23" t="s">
-        <v>160</v>
-      </c>
-      <c r="E108" s="23" t="s">
-        <v>14</v>
-      </c>
-      <c r="F108" s="31"/>
-      <c r="G108" s="31"/>
-      <c r="H108" s="32" t="s">
-        <v>161</v>
-      </c>
+    <row r="108" spans="1:26" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A108" s="67" t="s">
+        <v>145</v>
+      </c>
+      <c r="B108" s="104"/>
+      <c r="C108" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="D108" s="16"/>
+      <c r="E108" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="F108" s="67" t="s">
+        <v>133</v>
+      </c>
+      <c r="G108" s="98"/>
+      <c r="H108" s="99"/>
       <c r="I108" s="2"/>
       <c r="J108" s="2"/>
       <c r="K108" s="2"/>
@@ -5409,17 +5616,15 @@
       <c r="Y108" s="2"/>
       <c r="Z108" s="2"/>
     </row>
-    <row r="109" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A109" s="58" t="s">
-        <v>48</v>
-      </c>
-      <c r="B109" s="59"/>
-      <c r="C109" s="59"/>
-      <c r="D109" s="59"/>
-      <c r="E109" s="59"/>
-      <c r="F109" s="59"/>
-      <c r="G109" s="59"/>
-      <c r="H109" s="60"/>
+    <row r="109" spans="1:26" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A109" s="19"/>
+      <c r="B109" s="19"/>
+      <c r="C109" s="19"/>
+      <c r="D109" s="19"/>
+      <c r="E109" s="19"/>
+      <c r="F109" s="19"/>
+      <c r="G109" s="19"/>
+      <c r="H109" s="19"/>
       <c r="I109" s="2"/>
       <c r="J109" s="2"/>
       <c r="K109" s="2"/>
@@ -5440,24 +5645,18 @@
       <c r="Z109" s="2"/>
     </row>
     <row r="110" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A110" s="42" t="s">
-        <v>49</v>
-      </c>
-      <c r="B110" s="43"/>
-      <c r="C110" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D110" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="E110" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="F110" s="42" t="s">
-        <v>53</v>
-      </c>
-      <c r="G110" s="39"/>
-      <c r="H110" s="40"/>
+      <c r="A110" s="20" t="s">
+        <v>58</v>
+      </c>
+      <c r="B110" s="89" t="s">
+        <v>146</v>
+      </c>
+      <c r="C110" s="90"/>
+      <c r="D110" s="90"/>
+      <c r="E110" s="90"/>
+      <c r="F110" s="90"/>
+      <c r="G110" s="90"/>
+      <c r="H110" s="91"/>
       <c r="I110" s="2"/>
       <c r="J110" s="2"/>
       <c r="K110" s="2"/>
@@ -5478,22 +5677,18 @@
       <c r="Z110" s="2"/>
     </row>
     <row r="111" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A111" s="54" t="s">
-        <v>162</v>
-      </c>
-      <c r="B111" s="43"/>
-      <c r="C111" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="D111" s="16"/>
-      <c r="E111" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="F111" s="54" t="s">
-        <v>149</v>
-      </c>
-      <c r="G111" s="39"/>
-      <c r="H111" s="40"/>
+      <c r="A111" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B111" s="48" t="s">
+        <v>147</v>
+      </c>
+      <c r="C111" s="109"/>
+      <c r="D111" s="109"/>
+      <c r="E111" s="109"/>
+      <c r="F111" s="109"/>
+      <c r="G111" s="109"/>
+      <c r="H111" s="110"/>
       <c r="I111" s="2"/>
       <c r="J111" s="2"/>
       <c r="K111" s="2"/>
@@ -5514,22 +5709,16 @@
       <c r="Z111" s="2"/>
     </row>
     <row r="112" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A112" s="54" t="s">
-        <v>163</v>
-      </c>
-      <c r="B112" s="43"/>
-      <c r="C112" s="15"/>
-      <c r="D112" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="E112" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="F112" s="54" t="s">
-        <v>150</v>
-      </c>
-      <c r="G112" s="39"/>
-      <c r="H112" s="40"/>
+      <c r="A112" s="61" t="s">
+        <v>4</v>
+      </c>
+      <c r="B112" s="83"/>
+      <c r="C112" s="83"/>
+      <c r="D112" s="83"/>
+      <c r="E112" s="83"/>
+      <c r="F112" s="83"/>
+      <c r="G112" s="83"/>
+      <c r="H112" s="84"/>
       <c r="I112" s="2"/>
       <c r="J112" s="2"/>
       <c r="K112" s="2"/>
@@ -5550,14 +5739,28 @@
       <c r="Z112" s="2"/>
     </row>
     <row r="113" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A113" s="19"/>
-      <c r="B113" s="19"/>
-      <c r="C113" s="19"/>
-      <c r="D113" s="19"/>
-      <c r="E113" s="19"/>
-      <c r="F113" s="19"/>
-      <c r="G113" s="19"/>
-      <c r="H113" s="19"/>
+      <c r="A113" s="101" t="s">
+        <v>5</v>
+      </c>
+      <c r="B113" s="121"/>
+      <c r="C113" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D113" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E113" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F113" s="100" t="s">
+        <v>9</v>
+      </c>
+      <c r="G113" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H113" s="3" t="s">
+        <v>148</v>
+      </c>
       <c r="I113" s="2"/>
       <c r="J113" s="2"/>
       <c r="K113" s="2"/>
@@ -5578,18 +5781,26 @@
       <c r="Z113" s="2"/>
     </row>
     <row r="114" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A114" s="20" t="s">
-        <v>58</v>
-      </c>
-      <c r="B114" s="61" t="s">
-        <v>164</v>
-      </c>
-      <c r="C114" s="62"/>
-      <c r="D114" s="62"/>
-      <c r="E114" s="62"/>
-      <c r="F114" s="62"/>
-      <c r="G114" s="62"/>
-      <c r="H114" s="63"/>
+      <c r="A114" s="40" t="s">
+        <v>149</v>
+      </c>
+      <c r="B114" s="47"/>
+      <c r="C114" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D114" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E114" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F114" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G114" s="5"/>
+      <c r="H114" s="6" t="s">
+        <v>148</v>
+      </c>
       <c r="I114" s="2"/>
       <c r="J114" s="2"/>
       <c r="K114" s="2"/>
@@ -5610,18 +5821,26 @@
       <c r="Z114" s="2"/>
     </row>
     <row r="115" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A115" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B115" s="38" t="s">
-        <v>165</v>
-      </c>
-      <c r="C115" s="39"/>
-      <c r="D115" s="39"/>
-      <c r="E115" s="39"/>
-      <c r="F115" s="39"/>
-      <c r="G115" s="39"/>
-      <c r="H115" s="40"/>
+      <c r="A115" s="40" t="s">
+        <v>61</v>
+      </c>
+      <c r="B115" s="47"/>
+      <c r="C115" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D115" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E115" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F115" s="5"/>
+      <c r="G115" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H115" s="6" t="s">
+        <v>62</v>
+      </c>
       <c r="I115" s="2"/>
       <c r="J115" s="2"/>
       <c r="K115" s="2"/>
@@ -5642,16 +5861,24 @@
       <c r="Z115" s="2"/>
     </row>
     <row r="116" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A116" s="41" t="s">
-        <v>4</v>
-      </c>
-      <c r="B116" s="39"/>
-      <c r="C116" s="39"/>
-      <c r="D116" s="39"/>
-      <c r="E116" s="39"/>
-      <c r="F116" s="39"/>
-      <c r="G116" s="39"/>
-      <c r="H116" s="40"/>
+      <c r="A116" s="40" t="s">
+        <v>150</v>
+      </c>
+      <c r="B116" s="47"/>
+      <c r="C116" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="D116" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="E116" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F116" s="5"/>
+      <c r="G116" s="5"/>
+      <c r="H116" s="6" t="s">
+        <v>153</v>
+      </c>
       <c r="I116" s="2"/>
       <c r="J116" s="2"/>
       <c r="K116" s="2"/>
@@ -5672,27 +5899,23 @@
       <c r="Z116" s="2"/>
     </row>
     <row r="117" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A117" s="42" t="s">
-        <v>5</v>
-      </c>
-      <c r="B117" s="43"/>
-      <c r="C117" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D117" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E117" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F117" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G117" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H117" s="3" t="s">
-        <v>2</v>
+      <c r="A117" s="40" t="s">
+        <v>154</v>
+      </c>
+      <c r="B117" s="47"/>
+      <c r="C117" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D117" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E117" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F117" s="5"/>
+      <c r="G117" s="5"/>
+      <c r="H117" s="6" t="s">
+        <v>155</v>
       </c>
       <c r="I117" s="2"/>
       <c r="J117" s="2"/>
@@ -5714,25 +5937,23 @@
       <c r="Z117" s="2"/>
     </row>
     <row r="118" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A118" s="44" t="s">
-        <v>166</v>
-      </c>
-      <c r="B118" s="43"/>
+      <c r="A118" s="40" t="s">
+        <v>156</v>
+      </c>
+      <c r="B118" s="47"/>
       <c r="C118" s="4" t="s">
-        <v>12</v>
+        <v>29</v>
       </c>
       <c r="D118" s="4" t="s">
-        <v>13</v>
+        <v>30</v>
       </c>
       <c r="E118" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="F118" s="5" t="s">
-        <v>15</v>
-      </c>
+      <c r="F118" s="5"/>
       <c r="G118" s="5"/>
       <c r="H118" s="6" t="s">
-        <v>167</v>
+        <v>157</v>
       </c>
       <c r="I118" s="2"/>
       <c r="J118" s="2"/>
@@ -5753,26 +5974,24 @@
       <c r="Y118" s="2"/>
       <c r="Z118" s="2"/>
     </row>
-    <row r="119" spans="1:26" ht="15.75" customHeight="1">
+    <row r="119" spans="1:26" ht="15.75" customHeight="1" thickBot="1">
       <c r="A119" s="44" t="s">
-        <v>99</v>
-      </c>
-      <c r="B119" s="43"/>
-      <c r="C119" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D119" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E119" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="B119" s="92"/>
+      <c r="C119" s="23" t="s">
+        <v>159</v>
+      </c>
+      <c r="D119" s="23" t="s">
+        <v>160</v>
+      </c>
+      <c r="E119" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="F119" s="5"/>
-      <c r="G119" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="H119" s="6" t="s">
-        <v>168</v>
+      <c r="F119" s="31"/>
+      <c r="G119" s="31"/>
+      <c r="H119" s="32" t="s">
+        <v>161</v>
       </c>
       <c r="I119" s="2"/>
       <c r="J119" s="2"/>
@@ -5794,26 +6013,16 @@
       <c r="Z119" s="2"/>
     </row>
     <row r="120" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A120" s="44" t="s">
-        <v>61</v>
-      </c>
-      <c r="B120" s="43"/>
-      <c r="C120" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D120" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E120" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="F120" s="5"/>
-      <c r="G120" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="H120" s="6" t="s">
-        <v>62</v>
-      </c>
+      <c r="A120" s="114" t="s">
+        <v>48</v>
+      </c>
+      <c r="B120" s="115"/>
+      <c r="C120" s="115"/>
+      <c r="D120" s="115"/>
+      <c r="E120" s="115"/>
+      <c r="F120" s="115"/>
+      <c r="G120" s="115"/>
+      <c r="H120" s="116"/>
       <c r="I120" s="2"/>
       <c r="J120" s="2"/>
       <c r="K120" s="2"/>
@@ -5834,24 +6043,24 @@
       <c r="Z120" s="2"/>
     </row>
     <row r="121" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A121" s="44" t="s">
-        <v>111</v>
-      </c>
-      <c r="B121" s="43"/>
-      <c r="C121" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="D121" s="4" t="s">
-        <v>169</v>
-      </c>
-      <c r="E121" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="F121" s="5"/>
-      <c r="G121" s="5"/>
-      <c r="H121" s="6" t="s">
-        <v>170</v>
-      </c>
+      <c r="A121" s="101" t="s">
+        <v>49</v>
+      </c>
+      <c r="B121" s="121"/>
+      <c r="C121" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D121" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E121" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F121" s="101" t="s">
+        <v>53</v>
+      </c>
+      <c r="G121" s="102"/>
+      <c r="H121" s="103"/>
       <c r="I121" s="2"/>
       <c r="J121" s="2"/>
       <c r="K121" s="2"/>
@@ -5872,24 +6081,22 @@
       <c r="Z121" s="2"/>
     </row>
     <row r="122" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A122" s="56" t="s">
-        <v>119</v>
-      </c>
-      <c r="B122" s="57"/>
-      <c r="C122" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="D122" s="4" t="s">
-        <v>169</v>
-      </c>
-      <c r="E122" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="F122" s="29"/>
-      <c r="G122" s="29"/>
-      <c r="H122" s="30" t="s">
-        <v>171</v>
-      </c>
+      <c r="A122" s="43" t="s">
+        <v>162</v>
+      </c>
+      <c r="B122" s="87"/>
+      <c r="C122" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="D122" s="16"/>
+      <c r="E122" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="F122" s="66" t="s">
+        <v>149</v>
+      </c>
+      <c r="G122" s="96"/>
+      <c r="H122" s="97"/>
       <c r="I122" s="2"/>
       <c r="J122" s="2"/>
       <c r="K122" s="2"/>
@@ -5910,24 +6117,22 @@
       <c r="Z122" s="2"/>
     </row>
     <row r="123" spans="1:26" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A123" s="55" t="s">
-        <v>172</v>
-      </c>
-      <c r="B123" s="51"/>
-      <c r="C123" s="23" t="s">
-        <v>46</v>
-      </c>
-      <c r="D123" s="23" t="s">
-        <v>30</v>
-      </c>
-      <c r="E123" s="23" t="s">
-        <v>14</v>
-      </c>
-      <c r="F123" s="31"/>
-      <c r="G123" s="31"/>
-      <c r="H123" s="32" t="s">
-        <v>173</v>
-      </c>
+      <c r="A123" s="41" t="s">
+        <v>163</v>
+      </c>
+      <c r="B123" s="88"/>
+      <c r="C123" s="15"/>
+      <c r="D123" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="E123" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="F123" s="67" t="s">
+        <v>150</v>
+      </c>
+      <c r="G123" s="98"/>
+      <c r="H123" s="99"/>
       <c r="I123" s="2"/>
       <c r="J123" s="2"/>
       <c r="K123" s="2"/>
@@ -5947,17 +6152,15 @@
       <c r="Y123" s="2"/>
       <c r="Z123" s="2"/>
     </row>
-    <row r="124" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A124" s="58" t="s">
-        <v>48</v>
-      </c>
-      <c r="B124" s="59"/>
-      <c r="C124" s="59"/>
-      <c r="D124" s="59"/>
-      <c r="E124" s="59"/>
-      <c r="F124" s="59"/>
-      <c r="G124" s="59"/>
-      <c r="H124" s="60"/>
+    <row r="124" spans="1:26" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A124" s="19"/>
+      <c r="B124" s="19"/>
+      <c r="C124" s="19"/>
+      <c r="D124" s="19"/>
+      <c r="E124" s="19"/>
+      <c r="F124" s="19"/>
+      <c r="G124" s="19"/>
+      <c r="H124" s="19"/>
       <c r="I124" s="2"/>
       <c r="J124" s="2"/>
       <c r="K124" s="2"/>
@@ -5978,24 +6181,18 @@
       <c r="Z124" s="2"/>
     </row>
     <row r="125" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A125" s="42" t="s">
-        <v>49</v>
-      </c>
-      <c r="B125" s="43"/>
-      <c r="C125" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D125" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="E125" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="F125" s="42" t="s">
-        <v>53</v>
-      </c>
-      <c r="G125" s="39"/>
-      <c r="H125" s="40"/>
+      <c r="A125" s="20" t="s">
+        <v>58</v>
+      </c>
+      <c r="B125" s="111" t="s">
+        <v>164</v>
+      </c>
+      <c r="C125" s="112"/>
+      <c r="D125" s="112"/>
+      <c r="E125" s="112"/>
+      <c r="F125" s="112"/>
+      <c r="G125" s="112"/>
+      <c r="H125" s="113"/>
       <c r="I125" s="2"/>
       <c r="J125" s="2"/>
       <c r="K125" s="2"/>
@@ -6016,22 +6213,18 @@
       <c r="Z125" s="2"/>
     </row>
     <row r="126" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A126" s="50" t="s">
-        <v>174</v>
-      </c>
-      <c r="B126" s="51"/>
-      <c r="C126" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="D126" s="34"/>
-      <c r="E126" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="F126" s="50" t="s">
-        <v>166</v>
-      </c>
-      <c r="G126" s="52"/>
-      <c r="H126" s="53"/>
+      <c r="A126" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B126" s="48" t="s">
+        <v>165</v>
+      </c>
+      <c r="C126" s="109"/>
+      <c r="D126" s="109"/>
+      <c r="E126" s="109"/>
+      <c r="F126" s="109"/>
+      <c r="G126" s="109"/>
+      <c r="H126" s="110"/>
       <c r="I126" s="2"/>
       <c r="J126" s="2"/>
       <c r="K126" s="2"/>
@@ -6052,14 +6245,16 @@
       <c r="Z126" s="2"/>
     </row>
     <row r="127" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A127" s="2"/>
-      <c r="B127" s="2"/>
-      <c r="C127" s="2"/>
-      <c r="D127" s="2"/>
-      <c r="E127" s="2"/>
-      <c r="F127" s="2"/>
-      <c r="G127" s="2"/>
-      <c r="H127" s="2"/>
+      <c r="A127" s="61" t="s">
+        <v>4</v>
+      </c>
+      <c r="B127" s="83"/>
+      <c r="C127" s="83"/>
+      <c r="D127" s="83"/>
+      <c r="E127" s="83"/>
+      <c r="F127" s="83"/>
+      <c r="G127" s="83"/>
+      <c r="H127" s="84"/>
       <c r="I127" s="2"/>
       <c r="J127" s="2"/>
       <c r="K127" s="2"/>
@@ -6079,15 +6274,29 @@
       <c r="Y127" s="2"/>
       <c r="Z127" s="2"/>
     </row>
-    <row r="128" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A128" s="2"/>
-      <c r="B128" s="2"/>
-      <c r="C128" s="2"/>
-      <c r="D128" s="2"/>
-      <c r="E128" s="2"/>
-      <c r="F128" s="2"/>
-      <c r="G128" s="2"/>
-      <c r="H128" s="2"/>
+    <row r="128" spans="1:26" ht="15" customHeight="1">
+      <c r="A128" s="38" t="s">
+        <v>5</v>
+      </c>
+      <c r="B128" s="86"/>
+      <c r="C128" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D128" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E128" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F128" s="100" t="s">
+        <v>9</v>
+      </c>
+      <c r="G128" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H128" s="3" t="s">
+        <v>2</v>
+      </c>
       <c r="I128" s="2"/>
       <c r="J128" s="2"/>
       <c r="K128" s="2"/>
@@ -6108,14 +6317,26 @@
       <c r="Z128" s="2"/>
     </row>
     <row r="129" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A129" s="2"/>
-      <c r="B129" s="2"/>
-      <c r="C129" s="2"/>
-      <c r="D129" s="2"/>
-      <c r="E129" s="2"/>
-      <c r="F129" s="2"/>
-      <c r="G129" s="2"/>
-      <c r="H129" s="2"/>
+      <c r="A129" s="48" t="s">
+        <v>166</v>
+      </c>
+      <c r="B129" s="82"/>
+      <c r="C129" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D129" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E129" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F129" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G129" s="5"/>
+      <c r="H129" s="6" t="s">
+        <v>167</v>
+      </c>
       <c r="I129" s="2"/>
       <c r="J129" s="2"/>
       <c r="K129" s="2"/>
@@ -6136,14 +6357,26 @@
       <c r="Z129" s="2"/>
     </row>
     <row r="130" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A130" s="2"/>
-      <c r="B130" s="2"/>
-      <c r="C130" s="2"/>
-      <c r="D130" s="2"/>
-      <c r="E130" s="2"/>
-      <c r="F130" s="2"/>
-      <c r="G130" s="2"/>
-      <c r="H130" s="2"/>
+      <c r="A130" s="48" t="s">
+        <v>61</v>
+      </c>
+      <c r="B130" s="82"/>
+      <c r="C130" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D130" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E130" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F130" s="5"/>
+      <c r="G130" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H130" s="6" t="s">
+        <v>62</v>
+      </c>
       <c r="I130" s="2"/>
       <c r="J130" s="2"/>
       <c r="K130" s="2"/>
@@ -6163,15 +6396,25 @@
       <c r="Y130" s="2"/>
       <c r="Z130" s="2"/>
     </row>
-    <row r="131" spans="1:26" ht="15" customHeight="1">
-      <c r="A131" s="2"/>
-      <c r="B131" s="2"/>
-      <c r="C131" s="2"/>
-      <c r="D131" s="2"/>
-      <c r="E131" s="2"/>
-      <c r="F131" s="2"/>
-      <c r="G131" s="2"/>
-      <c r="H131" s="2"/>
+    <row r="131" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A131" s="48" t="s">
+        <v>111</v>
+      </c>
+      <c r="B131" s="82"/>
+      <c r="C131" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="D131" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="E131" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F131" s="5"/>
+      <c r="G131" s="5"/>
+      <c r="H131" s="6" t="s">
+        <v>169</v>
+      </c>
       <c r="I131" s="2"/>
       <c r="J131" s="2"/>
       <c r="K131" s="2"/>
@@ -6192,14 +6435,24 @@
       <c r="Z131" s="2"/>
     </row>
     <row r="132" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A132" s="2"/>
-      <c r="B132" s="2"/>
-      <c r="C132" s="2"/>
-      <c r="D132" s="2"/>
-      <c r="E132" s="2"/>
-      <c r="F132" s="2"/>
-      <c r="G132" s="2"/>
-      <c r="H132" s="2"/>
+      <c r="A132" s="48" t="s">
+        <v>119</v>
+      </c>
+      <c r="B132" s="82"/>
+      <c r="C132" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="D132" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="E132" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="F132" s="29"/>
+      <c r="G132" s="29"/>
+      <c r="H132" s="30" t="s">
+        <v>170</v>
+      </c>
       <c r="I132" s="2"/>
       <c r="J132" s="2"/>
       <c r="K132" s="2"/>
@@ -6219,15 +6472,25 @@
       <c r="Y132" s="2"/>
       <c r="Z132" s="2"/>
     </row>
-    <row r="133" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A133" s="2"/>
-      <c r="B133" s="2"/>
-      <c r="C133" s="2"/>
-      <c r="D133" s="2"/>
-      <c r="E133" s="2"/>
-      <c r="F133" s="2"/>
-      <c r="G133" s="2"/>
-      <c r="H133" s="2"/>
+    <row r="133" spans="1:26" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A133" s="75" t="s">
+        <v>171</v>
+      </c>
+      <c r="B133" s="85"/>
+      <c r="C133" s="23" t="s">
+        <v>46</v>
+      </c>
+      <c r="D133" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="E133" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="F133" s="31"/>
+      <c r="G133" s="31"/>
+      <c r="H133" s="32" t="s">
+        <v>172</v>
+      </c>
       <c r="I133" s="2"/>
       <c r="J133" s="2"/>
       <c r="K133" s="2"/>
@@ -6247,15 +6510,17 @@
       <c r="Y133" s="2"/>
       <c r="Z133" s="2"/>
     </row>
-    <row r="134" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A134" s="2"/>
-      <c r="B134" s="2"/>
-      <c r="C134" s="2"/>
-      <c r="D134" s="2"/>
-      <c r="E134" s="2"/>
-      <c r="F134" s="2"/>
-      <c r="G134" s="2"/>
-      <c r="H134" s="2"/>
+    <row r="134" spans="1:26" ht="15" customHeight="1">
+      <c r="A134" s="46" t="s">
+        <v>48</v>
+      </c>
+      <c r="B134" s="93"/>
+      <c r="C134" s="93"/>
+      <c r="D134" s="93"/>
+      <c r="E134" s="93"/>
+      <c r="F134" s="93"/>
+      <c r="G134" s="93"/>
+      <c r="H134" s="94"/>
       <c r="I134" s="2"/>
       <c r="J134" s="2"/>
       <c r="K134" s="2"/>
@@ -6276,14 +6541,24 @@
       <c r="Z134" s="2"/>
     </row>
     <row r="135" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A135" s="2"/>
-      <c r="B135" s="2"/>
-      <c r="C135" s="2"/>
-      <c r="D135" s="2"/>
-      <c r="E135" s="2"/>
-      <c r="F135" s="2"/>
-      <c r="G135" s="2"/>
-      <c r="H135" s="2"/>
+      <c r="A135" s="38" t="s">
+        <v>49</v>
+      </c>
+      <c r="B135" s="86"/>
+      <c r="C135" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D135" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E135" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F135" s="101" t="s">
+        <v>53</v>
+      </c>
+      <c r="G135" s="102"/>
+      <c r="H135" s="103"/>
       <c r="I135" s="2"/>
       <c r="J135" s="2"/>
       <c r="K135" s="2"/>
@@ -6303,15 +6578,23 @@
       <c r="Y135" s="2"/>
       <c r="Z135" s="2"/>
     </row>
-    <row r="136" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A136" s="2"/>
-      <c r="B136" s="2"/>
-      <c r="C136" s="2"/>
-      <c r="D136" s="2"/>
-      <c r="E136" s="2"/>
-      <c r="F136" s="2"/>
-      <c r="G136" s="2"/>
-      <c r="H136" s="2"/>
+    <row r="136" spans="1:26" ht="15" customHeight="1" thickBot="1">
+      <c r="A136" s="67" t="s">
+        <v>173</v>
+      </c>
+      <c r="B136" s="104"/>
+      <c r="C136" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="D136" s="34"/>
+      <c r="E136" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="F136" s="67" t="s">
+        <v>166</v>
+      </c>
+      <c r="G136" s="98"/>
+      <c r="H136" s="99"/>
       <c r="I136" s="2"/>
       <c r="J136" s="2"/>
       <c r="K136" s="2"/>
@@ -6331,15 +6614,7 @@
       <c r="Y136" s="2"/>
       <c r="Z136" s="2"/>
     </row>
-    <row r="137" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A137" s="2"/>
-      <c r="B137" s="2"/>
-      <c r="C137" s="2"/>
-      <c r="D137" s="2"/>
-      <c r="E137" s="2"/>
-      <c r="F137" s="2"/>
-      <c r="G137" s="2"/>
-      <c r="H137" s="2"/>
+    <row r="137" spans="1:26" ht="15.75" customHeight="1" thickBot="1">
       <c r="I137" s="2"/>
       <c r="J137" s="2"/>
       <c r="K137" s="2"/>
@@ -6359,15 +6634,19 @@
       <c r="Y137" s="2"/>
       <c r="Z137" s="2"/>
     </row>
-    <row r="138" spans="1:26" ht="15" customHeight="1">
-      <c r="A138" s="2"/>
-      <c r="B138" s="2"/>
-      <c r="C138" s="2"/>
-      <c r="D138" s="2"/>
-      <c r="E138" s="2"/>
-      <c r="F138" s="2"/>
-      <c r="G138" s="2"/>
-      <c r="H138" s="2"/>
+    <row r="138" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A138" s="107" t="s">
+        <v>58</v>
+      </c>
+      <c r="B138" s="111" t="s">
+        <v>183</v>
+      </c>
+      <c r="C138" s="112"/>
+      <c r="D138" s="112"/>
+      <c r="E138" s="112"/>
+      <c r="F138" s="112"/>
+      <c r="G138" s="112"/>
+      <c r="H138" s="113"/>
       <c r="I138" s="2"/>
       <c r="J138" s="2"/>
       <c r="K138" s="2"/>
@@ -6388,14 +6667,18 @@
       <c r="Z138" s="2"/>
     </row>
     <row r="139" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A139" s="2"/>
-      <c r="B139" s="2"/>
-      <c r="C139" s="2"/>
-      <c r="D139" s="2"/>
-      <c r="E139" s="2"/>
-      <c r="F139" s="2"/>
-      <c r="G139" s="2"/>
-      <c r="H139" s="2"/>
+      <c r="A139" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B139" s="48" t="s">
+        <v>184</v>
+      </c>
+      <c r="C139" s="109"/>
+      <c r="D139" s="109"/>
+      <c r="E139" s="109"/>
+      <c r="F139" s="109"/>
+      <c r="G139" s="109"/>
+      <c r="H139" s="110"/>
       <c r="I139" s="2"/>
       <c r="J139" s="2"/>
       <c r="K139" s="2"/>
@@ -6415,15 +6698,17 @@
       <c r="Y139" s="2"/>
       <c r="Z139" s="2"/>
     </row>
-    <row r="140" spans="1:26" ht="15" customHeight="1">
-      <c r="A140" s="2"/>
-      <c r="B140" s="2"/>
-      <c r="C140" s="2"/>
-      <c r="D140" s="2"/>
-      <c r="E140" s="2"/>
-      <c r="F140" s="2"/>
-      <c r="G140" s="2"/>
-      <c r="H140" s="2"/>
+    <row r="140" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A140" s="61" t="s">
+        <v>4</v>
+      </c>
+      <c r="B140" s="83"/>
+      <c r="C140" s="83"/>
+      <c r="D140" s="83"/>
+      <c r="E140" s="83"/>
+      <c r="F140" s="83"/>
+      <c r="G140" s="83"/>
+      <c r="H140" s="84"/>
       <c r="I140" s="2"/>
       <c r="J140" s="2"/>
       <c r="K140" s="2"/>
@@ -6444,14 +6729,28 @@
       <c r="Z140" s="2"/>
     </row>
     <row r="141" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A141" s="2"/>
-      <c r="B141" s="2"/>
-      <c r="C141" s="2"/>
-      <c r="D141" s="2"/>
-      <c r="E141" s="2"/>
-      <c r="F141" s="2"/>
-      <c r="G141" s="2"/>
-      <c r="H141" s="2"/>
+      <c r="A141" s="101" t="s">
+        <v>5</v>
+      </c>
+      <c r="B141" s="121"/>
+      <c r="C141" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D141" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E141" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F141" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G141" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H141" s="3" t="s">
+        <v>2</v>
+      </c>
       <c r="I141" s="2"/>
       <c r="J141" s="2"/>
       <c r="K141" s="2"/>
@@ -6472,14 +6771,26 @@
       <c r="Z141" s="2"/>
     </row>
     <row r="142" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A142" s="2"/>
-      <c r="B142" s="2"/>
-      <c r="C142" s="2"/>
-      <c r="D142" s="2"/>
-      <c r="E142" s="2"/>
-      <c r="F142" s="2"/>
-      <c r="G142" s="2"/>
-      <c r="H142" s="2"/>
+      <c r="A142" s="48" t="s">
+        <v>185</v>
+      </c>
+      <c r="B142" s="82"/>
+      <c r="C142" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D142" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E142" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F142" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G142" s="5"/>
+      <c r="H142" s="6" t="s">
+        <v>186</v>
+      </c>
       <c r="I142" s="2"/>
       <c r="J142" s="2"/>
       <c r="K142" s="2"/>
@@ -6499,15 +6810,27 @@
       <c r="Y142" s="2"/>
       <c r="Z142" s="2"/>
     </row>
-    <row r="143" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A143" s="2"/>
-      <c r="B143" s="2"/>
-      <c r="C143" s="2"/>
-      <c r="D143" s="2"/>
-      <c r="E143" s="2"/>
-      <c r="F143" s="2"/>
-      <c r="G143" s="2"/>
-      <c r="H143" s="2"/>
+    <row r="143" spans="1:26" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A143" s="75" t="s">
+        <v>166</v>
+      </c>
+      <c r="B143" s="85"/>
+      <c r="C143" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D143" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E143" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F143" s="5"/>
+      <c r="G143" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H143" s="6" t="s">
+        <v>187</v>
+      </c>
       <c r="I143" s="2"/>
       <c r="J143" s="2"/>
       <c r="K143" s="2"/>
@@ -6528,14 +6851,16 @@
       <c r="Z143" s="2"/>
     </row>
     <row r="144" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A144" s="2"/>
-      <c r="B144" s="2"/>
-      <c r="C144" s="2"/>
-      <c r="D144" s="2"/>
-      <c r="E144" s="2"/>
-      <c r="F144" s="2"/>
-      <c r="G144" s="2"/>
-      <c r="H144" s="2"/>
+      <c r="A144" s="114" t="s">
+        <v>48</v>
+      </c>
+      <c r="B144" s="115"/>
+      <c r="C144" s="115"/>
+      <c r="D144" s="115"/>
+      <c r="E144" s="115"/>
+      <c r="F144" s="115"/>
+      <c r="G144" s="115"/>
+      <c r="H144" s="116"/>
       <c r="I144" s="2"/>
       <c r="J144" s="2"/>
       <c r="K144" s="2"/>
@@ -6556,14 +6881,24 @@
       <c r="Z144" s="2"/>
     </row>
     <row r="145" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A145" s="2"/>
-      <c r="B145" s="2"/>
-      <c r="C145" s="2"/>
-      <c r="D145" s="2"/>
-      <c r="E145" s="2"/>
-      <c r="F145" s="2"/>
-      <c r="G145" s="2"/>
-      <c r="H145" s="2"/>
+      <c r="A145" s="101" t="s">
+        <v>49</v>
+      </c>
+      <c r="B145" s="121"/>
+      <c r="C145" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D145" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E145" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F145" s="101" t="s">
+        <v>53</v>
+      </c>
+      <c r="G145" s="102"/>
+      <c r="H145" s="103"/>
       <c r="I145" s="2"/>
       <c r="J145" s="2"/>
       <c r="K145" s="2"/>
@@ -6584,14 +6919,22 @@
       <c r="Z145" s="2"/>
     </row>
     <row r="146" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A146" s="2"/>
-      <c r="B146" s="2"/>
-      <c r="C146" s="2"/>
-      <c r="D146" s="2"/>
-      <c r="E146" s="2"/>
-      <c r="F146" s="2"/>
-      <c r="G146" s="2"/>
-      <c r="H146" s="2"/>
+      <c r="A146" s="66" t="s">
+        <v>188</v>
+      </c>
+      <c r="B146" s="105"/>
+      <c r="C146" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="D146" s="16"/>
+      <c r="E146" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="F146" s="66" t="s">
+        <v>185</v>
+      </c>
+      <c r="G146" s="96"/>
+      <c r="H146" s="97"/>
       <c r="I146" s="2"/>
       <c r="J146" s="2"/>
       <c r="K146" s="2"/>
@@ -6611,15 +6954,23 @@
       <c r="Y146" s="2"/>
       <c r="Z146" s="2"/>
     </row>
-    <row r="147" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A147" s="2"/>
-      <c r="B147" s="2"/>
-      <c r="C147" s="2"/>
-      <c r="D147" s="2"/>
-      <c r="E147" s="2"/>
-      <c r="F147" s="2"/>
-      <c r="G147" s="2"/>
-      <c r="H147" s="2"/>
+    <row r="147" spans="1:26" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A147" s="67" t="s">
+        <v>189</v>
+      </c>
+      <c r="B147" s="104"/>
+      <c r="C147" s="106"/>
+      <c r="D147" s="106" t="s">
+        <v>15</v>
+      </c>
+      <c r="E147" s="106" t="s">
+        <v>15</v>
+      </c>
+      <c r="F147" s="67" t="s">
+        <v>166</v>
+      </c>
+      <c r="G147" s="98"/>
+      <c r="H147" s="99"/>
       <c r="I147" s="2"/>
       <c r="J147" s="2"/>
       <c r="K147" s="2"/>
@@ -6640,14 +6991,6 @@
       <c r="Z147" s="2"/>
     </row>
     <row r="148" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A148" s="2"/>
-      <c r="B148" s="2"/>
-      <c r="C148" s="2"/>
-      <c r="D148" s="2"/>
-      <c r="E148" s="2"/>
-      <c r="F148" s="2"/>
-      <c r="G148" s="2"/>
-      <c r="H148" s="2"/>
       <c r="I148" s="2"/>
       <c r="J148" s="2"/>
       <c r="K148" s="2"/>
@@ -30523,170 +30866,76 @@
       <c r="Y1000" s="2"/>
       <c r="Z1000" s="2"/>
     </row>
-    <row r="1001" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A1001" s="2"/>
-      <c r="B1001" s="2"/>
-      <c r="C1001" s="2"/>
-      <c r="D1001" s="2"/>
-      <c r="E1001" s="2"/>
-      <c r="F1001" s="2"/>
-      <c r="G1001" s="2"/>
-      <c r="H1001" s="2"/>
-      <c r="I1001" s="2"/>
-      <c r="J1001" s="2"/>
-      <c r="K1001" s="2"/>
-      <c r="L1001" s="2"/>
-      <c r="M1001" s="2"/>
-      <c r="N1001" s="2"/>
-      <c r="O1001" s="2"/>
-      <c r="P1001" s="2"/>
-      <c r="Q1001" s="2"/>
-      <c r="R1001" s="2"/>
-      <c r="S1001" s="2"/>
-      <c r="T1001" s="2"/>
-      <c r="U1001" s="2"/>
-      <c r="V1001" s="2"/>
-      <c r="W1001" s="2"/>
-      <c r="X1001" s="2"/>
-      <c r="Y1001" s="2"/>
-      <c r="Z1001" s="2"/>
-    </row>
-    <row r="1002" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A1002" s="2"/>
-      <c r="B1002" s="2"/>
-      <c r="C1002" s="2"/>
-      <c r="D1002" s="2"/>
-      <c r="E1002" s="2"/>
-      <c r="F1002" s="2"/>
-      <c r="G1002" s="2"/>
-      <c r="H1002" s="2"/>
-      <c r="I1002" s="2"/>
-      <c r="J1002" s="2"/>
-      <c r="K1002" s="2"/>
-      <c r="L1002" s="2"/>
-      <c r="M1002" s="2"/>
-      <c r="N1002" s="2"/>
-      <c r="O1002" s="2"/>
-      <c r="P1002" s="2"/>
-      <c r="Q1002" s="2"/>
-      <c r="R1002" s="2"/>
-      <c r="S1002" s="2"/>
-      <c r="T1002" s="2"/>
-      <c r="U1002" s="2"/>
-      <c r="V1002" s="2"/>
-      <c r="W1002" s="2"/>
-      <c r="X1002" s="2"/>
-      <c r="Y1002" s="2"/>
-      <c r="Z1002" s="2"/>
-    </row>
-    <row r="1003" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A1003" s="2"/>
-      <c r="B1003" s="2"/>
-      <c r="C1003" s="2"/>
-      <c r="D1003" s="2"/>
-      <c r="E1003" s="2"/>
-      <c r="F1003" s="2"/>
-      <c r="G1003" s="2"/>
-      <c r="H1003" s="2"/>
-      <c r="I1003" s="2"/>
-      <c r="J1003" s="2"/>
-      <c r="K1003" s="2"/>
-      <c r="L1003" s="2"/>
-      <c r="M1003" s="2"/>
-      <c r="N1003" s="2"/>
-      <c r="O1003" s="2"/>
-      <c r="P1003" s="2"/>
-      <c r="Q1003" s="2"/>
-      <c r="R1003" s="2"/>
-      <c r="S1003" s="2"/>
-      <c r="T1003" s="2"/>
-      <c r="U1003" s="2"/>
-      <c r="V1003" s="2"/>
-      <c r="W1003" s="2"/>
-      <c r="X1003" s="2"/>
-      <c r="Y1003" s="2"/>
-      <c r="Z1003" s="2"/>
-    </row>
-    <row r="1004" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A1004" s="2"/>
-      <c r="B1004" s="2"/>
-      <c r="C1004" s="2"/>
-      <c r="D1004" s="2"/>
-      <c r="E1004" s="2"/>
-      <c r="F1004" s="2"/>
-      <c r="G1004" s="2"/>
-      <c r="H1004" s="2"/>
-      <c r="I1004" s="2"/>
-      <c r="J1004" s="2"/>
-      <c r="K1004" s="2"/>
-      <c r="L1004" s="2"/>
-      <c r="M1004" s="2"/>
-      <c r="N1004" s="2"/>
-      <c r="O1004" s="2"/>
-      <c r="P1004" s="2"/>
-      <c r="Q1004" s="2"/>
-      <c r="R1004" s="2"/>
-      <c r="S1004" s="2"/>
-      <c r="T1004" s="2"/>
-      <c r="U1004" s="2"/>
-      <c r="V1004" s="2"/>
-      <c r="W1004" s="2"/>
-      <c r="X1004" s="2"/>
-      <c r="Y1004" s="2"/>
-      <c r="Z1004" s="2"/>
-    </row>
   </sheetData>
-  <mergeCells count="139">
-    <mergeCell ref="A57:B57"/>
-    <mergeCell ref="A58:B58"/>
-    <mergeCell ref="A59:B59"/>
-    <mergeCell ref="A49:H49"/>
-    <mergeCell ref="F50:H50"/>
-    <mergeCell ref="A50:B50"/>
-    <mergeCell ref="A51:B51"/>
-    <mergeCell ref="F51:H51"/>
-    <mergeCell ref="B53:H53"/>
-    <mergeCell ref="B54:H54"/>
-    <mergeCell ref="A55:H55"/>
-    <mergeCell ref="A56:B56"/>
-    <mergeCell ref="B1:H1"/>
-    <mergeCell ref="B2:H2"/>
-    <mergeCell ref="A3:H3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A15:H15"/>
-    <mergeCell ref="F16:H16"/>
-    <mergeCell ref="F17:H17"/>
-    <mergeCell ref="F18:H18"/>
-    <mergeCell ref="F19:H19"/>
-    <mergeCell ref="F20:H20"/>
-    <mergeCell ref="B22:H22"/>
-    <mergeCell ref="B23:H23"/>
-    <mergeCell ref="A24:H24"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="A34:H34"/>
+  <mergeCells count="142">
+    <mergeCell ref="F146:H146"/>
+    <mergeCell ref="A147:B147"/>
+    <mergeCell ref="F147:H147"/>
+    <mergeCell ref="A146:B146"/>
+    <mergeCell ref="A143:B143"/>
+    <mergeCell ref="A142:B142"/>
+    <mergeCell ref="A133:B133"/>
+    <mergeCell ref="A132:B132"/>
+    <mergeCell ref="A131:B131"/>
+    <mergeCell ref="A136:B136"/>
+    <mergeCell ref="A91:B91"/>
+    <mergeCell ref="B138:H138"/>
+    <mergeCell ref="B139:H139"/>
+    <mergeCell ref="A140:H140"/>
+    <mergeCell ref="A141:B141"/>
+    <mergeCell ref="A144:H144"/>
+    <mergeCell ref="A145:B145"/>
+    <mergeCell ref="F145:H145"/>
+    <mergeCell ref="F135:H135"/>
+    <mergeCell ref="F136:H136"/>
+    <mergeCell ref="F92:H92"/>
+    <mergeCell ref="B84:H84"/>
+    <mergeCell ref="B85:H85"/>
+    <mergeCell ref="F91:H91"/>
+    <mergeCell ref="A86:H86"/>
+    <mergeCell ref="A90:H90"/>
+    <mergeCell ref="B95:H95"/>
+    <mergeCell ref="B96:H96"/>
+    <mergeCell ref="A97:H97"/>
+    <mergeCell ref="A87:B87"/>
+    <mergeCell ref="A98:B98"/>
+    <mergeCell ref="A106:H106"/>
+    <mergeCell ref="A107:B107"/>
+    <mergeCell ref="F107:H107"/>
+    <mergeCell ref="F108:H108"/>
+    <mergeCell ref="A108:B108"/>
+    <mergeCell ref="B111:H111"/>
+    <mergeCell ref="A112:H112"/>
+    <mergeCell ref="A113:B113"/>
+    <mergeCell ref="A129:B129"/>
+    <mergeCell ref="A93:B93"/>
+    <mergeCell ref="F93:H93"/>
+    <mergeCell ref="A120:H120"/>
+    <mergeCell ref="F121:H121"/>
+    <mergeCell ref="F122:H122"/>
+    <mergeCell ref="F123:H123"/>
+    <mergeCell ref="B126:H126"/>
+    <mergeCell ref="B125:H125"/>
+    <mergeCell ref="A127:H127"/>
+    <mergeCell ref="A82:B82"/>
+    <mergeCell ref="F82:H82"/>
+    <mergeCell ref="A73:B73"/>
+    <mergeCell ref="A71:B71"/>
+    <mergeCell ref="A72:B72"/>
+    <mergeCell ref="A74:B74"/>
+    <mergeCell ref="A75:B75"/>
+    <mergeCell ref="A76:B76"/>
+    <mergeCell ref="A77:B77"/>
+    <mergeCell ref="A78:B78"/>
+    <mergeCell ref="A80:H80"/>
+    <mergeCell ref="A81:B81"/>
+    <mergeCell ref="F81:H81"/>
+    <mergeCell ref="A121:B121"/>
+    <mergeCell ref="A130:B130"/>
+    <mergeCell ref="B68:H68"/>
+    <mergeCell ref="B69:H69"/>
+    <mergeCell ref="A79:B79"/>
+    <mergeCell ref="A70:H70"/>
     <mergeCell ref="A35:B35"/>
     <mergeCell ref="F35:H35"/>
     <mergeCell ref="A36:B36"/>
@@ -30711,71 +30960,56 @@
     <mergeCell ref="A46:B46"/>
     <mergeCell ref="A47:B47"/>
     <mergeCell ref="A48:B48"/>
-    <mergeCell ref="B68:H68"/>
-    <mergeCell ref="B69:H69"/>
-    <mergeCell ref="A106:B106"/>
-    <mergeCell ref="A107:B107"/>
-    <mergeCell ref="A92:B92"/>
-    <mergeCell ref="A89:B89"/>
-    <mergeCell ref="A93:B93"/>
-    <mergeCell ref="A94:B94"/>
-    <mergeCell ref="A95:H95"/>
-    <mergeCell ref="A96:B96"/>
-    <mergeCell ref="F96:H96"/>
-    <mergeCell ref="A97:B97"/>
-    <mergeCell ref="F97:H97"/>
-    <mergeCell ref="B99:H99"/>
-    <mergeCell ref="B100:H100"/>
-    <mergeCell ref="A101:H101"/>
-    <mergeCell ref="A102:B102"/>
-    <mergeCell ref="A103:B103"/>
-    <mergeCell ref="A104:B104"/>
-    <mergeCell ref="A88:B88"/>
-    <mergeCell ref="A90:B90"/>
-    <mergeCell ref="A91:B91"/>
-    <mergeCell ref="A79:B79"/>
-    <mergeCell ref="A70:H70"/>
-    <mergeCell ref="A126:B126"/>
-    <mergeCell ref="F126:H126"/>
-    <mergeCell ref="A105:B105"/>
-    <mergeCell ref="A111:B111"/>
-    <mergeCell ref="A112:B112"/>
-    <mergeCell ref="A123:B123"/>
-    <mergeCell ref="A122:B122"/>
-    <mergeCell ref="A120:B120"/>
-    <mergeCell ref="A121:B121"/>
-    <mergeCell ref="A124:H124"/>
-    <mergeCell ref="A125:B125"/>
-    <mergeCell ref="F125:H125"/>
-    <mergeCell ref="A117:B117"/>
-    <mergeCell ref="A118:B118"/>
-    <mergeCell ref="A119:B119"/>
-    <mergeCell ref="B114:H114"/>
-    <mergeCell ref="A108:B108"/>
-    <mergeCell ref="A109:H109"/>
-    <mergeCell ref="A110:B110"/>
-    <mergeCell ref="F110:H110"/>
-    <mergeCell ref="F111:H111"/>
-    <mergeCell ref="F112:H112"/>
-    <mergeCell ref="B115:H115"/>
-    <mergeCell ref="A116:H116"/>
-    <mergeCell ref="A71:B71"/>
-    <mergeCell ref="A72:B72"/>
-    <mergeCell ref="A74:B74"/>
-    <mergeCell ref="A75:B75"/>
-    <mergeCell ref="A76:B76"/>
-    <mergeCell ref="A77:B77"/>
-    <mergeCell ref="A78:B78"/>
-    <mergeCell ref="A80:H80"/>
-    <mergeCell ref="A81:B81"/>
-    <mergeCell ref="F81:H81"/>
-    <mergeCell ref="A82:B82"/>
-    <mergeCell ref="F82:H82"/>
-    <mergeCell ref="B84:H84"/>
-    <mergeCell ref="B85:H85"/>
-    <mergeCell ref="A86:H86"/>
-    <mergeCell ref="A87:B87"/>
-    <mergeCell ref="A73:B73"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="A34:H34"/>
+    <mergeCell ref="F17:H17"/>
+    <mergeCell ref="F18:H18"/>
+    <mergeCell ref="F19:H19"/>
+    <mergeCell ref="F20:H20"/>
+    <mergeCell ref="B22:H22"/>
+    <mergeCell ref="B23:H23"/>
+    <mergeCell ref="A24:H24"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="B1:H1"/>
+    <mergeCell ref="B2:H2"/>
+    <mergeCell ref="A3:H3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A15:H15"/>
+    <mergeCell ref="F16:H16"/>
+    <mergeCell ref="A57:B57"/>
+    <mergeCell ref="A58:B58"/>
+    <mergeCell ref="A59:B59"/>
+    <mergeCell ref="A49:H49"/>
+    <mergeCell ref="F50:H50"/>
+    <mergeCell ref="A50:B50"/>
+    <mergeCell ref="A51:B51"/>
+    <mergeCell ref="F51:H51"/>
+    <mergeCell ref="B53:H53"/>
+    <mergeCell ref="B54:H54"/>
+    <mergeCell ref="A55:H55"/>
+    <mergeCell ref="A56:B56"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>

<commit_message>
Interface gráfica finalizada, trigger de investimento atualizada e dicionário de dados corrigido
</commit_message>
<xml_diff>
--- a/Dicionário/Dicionario_de_dados.xlsx
+++ b/Dicionário/Dicionario_de_dados.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\migue\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luigi\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{899B0255-1917-47B0-B5A7-0BEBF9F5FCD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BA60065-79A4-4347-B256-3986BA81671D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dicionario" sheetId="1" r:id="rId1"/>
@@ -875,7 +875,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="45">
+  <borders count="48">
     <border>
       <left/>
       <right/>
@@ -1410,14 +1410,53 @@
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
-      <bottom/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="128">
+  <cellXfs count="133">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1581,16 +1620,7 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1599,46 +1629,37 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1656,65 +1677,41 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1738,11 +1735,68 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1961,9 +2015,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1056"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A196" workbookViewId="0">
-      <selection activeCell="C188" sqref="C188"/>
-    </sheetView>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1982,7 +2034,7 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="100" t="s">
+      <c r="B1" s="122" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="93"/>
@@ -2014,7 +2066,7 @@
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="99" t="s">
+      <c r="B2" s="115" t="s">
         <v>3</v>
       </c>
       <c r="C2" s="93"/>
@@ -2043,7 +2095,7 @@
       <c r="Z2" s="2"/>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A3" s="75" t="s">
+      <c r="A3" s="82" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="93"/>
@@ -2073,10 +2125,10 @@
       <c r="Z3" s="2"/>
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A4" s="92" t="s">
+      <c r="A4" s="95" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="88"/>
+      <c r="B4" s="92"/>
       <c r="C4" s="1" t="s">
         <v>6</v>
       </c>
@@ -2115,10 +2167,10 @@
       <c r="Z4" s="2"/>
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A5" s="72" t="s">
+      <c r="A5" s="73" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="88"/>
+      <c r="B5" s="92"/>
       <c r="C5" s="4" t="s">
         <v>12</v>
       </c>
@@ -2155,10 +2207,10 @@
       <c r="Z5" s="2"/>
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A6" s="72" t="s">
+      <c r="A6" s="73" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="88"/>
+      <c r="B6" s="92"/>
       <c r="C6" s="4" t="s">
         <v>18</v>
       </c>
@@ -2193,10 +2245,10 @@
       <c r="Z6" s="2"/>
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A7" s="72" t="s">
+      <c r="A7" s="73" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="88"/>
+      <c r="B7" s="92"/>
       <c r="C7" s="4" t="s">
         <v>21</v>
       </c>
@@ -2231,10 +2283,10 @@
       <c r="Z7" s="2"/>
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A8" s="72" t="s">
+      <c r="A8" s="73" t="s">
         <v>24</v>
       </c>
-      <c r="B8" s="88"/>
+      <c r="B8" s="92"/>
       <c r="C8" s="4" t="s">
         <v>25</v>
       </c>
@@ -2269,10 +2321,10 @@
       <c r="Z8" s="2"/>
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A9" s="72" t="s">
+      <c r="A9" s="73" t="s">
         <v>28</v>
       </c>
-      <c r="B9" s="88"/>
+      <c r="B9" s="92"/>
       <c r="C9" s="4" t="s">
         <v>29</v>
       </c>
@@ -2307,10 +2359,10 @@
       <c r="Z9" s="2"/>
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A10" s="72" t="s">
+      <c r="A10" s="73" t="s">
         <v>32</v>
       </c>
-      <c r="B10" s="88"/>
+      <c r="B10" s="92"/>
       <c r="C10" s="4" t="s">
         <v>33</v>
       </c>
@@ -2345,10 +2397,10 @@
       <c r="Z10" s="2"/>
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A11" s="103" t="s">
+      <c r="A11" s="118" t="s">
         <v>36</v>
       </c>
-      <c r="B11" s="88"/>
+      <c r="B11" s="92"/>
       <c r="C11" s="8" t="s">
         <v>37</v>
       </c>
@@ -2383,10 +2435,10 @@
       <c r="Z11" s="2"/>
     </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A12" s="103" t="s">
+      <c r="A12" s="118" t="s">
         <v>39</v>
       </c>
-      <c r="B12" s="88"/>
+      <c r="B12" s="92"/>
       <c r="C12" s="8" t="s">
         <v>21</v>
       </c>
@@ -2421,10 +2473,10 @@
       <c r="Z12" s="2"/>
     </row>
     <row r="13" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A13" s="103" t="s">
+      <c r="A13" s="118" t="s">
         <v>41</v>
       </c>
-      <c r="B13" s="88"/>
+      <c r="B13" s="92"/>
       <c r="C13" s="8" t="s">
         <v>42</v>
       </c>
@@ -2459,10 +2511,10 @@
       <c r="Z13" s="2"/>
     </row>
     <row r="14" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A14" s="101" t="s">
+      <c r="A14" s="116" t="s">
         <v>45</v>
       </c>
-      <c r="B14" s="102"/>
+      <c r="B14" s="117"/>
       <c r="C14" s="11" t="s">
         <v>46</v>
       </c>
@@ -2497,16 +2549,16 @@
       <c r="Z14" s="2"/>
     </row>
     <row r="15" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="89" t="s">
+      <c r="A15" s="123" t="s">
         <v>48</v>
       </c>
-      <c r="B15" s="90"/>
-      <c r="C15" s="90"/>
-      <c r="D15" s="90"/>
-      <c r="E15" s="90"/>
-      <c r="F15" s="90"/>
-      <c r="G15" s="90"/>
-      <c r="H15" s="91"/>
+      <c r="B15" s="124"/>
+      <c r="C15" s="124"/>
+      <c r="D15" s="124"/>
+      <c r="E15" s="124"/>
+      <c r="F15" s="124"/>
+      <c r="G15" s="124"/>
+      <c r="H15" s="125"/>
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
       <c r="K15" s="2"/>
@@ -2527,10 +2579,10 @@
       <c r="Z15" s="2"/>
     </row>
     <row r="16" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="92" t="s">
+      <c r="A16" s="95" t="s">
         <v>49</v>
       </c>
-      <c r="B16" s="88"/>
+      <c r="B16" s="92"/>
       <c r="C16" s="1" t="s">
         <v>50</v>
       </c>
@@ -2540,7 +2592,7 @@
       <c r="E16" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="F16" s="92" t="s">
+      <c r="F16" s="95" t="s">
         <v>53</v>
       </c>
       <c r="G16" s="93"/>
@@ -2565,10 +2617,10 @@
       <c r="Z16" s="2"/>
     </row>
     <row r="17" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A17" s="95" t="s">
+      <c r="A17" s="91" t="s">
         <v>54</v>
       </c>
-      <c r="B17" s="88"/>
+      <c r="B17" s="92"/>
       <c r="C17" s="15" t="s">
         <v>15</v>
       </c>
@@ -2576,7 +2628,7 @@
       <c r="E17" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="F17" s="95" t="s">
+      <c r="F17" s="91" t="s">
         <v>11</v>
       </c>
       <c r="G17" s="93"/>
@@ -2601,10 +2653,10 @@
       <c r="Z17" s="2"/>
     </row>
     <row r="18" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A18" s="95" t="s">
+      <c r="A18" s="91" t="s">
         <v>55</v>
       </c>
-      <c r="B18" s="88"/>
+      <c r="B18" s="92"/>
       <c r="C18" s="15"/>
       <c r="D18" s="15" t="s">
         <v>15</v>
@@ -2612,7 +2664,7 @@
       <c r="E18" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="F18" s="95" t="s">
+      <c r="F18" s="91" t="s">
         <v>24</v>
       </c>
       <c r="G18" s="93"/>
@@ -2637,10 +2689,10 @@
       <c r="Z18" s="2"/>
     </row>
     <row r="19" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A19" s="65" t="s">
+      <c r="A19" s="63" t="s">
         <v>56</v>
       </c>
-      <c r="B19" s="88"/>
+      <c r="B19" s="92"/>
       <c r="C19" s="15"/>
       <c r="D19" s="15" t="s">
         <v>15</v>
@@ -2648,7 +2700,7 @@
       <c r="E19" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="F19" s="65" t="s">
+      <c r="F19" s="63" t="s">
         <v>39</v>
       </c>
       <c r="G19" s="93"/>
@@ -2673,10 +2725,10 @@
       <c r="Z19" s="2"/>
     </row>
     <row r="20" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A20" s="104" t="s">
+      <c r="A20" s="66" t="s">
         <v>57</v>
       </c>
-      <c r="B20" s="107"/>
+      <c r="B20" s="111"/>
       <c r="C20" s="17"/>
       <c r="D20" s="18" t="s">
         <v>15</v>
@@ -2684,11 +2736,11 @@
       <c r="E20" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="F20" s="104" t="s">
+      <c r="F20" s="66" t="s">
         <v>32</v>
       </c>
-      <c r="G20" s="105"/>
-      <c r="H20" s="106"/>
+      <c r="G20" s="120"/>
+      <c r="H20" s="121"/>
       <c r="I20" s="2"/>
       <c r="J20" s="2"/>
       <c r="K20" s="2"/>
@@ -2740,15 +2792,15 @@
       <c r="A22" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="B22" s="96" t="s">
+      <c r="B22" s="104" t="s">
         <v>59</v>
       </c>
-      <c r="C22" s="97"/>
-      <c r="D22" s="97"/>
-      <c r="E22" s="97"/>
-      <c r="F22" s="97"/>
-      <c r="G22" s="97"/>
-      <c r="H22" s="98"/>
+      <c r="C22" s="105"/>
+      <c r="D22" s="105"/>
+      <c r="E22" s="105"/>
+      <c r="F22" s="105"/>
+      <c r="G22" s="105"/>
+      <c r="H22" s="106"/>
       <c r="I22" s="2"/>
       <c r="J22" s="2"/>
       <c r="K22" s="2"/>
@@ -2772,7 +2824,7 @@
       <c r="A23" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B23" s="99" t="s">
+      <c r="B23" s="115" t="s">
         <v>60</v>
       </c>
       <c r="C23" s="93"/>
@@ -2801,7 +2853,7 @@
       <c r="Z23" s="2"/>
     </row>
     <row r="24" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="75" t="s">
+      <c r="A24" s="82" t="s">
         <v>4</v>
       </c>
       <c r="B24" s="93"/>
@@ -2831,10 +2883,10 @@
       <c r="Z24" s="2"/>
     </row>
     <row r="25" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="92" t="s">
+      <c r="A25" s="95" t="s">
         <v>5</v>
       </c>
-      <c r="B25" s="88"/>
+      <c r="B25" s="92"/>
       <c r="C25" s="1" t="s">
         <v>6</v>
       </c>
@@ -2873,10 +2925,10 @@
       <c r="Z25" s="2"/>
     </row>
     <row r="26" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="72" t="s">
+      <c r="A26" s="73" t="s">
         <v>61</v>
       </c>
-      <c r="B26" s="88"/>
+      <c r="B26" s="92"/>
       <c r="C26" s="4" t="s">
         <v>12</v>
       </c>
@@ -2913,10 +2965,10 @@
       <c r="Z26" s="2"/>
     </row>
     <row r="27" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="72" t="s">
+      <c r="A27" s="73" t="s">
         <v>11</v>
       </c>
-      <c r="B27" s="88"/>
+      <c r="B27" s="92"/>
       <c r="C27" s="4" t="s">
         <v>12</v>
       </c>
@@ -2953,10 +3005,10 @@
       <c r="Z27" s="2"/>
     </row>
     <row r="28" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="72" t="s">
+      <c r="A28" s="73" t="s">
         <v>64</v>
       </c>
-      <c r="B28" s="88"/>
+      <c r="B28" s="92"/>
       <c r="C28" s="4" t="s">
         <v>42</v>
       </c>
@@ -2991,10 +3043,10 @@
       <c r="Z28" s="2"/>
     </row>
     <row r="29" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="72" t="s">
+      <c r="A29" s="73" t="s">
         <v>66</v>
       </c>
-      <c r="B29" s="88"/>
+      <c r="B29" s="92"/>
       <c r="C29" s="4" t="s">
         <v>67</v>
       </c>
@@ -3029,10 +3081,10 @@
       <c r="Z29" s="2"/>
     </row>
     <row r="30" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="72" t="s">
+      <c r="A30" s="73" t="s">
         <v>70</v>
       </c>
-      <c r="B30" s="88"/>
+      <c r="B30" s="92"/>
       <c r="C30" s="4" t="s">
         <v>67</v>
       </c>
@@ -3067,10 +3119,10 @@
       <c r="Z30" s="2"/>
     </row>
     <row r="31" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="72" t="s">
+      <c r="A31" s="73" t="s">
         <v>72</v>
       </c>
-      <c r="B31" s="88"/>
+      <c r="B31" s="92"/>
       <c r="C31" s="4" t="s">
         <v>67</v>
       </c>
@@ -3105,10 +3157,10 @@
       <c r="Z31" s="2"/>
     </row>
     <row r="32" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="103" t="s">
+      <c r="A32" s="118" t="s">
         <v>74</v>
       </c>
-      <c r="B32" s="88"/>
+      <c r="B32" s="92"/>
       <c r="C32" s="4" t="s">
         <v>67</v>
       </c>
@@ -3143,10 +3195,10 @@
       <c r="Z32" s="2"/>
     </row>
     <row r="33" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="108" t="s">
+      <c r="A33" s="119" t="s">
         <v>76</v>
       </c>
-      <c r="B33" s="107"/>
+      <c r="B33" s="111"/>
       <c r="C33" s="23" t="s">
         <v>67</v>
       </c>
@@ -3181,16 +3233,16 @@
       <c r="Z33" s="2"/>
     </row>
     <row r="34" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="109" t="s">
+      <c r="A34" s="112" t="s">
         <v>48</v>
       </c>
-      <c r="B34" s="110"/>
-      <c r="C34" s="110"/>
-      <c r="D34" s="110"/>
-      <c r="E34" s="110"/>
-      <c r="F34" s="110"/>
-      <c r="G34" s="110"/>
-      <c r="H34" s="111"/>
+      <c r="B34" s="113"/>
+      <c r="C34" s="113"/>
+      <c r="D34" s="113"/>
+      <c r="E34" s="113"/>
+      <c r="F34" s="113"/>
+      <c r="G34" s="113"/>
+      <c r="H34" s="114"/>
       <c r="I34" s="2"/>
       <c r="J34" s="2"/>
       <c r="K34" s="2"/>
@@ -3211,10 +3263,10 @@
       <c r="Z34" s="2"/>
     </row>
     <row r="35" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="92" t="s">
+      <c r="A35" s="95" t="s">
         <v>49</v>
       </c>
-      <c r="B35" s="88"/>
+      <c r="B35" s="92"/>
       <c r="C35" s="1" t="s">
         <v>50</v>
       </c>
@@ -3224,7 +3276,7 @@
       <c r="E35" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="F35" s="92" t="s">
+      <c r="F35" s="95" t="s">
         <v>53</v>
       </c>
       <c r="G35" s="93"/>
@@ -3249,10 +3301,10 @@
       <c r="Z35" s="2"/>
     </row>
     <row r="36" spans="1:26" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="95" t="s">
+      <c r="A36" s="91" t="s">
         <v>78</v>
       </c>
-      <c r="B36" s="88"/>
+      <c r="B36" s="92"/>
       <c r="C36" s="15" t="s">
         <v>15</v>
       </c>
@@ -3260,7 +3312,7 @@
       <c r="E36" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="F36" s="95" t="s">
+      <c r="F36" s="91" t="s">
         <v>61</v>
       </c>
       <c r="G36" s="93"/>
@@ -3316,15 +3368,15 @@
       <c r="A38" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="B38" s="96" t="s">
+      <c r="B38" s="104" t="s">
         <v>79</v>
       </c>
-      <c r="C38" s="97"/>
-      <c r="D38" s="97"/>
-      <c r="E38" s="97"/>
-      <c r="F38" s="97"/>
-      <c r="G38" s="97"/>
-      <c r="H38" s="98"/>
+      <c r="C38" s="105"/>
+      <c r="D38" s="105"/>
+      <c r="E38" s="105"/>
+      <c r="F38" s="105"/>
+      <c r="G38" s="105"/>
+      <c r="H38" s="106"/>
       <c r="I38" s="2"/>
       <c r="J38" s="2"/>
       <c r="K38" s="2"/>
@@ -3348,7 +3400,7 @@
       <c r="A39" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B39" s="99" t="s">
+      <c r="B39" s="115" t="s">
         <v>80</v>
       </c>
       <c r="C39" s="93"/>
@@ -3377,7 +3429,7 @@
       <c r="Z39" s="2"/>
     </row>
     <row r="40" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="75" t="s">
+      <c r="A40" s="82" t="s">
         <v>4</v>
       </c>
       <c r="B40" s="93"/>
@@ -3407,10 +3459,10 @@
       <c r="Z40" s="2"/>
     </row>
     <row r="41" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="92" t="s">
+      <c r="A41" s="95" t="s">
         <v>5</v>
       </c>
-      <c r="B41" s="88"/>
+      <c r="B41" s="92"/>
       <c r="C41" s="1" t="s">
         <v>6</v>
       </c>
@@ -3449,10 +3501,10 @@
       <c r="Z41" s="2"/>
     </row>
     <row r="42" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="72" t="s">
+      <c r="A42" s="73" t="s">
         <v>81</v>
       </c>
-      <c r="B42" s="88"/>
+      <c r="B42" s="92"/>
       <c r="C42" s="4" t="s">
         <v>12</v>
       </c>
@@ -3489,10 +3541,10 @@
       <c r="Z42" s="2"/>
     </row>
     <row r="43" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="72" t="s">
+      <c r="A43" s="73" t="s">
         <v>61</v>
       </c>
-      <c r="B43" s="88"/>
+      <c r="B43" s="92"/>
       <c r="C43" s="4" t="s">
         <v>12</v>
       </c>
@@ -3529,10 +3581,10 @@
       <c r="Z43" s="2"/>
     </row>
     <row r="44" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="72" t="s">
+      <c r="A44" s="73" t="s">
         <v>84</v>
       </c>
-      <c r="B44" s="88"/>
+      <c r="B44" s="92"/>
       <c r="C44" s="4" t="s">
         <v>85</v>
       </c>
@@ -3567,10 +3619,10 @@
       <c r="Z44" s="2"/>
     </row>
     <row r="45" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="72" t="s">
+      <c r="A45" s="73" t="s">
         <v>88</v>
       </c>
-      <c r="B45" s="88"/>
+      <c r="B45" s="92"/>
       <c r="C45" s="4" t="s">
         <v>85</v>
       </c>
@@ -3605,10 +3657,10 @@
       <c r="Z45" s="2"/>
     </row>
     <row r="46" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="72" t="s">
+      <c r="A46" s="73" t="s">
         <v>90</v>
       </c>
-      <c r="B46" s="88"/>
+      <c r="B46" s="92"/>
       <c r="C46" s="4" t="s">
         <v>67</v>
       </c>
@@ -3643,10 +3695,10 @@
       <c r="Z46" s="2"/>
     </row>
     <row r="47" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="72" t="s">
+      <c r="A47" s="73" t="s">
         <v>92</v>
       </c>
-      <c r="B47" s="88"/>
+      <c r="B47" s="92"/>
       <c r="C47" s="4" t="s">
         <v>67</v>
       </c>
@@ -3681,10 +3733,10 @@
       <c r="Z47" s="2"/>
     </row>
     <row r="48" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="101" t="s">
+      <c r="A48" s="116" t="s">
         <v>94</v>
       </c>
-      <c r="B48" s="102"/>
+      <c r="B48" s="117"/>
       <c r="C48" s="11" t="s">
         <v>46</v>
       </c>
@@ -3719,16 +3771,16 @@
       <c r="Z48" s="2"/>
     </row>
     <row r="49" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="89" t="s">
+      <c r="A49" s="123" t="s">
         <v>48</v>
       </c>
-      <c r="B49" s="90"/>
-      <c r="C49" s="90"/>
-      <c r="D49" s="90"/>
-      <c r="E49" s="90"/>
-      <c r="F49" s="90"/>
-      <c r="G49" s="90"/>
-      <c r="H49" s="91"/>
+      <c r="B49" s="124"/>
+      <c r="C49" s="124"/>
+      <c r="D49" s="124"/>
+      <c r="E49" s="124"/>
+      <c r="F49" s="124"/>
+      <c r="G49" s="124"/>
+      <c r="H49" s="125"/>
       <c r="I49" s="2"/>
       <c r="J49" s="2"/>
       <c r="K49" s="2"/>
@@ -3749,10 +3801,10 @@
       <c r="Z49" s="2"/>
     </row>
     <row r="50" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="92" t="s">
+      <c r="A50" s="95" t="s">
         <v>49</v>
       </c>
-      <c r="B50" s="88"/>
+      <c r="B50" s="92"/>
       <c r="C50" s="1" t="s">
         <v>50</v>
       </c>
@@ -3762,7 +3814,7 @@
       <c r="E50" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="F50" s="92" t="s">
+      <c r="F50" s="95" t="s">
         <v>53</v>
       </c>
       <c r="G50" s="93"/>
@@ -3787,10 +3839,10 @@
       <c r="Z50" s="2"/>
     </row>
     <row r="51" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="95" t="s">
+      <c r="A51" s="91" t="s">
         <v>96</v>
       </c>
-      <c r="B51" s="88"/>
+      <c r="B51" s="92"/>
       <c r="C51" s="15" t="s">
         <v>15</v>
       </c>
@@ -3798,7 +3850,7 @@
       <c r="E51" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="F51" s="95" t="s">
+      <c r="F51" s="91" t="s">
         <v>81</v>
       </c>
       <c r="G51" s="93"/>
@@ -3854,15 +3906,15 @@
       <c r="A53" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="B53" s="96" t="s">
+      <c r="B53" s="104" t="s">
         <v>97</v>
       </c>
-      <c r="C53" s="97"/>
-      <c r="D53" s="97"/>
-      <c r="E53" s="97"/>
-      <c r="F53" s="97"/>
-      <c r="G53" s="97"/>
-      <c r="H53" s="98"/>
+      <c r="C53" s="105"/>
+      <c r="D53" s="105"/>
+      <c r="E53" s="105"/>
+      <c r="F53" s="105"/>
+      <c r="G53" s="105"/>
+      <c r="H53" s="106"/>
       <c r="I53" s="2"/>
       <c r="J53" s="2"/>
       <c r="K53" s="2"/>
@@ -3886,7 +3938,7 @@
       <c r="A54" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B54" s="99" t="s">
+      <c r="B54" s="115" t="s">
         <v>98</v>
       </c>
       <c r="C54" s="93"/>
@@ -3915,7 +3967,7 @@
       <c r="Z54" s="2"/>
     </row>
     <row r="55" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="75" t="s">
+      <c r="A55" s="82" t="s">
         <v>4</v>
       </c>
       <c r="B55" s="93"/>
@@ -3945,10 +3997,10 @@
       <c r="Z55" s="2"/>
     </row>
     <row r="56" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="92" t="s">
+      <c r="A56" s="95" t="s">
         <v>5</v>
       </c>
-      <c r="B56" s="88"/>
+      <c r="B56" s="92"/>
       <c r="C56" s="1" t="s">
         <v>6</v>
       </c>
@@ -3987,10 +4039,10 @@
       <c r="Z56" s="2"/>
     </row>
     <row r="57" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="72" t="s">
+      <c r="A57" s="73" t="s">
         <v>99</v>
       </c>
-      <c r="B57" s="88"/>
+      <c r="B57" s="92"/>
       <c r="C57" s="4" t="s">
         <v>12</v>
       </c>
@@ -4027,10 +4079,10 @@
       <c r="Z57" s="2"/>
     </row>
     <row r="58" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="72" t="s">
+      <c r="A58" s="73" t="s">
         <v>61</v>
       </c>
-      <c r="B58" s="88"/>
+      <c r="B58" s="92"/>
       <c r="C58" s="4" t="s">
         <v>12</v>
       </c>
@@ -4067,10 +4119,10 @@
       <c r="Z58" s="2"/>
     </row>
     <row r="59" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="72" t="s">
+      <c r="A59" s="73" t="s">
         <v>11</v>
       </c>
-      <c r="B59" s="88"/>
+      <c r="B59" s="92"/>
       <c r="C59" s="4" t="s">
         <v>12</v>
       </c>
@@ -4107,10 +4159,10 @@
       <c r="Z59" s="2"/>
     </row>
     <row r="60" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="72" t="s">
+      <c r="A60" s="73" t="s">
         <v>103</v>
       </c>
-      <c r="B60" s="88"/>
+      <c r="B60" s="92"/>
       <c r="C60" s="4" t="s">
         <v>46</v>
       </c>
@@ -4145,10 +4197,10 @@
       <c r="Z60" s="2"/>
     </row>
     <row r="61" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="72" t="s">
+      <c r="A61" s="73" t="s">
         <v>105</v>
       </c>
-      <c r="B61" s="88"/>
+      <c r="B61" s="92"/>
       <c r="C61" s="4" t="s">
         <v>42</v>
       </c>
@@ -4183,10 +4235,10 @@
       <c r="Z61" s="2"/>
     </row>
     <row r="62" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="72" t="s">
+      <c r="A62" s="73" t="s">
         <v>106</v>
       </c>
-      <c r="B62" s="88"/>
+      <c r="B62" s="92"/>
       <c r="C62" s="12" t="s">
         <v>107</v>
       </c>
@@ -4221,10 +4273,10 @@
       <c r="Z62" s="2"/>
     </row>
     <row r="63" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="81" t="s">
+      <c r="A63" s="71" t="s">
         <v>109</v>
       </c>
-      <c r="B63" s="107"/>
+      <c r="B63" s="111"/>
       <c r="C63" s="23" t="s">
         <v>67</v>
       </c>
@@ -4259,16 +4311,16 @@
       <c r="Z63" s="2"/>
     </row>
     <row r="64" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="109" t="s">
+      <c r="A64" s="112" t="s">
         <v>48</v>
       </c>
-      <c r="B64" s="110"/>
-      <c r="C64" s="110"/>
-      <c r="D64" s="110"/>
-      <c r="E64" s="110"/>
-      <c r="F64" s="110"/>
-      <c r="G64" s="110"/>
-      <c r="H64" s="111"/>
+      <c r="B64" s="113"/>
+      <c r="C64" s="113"/>
+      <c r="D64" s="113"/>
+      <c r="E64" s="113"/>
+      <c r="F64" s="113"/>
+      <c r="G64" s="113"/>
+      <c r="H64" s="114"/>
       <c r="I64" s="2"/>
       <c r="J64" s="2"/>
       <c r="K64" s="2"/>
@@ -4289,10 +4341,10 @@
       <c r="Z64" s="2"/>
     </row>
     <row r="65" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="92" t="s">
+      <c r="A65" s="95" t="s">
         <v>49</v>
       </c>
-      <c r="B65" s="88"/>
+      <c r="B65" s="92"/>
       <c r="C65" s="1" t="s">
         <v>50</v>
       </c>
@@ -4302,7 +4354,7 @@
       <c r="E65" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="F65" s="92" t="s">
+      <c r="F65" s="95" t="s">
         <v>53</v>
       </c>
       <c r="G65" s="93"/>
@@ -4327,10 +4379,10 @@
       <c r="Z65" s="2"/>
     </row>
     <row r="66" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="95" t="s">
+      <c r="A66" s="91" t="s">
         <v>111</v>
       </c>
-      <c r="B66" s="88"/>
+      <c r="B66" s="92"/>
       <c r="C66" s="15" t="s">
         <v>15</v>
       </c>
@@ -4338,7 +4390,7 @@
       <c r="E66" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="F66" s="95" t="s">
+      <c r="F66" s="91" t="s">
         <v>99</v>
       </c>
       <c r="G66" s="93"/>
@@ -4394,15 +4446,15 @@
       <c r="A68" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="B68" s="96" t="s">
+      <c r="B68" s="104" t="s">
         <v>112</v>
       </c>
-      <c r="C68" s="97"/>
-      <c r="D68" s="97"/>
-      <c r="E68" s="97"/>
-      <c r="F68" s="97"/>
-      <c r="G68" s="97"/>
-      <c r="H68" s="98"/>
+      <c r="C68" s="105"/>
+      <c r="D68" s="105"/>
+      <c r="E68" s="105"/>
+      <c r="F68" s="105"/>
+      <c r="G68" s="105"/>
+      <c r="H68" s="106"/>
       <c r="I68" s="2"/>
       <c r="J68" s="2"/>
       <c r="K68" s="2"/>
@@ -4426,15 +4478,15 @@
       <c r="A69" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B69" s="112" t="s">
+      <c r="B69" s="107" t="s">
         <v>113</v>
       </c>
-      <c r="C69" s="97"/>
-      <c r="D69" s="97"/>
-      <c r="E69" s="97"/>
-      <c r="F69" s="97"/>
-      <c r="G69" s="97"/>
-      <c r="H69" s="98"/>
+      <c r="C69" s="105"/>
+      <c r="D69" s="105"/>
+      <c r="E69" s="105"/>
+      <c r="F69" s="105"/>
+      <c r="G69" s="105"/>
+      <c r="H69" s="106"/>
       <c r="I69" s="2"/>
       <c r="J69" s="2"/>
       <c r="K69" s="2"/>
@@ -4455,7 +4507,7 @@
       <c r="Z69" s="2"/>
     </row>
     <row r="70" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="75" t="s">
+      <c r="A70" s="82" t="s">
         <v>4</v>
       </c>
       <c r="B70" s="93"/>
@@ -4464,7 +4516,7 @@
       <c r="E70" s="93"/>
       <c r="F70" s="93"/>
       <c r="G70" s="93"/>
-      <c r="H70" s="115"/>
+      <c r="H70" s="110"/>
       <c r="I70" s="33"/>
       <c r="J70" s="2"/>
       <c r="K70" s="2"/>
@@ -4485,10 +4537,10 @@
       <c r="Z70" s="2"/>
     </row>
     <row r="71" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="92" t="s">
+      <c r="A71" s="95" t="s">
         <v>5</v>
       </c>
-      <c r="B71" s="88"/>
+      <c r="B71" s="92"/>
       <c r="C71" s="1" t="s">
         <v>6</v>
       </c>
@@ -4527,10 +4579,10 @@
       <c r="Z71" s="2"/>
     </row>
     <row r="72" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="72" t="s">
+      <c r="A72" s="73" t="s">
         <v>114</v>
       </c>
-      <c r="B72" s="88"/>
+      <c r="B72" s="92"/>
       <c r="C72" s="4" t="s">
         <v>12</v>
       </c>
@@ -4567,10 +4619,10 @@
       <c r="Z72" s="2"/>
     </row>
     <row r="73" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="72" t="s">
+      <c r="A73" s="73" t="s">
         <v>17</v>
       </c>
-      <c r="B73" s="80"/>
+      <c r="B73" s="74"/>
       <c r="C73" s="4" t="s">
         <v>18</v>
       </c>
@@ -4605,10 +4657,10 @@
       <c r="Z73" s="2"/>
     </row>
     <row r="74" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="72" t="s">
+      <c r="A74" s="73" t="s">
         <v>61</v>
       </c>
-      <c r="B74" s="88"/>
+      <c r="B74" s="92"/>
       <c r="C74" s="4" t="s">
         <v>12</v>
       </c>
@@ -4645,10 +4697,10 @@
       <c r="Z74" s="2"/>
     </row>
     <row r="75" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="72" t="s">
+      <c r="A75" s="73" t="s">
         <v>117</v>
       </c>
-      <c r="B75" s="88"/>
+      <c r="B75" s="92"/>
       <c r="C75" s="4" t="s">
         <v>67</v>
       </c>
@@ -4683,10 +4735,10 @@
       <c r="Z75" s="2"/>
     </row>
     <row r="76" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="72" t="s">
+      <c r="A76" s="73" t="s">
         <v>119</v>
       </c>
-      <c r="B76" s="88"/>
+      <c r="B76" s="92"/>
       <c r="C76" s="4" t="s">
         <v>67</v>
       </c>
@@ -4721,10 +4773,10 @@
       <c r="Z76" s="2"/>
     </row>
     <row r="77" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="72" t="s">
+      <c r="A77" s="73" t="s">
         <v>122</v>
       </c>
-      <c r="B77" s="88"/>
+      <c r="B77" s="92"/>
       <c r="C77" s="4" t="s">
         <v>46</v>
       </c>
@@ -4759,10 +4811,10 @@
       <c r="Z77" s="2"/>
     </row>
     <row r="78" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="118" t="s">
+      <c r="A78" s="96" t="s">
         <v>124</v>
       </c>
-      <c r="B78" s="119"/>
+      <c r="B78" s="97"/>
       <c r="C78" s="12" t="s">
         <v>46</v>
       </c>
@@ -4797,10 +4849,10 @@
       <c r="Z78" s="2"/>
     </row>
     <row r="79" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A79" s="113" t="s">
+      <c r="A79" s="108" t="s">
         <v>126</v>
       </c>
-      <c r="B79" s="114"/>
+      <c r="B79" s="109"/>
       <c r="C79" s="35" t="s">
         <v>67</v>
       </c>
@@ -4835,16 +4887,16 @@
       <c r="Z79" s="2"/>
     </row>
     <row r="80" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="120" t="s">
+      <c r="A80" s="98" t="s">
         <v>48</v>
       </c>
-      <c r="B80" s="121"/>
-      <c r="C80" s="121"/>
-      <c r="D80" s="121"/>
-      <c r="E80" s="121"/>
-      <c r="F80" s="121"/>
-      <c r="G80" s="121"/>
-      <c r="H80" s="122"/>
+      <c r="B80" s="99"/>
+      <c r="C80" s="99"/>
+      <c r="D80" s="99"/>
+      <c r="E80" s="99"/>
+      <c r="F80" s="99"/>
+      <c r="G80" s="99"/>
+      <c r="H80" s="100"/>
       <c r="I80" s="2"/>
       <c r="J80" s="2"/>
       <c r="K80" s="2"/>
@@ -4865,10 +4917,10 @@
       <c r="Z80" s="2"/>
     </row>
     <row r="81" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="92" t="s">
+      <c r="A81" s="95" t="s">
         <v>49</v>
       </c>
-      <c r="B81" s="88"/>
+      <c r="B81" s="92"/>
       <c r="C81" s="1" t="s">
         <v>50</v>
       </c>
@@ -4878,7 +4930,7 @@
       <c r="E81" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="F81" s="92" t="s">
+      <c r="F81" s="95" t="s">
         <v>53</v>
       </c>
       <c r="G81" s="93"/>
@@ -4903,10 +4955,10 @@
       <c r="Z81" s="2"/>
     </row>
     <row r="82" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A82" s="95" t="s">
+      <c r="A82" s="91" t="s">
         <v>128</v>
       </c>
-      <c r="B82" s="88"/>
+      <c r="B82" s="92"/>
       <c r="C82" s="15" t="s">
         <v>15</v>
       </c>
@@ -4914,7 +4966,7 @@
       <c r="E82" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="F82" s="95" t="s">
+      <c r="F82" s="91" t="s">
         <v>114</v>
       </c>
       <c r="G82" s="93"/>
@@ -4970,15 +5022,15 @@
       <c r="A84" s="61" t="s">
         <v>58</v>
       </c>
-      <c r="B84" s="69" t="s">
+      <c r="B84" s="88" t="s">
         <v>174</v>
       </c>
-      <c r="C84" s="70"/>
-      <c r="D84" s="70"/>
-      <c r="E84" s="70"/>
-      <c r="F84" s="70"/>
-      <c r="G84" s="70"/>
-      <c r="H84" s="71"/>
+      <c r="C84" s="89"/>
+      <c r="D84" s="89"/>
+      <c r="E84" s="89"/>
+      <c r="F84" s="89"/>
+      <c r="G84" s="89"/>
+      <c r="H84" s="90"/>
       <c r="I84" s="2"/>
       <c r="J84" s="2"/>
       <c r="K84" s="2"/>
@@ -5002,15 +5054,15 @@
       <c r="A85" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B85" s="72" t="s">
+      <c r="B85" s="73" t="s">
         <v>175</v>
       </c>
-      <c r="C85" s="73"/>
-      <c r="D85" s="73"/>
-      <c r="E85" s="73"/>
-      <c r="F85" s="73"/>
-      <c r="G85" s="73"/>
-      <c r="H85" s="74"/>
+      <c r="C85" s="84"/>
+      <c r="D85" s="84"/>
+      <c r="E85" s="84"/>
+      <c r="F85" s="84"/>
+      <c r="G85" s="84"/>
+      <c r="H85" s="85"/>
       <c r="I85" s="2"/>
       <c r="J85" s="2"/>
       <c r="K85" s="2"/>
@@ -5031,16 +5083,16 @@
       <c r="Z85" s="2"/>
     </row>
     <row r="86" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="75" t="s">
+      <c r="A86" s="82" t="s">
         <v>4</v>
       </c>
-      <c r="B86" s="76"/>
-      <c r="C86" s="76"/>
-      <c r="D86" s="76"/>
-      <c r="E86" s="76"/>
-      <c r="F86" s="76"/>
-      <c r="G86" s="76"/>
-      <c r="H86" s="77"/>
+      <c r="B86" s="86"/>
+      <c r="C86" s="86"/>
+      <c r="D86" s="86"/>
+      <c r="E86" s="86"/>
+      <c r="F86" s="86"/>
+      <c r="G86" s="86"/>
+      <c r="H86" s="87"/>
       <c r="I86" s="2"/>
       <c r="J86" s="2"/>
       <c r="K86" s="2"/>
@@ -5061,10 +5113,10 @@
       <c r="Z86" s="2"/>
     </row>
     <row r="87" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="78" t="s">
+      <c r="A87" s="75" t="s">
         <v>5</v>
       </c>
-      <c r="B87" s="79"/>
+      <c r="B87" s="76"/>
       <c r="C87" s="1" t="s">
         <v>6</v>
       </c>
@@ -5183,16 +5235,16 @@
       <c r="Z89" s="2"/>
     </row>
     <row r="90" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="83" t="s">
+      <c r="A90" s="77" t="s">
         <v>48</v>
       </c>
-      <c r="B90" s="84"/>
-      <c r="C90" s="84"/>
-      <c r="D90" s="84"/>
-      <c r="E90" s="84"/>
-      <c r="F90" s="84"/>
-      <c r="G90" s="84"/>
-      <c r="H90" s="85"/>
+      <c r="B90" s="78"/>
+      <c r="C90" s="78"/>
+      <c r="D90" s="78"/>
+      <c r="E90" s="78"/>
+      <c r="F90" s="78"/>
+      <c r="G90" s="78"/>
+      <c r="H90" s="79"/>
       <c r="I90" s="2"/>
       <c r="J90" s="2"/>
       <c r="K90" s="2"/>
@@ -5213,10 +5265,10 @@
       <c r="Z90" s="2"/>
     </row>
     <row r="91" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="78" t="s">
+      <c r="A91" s="75" t="s">
         <v>49</v>
       </c>
-      <c r="B91" s="79"/>
+      <c r="B91" s="76"/>
       <c r="C91" s="1" t="s">
         <v>50</v>
       </c>
@@ -5226,11 +5278,11 @@
       <c r="E91" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="F91" s="78" t="s">
+      <c r="F91" s="75" t="s">
         <v>53</v>
       </c>
-      <c r="G91" s="86"/>
-      <c r="H91" s="87"/>
+      <c r="G91" s="80"/>
+      <c r="H91" s="81"/>
       <c r="I91" s="2"/>
       <c r="J91" s="2"/>
       <c r="K91" s="2"/>
@@ -5262,11 +5314,11 @@
       <c r="E92" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="F92" s="65" t="s">
+      <c r="F92" s="63" t="s">
         <v>176</v>
       </c>
-      <c r="G92" s="67"/>
-      <c r="H92" s="68"/>
+      <c r="G92" s="64"/>
+      <c r="H92" s="65"/>
       <c r="I92" s="2"/>
       <c r="J92" s="2"/>
       <c r="K92" s="2"/>
@@ -5287,10 +5339,10 @@
       <c r="Z92" s="2"/>
     </row>
     <row r="93" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A93" s="104" t="s">
+      <c r="A93" s="66" t="s">
         <v>179</v>
       </c>
-      <c r="B93" s="126"/>
+      <c r="B93" s="67"/>
       <c r="C93" s="60"/>
       <c r="D93" s="60" t="s">
         <v>15</v>
@@ -5298,11 +5350,11 @@
       <c r="E93" s="60" t="s">
         <v>15</v>
       </c>
-      <c r="F93" s="104" t="s">
+      <c r="F93" s="66" t="s">
         <v>114</v>
       </c>
-      <c r="G93" s="116"/>
-      <c r="H93" s="117"/>
+      <c r="G93" s="68"/>
+      <c r="H93" s="69"/>
       <c r="I93" s="2"/>
       <c r="J93" s="2"/>
       <c r="K93" s="2"/>
@@ -5354,15 +5406,15 @@
       <c r="A95" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="B95" s="123" t="s">
+      <c r="B95" s="101" t="s">
         <v>129</v>
       </c>
-      <c r="C95" s="124"/>
-      <c r="D95" s="124"/>
-      <c r="E95" s="124"/>
-      <c r="F95" s="124"/>
-      <c r="G95" s="124"/>
-      <c r="H95" s="125"/>
+      <c r="C95" s="102"/>
+      <c r="D95" s="102"/>
+      <c r="E95" s="102"/>
+      <c r="F95" s="102"/>
+      <c r="G95" s="102"/>
+      <c r="H95" s="103"/>
       <c r="I95" s="2"/>
       <c r="J95" s="2"/>
       <c r="K95" s="2"/>
@@ -5386,15 +5438,15 @@
       <c r="A96" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B96" s="72" t="s">
+      <c r="B96" s="73" t="s">
         <v>130</v>
       </c>
-      <c r="C96" s="73"/>
-      <c r="D96" s="73"/>
-      <c r="E96" s="73"/>
-      <c r="F96" s="73"/>
-      <c r="G96" s="73"/>
-      <c r="H96" s="74"/>
+      <c r="C96" s="84"/>
+      <c r="D96" s="84"/>
+      <c r="E96" s="84"/>
+      <c r="F96" s="84"/>
+      <c r="G96" s="84"/>
+      <c r="H96" s="85"/>
       <c r="I96" s="2"/>
       <c r="J96" s="2"/>
       <c r="K96" s="2"/>
@@ -5415,16 +5467,16 @@
       <c r="Z96" s="2"/>
     </row>
     <row r="97" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="75" t="s">
+      <c r="A97" s="82" t="s">
         <v>4</v>
       </c>
-      <c r="B97" s="76"/>
-      <c r="C97" s="76"/>
-      <c r="D97" s="76"/>
-      <c r="E97" s="76"/>
-      <c r="F97" s="76"/>
-      <c r="G97" s="76"/>
-      <c r="H97" s="77"/>
+      <c r="B97" s="86"/>
+      <c r="C97" s="86"/>
+      <c r="D97" s="86"/>
+      <c r="E97" s="86"/>
+      <c r="F97" s="86"/>
+      <c r="G97" s="86"/>
+      <c r="H97" s="87"/>
       <c r="I97" s="2"/>
       <c r="J97" s="2"/>
       <c r="K97" s="2"/>
@@ -5445,10 +5497,10 @@
       <c r="Z97" s="2"/>
     </row>
     <row r="98" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A98" s="78" t="s">
+      <c r="A98" s="75" t="s">
         <v>5</v>
       </c>
-      <c r="B98" s="79"/>
+      <c r="B98" s="76"/>
       <c r="C98" s="1" t="s">
         <v>6</v>
       </c>
@@ -5757,16 +5809,16 @@
       <c r="Z105" s="2"/>
     </row>
     <row r="106" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A106" s="83" t="s">
+      <c r="A106" s="77" t="s">
         <v>48</v>
       </c>
-      <c r="B106" s="84"/>
-      <c r="C106" s="84"/>
-      <c r="D106" s="84"/>
-      <c r="E106" s="84"/>
-      <c r="F106" s="84"/>
-      <c r="G106" s="84"/>
-      <c r="H106" s="85"/>
+      <c r="B106" s="78"/>
+      <c r="C106" s="78"/>
+      <c r="D106" s="78"/>
+      <c r="E106" s="78"/>
+      <c r="F106" s="78"/>
+      <c r="G106" s="78"/>
+      <c r="H106" s="79"/>
       <c r="I106" s="2"/>
       <c r="J106" s="2"/>
       <c r="K106" s="2"/>
@@ -5787,10 +5839,10 @@
       <c r="Z106" s="2"/>
     </row>
     <row r="107" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A107" s="75" t="s">
+      <c r="A107" s="82" t="s">
         <v>49</v>
       </c>
-      <c r="B107" s="127"/>
+      <c r="B107" s="83"/>
       <c r="C107" s="1" t="s">
         <v>50</v>
       </c>
@@ -5800,11 +5852,11 @@
       <c r="E107" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="F107" s="78" t="s">
+      <c r="F107" s="75" t="s">
         <v>53</v>
       </c>
-      <c r="G107" s="86"/>
-      <c r="H107" s="87"/>
+      <c r="G107" s="80"/>
+      <c r="H107" s="81"/>
       <c r="I107" s="2"/>
       <c r="J107" s="2"/>
       <c r="K107" s="2"/>
@@ -5825,10 +5877,10 @@
       <c r="Z107" s="2"/>
     </row>
     <row r="108" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A108" s="104" t="s">
+      <c r="A108" s="66" t="s">
         <v>143</v>
       </c>
-      <c r="B108" s="126"/>
+      <c r="B108" s="67"/>
       <c r="C108" s="15" t="s">
         <v>15</v>
       </c>
@@ -5836,11 +5888,11 @@
       <c r="E108" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="F108" s="104" t="s">
+      <c r="F108" s="66" t="s">
         <v>131</v>
       </c>
-      <c r="G108" s="116"/>
-      <c r="H108" s="117"/>
+      <c r="G108" s="68"/>
+      <c r="H108" s="69"/>
       <c r="I108" s="2"/>
       <c r="J108" s="2"/>
       <c r="K108" s="2"/>
@@ -5924,15 +5976,15 @@
       <c r="A111" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B111" s="72" t="s">
+      <c r="B111" s="73" t="s">
         <v>145</v>
       </c>
-      <c r="C111" s="73"/>
-      <c r="D111" s="73"/>
-      <c r="E111" s="73"/>
-      <c r="F111" s="73"/>
-      <c r="G111" s="73"/>
-      <c r="H111" s="74"/>
+      <c r="C111" s="84"/>
+      <c r="D111" s="84"/>
+      <c r="E111" s="84"/>
+      <c r="F111" s="84"/>
+      <c r="G111" s="84"/>
+      <c r="H111" s="85"/>
       <c r="I111" s="2"/>
       <c r="J111" s="2"/>
       <c r="K111" s="2"/>
@@ -5953,16 +6005,16 @@
       <c r="Z111" s="2"/>
     </row>
     <row r="112" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A112" s="75" t="s">
+      <c r="A112" s="82" t="s">
         <v>4</v>
       </c>
-      <c r="B112" s="76"/>
-      <c r="C112" s="76"/>
-      <c r="D112" s="76"/>
-      <c r="E112" s="76"/>
-      <c r="F112" s="76"/>
-      <c r="G112" s="76"/>
-      <c r="H112" s="77"/>
+      <c r="B112" s="86"/>
+      <c r="C112" s="86"/>
+      <c r="D112" s="86"/>
+      <c r="E112" s="86"/>
+      <c r="F112" s="86"/>
+      <c r="G112" s="86"/>
+      <c r="H112" s="87"/>
       <c r="I112" s="2"/>
       <c r="J112" s="2"/>
       <c r="K112" s="2"/>
@@ -5983,10 +6035,10 @@
       <c r="Z112" s="2"/>
     </row>
     <row r="113" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A113" s="78" t="s">
+      <c r="A113" s="75" t="s">
         <v>5</v>
       </c>
-      <c r="B113" s="79"/>
+      <c r="B113" s="76"/>
       <c r="C113" s="1" t="s">
         <v>6</v>
       </c>
@@ -6295,16 +6347,16 @@
       <c r="Z120" s="2"/>
     </row>
     <row r="121" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A121" s="83" t="s">
+      <c r="A121" s="77" t="s">
         <v>48</v>
       </c>
-      <c r="B121" s="84"/>
-      <c r="C121" s="84"/>
-      <c r="D121" s="84"/>
-      <c r="E121" s="84"/>
-      <c r="F121" s="84"/>
-      <c r="G121" s="84"/>
-      <c r="H121" s="85"/>
+      <c r="B121" s="78"/>
+      <c r="C121" s="78"/>
+      <c r="D121" s="78"/>
+      <c r="E121" s="78"/>
+      <c r="F121" s="78"/>
+      <c r="G121" s="78"/>
+      <c r="H121" s="79"/>
       <c r="I121" s="2"/>
       <c r="J121" s="2"/>
       <c r="K121" s="2"/>
@@ -6325,10 +6377,10 @@
       <c r="Z121" s="2"/>
     </row>
     <row r="122" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A122" s="78" t="s">
+      <c r="A122" s="75" t="s">
         <v>49</v>
       </c>
-      <c r="B122" s="79"/>
+      <c r="B122" s="76"/>
       <c r="C122" s="1" t="s">
         <v>50</v>
       </c>
@@ -6338,11 +6390,11 @@
       <c r="E122" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="F122" s="78" t="s">
+      <c r="F122" s="75" t="s">
         <v>53</v>
       </c>
-      <c r="G122" s="86"/>
-      <c r="H122" s="87"/>
+      <c r="G122" s="80"/>
+      <c r="H122" s="81"/>
       <c r="I122" s="2"/>
       <c r="J122" s="2"/>
       <c r="K122" s="2"/>
@@ -6374,11 +6426,11 @@
       <c r="E123" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="F123" s="65" t="s">
+      <c r="F123" s="63" t="s">
         <v>147</v>
       </c>
-      <c r="G123" s="67"/>
-      <c r="H123" s="68"/>
+      <c r="G123" s="64"/>
+      <c r="H123" s="65"/>
       <c r="I123" s="2"/>
       <c r="J123" s="2"/>
       <c r="K123" s="2"/>
@@ -6410,11 +6462,11 @@
       <c r="E124" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="F124" s="104" t="s">
+      <c r="F124" s="66" t="s">
         <v>148</v>
       </c>
-      <c r="G124" s="116"/>
-      <c r="H124" s="117"/>
+      <c r="G124" s="68"/>
+      <c r="H124" s="69"/>
       <c r="I124" s="2"/>
       <c r="J124" s="2"/>
       <c r="K124" s="2"/>
@@ -6466,15 +6518,15 @@
       <c r="A126" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="B126" s="69" t="s">
+      <c r="B126" s="88" t="s">
         <v>162</v>
       </c>
-      <c r="C126" s="70"/>
-      <c r="D126" s="70"/>
-      <c r="E126" s="70"/>
-      <c r="F126" s="70"/>
-      <c r="G126" s="70"/>
-      <c r="H126" s="71"/>
+      <c r="C126" s="89"/>
+      <c r="D126" s="89"/>
+      <c r="E126" s="89"/>
+      <c r="F126" s="89"/>
+      <c r="G126" s="89"/>
+      <c r="H126" s="90"/>
       <c r="I126" s="2"/>
       <c r="J126" s="2"/>
       <c r="K126" s="2"/>
@@ -6498,15 +6550,15 @@
       <c r="A127" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B127" s="72" t="s">
+      <c r="B127" s="73" t="s">
         <v>163</v>
       </c>
-      <c r="C127" s="73"/>
-      <c r="D127" s="73"/>
-      <c r="E127" s="73"/>
-      <c r="F127" s="73"/>
-      <c r="G127" s="73"/>
-      <c r="H127" s="74"/>
+      <c r="C127" s="84"/>
+      <c r="D127" s="84"/>
+      <c r="E127" s="84"/>
+      <c r="F127" s="84"/>
+      <c r="G127" s="84"/>
+      <c r="H127" s="85"/>
       <c r="I127" s="2"/>
       <c r="J127" s="2"/>
       <c r="K127" s="2"/>
@@ -6527,16 +6579,16 @@
       <c r="Z127" s="2"/>
     </row>
     <row r="128" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A128" s="75" t="s">
+      <c r="A128" s="82" t="s">
         <v>4</v>
       </c>
-      <c r="B128" s="76"/>
-      <c r="C128" s="76"/>
-      <c r="D128" s="76"/>
-      <c r="E128" s="76"/>
-      <c r="F128" s="76"/>
-      <c r="G128" s="76"/>
-      <c r="H128" s="77"/>
+      <c r="B128" s="86"/>
+      <c r="C128" s="86"/>
+      <c r="D128" s="86"/>
+      <c r="E128" s="86"/>
+      <c r="F128" s="86"/>
+      <c r="G128" s="86"/>
+      <c r="H128" s="87"/>
       <c r="I128" s="2"/>
       <c r="J128" s="2"/>
       <c r="K128" s="2"/>
@@ -6599,10 +6651,10 @@
       <c r="Z129" s="2"/>
     </row>
     <row r="130" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A130" s="72" t="s">
+      <c r="A130" s="73" t="s">
         <v>164</v>
       </c>
-      <c r="B130" s="80"/>
+      <c r="B130" s="74"/>
       <c r="C130" s="4" t="s">
         <v>12</v>
       </c>
@@ -6677,10 +6729,10 @@
       <c r="Z131" s="2"/>
     </row>
     <row r="132" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A132" s="72" t="s">
+      <c r="A132" s="73" t="s">
         <v>61</v>
       </c>
-      <c r="B132" s="80"/>
+      <c r="B132" s="74"/>
       <c r="C132" s="4" t="s">
         <v>12</v>
       </c>
@@ -6717,10 +6769,10 @@
       <c r="Z132" s="2"/>
     </row>
     <row r="133" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A133" s="72" t="s">
+      <c r="A133" s="73" t="s">
         <v>109</v>
       </c>
-      <c r="B133" s="80"/>
+      <c r="B133" s="74"/>
       <c r="C133" s="4" t="s">
         <v>67</v>
       </c>
@@ -6755,10 +6807,10 @@
       <c r="Z133" s="2"/>
     </row>
     <row r="134" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A134" s="72" t="s">
+      <c r="A134" s="73" t="s">
         <v>117</v>
       </c>
-      <c r="B134" s="80"/>
+      <c r="B134" s="74"/>
       <c r="C134" s="12" t="s">
         <v>67</v>
       </c>
@@ -6793,10 +6845,10 @@
       <c r="Z134" s="2"/>
     </row>
     <row r="135" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A135" s="81" t="s">
+      <c r="A135" s="71" t="s">
         <v>169</v>
       </c>
-      <c r="B135" s="82"/>
+      <c r="B135" s="72"/>
       <c r="C135" s="23" t="s">
         <v>46</v>
       </c>
@@ -6874,11 +6926,11 @@
       <c r="E137" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="F137" s="78" t="s">
+      <c r="F137" s="75" t="s">
         <v>53</v>
       </c>
-      <c r="G137" s="86"/>
-      <c r="H137" s="87"/>
+      <c r="G137" s="80"/>
+      <c r="H137" s="81"/>
       <c r="I137" s="2"/>
       <c r="J137" s="2"/>
       <c r="K137" s="2"/>
@@ -6899,10 +6951,10 @@
       <c r="Z137" s="2"/>
     </row>
     <row r="138" spans="1:26" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A138" s="104" t="s">
+      <c r="A138" s="66" t="s">
         <v>171</v>
       </c>
-      <c r="B138" s="126"/>
+      <c r="B138" s="67"/>
       <c r="C138" s="18" t="s">
         <v>15</v>
       </c>
@@ -6910,11 +6962,11 @@
       <c r="E138" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="F138" s="104" t="s">
+      <c r="F138" s="66" t="s">
         <v>164</v>
       </c>
-      <c r="G138" s="116"/>
-      <c r="H138" s="117"/>
+      <c r="G138" s="68"/>
+      <c r="H138" s="69"/>
       <c r="I138" s="2"/>
       <c r="J138" s="2"/>
       <c r="K138" s="2"/>
@@ -6958,15 +7010,15 @@
       <c r="A140" s="61" t="s">
         <v>58</v>
       </c>
-      <c r="B140" s="69" t="s">
+      <c r="B140" s="88" t="s">
         <v>181</v>
       </c>
-      <c r="C140" s="70"/>
-      <c r="D140" s="70"/>
-      <c r="E140" s="70"/>
-      <c r="F140" s="70"/>
-      <c r="G140" s="70"/>
-      <c r="H140" s="71"/>
+      <c r="C140" s="89"/>
+      <c r="D140" s="89"/>
+      <c r="E140" s="89"/>
+      <c r="F140" s="89"/>
+      <c r="G140" s="89"/>
+      <c r="H140" s="90"/>
       <c r="I140" s="2"/>
       <c r="J140" s="2"/>
       <c r="K140" s="2"/>
@@ -6990,15 +7042,15 @@
       <c r="A141" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B141" s="72" t="s">
+      <c r="B141" s="73" t="s">
         <v>182</v>
       </c>
-      <c r="C141" s="73"/>
-      <c r="D141" s="73"/>
-      <c r="E141" s="73"/>
-      <c r="F141" s="73"/>
-      <c r="G141" s="73"/>
-      <c r="H141" s="74"/>
+      <c r="C141" s="84"/>
+      <c r="D141" s="84"/>
+      <c r="E141" s="84"/>
+      <c r="F141" s="84"/>
+      <c r="G141" s="84"/>
+      <c r="H141" s="85"/>
       <c r="I141" s="2"/>
       <c r="J141" s="2"/>
       <c r="K141" s="2"/>
@@ -7019,16 +7071,16 @@
       <c r="Z141" s="2"/>
     </row>
     <row r="142" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A142" s="75" t="s">
+      <c r="A142" s="82" t="s">
         <v>4</v>
       </c>
-      <c r="B142" s="76"/>
-      <c r="C142" s="76"/>
-      <c r="D142" s="76"/>
-      <c r="E142" s="76"/>
-      <c r="F142" s="76"/>
-      <c r="G142" s="76"/>
-      <c r="H142" s="77"/>
+      <c r="B142" s="86"/>
+      <c r="C142" s="86"/>
+      <c r="D142" s="86"/>
+      <c r="E142" s="86"/>
+      <c r="F142" s="86"/>
+      <c r="G142" s="86"/>
+      <c r="H142" s="87"/>
       <c r="I142" s="2"/>
       <c r="J142" s="2"/>
       <c r="K142" s="2"/>
@@ -7049,10 +7101,10 @@
       <c r="Z142" s="2"/>
     </row>
     <row r="143" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A143" s="78" t="s">
+      <c r="A143" s="75" t="s">
         <v>5</v>
       </c>
-      <c r="B143" s="79"/>
+      <c r="B143" s="76"/>
       <c r="C143" s="1" t="s">
         <v>6</v>
       </c>
@@ -7091,10 +7143,10 @@
       <c r="Z143" s="2"/>
     </row>
     <row r="144" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A144" s="72" t="s">
+      <c r="A144" s="73" t="s">
         <v>183</v>
       </c>
-      <c r="B144" s="80"/>
+      <c r="B144" s="74"/>
       <c r="C144" s="4" t="s">
         <v>12</v>
       </c>
@@ -7131,10 +7183,10 @@
       <c r="Z144" s="2"/>
     </row>
     <row r="145" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A145" s="81" t="s">
+      <c r="A145" s="71" t="s">
         <v>164</v>
       </c>
-      <c r="B145" s="82"/>
+      <c r="B145" s="72"/>
       <c r="C145" s="4" t="s">
         <v>12</v>
       </c>
@@ -7171,16 +7223,16 @@
       <c r="Z145" s="2"/>
     </row>
     <row r="146" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A146" s="83" t="s">
+      <c r="A146" s="77" t="s">
         <v>48</v>
       </c>
-      <c r="B146" s="84"/>
-      <c r="C146" s="84"/>
-      <c r="D146" s="84"/>
-      <c r="E146" s="84"/>
-      <c r="F146" s="84"/>
-      <c r="G146" s="84"/>
-      <c r="H146" s="85"/>
+      <c r="B146" s="78"/>
+      <c r="C146" s="78"/>
+      <c r="D146" s="78"/>
+      <c r="E146" s="78"/>
+      <c r="F146" s="78"/>
+      <c r="G146" s="78"/>
+      <c r="H146" s="79"/>
       <c r="I146" s="2"/>
       <c r="J146" s="2"/>
       <c r="K146" s="2"/>
@@ -7201,10 +7253,10 @@
       <c r="Z146" s="2"/>
     </row>
     <row r="147" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A147" s="78" t="s">
+      <c r="A147" s="75" t="s">
         <v>49</v>
       </c>
-      <c r="B147" s="79"/>
+      <c r="B147" s="76"/>
       <c r="C147" s="1" t="s">
         <v>50</v>
       </c>
@@ -7214,11 +7266,11 @@
       <c r="E147" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="F147" s="78" t="s">
+      <c r="F147" s="75" t="s">
         <v>53</v>
       </c>
-      <c r="G147" s="86"/>
-      <c r="H147" s="87"/>
+      <c r="G147" s="80"/>
+      <c r="H147" s="81"/>
       <c r="I147" s="2"/>
       <c r="J147" s="2"/>
       <c r="K147" s="2"/>
@@ -7239,10 +7291,10 @@
       <c r="Z147" s="2"/>
     </row>
     <row r="148" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A148" s="65" t="s">
+      <c r="A148" s="63" t="s">
         <v>186</v>
       </c>
-      <c r="B148" s="66"/>
+      <c r="B148" s="70"/>
       <c r="C148" s="15" t="s">
         <v>15</v>
       </c>
@@ -7250,11 +7302,11 @@
       <c r="E148" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="F148" s="65" t="s">
+      <c r="F148" s="63" t="s">
         <v>183</v>
       </c>
-      <c r="G148" s="67"/>
-      <c r="H148" s="68"/>
+      <c r="G148" s="64"/>
+      <c r="H148" s="65"/>
       <c r="I148" s="2"/>
       <c r="J148" s="2"/>
       <c r="K148" s="2"/>
@@ -7275,10 +7327,10 @@
       <c r="Z148" s="2"/>
     </row>
     <row r="149" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A149" s="104" t="s">
+      <c r="A149" s="66" t="s">
         <v>187</v>
       </c>
-      <c r="B149" s="126"/>
+      <c r="B149" s="67"/>
       <c r="C149" s="60"/>
       <c r="D149" s="60" t="s">
         <v>15</v>
@@ -7286,11 +7338,11 @@
       <c r="E149" s="60" t="s">
         <v>15</v>
       </c>
-      <c r="F149" s="104" t="s">
+      <c r="F149" s="66" t="s">
         <v>164</v>
       </c>
-      <c r="G149" s="116"/>
-      <c r="H149" s="117"/>
+      <c r="G149" s="68"/>
+      <c r="H149" s="69"/>
       <c r="I149" s="2"/>
       <c r="J149" s="2"/>
       <c r="K149" s="2"/>
@@ -7334,15 +7386,15 @@
       <c r="A151" s="61" t="s">
         <v>58</v>
       </c>
-      <c r="B151" s="69" t="s">
+      <c r="B151" s="88" t="s">
         <v>193</v>
       </c>
-      <c r="C151" s="70"/>
-      <c r="D151" s="70"/>
-      <c r="E151" s="70"/>
-      <c r="F151" s="70"/>
-      <c r="G151" s="70"/>
-      <c r="H151" s="71"/>
+      <c r="C151" s="89"/>
+      <c r="D151" s="89"/>
+      <c r="E151" s="89"/>
+      <c r="F151" s="89"/>
+      <c r="G151" s="89"/>
+      <c r="H151" s="90"/>
       <c r="I151" s="2"/>
       <c r="J151" s="2"/>
       <c r="K151" s="2"/>
@@ -7366,15 +7418,15 @@
       <c r="A152" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B152" s="72" t="s">
+      <c r="B152" s="73" t="s">
         <v>194</v>
       </c>
-      <c r="C152" s="73"/>
-      <c r="D152" s="73"/>
-      <c r="E152" s="73"/>
-      <c r="F152" s="73"/>
-      <c r="G152" s="73"/>
-      <c r="H152" s="74"/>
+      <c r="C152" s="84"/>
+      <c r="D152" s="84"/>
+      <c r="E152" s="84"/>
+      <c r="F152" s="84"/>
+      <c r="G152" s="84"/>
+      <c r="H152" s="85"/>
       <c r="I152" s="2"/>
       <c r="J152" s="2"/>
       <c r="K152" s="2"/>
@@ -7395,16 +7447,16 @@
       <c r="Z152" s="2"/>
     </row>
     <row r="153" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A153" s="75" t="s">
+      <c r="A153" s="82" t="s">
         <v>4</v>
       </c>
-      <c r="B153" s="76"/>
-      <c r="C153" s="76"/>
-      <c r="D153" s="76"/>
-      <c r="E153" s="76"/>
-      <c r="F153" s="76"/>
-      <c r="G153" s="76"/>
-      <c r="H153" s="77"/>
+      <c r="B153" s="86"/>
+      <c r="C153" s="86"/>
+      <c r="D153" s="86"/>
+      <c r="E153" s="86"/>
+      <c r="F153" s="86"/>
+      <c r="G153" s="86"/>
+      <c r="H153" s="87"/>
       <c r="I153" s="2"/>
       <c r="J153" s="2"/>
       <c r="K153" s="2"/>
@@ -7425,10 +7477,10 @@
       <c r="Z153" s="2"/>
     </row>
     <row r="154" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A154" s="78" t="s">
+      <c r="A154" s="75" t="s">
         <v>5</v>
       </c>
-      <c r="B154" s="79"/>
+      <c r="B154" s="76"/>
       <c r="C154" s="1" t="s">
         <v>6</v>
       </c>
@@ -7467,10 +7519,10 @@
       <c r="Z154" s="2"/>
     </row>
     <row r="155" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A155" s="72" t="s">
+      <c r="A155" s="73" t="s">
         <v>195</v>
       </c>
-      <c r="B155" s="80"/>
+      <c r="B155" s="74"/>
       <c r="C155" s="4" t="s">
         <v>12</v>
       </c>
@@ -7507,10 +7559,10 @@
       <c r="Z155" s="2"/>
     </row>
     <row r="156" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A156" s="63" t="s">
+      <c r="A156" s="73" t="s">
         <v>11</v>
       </c>
-      <c r="B156" s="64"/>
+      <c r="B156" s="74"/>
       <c r="C156" s="4" t="s">
         <v>12</v>
       </c>
@@ -7545,10 +7597,10 @@
       <c r="Z156" s="2"/>
     </row>
     <row r="157" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A157" s="63" t="s">
+      <c r="A157" s="73" t="s">
         <v>17</v>
       </c>
-      <c r="B157" s="64"/>
+      <c r="B157" s="74"/>
       <c r="C157" s="4" t="s">
         <v>18</v>
       </c>
@@ -7583,10 +7635,10 @@
       <c r="Z157" s="2"/>
     </row>
     <row r="158" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A158" s="63" t="s">
+      <c r="A158" s="73" t="s">
         <v>20</v>
       </c>
-      <c r="B158" s="64"/>
+      <c r="B158" s="74"/>
       <c r="C158" s="4" t="s">
         <v>21</v>
       </c>
@@ -7621,10 +7673,10 @@
       <c r="Z158" s="2"/>
     </row>
     <row r="159" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A159" s="63" t="s">
+      <c r="A159" s="73" t="s">
         <v>24</v>
       </c>
-      <c r="B159" s="64"/>
+      <c r="B159" s="74"/>
       <c r="C159" s="4" t="s">
         <v>25</v>
       </c>
@@ -7659,10 +7711,10 @@
       <c r="Z159" s="2"/>
     </row>
     <row r="160" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A160" s="63" t="s">
+      <c r="A160" s="73" t="s">
         <v>28</v>
       </c>
-      <c r="B160" s="64"/>
+      <c r="B160" s="74"/>
       <c r="C160" s="4" t="s">
         <v>29</v>
       </c>
@@ -7697,10 +7749,10 @@
       <c r="Z160" s="2"/>
     </row>
     <row r="161" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A161" s="63" t="s">
+      <c r="A161" s="73" t="s">
         <v>32</v>
       </c>
-      <c r="B161" s="64"/>
+      <c r="B161" s="74"/>
       <c r="C161" s="4" t="s">
         <v>33</v>
       </c>
@@ -7735,10 +7787,10 @@
       <c r="Z161" s="2"/>
     </row>
     <row r="162" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A162" s="63" t="s">
+      <c r="A162" s="73" t="s">
         <v>36</v>
       </c>
-      <c r="B162" s="64"/>
+      <c r="B162" s="74"/>
       <c r="C162" s="4" t="s">
         <v>37</v>
       </c>
@@ -7773,10 +7825,10 @@
       <c r="Z162" s="2"/>
     </row>
     <row r="163" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A163" s="63" t="s">
+      <c r="A163" s="73" t="s">
         <v>39</v>
       </c>
-      <c r="B163" s="64"/>
+      <c r="B163" s="74"/>
       <c r="C163" s="4" t="s">
         <v>21</v>
       </c>
@@ -7811,10 +7863,10 @@
       <c r="Z163" s="2"/>
     </row>
     <row r="164" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A164" s="63" t="s">
+      <c r="A164" s="73" t="s">
         <v>41</v>
       </c>
-      <c r="B164" s="64"/>
+      <c r="B164" s="74"/>
       <c r="C164" s="4" t="s">
         <v>42</v>
       </c>
@@ -7849,10 +7901,10 @@
       <c r="Z164" s="2"/>
     </row>
     <row r="165" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A165" s="63" t="s">
+      <c r="A165" s="73" t="s">
         <v>45</v>
       </c>
-      <c r="B165" s="64"/>
+      <c r="B165" s="74"/>
       <c r="C165" s="4" t="s">
         <v>46</v>
       </c>
@@ -7887,10 +7939,10 @@
       <c r="Z165" s="2"/>
     </row>
     <row r="166" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A166" s="63" t="s">
+      <c r="A166" s="73" t="s">
         <v>61</v>
       </c>
-      <c r="B166" s="64"/>
+      <c r="B166" s="74"/>
       <c r="C166" s="4" t="s">
         <v>12</v>
       </c>
@@ -7925,10 +7977,10 @@
       <c r="Z166" s="2"/>
     </row>
     <row r="167" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A167" s="63" t="s">
+      <c r="A167" s="73" t="s">
         <v>64</v>
       </c>
-      <c r="B167" s="64"/>
+      <c r="B167" s="74"/>
       <c r="C167" s="4" t="s">
         <v>42</v>
       </c>
@@ -7963,10 +8015,10 @@
       <c r="Z167" s="2"/>
     </row>
     <row r="168" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A168" s="63" t="s">
+      <c r="A168" s="73" t="s">
         <v>66</v>
       </c>
-      <c r="B168" s="64"/>
+      <c r="B168" s="74"/>
       <c r="C168" s="4" t="s">
         <v>67</v>
       </c>
@@ -8001,10 +8053,10 @@
       <c r="Z168" s="2"/>
     </row>
     <row r="169" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A169" s="63" t="s">
+      <c r="A169" s="73" t="s">
         <v>70</v>
       </c>
-      <c r="B169" s="64"/>
+      <c r="B169" s="74"/>
       <c r="C169" s="4" t="s">
         <v>67</v>
       </c>
@@ -8039,10 +8091,10 @@
       <c r="Z169" s="2"/>
     </row>
     <row r="170" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A170" s="63" t="s">
+      <c r="A170" s="73" t="s">
         <v>72</v>
       </c>
-      <c r="B170" s="64"/>
+      <c r="B170" s="74"/>
       <c r="C170" s="4" t="s">
         <v>67</v>
       </c>
@@ -8077,10 +8129,10 @@
       <c r="Z170" s="2"/>
     </row>
     <row r="171" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A171" s="63" t="s">
+      <c r="A171" s="73" t="s">
         <v>74</v>
       </c>
-      <c r="B171" s="64"/>
+      <c r="B171" s="74"/>
       <c r="C171" s="4" t="s">
         <v>67</v>
       </c>
@@ -8115,10 +8167,10 @@
       <c r="Z171" s="2"/>
     </row>
     <row r="172" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A172" s="63" t="s">
+      <c r="A172" s="73" t="s">
         <v>76</v>
       </c>
-      <c r="B172" s="64"/>
+      <c r="B172" s="74"/>
       <c r="C172" s="4" t="s">
         <v>67</v>
       </c>
@@ -8153,10 +8205,10 @@
       <c r="Z172" s="2"/>
     </row>
     <row r="173" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A173" s="63" t="s">
+      <c r="A173" s="73" t="s">
         <v>81</v>
       </c>
-      <c r="B173" s="64"/>
+      <c r="B173" s="74"/>
       <c r="C173" s="4" t="s">
         <v>12</v>
       </c>
@@ -8191,10 +8243,10 @@
       <c r="Z173" s="2"/>
     </row>
     <row r="174" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A174" s="63" t="s">
+      <c r="A174" s="73" t="s">
         <v>84</v>
       </c>
-      <c r="B174" s="64"/>
+      <c r="B174" s="74"/>
       <c r="C174" s="4" t="s">
         <v>85</v>
       </c>
@@ -8229,10 +8281,10 @@
       <c r="Z174" s="2"/>
     </row>
     <row r="175" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A175" s="63" t="s">
+      <c r="A175" s="73" t="s">
         <v>88</v>
       </c>
-      <c r="B175" s="64"/>
+      <c r="B175" s="74"/>
       <c r="C175" s="4" t="s">
         <v>85</v>
       </c>
@@ -8267,10 +8319,10 @@
       <c r="Z175" s="2"/>
     </row>
     <row r="176" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A176" s="63" t="s">
+      <c r="A176" s="73" t="s">
         <v>90</v>
       </c>
-      <c r="B176" s="64"/>
+      <c r="B176" s="74"/>
       <c r="C176" s="4" t="s">
         <v>67</v>
       </c>
@@ -8305,10 +8357,10 @@
       <c r="Z176" s="2"/>
     </row>
     <row r="177" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A177" s="63" t="s">
+      <c r="A177" s="73" t="s">
         <v>92</v>
       </c>
-      <c r="B177" s="64"/>
+      <c r="B177" s="74"/>
       <c r="C177" s="4" t="s">
         <v>67</v>
       </c>
@@ -8343,10 +8395,10 @@
       <c r="Z177" s="2"/>
     </row>
     <row r="178" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A178" s="63" t="s">
+      <c r="A178" s="73" t="s">
         <v>94</v>
       </c>
-      <c r="B178" s="64"/>
+      <c r="B178" s="74"/>
       <c r="C178" s="4" t="s">
         <v>46</v>
       </c>
@@ -8381,10 +8433,10 @@
       <c r="Z178" s="2"/>
     </row>
     <row r="179" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A179" s="63" t="s">
+      <c r="A179" s="73" t="s">
         <v>131</v>
       </c>
-      <c r="B179" s="64"/>
+      <c r="B179" s="74"/>
       <c r="C179" s="4" t="s">
         <v>12</v>
       </c>
@@ -8419,10 +8471,10 @@
       <c r="Z179" s="2"/>
     </row>
     <row r="180" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A180" s="63" t="s">
+      <c r="A180" s="73" t="s">
         <v>219</v>
       </c>
-      <c r="B180" s="64"/>
+      <c r="B180" s="74"/>
       <c r="C180" s="4" t="s">
         <v>18</v>
       </c>
@@ -8457,10 +8509,10 @@
       <c r="Z180" s="2"/>
     </row>
     <row r="181" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A181" s="63" t="s">
+      <c r="A181" s="73" t="s">
         <v>135</v>
       </c>
-      <c r="B181" s="64"/>
+      <c r="B181" s="74"/>
       <c r="C181" s="4" t="s">
         <v>42</v>
       </c>
@@ -8495,10 +8547,10 @@
       <c r="Z181" s="2"/>
     </row>
     <row r="182" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A182" s="63" t="s">
+      <c r="A182" s="73" t="s">
         <v>137</v>
       </c>
-      <c r="B182" s="64"/>
+      <c r="B182" s="74"/>
       <c r="C182" s="4" t="s">
         <v>67</v>
       </c>
@@ -8533,10 +8585,10 @@
       <c r="Z182" s="2"/>
     </row>
     <row r="183" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A183" s="63" t="s">
+      <c r="A183" s="73" t="s">
         <v>139</v>
       </c>
-      <c r="B183" s="64"/>
+      <c r="B183" s="74"/>
       <c r="C183" s="4" t="s">
         <v>67</v>
       </c>
@@ -8571,10 +8623,10 @@
       <c r="Z183" s="2"/>
     </row>
     <row r="184" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A184" s="63" t="s">
+      <c r="A184" s="73" t="s">
         <v>141</v>
       </c>
-      <c r="B184" s="64"/>
+      <c r="B184" s="74"/>
       <c r="C184" s="4" t="s">
         <v>46</v>
       </c>
@@ -8609,10 +8661,10 @@
       <c r="Z184" s="2"/>
     </row>
     <row r="185" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A185" s="63" t="s">
+      <c r="A185" s="73" t="s">
         <v>114</v>
       </c>
-      <c r="B185" s="64"/>
+      <c r="B185" s="74"/>
       <c r="C185" s="4" t="s">
         <v>12</v>
       </c>
@@ -8647,10 +8699,10 @@
       <c r="Z185" s="2"/>
     </row>
     <row r="186" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A186" s="63" t="s">
+      <c r="A186" s="73" t="s">
         <v>225</v>
       </c>
-      <c r="B186" s="64"/>
+      <c r="B186" s="74"/>
       <c r="C186" s="4" t="s">
         <v>18</v>
       </c>
@@ -8685,10 +8737,10 @@
       <c r="Z186" s="2"/>
     </row>
     <row r="187" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A187" s="63" t="s">
+      <c r="A187" s="73" t="s">
         <v>117</v>
       </c>
-      <c r="B187" s="64"/>
+      <c r="B187" s="74"/>
       <c r="C187" s="4" t="s">
         <v>67</v>
       </c>
@@ -8723,10 +8775,10 @@
       <c r="Z187" s="2"/>
     </row>
     <row r="188" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A188" s="63" t="s">
+      <c r="A188" s="73" t="s">
         <v>119</v>
       </c>
-      <c r="B188" s="64"/>
+      <c r="B188" s="74"/>
       <c r="C188" s="4" t="s">
         <v>67</v>
       </c>
@@ -8761,10 +8813,10 @@
       <c r="Z188" s="2"/>
     </row>
     <row r="189" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A189" s="63" t="s">
+      <c r="A189" s="73" t="s">
         <v>122</v>
       </c>
-      <c r="B189" s="64"/>
+      <c r="B189" s="74"/>
       <c r="C189" s="4" t="s">
         <v>46</v>
       </c>
@@ -8799,10 +8851,10 @@
       <c r="Z189" s="2"/>
     </row>
     <row r="190" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A190" s="63" t="s">
+      <c r="A190" s="73" t="s">
         <v>124</v>
       </c>
-      <c r="B190" s="64"/>
+      <c r="B190" s="74"/>
       <c r="C190" s="4" t="s">
         <v>46</v>
       </c>
@@ -8837,10 +8889,10 @@
       <c r="Z190" s="2"/>
     </row>
     <row r="191" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A191" s="63" t="s">
+      <c r="A191" s="73" t="s">
         <v>126</v>
       </c>
-      <c r="B191" s="64"/>
+      <c r="B191" s="74"/>
       <c r="C191" s="4" t="s">
         <v>67</v>
       </c>
@@ -8875,10 +8927,10 @@
       <c r="Z191" s="2"/>
     </row>
     <row r="192" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A192" s="63" t="s">
+      <c r="A192" s="73" t="s">
         <v>176</v>
       </c>
-      <c r="B192" s="64"/>
+      <c r="B192" s="74"/>
       <c r="C192" s="4" t="s">
         <v>12</v>
       </c>
@@ -8913,10 +8965,10 @@
       <c r="Z192" s="2"/>
     </row>
     <row r="193" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A193" s="63" t="s">
+      <c r="A193" s="73" t="s">
         <v>164</v>
       </c>
-      <c r="B193" s="64"/>
+      <c r="B193" s="74"/>
       <c r="C193" s="4" t="s">
         <v>12</v>
       </c>
@@ -8951,10 +9003,10 @@
       <c r="Z193" s="2"/>
     </row>
     <row r="194" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A194" s="63" t="s">
+      <c r="A194" s="73" t="s">
         <v>234</v>
       </c>
-      <c r="B194" s="64"/>
+      <c r="B194" s="74"/>
       <c r="C194" s="4" t="s">
         <v>18</v>
       </c>
@@ -8989,10 +9041,10 @@
       <c r="Z194" s="2"/>
     </row>
     <row r="195" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A195" s="63" t="s">
+      <c r="A195" s="73" t="s">
         <v>235</v>
       </c>
-      <c r="B195" s="64"/>
+      <c r="B195" s="74"/>
       <c r="C195" s="4" t="s">
         <v>67</v>
       </c>
@@ -9027,10 +9079,10 @@
       <c r="Z195" s="2"/>
     </row>
     <row r="196" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A196" s="63" t="s">
+      <c r="A196" s="73" t="s">
         <v>236</v>
       </c>
-      <c r="B196" s="64"/>
+      <c r="B196" s="74"/>
       <c r="C196" s="4" t="s">
         <v>67</v>
       </c>
@@ -9065,10 +9117,10 @@
       <c r="Z196" s="2"/>
     </row>
     <row r="197" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A197" s="63" t="s">
+      <c r="A197" s="73" t="s">
         <v>169</v>
       </c>
-      <c r="B197" s="64"/>
+      <c r="B197" s="74"/>
       <c r="C197" s="4" t="s">
         <v>46</v>
       </c>
@@ -9103,10 +9155,10 @@
       <c r="Z197" s="2"/>
     </row>
     <row r="198" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A198" s="63" t="s">
+      <c r="A198" s="131" t="s">
         <v>183</v>
       </c>
-      <c r="B198" s="64"/>
+      <c r="B198" s="132"/>
       <c r="C198" s="4" t="s">
         <v>12</v>
       </c>
@@ -9141,10 +9193,10 @@
       <c r="Z198" s="2"/>
     </row>
     <row r="199" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A199" s="63" t="s">
+      <c r="A199" s="73" t="s">
         <v>147</v>
       </c>
-      <c r="B199" s="64"/>
+      <c r="B199" s="74"/>
       <c r="C199" s="4" t="s">
         <v>12</v>
       </c>
@@ -9179,10 +9231,10 @@
       <c r="Z199" s="2"/>
     </row>
     <row r="200" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A200" s="63" t="s">
+      <c r="A200" s="73" t="s">
         <v>237</v>
       </c>
-      <c r="B200" s="64"/>
+      <c r="B200" s="74"/>
       <c r="C200" s="4" t="s">
         <v>18</v>
       </c>
@@ -9217,10 +9269,10 @@
       <c r="Z200" s="2"/>
     </row>
     <row r="201" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A201" s="63" t="s">
+      <c r="A201" s="73" t="s">
         <v>148</v>
       </c>
-      <c r="B201" s="64"/>
+      <c r="B201" s="74"/>
       <c r="C201" s="4" t="s">
         <v>149</v>
       </c>
@@ -9255,10 +9307,10 @@
       <c r="Z201" s="2"/>
     </row>
     <row r="202" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A202" s="63" t="s">
+      <c r="A202" s="73" t="s">
         <v>152</v>
       </c>
-      <c r="B202" s="64"/>
+      <c r="B202" s="74"/>
       <c r="C202" s="4" t="s">
         <v>21</v>
       </c>
@@ -9293,10 +9345,10 @@
       <c r="Z202" s="2"/>
     </row>
     <row r="203" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A203" s="63" t="s">
+      <c r="A203" s="73" t="s">
         <v>154</v>
       </c>
-      <c r="B203" s="64"/>
+      <c r="B203" s="74"/>
       <c r="C203" s="4" t="s">
         <v>29</v>
       </c>
@@ -9331,10 +9383,10 @@
       <c r="Z203" s="2"/>
     </row>
     <row r="204" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A204" s="63" t="s">
+      <c r="A204" s="73" t="s">
         <v>156</v>
       </c>
-      <c r="B204" s="64"/>
+      <c r="B204" s="74"/>
       <c r="C204" s="4" t="s">
         <v>157</v>
       </c>
@@ -9369,10 +9421,10 @@
       <c r="Z204" s="2"/>
     </row>
     <row r="205" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A205" s="63" t="s">
+      <c r="A205" s="73" t="s">
         <v>99</v>
       </c>
-      <c r="B205" s="64"/>
+      <c r="B205" s="74"/>
       <c r="C205" s="4" t="s">
         <v>12</v>
       </c>
@@ -9407,10 +9459,10 @@
       <c r="Z205" s="2"/>
     </row>
     <row r="206" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A206" s="63" t="s">
+      <c r="A206" s="73" t="s">
         <v>253</v>
       </c>
-      <c r="B206" s="64"/>
+      <c r="B206" s="74"/>
       <c r="C206" s="4" t="s">
         <v>12</v>
       </c>
@@ -9445,10 +9497,10 @@
       <c r="Z206" s="2"/>
     </row>
     <row r="207" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A207" s="63" t="s">
+      <c r="A207" s="73" t="s">
         <v>254</v>
       </c>
-      <c r="B207" s="64"/>
+      <c r="B207" s="74"/>
       <c r="C207" s="4" t="s">
         <v>12</v>
       </c>
@@ -9483,10 +9535,10 @@
       <c r="Z207" s="2"/>
     </row>
     <row r="208" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A208" s="63" t="s">
+      <c r="A208" s="73" t="s">
         <v>255</v>
       </c>
-      <c r="B208" s="64"/>
+      <c r="B208" s="74"/>
       <c r="C208" s="4" t="s">
         <v>46</v>
       </c>
@@ -9521,10 +9573,10 @@
       <c r="Z208" s="2"/>
     </row>
     <row r="209" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A209" s="63" t="s">
+      <c r="A209" s="73" t="s">
         <v>105</v>
       </c>
-      <c r="B209" s="64"/>
+      <c r="B209" s="74"/>
       <c r="C209" s="4" t="s">
         <v>42</v>
       </c>
@@ -9559,10 +9611,10 @@
       <c r="Z209" s="2"/>
     </row>
     <row r="210" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A210" s="63" t="s">
+      <c r="A210" s="73" t="s">
         <v>106</v>
       </c>
-      <c r="B210" s="64"/>
+      <c r="B210" s="74"/>
       <c r="C210" s="4" t="s">
         <v>107</v>
       </c>
@@ -9597,10 +9649,10 @@
       <c r="Z210" s="2"/>
     </row>
     <row r="211" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A211" s="81" t="s">
+      <c r="A211" s="71" t="s">
         <v>256</v>
       </c>
-      <c r="B211" s="82"/>
+      <c r="B211" s="72"/>
       <c r="C211" s="4" t="s">
         <v>46</v>
       </c>
@@ -9635,16 +9687,16 @@
       <c r="Z211" s="2"/>
     </row>
     <row r="212" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A212" s="83" t="s">
+      <c r="A212" s="77" t="s">
         <v>48</v>
       </c>
-      <c r="B212" s="84"/>
-      <c r="C212" s="84"/>
-      <c r="D212" s="84"/>
-      <c r="E212" s="84"/>
-      <c r="F212" s="84"/>
-      <c r="G212" s="84"/>
-      <c r="H212" s="85"/>
+      <c r="B212" s="78"/>
+      <c r="C212" s="78"/>
+      <c r="D212" s="78"/>
+      <c r="E212" s="78"/>
+      <c r="F212" s="78"/>
+      <c r="G212" s="78"/>
+      <c r="H212" s="79"/>
       <c r="I212" s="2"/>
       <c r="J212" s="2"/>
       <c r="K212" s="2"/>
@@ -9665,10 +9717,10 @@
       <c r="Z212" s="2"/>
     </row>
     <row r="213" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A213" s="78" t="s">
+      <c r="A213" s="75" t="s">
         <v>49</v>
       </c>
-      <c r="B213" s="79"/>
+      <c r="B213" s="76"/>
       <c r="C213" s="1" t="s">
         <v>50</v>
       </c>
@@ -9678,11 +9730,11 @@
       <c r="E213" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="F213" s="78" t="s">
+      <c r="F213" s="75" t="s">
         <v>53</v>
       </c>
-      <c r="G213" s="86"/>
-      <c r="H213" s="87"/>
+      <c r="G213" s="80"/>
+      <c r="H213" s="81"/>
       <c r="I213" s="2"/>
       <c r="J213" s="2"/>
       <c r="K213" s="2"/>
@@ -9702,23 +9754,23 @@
       <c r="Y213" s="2"/>
       <c r="Z213" s="2"/>
     </row>
-    <row r="214" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A214" s="65" t="s">
+    <row r="214" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A214" s="126" t="s">
         <v>263</v>
       </c>
-      <c r="B214" s="66"/>
-      <c r="C214" s="15" t="s">
+      <c r="B214" s="130"/>
+      <c r="C214" s="60" t="s">
         <v>15</v>
       </c>
-      <c r="D214" s="16"/>
-      <c r="E214" s="15" t="s">
+      <c r="D214" s="129"/>
+      <c r="E214" s="60" t="s">
         <v>15</v>
       </c>
-      <c r="F214" s="65" t="s">
+      <c r="F214" s="126" t="s">
         <v>195</v>
       </c>
-      <c r="G214" s="67"/>
-      <c r="H214" s="68"/>
+      <c r="G214" s="127"/>
+      <c r="H214" s="128"/>
       <c r="I214" s="2"/>
       <c r="J214" s="2"/>
       <c r="K214" s="2"/>
@@ -33315,75 +33367,123 @@
       <c r="Z1056" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="153">
-    <mergeCell ref="F148:H148"/>
-    <mergeCell ref="A149:B149"/>
-    <mergeCell ref="F149:H149"/>
-    <mergeCell ref="A148:B148"/>
-    <mergeCell ref="A145:B145"/>
-    <mergeCell ref="A144:B144"/>
-    <mergeCell ref="A135:B135"/>
-    <mergeCell ref="A134:B134"/>
-    <mergeCell ref="A133:B133"/>
-    <mergeCell ref="A138:B138"/>
-    <mergeCell ref="A143:B143"/>
-    <mergeCell ref="A146:H146"/>
-    <mergeCell ref="A147:B147"/>
-    <mergeCell ref="F147:H147"/>
-    <mergeCell ref="F137:H137"/>
-    <mergeCell ref="F138:H138"/>
-    <mergeCell ref="F92:H92"/>
-    <mergeCell ref="A98:B98"/>
-    <mergeCell ref="A106:H106"/>
-    <mergeCell ref="A107:B107"/>
-    <mergeCell ref="F107:H107"/>
-    <mergeCell ref="F108:H108"/>
-    <mergeCell ref="A108:B108"/>
-    <mergeCell ref="B111:H111"/>
-    <mergeCell ref="A112:H112"/>
-    <mergeCell ref="A113:B113"/>
-    <mergeCell ref="A130:B130"/>
-    <mergeCell ref="A121:H121"/>
-    <mergeCell ref="F122:H122"/>
-    <mergeCell ref="F123:H123"/>
-    <mergeCell ref="B96:H96"/>
-    <mergeCell ref="A97:H97"/>
-    <mergeCell ref="A87:B87"/>
-    <mergeCell ref="A93:B93"/>
-    <mergeCell ref="F93:H93"/>
-    <mergeCell ref="A91:B91"/>
-    <mergeCell ref="B140:H140"/>
-    <mergeCell ref="B141:H141"/>
-    <mergeCell ref="A142:H142"/>
-    <mergeCell ref="F124:H124"/>
-    <mergeCell ref="B127:H127"/>
-    <mergeCell ref="B126:H126"/>
-    <mergeCell ref="A128:H128"/>
-    <mergeCell ref="A82:B82"/>
-    <mergeCell ref="F82:H82"/>
-    <mergeCell ref="A73:B73"/>
-    <mergeCell ref="A71:B71"/>
-    <mergeCell ref="A72:B72"/>
-    <mergeCell ref="A74:B74"/>
-    <mergeCell ref="A75:B75"/>
-    <mergeCell ref="A76:B76"/>
-    <mergeCell ref="A77:B77"/>
-    <mergeCell ref="A78:B78"/>
-    <mergeCell ref="A80:H80"/>
-    <mergeCell ref="A81:B81"/>
-    <mergeCell ref="F81:H81"/>
-    <mergeCell ref="A122:B122"/>
-    <mergeCell ref="B84:H84"/>
-    <mergeCell ref="B85:H85"/>
-    <mergeCell ref="F91:H91"/>
-    <mergeCell ref="A86:H86"/>
-    <mergeCell ref="A90:H90"/>
-    <mergeCell ref="B95:H95"/>
-    <mergeCell ref="A132:B132"/>
-    <mergeCell ref="B68:H68"/>
-    <mergeCell ref="B69:H69"/>
-    <mergeCell ref="A79:B79"/>
-    <mergeCell ref="A70:H70"/>
+  <mergeCells count="208">
+    <mergeCell ref="A205:B205"/>
+    <mergeCell ref="A206:B206"/>
+    <mergeCell ref="A207:B207"/>
+    <mergeCell ref="A208:B208"/>
+    <mergeCell ref="A209:B209"/>
+    <mergeCell ref="A210:B210"/>
+    <mergeCell ref="A196:B196"/>
+    <mergeCell ref="A197:B197"/>
+    <mergeCell ref="A198:B198"/>
+    <mergeCell ref="A199:B199"/>
+    <mergeCell ref="A200:B200"/>
+    <mergeCell ref="A201:B201"/>
+    <mergeCell ref="A202:B202"/>
+    <mergeCell ref="A203:B203"/>
+    <mergeCell ref="A204:B204"/>
+    <mergeCell ref="A187:B187"/>
+    <mergeCell ref="A188:B188"/>
+    <mergeCell ref="A189:B189"/>
+    <mergeCell ref="A190:B190"/>
+    <mergeCell ref="A191:B191"/>
+    <mergeCell ref="A192:B192"/>
+    <mergeCell ref="A193:B193"/>
+    <mergeCell ref="A194:B194"/>
+    <mergeCell ref="A195:B195"/>
+    <mergeCell ref="A178:B178"/>
+    <mergeCell ref="A179:B179"/>
+    <mergeCell ref="A180:B180"/>
+    <mergeCell ref="A181:B181"/>
+    <mergeCell ref="A182:B182"/>
+    <mergeCell ref="A183:B183"/>
+    <mergeCell ref="A184:B184"/>
+    <mergeCell ref="A185:B185"/>
+    <mergeCell ref="A186:B186"/>
+    <mergeCell ref="A169:B169"/>
+    <mergeCell ref="A170:B170"/>
+    <mergeCell ref="A171:B171"/>
+    <mergeCell ref="A172:B172"/>
+    <mergeCell ref="A173:B173"/>
+    <mergeCell ref="A174:B174"/>
+    <mergeCell ref="A175:B175"/>
+    <mergeCell ref="A176:B176"/>
+    <mergeCell ref="A177:B177"/>
+    <mergeCell ref="A214:B214"/>
+    <mergeCell ref="F214:H214"/>
+    <mergeCell ref="B151:H151"/>
+    <mergeCell ref="B152:H152"/>
+    <mergeCell ref="A153:H153"/>
+    <mergeCell ref="A154:B154"/>
+    <mergeCell ref="A155:B155"/>
+    <mergeCell ref="A211:B211"/>
+    <mergeCell ref="A212:H212"/>
+    <mergeCell ref="A213:B213"/>
+    <mergeCell ref="F213:H213"/>
+    <mergeCell ref="A156:B156"/>
+    <mergeCell ref="A157:B157"/>
+    <mergeCell ref="A158:B158"/>
+    <mergeCell ref="A159:B159"/>
+    <mergeCell ref="A160:B160"/>
+    <mergeCell ref="A161:B161"/>
+    <mergeCell ref="A162:B162"/>
+    <mergeCell ref="A163:B163"/>
+    <mergeCell ref="A164:B164"/>
+    <mergeCell ref="A165:B165"/>
+    <mergeCell ref="A166:B166"/>
+    <mergeCell ref="A167:B167"/>
+    <mergeCell ref="A168:B168"/>
+    <mergeCell ref="A57:B57"/>
+    <mergeCell ref="A58:B58"/>
+    <mergeCell ref="A59:B59"/>
+    <mergeCell ref="A49:H49"/>
+    <mergeCell ref="F50:H50"/>
+    <mergeCell ref="A50:B50"/>
+    <mergeCell ref="A51:B51"/>
+    <mergeCell ref="F51:H51"/>
+    <mergeCell ref="B53:H53"/>
+    <mergeCell ref="B54:H54"/>
+    <mergeCell ref="A55:H55"/>
+    <mergeCell ref="A56:B56"/>
+    <mergeCell ref="B1:H1"/>
+    <mergeCell ref="B2:H2"/>
+    <mergeCell ref="A3:H3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A15:H15"/>
+    <mergeCell ref="F16:H16"/>
+    <mergeCell ref="F17:H17"/>
+    <mergeCell ref="F18:H18"/>
+    <mergeCell ref="F19:H19"/>
+    <mergeCell ref="F20:H20"/>
+    <mergeCell ref="B22:H22"/>
+    <mergeCell ref="B23:H23"/>
+    <mergeCell ref="A24:H24"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="A34:H34"/>
     <mergeCell ref="A35:B35"/>
     <mergeCell ref="F35:H35"/>
     <mergeCell ref="A36:B36"/>
@@ -33408,69 +33508,76 @@
     <mergeCell ref="A46:B46"/>
     <mergeCell ref="A47:B47"/>
     <mergeCell ref="A48:B48"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="A34:H34"/>
-    <mergeCell ref="F17:H17"/>
-    <mergeCell ref="F18:H18"/>
-    <mergeCell ref="F19:H19"/>
-    <mergeCell ref="F20:H20"/>
-    <mergeCell ref="B22:H22"/>
-    <mergeCell ref="B23:H23"/>
-    <mergeCell ref="A24:H24"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="B1:H1"/>
-    <mergeCell ref="B2:H2"/>
-    <mergeCell ref="A3:H3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A15:H15"/>
-    <mergeCell ref="F16:H16"/>
-    <mergeCell ref="A57:B57"/>
-    <mergeCell ref="A58:B58"/>
-    <mergeCell ref="A59:B59"/>
-    <mergeCell ref="A49:H49"/>
-    <mergeCell ref="F50:H50"/>
-    <mergeCell ref="A50:B50"/>
-    <mergeCell ref="A51:B51"/>
-    <mergeCell ref="F51:H51"/>
-    <mergeCell ref="B53:H53"/>
-    <mergeCell ref="B54:H54"/>
-    <mergeCell ref="A55:H55"/>
-    <mergeCell ref="A56:B56"/>
-    <mergeCell ref="A214:B214"/>
-    <mergeCell ref="F214:H214"/>
-    <mergeCell ref="B151:H151"/>
-    <mergeCell ref="B152:H152"/>
-    <mergeCell ref="A153:H153"/>
-    <mergeCell ref="A154:B154"/>
-    <mergeCell ref="A155:B155"/>
-    <mergeCell ref="A211:B211"/>
-    <mergeCell ref="A212:H212"/>
-    <mergeCell ref="A213:B213"/>
-    <mergeCell ref="F213:H213"/>
+    <mergeCell ref="B84:H84"/>
+    <mergeCell ref="B85:H85"/>
+    <mergeCell ref="F91:H91"/>
+    <mergeCell ref="A86:H86"/>
+    <mergeCell ref="A90:H90"/>
+    <mergeCell ref="B95:H95"/>
+    <mergeCell ref="A132:B132"/>
+    <mergeCell ref="B68:H68"/>
+    <mergeCell ref="B69:H69"/>
+    <mergeCell ref="A79:B79"/>
+    <mergeCell ref="A70:H70"/>
+    <mergeCell ref="A82:B82"/>
+    <mergeCell ref="F82:H82"/>
+    <mergeCell ref="A73:B73"/>
+    <mergeCell ref="A71:B71"/>
+    <mergeCell ref="A72:B72"/>
+    <mergeCell ref="A74:B74"/>
+    <mergeCell ref="A75:B75"/>
+    <mergeCell ref="A76:B76"/>
+    <mergeCell ref="A77:B77"/>
+    <mergeCell ref="A78:B78"/>
+    <mergeCell ref="A80:H80"/>
+    <mergeCell ref="A81:B81"/>
+    <mergeCell ref="F81:H81"/>
+    <mergeCell ref="A113:B113"/>
+    <mergeCell ref="A130:B130"/>
+    <mergeCell ref="A121:H121"/>
+    <mergeCell ref="F122:H122"/>
+    <mergeCell ref="F123:H123"/>
+    <mergeCell ref="B96:H96"/>
+    <mergeCell ref="A97:H97"/>
+    <mergeCell ref="A87:B87"/>
+    <mergeCell ref="A93:B93"/>
+    <mergeCell ref="F93:H93"/>
+    <mergeCell ref="A91:B91"/>
+    <mergeCell ref="F124:H124"/>
+    <mergeCell ref="B127:H127"/>
+    <mergeCell ref="B126:H126"/>
+    <mergeCell ref="A128:H128"/>
+    <mergeCell ref="A122:B122"/>
+    <mergeCell ref="F92:H92"/>
+    <mergeCell ref="A98:B98"/>
+    <mergeCell ref="A106:H106"/>
+    <mergeCell ref="A107:B107"/>
+    <mergeCell ref="F107:H107"/>
+    <mergeCell ref="F108:H108"/>
+    <mergeCell ref="A108:B108"/>
+    <mergeCell ref="B111:H111"/>
+    <mergeCell ref="A112:H112"/>
+    <mergeCell ref="F148:H148"/>
+    <mergeCell ref="A149:B149"/>
+    <mergeCell ref="F149:H149"/>
+    <mergeCell ref="A148:B148"/>
+    <mergeCell ref="A145:B145"/>
+    <mergeCell ref="A144:B144"/>
+    <mergeCell ref="A135:B135"/>
+    <mergeCell ref="A134:B134"/>
+    <mergeCell ref="A133:B133"/>
+    <mergeCell ref="A138:B138"/>
+    <mergeCell ref="A143:B143"/>
+    <mergeCell ref="A146:H146"/>
+    <mergeCell ref="A147:B147"/>
+    <mergeCell ref="F147:H147"/>
+    <mergeCell ref="F137:H137"/>
+    <mergeCell ref="F138:H138"/>
+    <mergeCell ref="B140:H140"/>
+    <mergeCell ref="B141:H141"/>
+    <mergeCell ref="A142:H142"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0" footer="0"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>